<commit_message>
Add Vapor Quality Estimates
</commit_message>
<xml_diff>
--- a/TheEngine/Regen Solver/enginefiles/solverdata.xlsx
+++ b/TheEngine/Regen Solver/enginefiles/solverdata.xlsx
@@ -438,10 +438,10 @@
         <v>300</v>
       </c>
       <c r="F2">
-        <v>5.040835337370684</v>
+        <v>4.905011801081626</v>
       </c>
       <c r="G2">
-        <v>0.003532888033379544</v>
+        <v>0.002849206603787273</v>
       </c>
       <c r="H2">
         <v>0.006542436735388365</v>
@@ -458,16 +458,16 @@
         <v>0.03093226317788614</v>
       </c>
       <c r="D3">
-        <v>3999788.486338295</v>
+        <v>3999776.610203336</v>
       </c>
       <c r="E3">
         <v>300.3344679217842</v>
       </c>
       <c r="F3">
-        <v>5.649609025434406</v>
+        <v>5.48904777647008</v>
       </c>
       <c r="G3">
-        <v>0.003297378786112454</v>
+        <v>0.002637155852782424</v>
       </c>
       <c r="H3">
         <v>0.005942060430261161</v>
@@ -484,16 +484,16 @@
         <v>0.03010170940624797</v>
       </c>
       <c r="D4">
-        <v>3999505.900342832</v>
+        <v>3999477.250081811</v>
       </c>
       <c r="E4">
-        <v>300.6909806555503</v>
+        <v>300.6909813421665</v>
       </c>
       <c r="F4">
-        <v>6.345518720237725</v>
+        <v>6.155198255148112</v>
       </c>
       <c r="G4">
-        <v>0.003077482031081337</v>
+        <v>0.002439013086187956</v>
       </c>
       <c r="H4">
         <v>0.005386125297889534</v>
@@ -510,16 +510,16 @@
         <v>0.02927115563460979</v>
       </c>
       <c r="D5">
-        <v>3999126.438486568</v>
+        <v>3999073.958072922</v>
       </c>
       <c r="E5">
-        <v>301.07156825841</v>
+        <v>301.071570713086</v>
       </c>
       <c r="F5">
-        <v>7.144114098599627</v>
+        <v>6.91781991444688</v>
       </c>
       <c r="G5">
-        <v>0.002872108554920986</v>
+        <v>0.002253751992788962</v>
       </c>
       <c r="H5">
         <v>0.00487171151677468</v>
@@ -536,16 +536,16 @@
         <v>0.02844060186297162</v>
       </c>
       <c r="D6">
-        <v>3998614.035712085</v>
+        <v>3998527.480723054</v>
       </c>
       <c r="E6">
-        <v>301.4785261166659</v>
+        <v>301.4785320338666</v>
       </c>
       <c r="F6">
-        <v>8.06443012130919</v>
+        <v>7.794417485639511</v>
       </c>
       <c r="G6">
-        <v>0.002680265574964297</v>
+        <v>0.00208042772103773</v>
       </c>
       <c r="H6">
         <v>0.004396092827715485</v>
@@ -562,16 +562,16 @@
         <v>0.02761004809133344</v>
       </c>
       <c r="D7">
-        <v>3997917.84504006</v>
+        <v>3997782.213071322</v>
       </c>
       <c r="E7">
-        <v>301.9144637466343</v>
+        <v>301.9144757798911</v>
       </c>
       <c r="F7">
-        <v>9.129969220319737</v>
+        <v>8.806511995106687</v>
       </c>
       <c r="G7">
-        <v>0.002501046060202221</v>
+        <v>0.001918165903864194</v>
       </c>
       <c r="H7">
         <v>0.00395671747536446</v>
@@ -588,16 +588,16 @@
         <v>0.02677949431969527</v>
       </c>
       <c r="D8">
-        <v>3996965.488309265</v>
+        <v>3996758.597779526</v>
       </c>
       <c r="E8">
-        <v>302.3823663347757</v>
+        <v>302.3823886517101</v>
       </c>
       <c r="F8">
-        <v>10.37003547117806</v>
+        <v>9.980814614497675</v>
       </c>
       <c r="G8">
-        <v>0.002333618114626467</v>
+        <v>0.001766151593049934</v>
       </c>
       <c r="H8">
         <v>0.003551189604397998</v>
@@ -614,16 +614,16 @@
         <v>0.02594894054805708</v>
       </c>
       <c r="D9">
-        <v>3995652.83329915</v>
+        <v>3995341.535888504</v>
       </c>
       <c r="E9">
-        <v>302.8856737675035</v>
+        <v>302.8857129513292</v>
       </c>
       <c r="F9">
-        <v>11.82158491569118</v>
+        <v>11.35084714915075</v>
       </c>
       <c r="G9">
-        <v>0.002177213420773393</v>
+        <v>0.001623617318988921</v>
       </c>
       <c r="H9">
         <v>0.003177250208647025</v>
@@ -640,16 +640,16 @@
         <v>0.02511838677641891</v>
       </c>
       <c r="D10">
-        <v>3993828.252450201</v>
+        <v>3993362.41360171</v>
       </c>
       <c r="E10">
-        <v>303.4283843955078</v>
+        <v>303.4284509301681</v>
       </c>
       <c r="F10">
-        <v>13.5318589028469</v>
+        <v>12.95923830117153</v>
       </c>
       <c r="G10">
-        <v>0.002031112905532949</v>
+        <v>0.001489828972181673</v>
       </c>
       <c r="H10">
         <v>0.002832756114070572</v>
@@ -666,16 +666,16 @@
         <v>0.02428783300478073</v>
       </c>
       <c r="D11">
-        <v>3991267.912800594</v>
+        <v>3990570.669999055</v>
       </c>
       <c r="E11">
-        <v>304.0151950650875</v>
+        <v>304.0153058213451</v>
       </c>
       <c r="F11">
-        <v>15.56225841974068</v>
+        <v>14.86108918561069</v>
       </c>
       <c r="G11">
-        <v>0.001894625951999882</v>
+        <v>0.001364067122881179</v>
       </c>
       <c r="H11">
         <v>0.002515654229479245</v>
@@ -692,16 +692,16 @@
         <v>0.02345727923314256</v>
       </c>
       <c r="D12">
-        <v>3987636.078068059</v>
+        <v>3986587.737230955</v>
       </c>
       <c r="E12">
-        <v>304.651696756907</v>
+        <v>304.651879230879</v>
       </c>
       <c r="F12">
-        <v>17.99430304286021</v>
+        <v>17.12913436781196</v>
       </c>
       <c r="G12">
-        <v>0.001767055152802872</v>
+        <v>0.001245598966604661</v>
       </c>
       <c r="H12">
         <v>0.002223945332654902</v>
@@ -718,16 +718,16 @@
         <v>0.02262672546150438</v>
       </c>
       <c r="D13">
-        <v>3982419.463321049</v>
+        <v>3980830.190098177</v>
       </c>
       <c r="E13">
-        <v>305.3446604478437</v>
+        <v>305.344960142939</v>
       </c>
       <c r="F13">
-        <v>20.93938267201884</v>
+        <v>19.86217358022127</v>
       </c>
       <c r="G13">
-        <v>0.001647627512501713</v>
+        <v>0.001133630102095071</v>
       </c>
       <c r="H13">
         <v>0.00195562434030411</v>
@@ -744,16 +744,16 @@
         <v>0.0217961716898662</v>
       </c>
       <c r="D14">
-        <v>3974814.497898826</v>
+        <v>3972376.499475443</v>
       </c>
       <c r="E14">
-        <v>306.1024805800348</v>
+        <v>306.102974195615</v>
       </c>
       <c r="F14">
-        <v>24.55624124562735</v>
+        <v>23.2001899087946</v>
       </c>
       <c r="G14">
-        <v>0.001535340876074028</v>
+        <v>0.001027208451763175</v>
       </c>
       <c r="H14">
         <v>0.001708562832462672</v>
@@ -770,16 +770,16 @@
         <v>0.02096561791822803</v>
       </c>
       <c r="D15">
-        <v>3963523.164127846</v>
+        <v>3959723.300935372</v>
       </c>
       <c r="E15">
-        <v>306.9359230914835</v>
+        <v>306.9367428490476</v>
       </c>
       <c r="F15">
-        <v>29.08714405484334</v>
+        <v>27.35569291313612</v>
       </c>
       <c r="G15">
-        <v>0.001428563271735044</v>
+        <v>0.0009249950203275085</v>
       </c>
       <c r="H15">
         <v>0.001480226068461778</v>
@@ -796,16 +796,16 @@
         <v>0.02013506414658983</v>
       </c>
       <c r="D16">
-        <v>3946351.594622796</v>
+        <v>3940301.324010564</v>
       </c>
       <c r="E16">
-        <v>307.8595557735988</v>
+        <v>307.8609362505192</v>
       </c>
       <c r="F16">
-        <v>34.95354815431989</v>
+        <v>32.69700460986854</v>
       </c>
       <c r="G16">
-        <v>0.001323712314616638</v>
+        <v>0.0008245508884374054</v>
       </c>
       <c r="H16">
         <v>0.001266772068834776</v>
@@ -822,16 +822,16 @@
         <v>0.01930451037495166</v>
       </c>
       <c r="D17">
-        <v>3919294.336879671</v>
+        <v>3909360.812148617</v>
       </c>
       <c r="E17">
-        <v>308.8951274506359</v>
+        <v>308.8975018887731</v>
       </c>
       <c r="F17">
-        <v>43.18312987453626</v>
+        <v>40.12263077154041</v>
       </c>
       <c r="G17">
-        <v>0.001208130966363585</v>
+        <v>0.0007185636239751408</v>
       </c>
       <c r="H17">
         <v>0.001058130323103295</v>
@@ -848,16 +848,16 @@
         <v>0.01956298682688029</v>
       </c>
       <c r="D18">
-        <v>3873527.193732539</v>
+        <v>3856291.151585984</v>
       </c>
       <c r="E18">
-        <v>310.0842419281285</v>
+        <v>310.0884696275555</v>
       </c>
       <c r="F18">
-        <v>54.6231150476366</v>
+        <v>50.37010396659633</v>
       </c>
       <c r="G18">
-        <v>0.0009149962371608305</v>
+        <v>0.0005577303174063409</v>
       </c>
       <c r="H18">
         <v>0.0008541012114779965</v>
@@ -874,16 +874,16 @@
         <v>0.02135258148578198</v>
       </c>
       <c r="D19">
-        <v>3774472.645283897</v>
+        <v>3739606.498871365</v>
       </c>
       <c r="E19">
-        <v>311.5797803864489</v>
+        <v>311.5879780933276</v>
       </c>
       <c r="F19">
-        <v>48.04341102675494</v>
+        <v>44.62441060095711</v>
       </c>
       <c r="G19">
-        <v>0.0008141063899768637</v>
+        <v>0.000542265367818076</v>
       </c>
       <c r="H19">
         <v>0.0009463339455950721</v>
@@ -900,16 +900,16 @@
         <v>0.0231421761446837</v>
       </c>
       <c r="D20">
-        <v>3694134.154790155</v>
+        <v>3646202.960067133</v>
       </c>
       <c r="E20">
-        <v>313.0757795762041</v>
+        <v>313.0917013012407</v>
       </c>
       <c r="F20">
-        <v>41.5007411515905</v>
+        <v>38.82946300048378</v>
       </c>
       <c r="G20">
-        <v>0.0007732480305737462</v>
+        <v>0.0005471647209861363</v>
       </c>
       <c r="H20">
         <v>0.001069404477373927</v>
@@ -926,16 +926,16 @@
         <v>0.02493177080358538</v>
       </c>
       <c r="D21">
-        <v>3633223.360633792</v>
+        <v>3576350.577169761</v>
       </c>
       <c r="E21">
-        <v>314.5288752483295</v>
+        <v>314.5547995954685</v>
       </c>
       <c r="F21">
-        <v>35.96835522084915</v>
+        <v>33.86687367475206</v>
       </c>
       <c r="G21">
-        <v>0.0007561417470730942</v>
+        <v>0.0005592877113105684</v>
       </c>
       <c r="H21">
         <v>0.001208072179267094</v>
@@ -952,16 +952,16 @@
         <v>0.0267213654624871</v>
       </c>
       <c r="D22">
-        <v>3587435.028487478</v>
+        <v>3524470.394304341</v>
       </c>
       <c r="E22">
-        <v>315.9282649509464</v>
+        <v>315.9653647690192</v>
       </c>
       <c r="F22">
-        <v>31.39265900094465</v>
+        <v>29.71775728473478</v>
       </c>
       <c r="G22">
-        <v>0.0007516923140763166</v>
+        <v>0.0005751899114771566</v>
       </c>
       <c r="H22">
         <v>0.001358867032755786</v>
@@ -978,16 +978,16 @@
         <v>0.02851096012138879</v>
       </c>
       <c r="D23">
-        <v>3552853.463419101</v>
+        <v>3485689.213575249</v>
       </c>
       <c r="E23">
-        <v>317.2717931488573</v>
+        <v>317.3205769244773</v>
       </c>
       <c r="F23">
-        <v>27.60739522054747</v>
+        <v>26.25397418616662</v>
       </c>
       <c r="G23">
-        <v>0.0007548882371209399</v>
+        <v>0.0005933740930978196</v>
       </c>
       <c r="H23">
         <v>0.001520395727963033</v>
@@ -1004,16 +1004,16 @@
         <v>0.03030055478029048</v>
       </c>
       <c r="D24">
-        <v>3526496.956113954</v>
+        <v>3456389.216803909</v>
       </c>
       <c r="E24">
-        <v>318.5606673611311</v>
+        <v>318.6212618077764</v>
       </c>
       <c r="F24">
-        <v>24.45609158723162</v>
+        <v>23.34808244128254</v>
       </c>
       <c r="G24">
-        <v>0.0007630690794737898</v>
+        <v>0.00061304773703215</v>
       </c>
       <c r="H24">
         <v>0.001691941174899729</v>
@@ -1030,16 +1030,16 @@
         <v>0.03209014943919218</v>
       </c>
       <c r="D25">
-        <v>3506195.322731551</v>
+        <v>3433987.903630811</v>
       </c>
       <c r="E25">
-        <v>319.797491043022</v>
+        <v>319.8698074957406</v>
       </c>
       <c r="F25">
-        <v>21.81122528056344</v>
+        <v>20.89323199552232</v>
       </c>
       <c r="G25">
-        <v>0.000774677808468018</v>
+        <v>0.0006337430556593427</v>
       </c>
       <c r="H25">
         <v>0.001873074068597041</v>
@@ -1056,16 +1056,16 @@
         <v>0.03387974409809387</v>
       </c>
       <c r="D26">
-        <v>3490386.555014883</v>
+        <v>3416655.380971263</v>
       </c>
       <c r="E26">
-        <v>320.9853916464118</v>
+        <v>321.0692225956166</v>
       </c>
       <c r="F26">
-        <v>19.57273901108171</v>
+        <v>18.80392174771049</v>
       </c>
       <c r="G26">
-        <v>0.0007887392606650493</v>
+        <v>0.0006551638035196973</v>
       </c>
       <c r="H26">
         <v>0.002063509283295386</v>
@@ -1082,16 +1082,16 @@
         <v>0.03566933875699557</v>
       </c>
       <c r="D27">
-        <v>3477944.800944505</v>
+        <v>3403089.676003241</v>
       </c>
       <c r="E27">
-        <v>322.1276068153537</v>
+        <v>322.2226820445551</v>
       </c>
       <c r="F27">
-        <v>17.66280112036845</v>
+        <v>17.0126280416103</v>
       </c>
       <c r="G27">
-        <v>0.0008046109182510157</v>
+        <v>0.0006771127808027774</v>
       </c>
       <c r="H27">
         <v>0.002263042612275085</v>
@@ -1108,16 +1108,16 @@
         <v>0.03745893341589727</v>
       </c>
       <c r="D28">
-        <v>3468053.079261593</v>
+        <v>3392356.229944909</v>
       </c>
       <c r="E28">
-        <v>323.2272856879708</v>
+        <v>323.333305095259</v>
       </c>
       <c r="F28">
-        <v>16.0207474640868</v>
+        <v>15.46607156678846</v>
       </c>
       <c r="G28">
-        <v>0.0008218522709723224</v>
+        <v>0.0006994537009999353</v>
       </c>
       <c r="H28">
         <v>0.0024715192954805</v>
@@ -1134,16 +1134,16 @@
         <v>0.03924852807479898</v>
       </c>
       <c r="D29">
-        <v>3460113.123739185</v>
+        <v>3383776.991143041</v>
       </c>
       <c r="E29">
-        <v>324.2873975200711</v>
+        <v>324.4040503517729</v>
       </c>
       <c r="F29">
-        <v>14.59899709777522</v>
+        <v>14.12203395015133</v>
       </c>
       <c r="G29">
-        <v>0.0008401514358449833</v>
+        <v>0.0007220895634491635</v>
       </c>
       <c r="H29">
         <v>0.002688816871064464</v>
@@ -1160,16 +1160,16 @@
         <v>0.04103812273370067</v>
       </c>
       <c r="D30">
-        <v>3453682.410733139</v>
+        <v>3376854.409963838</v>
       </c>
       <c r="E30">
-        <v>325.3106954656657</v>
+        <v>325.4376715317665</v>
       </c>
       <c r="F30">
-        <v>13.35993195857892</v>
+        <v>12.94684529119103</v>
       </c>
       <c r="G30">
-        <v>0.0008592816403678695</v>
+        <v>0.0007449496695258027</v>
       </c>
       <c r="H30">
         <v>0.00291483514110167</v>
@@ -1186,16 +1186,16 @@
         <v>0.04282771739260237</v>
       </c>
       <c r="D31">
-        <v>3448430.236319737</v>
+        <v>3371219.234501278</v>
       </c>
       <c r="E31">
-        <v>326.29970887587</v>
+        <v>326.4367049772629</v>
       </c>
       <c r="F31">
-        <v>12.27355636724148</v>
+        <v>11.91345590160809</v>
       </c>
       <c r="G31">
-        <v>0.000879074253912427</v>
+        <v>0.0007679814720056848</v>
       </c>
       <c r="H31">
         <v>0.003149489950879344</v>
@@ -1212,16 +1212,16 @@
         <v>0.04461731205150407</v>
       </c>
       <c r="D32">
-        <v>3444106.942608105</v>
+        <v>3366594.398878599</v>
       </c>
       <c r="E32">
-        <v>327.2567500517925</v>
+        <v>327.4034735212522</v>
       </c>
       <c r="F32">
-        <v>11.31574792202437</v>
+        <v>10.99996968058679</v>
       </c>
       <c r="G32">
-        <v>0.0008994014512016542</v>
+        <v>0.0007911452699057156</v>
       </c>
       <c r="H32">
         <v>0.003392709143079871</v>
@@ -1238,16 +1238,16 @@
         <v>0.04640690671040576</v>
       </c>
       <c r="D33">
-        <v>3440522.196563589</v>
+        <v>3362769.808796308</v>
       </c>
       <c r="E33">
-        <v>328.1839278851081</v>
+        <v>328.3400983788061</v>
       </c>
       <c r="F33">
-        <v>10.46694656193384</v>
+        <v>10.18852916063212</v>
       </c>
       <c r="G33">
-        <v>0.0009201647164938942</v>
+        <v>0.0008144106499937629</v>
       </c>
       <c r="H33">
         <v>0.003644429817577348</v>
@@ -1264,16 +1264,16 @@
         <v>0.04819650136930748</v>
       </c>
       <c r="D34">
-        <v>3437529.52262989</v>
+        <v>3359584.553136025</v>
       </c>
       <c r="E34">
-        <v>329.0831642921338</v>
+        <v>329.2485145205685</v>
       </c>
       <c r="F34">
-        <v>9.711166114824609</v>
+        <v>9.464464807376389</v>
       </c>
       <c r="G34">
-        <v>0.0009412870146493105</v>
+        <v>0.0008377540383665035</v>
       </c>
       <c r="H34">
         <v>0.003904596410081231</v>
@@ -1290,16 +1290,16 @@
         <v>0.04998609602820916</v>
       </c>
       <c r="D35">
-        <v>3435015.18424392</v>
+        <v>3356914.220354675</v>
       </c>
       <c r="E35">
-        <v>329.9562112454624</v>
+        <v>330.1304870661394</v>
       </c>
       <c r="F35">
-        <v>9.035243426458154</v>
+        <v>8.815642231719297</v>
       </c>
       <c r="G35">
-        <v>0.0009627073341337943</v>
+        <v>0.0008611569784819222</v>
       </c>
       <c r="H35">
         <v>0.004173159303741212</v>
@@ -1316,16 +1316,16 @@
         <v>0.05177569068711085</v>
       </c>
       <c r="D36">
-        <v>3432890.114421577</v>
+        <v>3354661.758579374</v>
       </c>
       <c r="E36">
-        <v>330.8046672602125</v>
+        <v>330.9876273933657</v>
       </c>
       <c r="F36">
-        <v>8.428263357134931</v>
+        <v>8.231957904509787</v>
       </c>
       <c r="G36">
-        <v>0.0009843768048463061</v>
+        <v>0.0008846048967679329</v>
       </c>
       <c r="H36">
         <v>0.004450073799171029</v>
@@ -1342,16 +1342,16 @@
         <v>0.05356528534601257</v>
       </c>
       <c r="D37">
-        <v>3431084.003308685</v>
+        <v>3352750.821016089</v>
       </c>
       <c r="E37">
-        <v>331.6299927797102</v>
+        <v>331.8214083096973</v>
       </c>
       <c r="F37">
-        <v>7.881114832467551</v>
+        <v>7.704946808533583</v>
       </c>
       <c r="G37">
-        <v>0.001006255885791332</v>
+        <v>0.0009080862027412731</v>
       </c>
       <c r="H37">
         <v>0.004735299332450548</v>
@@ -1368,16 +1368,16 @@
         <v>0.05535488000491426</v>
       </c>
       <c r="D38">
-        <v>3429540.92577199</v>
+        <v>3351120.872404031</v>
       </c>
       <c r="E38">
-        <v>332.433524232551</v>
+        <v>332.6331779963685</v>
       </c>
       <c r="F38">
-        <v>7.386145293850942</v>
+        <v>7.227474970243511</v>
       </c>
       <c r="G38">
-        <v>0.00102831229451356</v>
+        <v>0.00093159162311481</v>
       </c>
       <c r="H38">
         <v>0.005028798869115337</v>
@@ -1394,16 +1394,16 @@
         <v>0.05714447466381595</v>
       </c>
       <c r="D39">
-        <v>3428216.078778824</v>
+        <v>3349723.555996133</v>
       </c>
       <c r="E39">
-        <v>333.2164867122806</v>
+        <v>333.4241726383011</v>
       </c>
       <c r="F39">
-        <v>6.936889617024696</v>
+        <v>6.793496784176314</v>
       </c>
       <c r="G39">
-        <v>0.001050519460240233</v>
+        <v>0.0009551137023758545</v>
       </c>
       <c r="H39">
         <v>0.005330538425664675</v>
@@ -1420,16 +1420,16 @@
         <v>0.05893406932271766</v>
       </c>
       <c r="D40">
-        <v>3427073.325831586</v>
+        <v>3348519.971708253</v>
       </c>
       <c r="E40">
-        <v>333.9800053258336</v>
+        <v>334.1955277616438</v>
       </c>
       <c r="F40">
-        <v>6.527855836186812</v>
+        <v>6.397862140337804</v>
       </c>
       <c r="G40">
-        <v>0.001072855353048263</v>
+        <v>0.0009786464237734201</v>
       </c>
       <c r="H40">
         <v>0.00564048668604419</v>
@@ -1446,16 +1446,16 @@
         <v>0.06072366398161935</v>
       </c>
       <c r="D41">
-        <v>3426083.333528778</v>
+        <v>3347478.619170708</v>
       </c>
       <c r="E41">
-        <v>334.7251153034298</v>
+        <v>334.9482883562499</v>
       </c>
       <c r="F41">
-        <v>6.154354542821734</v>
+        <v>6.036162103601146</v>
       </c>
       <c r="G41">
-        <v>0.001095301586792289</v>
+        <v>0.001002184918368445</v>
       </c>
       <c r="H41">
         <v>0.005958614688860019</v>
@@ -1472,16 +1472,16 @@
         <v>0.06251325864052105</v>
       </c>
       <c r="D42">
-        <v>3425222.1462981</v>
+        <v>3346573.830401494</v>
       </c>
       <c r="E42">
-        <v>335.4527709820812</v>
+        <v>335.6834178854317</v>
       </c>
       <c r="F42">
-        <v>5.812362117588775</v>
+        <v>5.704604640569664</v>
       </c>
       <c r="G42">
-        <v>0.00111784272437835</v>
+        <v>0.001025725239597351</v>
       </c>
       <c r="H42">
         <v>0.006284895569669207</v>
@@ -1498,16 +1498,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D43">
-        <v>3424470.088058893</v>
+        <v>3345784.566173799</v>
       </c>
       <c r="E43">
-        <v>336.1638537788124</v>
+        <v>336.401806292841</v>
       </c>
       <c r="F43">
-        <v>5.646975330257583</v>
+        <v>5.54436997722534</v>
       </c>
       <c r="G43">
-        <v>0.001128082524443627</v>
+        <v>0.001036638150099113</v>
       </c>
       <c r="H43">
         <v>0.006468277148910672</v>
@@ -1524,16 +1524,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D44">
-        <v>3423861.199129451</v>
+        <v>3345145.874705372</v>
       </c>
       <c r="E44">
-        <v>336.8661814718685</v>
+        <v>337.1113512771659</v>
       </c>
       <c r="F44">
-        <v>5.671475516610466</v>
+        <v>5.568675918974766</v>
       </c>
       <c r="G44">
-        <v>0.001123161165886009</v>
+        <v>0.001032067158003627</v>
       </c>
       <c r="H44">
         <v>0.006468277148910672</v>
@@ -1550,16 +1550,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D45">
-        <v>3423244.433631697</v>
+        <v>3344498.817383963</v>
       </c>
       <c r="E45">
-        <v>337.5685654364324</v>
+        <v>337.8209544012248</v>
       </c>
       <c r="F45">
-        <v>5.696188783424006</v>
+        <v>5.593195682262315</v>
       </c>
       <c r="G45">
-        <v>0.001118239694545118</v>
+        <v>0.00102749601242939</v>
       </c>
       <c r="H45">
         <v>0.006468277148910672</v>
@@ -1576,16 +1576,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D46">
-        <v>3422619.653879727</v>
+        <v>3343843.246173757</v>
       </c>
       <c r="E46">
-        <v>338.2710063936146</v>
+        <v>338.5306164193937</v>
       </c>
       <c r="F46">
-        <v>5.721117943236465</v>
+        <v>5.617932122011637</v>
       </c>
       <c r="G46">
-        <v>0.001113318103783921</v>
+        <v>0.001022924706966759</v>
       </c>
       <c r="H46">
         <v>0.006468277148910672</v>
@@ -1602,16 +1602,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D47">
-        <v>3421986.719145086</v>
+        <v>3343179.009727658</v>
       </c>
       <c r="E47">
-        <v>338.9735050769862</v>
+        <v>339.2403380992432</v>
       </c>
       <c r="F47">
-        <v>5.746265858655887</v>
+        <v>5.642888144558273</v>
       </c>
       <c r="G47">
-        <v>0.001108396386851186</v>
+        <v>0.001018353235094684</v>
       </c>
       <c r="H47">
         <v>0.006468277148910672</v>
@@ -1628,16 +1628,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D48">
-        <v>3421345.485575247</v>
+        <v>3342505.95329748</v>
       </c>
       <c r="E48">
-        <v>339.6760622328501</v>
+        <v>339.9501202218298</v>
       </c>
       <c r="F48">
-        <v>5.771635443486542</v>
+        <v>5.668066708819723</v>
       </c>
       <c r="G48">
-        <v>0.001103474536879033</v>
+        <v>0.001013781590178275</v>
       </c>
       <c r="H48">
         <v>0.006468277148910672</v>
@@ -1654,16 +1654,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D49">
-        <v>3420695.806109505</v>
+        <v>3341823.918641261</v>
       </c>
       <c r="E49">
-        <v>340.37867862052</v>
+        <v>340.6599635819945</v>
       </c>
       <c r="F49">
-        <v>5.797229663886126</v>
+        <v>5.693470827497718</v>
       </c>
       <c r="G49">
-        <v>0.001098552546880421</v>
+        <v>0.001009209765466342</v>
       </c>
       <c r="H49">
         <v>0.006468277148910672</v>
@@ -1680,16 +1680,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D50">
-        <v>3420037.530392215</v>
+        <v>3341132.7439276</v>
       </c>
       <c r="E50">
-        <v>341.0813550126065</v>
+        <v>341.36986898867</v>
       </c>
       <c r="F50">
-        <v>5.823051539554686</v>
+        <v>5.719103568313937</v>
       </c>
       <c r="G50">
-        <v>0.001093630409746566</v>
+        <v>0.001004637754088823</v>
       </c>
       <c r="H50">
         <v>0.006468277148910672</v>
@@ -1706,16 +1706,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D51">
-        <v>3419370.504683257</v>
+        <v>3340432.263636915</v>
       </c>
       <c r="E51">
-        <v>341.784092195311</v>
+        <v>342.0798372651959</v>
       </c>
       <c r="F51">
-        <v>5.849104144956302</v>
+        <v>5.744968055280063</v>
       </c>
       <c r="G51">
-        <v>0.001088708118244292</v>
+        <v>0.001000065549054182</v>
       </c>
       <c r="H51">
         <v>0.006468277148910672</v>
@@ -1732,16 +1732,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D52">
-        <v>3418694.571765632</v>
+        <v>3339722.308459487</v>
       </c>
       <c r="E52">
-        <v>342.4868909687273</v>
+        <v>342.789869249642</v>
       </c>
       <c r="F52">
-        <v>5.875390610574518</v>
+        <v>5.771067470003406</v>
       </c>
       <c r="G52">
-        <v>0.001083785665013317</v>
+        <v>0.0009954931432467218</v>
       </c>
       <c r="H52">
         <v>0.006468277148910672</v>
@@ -1758,16 +1758,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D53">
-        <v>3418009.570850095</v>
+        <v>3339002.705190194</v>
       </c>
       <c r="E53">
-        <v>343.1897521471511</v>
+        <v>343.4999657951416</v>
       </c>
       <c r="F53">
-        <v>5.901914124202739</v>
+        <v>5.797405053029354</v>
       </c>
       <c r="G53">
-        <v>0.001078863042563462</v>
+        <v>0.0009909205294238179</v>
       </c>
       <c r="H53">
         <v>0.006468277148910672</v>
@@ -1784,16 +1784,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D54">
-        <v>3417315.33747669</v>
+        <v>3338273.276619792</v>
       </c>
       <c r="E54">
-        <v>343.8926765593985</v>
+        <v>344.2101277702324</v>
       </c>
       <c r="F54">
-        <v>5.928677932270616</v>
+        <v>5.823984105221584</v>
       </c>
       <c r="G54">
-        <v>0.001073940243271792</v>
+        <v>0.0009863477002130957</v>
       </c>
       <c r="H54">
         <v>0.006468277148910672</v>
@@ -1810,16 +1810,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D55">
-        <v>3416611.703413099</v>
+        <v>3337533.841422617</v>
       </c>
       <c r="E55">
-        <v>344.5956650491327</v>
+        <v>344.9203560592078</v>
       </c>
       <c r="F55">
-        <v>5.955685341207746</v>
+        <v>5.850807989181658</v>
       </c>
       <c r="G55">
-        <v>0.001069017259379669</v>
+        <v>0.0009817746481095202</v>
       </c>
       <c r="H55">
         <v>0.006468277148910672</v>
@@ -1836,16 +1836,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D56">
-        <v>3415898.496549666</v>
+        <v>3336784.214040587</v>
       </c>
       <c r="E56">
-        <v>345.2987184751992</v>
+        <v>345.6306515624777</v>
       </c>
       <c r="F56">
-        <v>5.982939718845768</v>
+        <v>5.877880130709041</v>
       </c>
       <c r="G56">
-        <v>0.001064094082989743</v>
+        <v>0.00097720136547241</v>
       </c>
       <c r="H56">
         <v>0.006468277148910672</v>
@@ -1862,16 +1862,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D57">
-        <v>3415175.540790979</v>
+        <v>3336024.204563329</v>
       </c>
       <c r="E57">
-        <v>346.0018377119714</v>
+        <v>346.3410151969389</v>
       </c>
       <c r="F57">
-        <v>6.010444495860226</v>
+        <v>5.905204020303027</v>
       </c>
       <c r="G57">
-        <v>0.00105917070606285</v>
+        <v>0.0009726278445223701</v>
       </c>
       <c r="H57">
         <v>0.006468277148910672</v>
@@ -1888,16 +1888,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D58">
-        <v>3414442.655943872</v>
+        <v>3335253.618604323</v>
       </c>
       <c r="E58">
-        <v>346.7050236497041</v>
+        <v>347.0514478963564</v>
       </c>
       <c r="F58">
-        <v>6.03820316725352</v>
+        <v>5.932783214707966</v>
       </c>
       <c r="G58">
-        <v>0.001054247120414831</v>
+        <v>0.0009680540773381412</v>
       </c>
       <c r="H58">
         <v>0.006468277148910672</v>
@@ -1914,16 +1914,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D59">
-        <v>3413699.65760173</v>
+        <v>3334472.257172881</v>
       </c>
       <c r="E59">
-        <v>347.4082771948982</v>
+        <v>347.7619506117549</v>
       </c>
       <c r="F59">
-        <v>6.066219293880318</v>
+        <v>5.960621338503279</v>
       </c>
       <c r="G59">
-        <v>0.001049323317713263</v>
+        <v>0.0009634800558533623</v>
       </c>
       <c r="H59">
         <v>0.006468277148910672</v>
@@ -1940,16 +1940,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D60">
-        <v>3412946.357024928</v>
+        <v>3333679.916541805</v>
       </c>
       <c r="E60">
-        <v>348.1115992706744</v>
+        <v>348.4725243118212</v>
       </c>
       <c r="F60">
-        <v>6.094496504016807</v>
+        <v>5.988722085739762</v>
       </c>
       <c r="G60">
-        <v>0.001044399289474104</v>
+        <v>0.0009589057718532379</v>
       </c>
       <c r="H60">
         <v>0.006468277148910672</v>
@@ -1966,16 +1966,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D61">
-        <v>3412182.561017275</v>
+        <v>3332876.388110569</v>
       </c>
       <c r="E61">
-        <v>348.8149908171585</v>
+        <v>349.1831699833191</v>
       </c>
       <c r="F61">
-        <v>6.123038494975364</v>
+        <v>6.017089221623735</v>
       </c>
       <c r="G61">
-        <v>0.001039475027058243</v>
+        <v>0.0009543312169711334</v>
       </c>
       <c r="H61">
         <v>0.006468277148910672</v>
@@ -1992,16 +1992,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D62">
-        <v>3411408.071798308</v>
+        <v>3332061.458263829</v>
       </c>
       <c r="E62">
-        <v>349.5184527918761</v>
+        <v>349.8938886315144</v>
       </c>
       <c r="F62">
-        <v>6.151849034766138</v>
+        <v>6.045726584250832</v>
       </c>
       <c r="G62">
-        <v>0.001034550521667954</v>
+        <v>0.0009497563826850454</v>
       </c>
       <c r="H62">
         <v>0.006468277148910672</v>
@@ -2018,16 +2018,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D63">
-        <v>3410622.686871263</v>
+        <v>3331234.908225097</v>
       </c>
       <c r="E63">
-        <v>350.2219861701599</v>
+        <v>350.6046812806129</v>
       </c>
       <c r="F63">
-        <v>6.180931963807151</v>
+        <v>6.074638086390945</v>
       </c>
       <c r="G63">
-        <v>0.001029625764343261</v>
+        <v>0.0009451812603139994</v>
       </c>
       <c r="H63">
         <v>0.006468277148910672</v>
@@ -2044,16 +2044,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D64">
-        <v>3409826.198886561</v>
+        <v>3330396.513905375</v>
       </c>
       <c r="E64">
-        <v>350.925591945567</v>
+        <v>351.3155489742116</v>
       </c>
       <c r="F64">
-        <v>6.210291196684588</v>
+        <v>6.10382771732628</v>
       </c>
       <c r="G64">
-        <v>0.001024700745958189</v>
+        <v>0.0009406058410143347</v>
       </c>
       <c r="H64">
         <v>0.006468277148910672</v>
@@ -2070,16 +2070,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D65">
-        <v>3409018.395500643</v>
+        <v>3329546.045746549</v>
       </c>
       <c r="E65">
-        <v>351.6292711303096</v>
+        <v>352.0264927757615</v>
       </c>
       <c r="F65">
-        <v>6.239930723965037</v>
+        <v>6.133299544744305</v>
       </c>
       <c r="G65">
-        <v>0.001019775457216926</v>
+        <v>0.0009360301157758852</v>
       </c>
       <c r="H65">
         <v>0.006468277148910672</v>
@@ -2096,16 +2096,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D66">
-        <v>3408199.059229947</v>
+        <v>3328683.268559345</v>
       </c>
       <c r="E66">
-        <v>352.3330247556966</v>
+        <v>352.7375137690448</v>
       </c>
       <c r="F66">
-        <v>6.269854614061494</v>
+        <v>6.163057716687503</v>
       </c>
       <c r="G66">
-        <v>0.001014849888649857</v>
+        <v>0.0009314540754180523</v>
       </c>
       <c r="H66">
         <v>0.006468277148910672</v>
@@ -2122,16 +2122,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D67">
-        <v>3407367.967299861</v>
+        <v>3327807.941355614</v>
       </c>
       <c r="E67">
-        <v>353.0368538725891</v>
+        <v>353.4486130586656</v>
       </c>
       <c r="F67">
-        <v>6.300067015154909</v>
+        <v>6.193106463562032</v>
       </c>
       <c r="G67">
-        <v>0.001009924030609516</v>
+        <v>0.000926877710585768</v>
       </c>
       <c r="H67">
         <v>0.006468277148910672</v>
@@ -2148,16 +2148,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D68">
-        <v>3406524.891488431</v>
+        <v>3326919.817174727</v>
       </c>
       <c r="E68">
-        <v>353.7407595518679</v>
+        <v>354.1597917705553</v>
       </c>
       <c r="F68">
-        <v>6.330572157173423</v>
+        <v>6.223450100207266</v>
       </c>
       <c r="G68">
-        <v>0.001004997873266385</v>
+        <v>0.0009223010117453402</v>
       </c>
       <c r="H68">
         <v>0.006468277148910672</v>
@@ -2174,16 +2174,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D69">
-        <v>3405669.597964626</v>
+        <v>3326018.642903836</v>
       </c>
       <c r="E69">
-        <v>354.444742884916</v>
+        <v>354.8710510524924</v>
       </c>
       <c r="F69">
-        <v>6.361374353831108</v>
+        <v>6.25409302802852</v>
       </c>
       <c r="G69">
-        <v>0.001000071406604619</v>
+        <v>0.0009177239691801812</v>
       </c>
       <c r="H69">
         <v>0.006468277148910672</v>
@@ -2200,16 +2200,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D70">
-        <v>3404801.847120934</v>
+        <v>3325104.159091754</v>
       </c>
       <c r="E70">
-        <v>355.1488049841132</v>
+        <v>355.5823920746376</v>
       </c>
       <c r="F70">
-        <v>6.392478004728508</v>
+        <v>6.285039737195116</v>
       </c>
       <c r="G70">
-        <v>0.0009951446204176019</v>
+        <v>0.0009131465729864106</v>
       </c>
       <c r="H70">
         <v>0.006468277148910672</v>
@@ -2226,16 +2226,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D71">
-        <v>3403921.393400068</v>
+        <v>3324176.099756186</v>
       </c>
       <c r="E71">
-        <v>355.8529469833471</v>
+        <v>356.2938160300857</v>
       </c>
       <c r="F71">
-        <v>6.423887597517061</v>
+        <v>6.316294808906246</v>
       </c>
       <c r="G71">
-        <v>0.0009902175043034177</v>
+        <v>0.0009085688130683294</v>
       </c>
       <c r="H71">
         <v>0.006468277148910672</v>
@@ -2252,16 +2252,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D72">
-        <v>3403027.985115532</v>
+        <v>3323234.192184047</v>
       </c>
       <c r="E72">
-        <v>356.5571700385382</v>
+        <v>357.0053241354327</v>
       </c>
       <c r="F72">
-        <v>6.455607710129782</v>
+        <v>6.347862917727046</v>
       </c>
       <c r="G72">
-        <v>0.0009852900476601577</v>
+        <v>0.0009039906791337652</v>
       </c>
       <c r="H72">
         <v>0.006468277148910672</v>
@@ -2278,16 +2278,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D73">
-        <v>3402121.364265801</v>
+        <v>3322278.156724571</v>
       </c>
       <c r="E73">
-        <v>357.2614753281806</v>
+        <v>357.716917631361</v>
       </c>
       <c r="F73">
-        <v>6.487643013080545</v>
+        <v>6.37974883399744</v>
       </c>
       <c r="G73">
-        <v>0.0009803622396811194</v>
+        <v>0.000899412160689279</v>
       </c>
       <c r="H73">
         <v>0.006468277148910672</v>
@@ -2304,16 +2304,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D74">
-        <v>3401201.266341854</v>
+        <v>3321307.706574913</v>
       </c>
       <c r="E74">
-        <v>357.9658640538987</v>
+        <v>358.4285977832414</v>
       </c>
       <c r="F74">
-        <v>6.519998271834464</v>
+        <v>6.411957426316483</v>
       </c>
       <c r="G74">
-        <v>0.0009754340693498417</v>
+        <v>0.0008948332470352343</v>
       </c>
       <c r="H74">
         <v>0.006468277148910672</v>
@@ -2330,16 +2330,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D75">
-        <v>3400267.420127783</v>
+        <v>3320322.547557929</v>
       </c>
       <c r="E75">
-        <v>358.6703374410209</v>
+        <v>359.1403658817539</v>
       </c>
       <c r="F75">
-        <v>6.552678349252003</v>
+        <v>6.444493664104918</v>
       </c>
       <c r="G75">
-        <v>0.0009705055254350116</v>
+        <v>0.0008902539272607106</v>
       </c>
       <c r="H75">
         <v>0.006468277148910672</v>
@@ -2356,16 +2356,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D76">
-        <v>3399319.547494187</v>
+        <v>3319322.377891812</v>
       </c>
       <c r="E76">
-        <v>359.3748967391704</v>
+        <v>359.8522232435273</v>
       </c>
       <c r="F76">
-        <v>6.585688208109428</v>
+        <v>6.477362620248942</v>
       </c>
       <c r="G76">
-        <v>0.0009655765964852125</v>
+        <v>0.0008856741902382743</v>
       </c>
       <c r="H76">
         <v>0.006468277148910672</v>
@@ -2382,16 +2382,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D77">
-        <v>3398357.363184062</v>
+        <v>3318306.887951222</v>
       </c>
       <c r="E77">
-        <v>360.0795432228737</v>
+        <v>360.5641712117983</v>
       </c>
       <c r="F77">
-        <v>6.619032913698535</v>
+        <v>6.510569473828069</v>
       </c>
       <c r="G77">
-        <v>0.0009606472708235267</v>
+        <v>0.0008810940246185995</v>
       </c>
       <c r="H77">
         <v>0.006468277148910681</v>
@@ -2408,16 +2408,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D78">
-        <v>3397380.574590846</v>
+        <v>3317275.760019564</v>
       </c>
       <c r="E78">
-        <v>360.7842781921876</v>
+        <v>361.2762111570909</v>
       </c>
       <c r="F78">
-        <v>6.652717636508519</v>
+        <v>6.544119512930488</v>
       </c>
       <c r="G78">
-        <v>0.0009557175365419666</v>
+        <v>0.0008765134188249018</v>
       </c>
       <c r="H78">
         <v>0.006468277148910681</v>
@@ -2434,16 +2434,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D79">
-        <v>3396388.881528321</v>
+        <v>3316228.668032021</v>
       </c>
       <c r="E79">
-        <v>361.4891029733456</v>
+        <v>361.9883444779169</v>
       </c>
       <c r="F79">
-        <v>6.686747654993023</v>
+        <v>6.578018137558922</v>
       </c>
       <c r="G79">
-        <v>0.0009507873814957453</v>
+        <v>0.000871932361047239</v>
       </c>
       <c r="H79">
         <v>0.006468277148910681</v>
@@ -2460,16 +2460,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D80">
-        <v>3395381.975991998</v>
+        <v>3315165.277308962</v>
       </c>
       <c r="E80">
-        <v>362.1940189194237</v>
+        <v>362.700572601498</v>
       </c>
       <c r="F80">
-        <v>6.721128358425659</v>
+        <v>6.612270862630695</v>
       </c>
       <c r="G80">
-        <v>0.0009458567932973814</v>
+        <v>0.0008673508392366054</v>
       </c>
       <c r="H80">
         <v>0.006468277148910681</v>
@@ -2486,16 +2486,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D81">
-        <v>3394359.541911634</v>
+        <v>3314085.244279277</v>
       </c>
       <c r="E81">
-        <v>362.8990274110273</v>
+        <v>363.4128969845111</v>
       </c>
       <c r="F81">
-        <v>6.755865249847219</v>
+        <v>6.646883321075436</v>
       </c>
       <c r="G81">
-        <v>0.0009409257593106144</v>
+        <v>0.000862768841098868</v>
       </c>
       <c r="H81">
         <v>0.006468277148910681</v>
@@ -2512,16 +2512,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D82">
-        <v>3393321.254894496</v>
+        <v>3312988.216193237</v>
       </c>
       <c r="E82">
-        <v>363.6041298569987</v>
+        <v>364.125319113856</v>
       </c>
       <c r="F82">
-        <v>6.790963949108149</v>
+        <v>6.681861267034241</v>
       </c>
       <c r="G82">
-        <v>0.0009359942666441432</v>
+        <v>0.0008581863540885112</v>
       </c>
       <c r="H82">
         <v>0.006468277148910681</v>
@@ -2538,16 +2538,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D83">
-        <v>3392266.78195898</v>
+        <v>3311873.830824388</v>
       </c>
       <c r="E83">
-        <v>364.3093276951475</v>
+        <v>364.8378405074485</v>
       </c>
       <c r="F83">
-        <v>6.826430196009864</v>
+        <v>6.717210579164193</v>
       </c>
       <c r="G83">
-        <v>0.000931062302145176</v>
+        <v>0.000853603365402178</v>
       </c>
       <c r="H83">
         <v>0.006468277148910681</v>
@@ -2564,16 +2564,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D84">
-        <v>3391195.781258145</v>
+        <v>3310741.71616001</v>
       </c>
       <c r="E84">
-        <v>365.014622393003</v>
+        <v>365.5504627150381</v>
       </c>
       <c r="F84">
-        <v>6.862269853548676</v>
+        <v>6.752937264052361</v>
       </c>
       <c r="G84">
-        <v>0.0009261298523927779</v>
+        <v>0.0008490198619720312</v>
       </c>
       <c r="H84">
         <v>0.006468277148910681</v>
@@ -2590,16 +2590,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D85">
-        <v>3390107.901792753</v>
+        <v>3309591.490079639</v>
       </c>
       <c r="E85">
-        <v>365.7200154485911</v>
+        <v>366.2631873190517</v>
       </c>
       <c r="F85">
-        <v>6.898488911266385</v>
+        <v>6.789047459743499</v>
       </c>
       <c r="G85">
-        <v>0.0009211969036910172</v>
+        <v>0.0008444358304588856</v>
       </c>
       <c r="H85">
         <v>0.006468277148910681</v>
@@ -2616,16 +2616,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D86">
-        <v>3389002.783113322</v>
+        <v>3308422.7600211</v>
       </c>
       <c r="E86">
-        <v>366.4255083912355</v>
+        <v>366.976015935465</v>
       </c>
       <c r="F86">
-        <v>6.935093488711545</v>
+        <v>6.825547439385984</v>
       </c>
       <c r="G86">
-        <v>0.0009162634420618981</v>
+        <v>0.000839851257245142</v>
       </c>
       <c r="H86">
         <v>0.006468277148910681</v>
@@ -2642,16 +2642,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D87">
-        <v>3387880.055010722</v>
+        <v>3307235.122633511</v>
       </c>
       <c r="E87">
-        <v>367.1311027823839</v>
+        <v>367.6889502147018</v>
       </c>
       <c r="F87">
-        <v>6.972089839015827</v>
+        <v>6.862443615000607</v>
       </c>
       <c r="G87">
-        <v>0.0009113294532380726</v>
+        <v>0.0008352661284274916</v>
       </c>
       <c r="H87">
         <v>0.006468277148910681</v>
@@ -2668,16 +2668,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D88">
-        <v>3386739.337194806</v>
+        <v>3306028.163416653</v>
       </c>
       <c r="E88">
-        <v>367.8368002164619</v>
+        <v>368.4019918425624</v>
       </c>
       <c r="F88">
-        <v>7.009484352589893</v>
+        <v>6.899742541377174</v>
       </c>
       <c r="G88">
-        <v>0.0009063949226553357</v>
+        <v>0.000830680429809386</v>
       </c>
       <c r="H88">
         <v>0.006468277148910681</v>
@@ -2694,16 +2694,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D89">
-        <v>3385580.238960535</v>
+        <v>3304801.456346103</v>
       </c>
       <c r="E89">
-        <v>368.5426023217532</v>
+        <v>369.1151425411824</v>
       </c>
       <c r="F89">
-        <v>7.047283560943653</v>
+        <v>6.937450920103951</v>
       </c>
       <c r="G89">
-        <v>0.0009014598354448656</v>
+        <v>0.0008260941468932742</v>
       </c>
       <c r="H89">
         <v>0.006468277148910681</v>
@@ -2720,16 +2720,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D90">
-        <v>3384402.35884103</v>
+        <v>3303554.563483458</v>
       </c>
       <c r="E90">
-        <v>369.248510761309</v>
+        <v>369.8284040700232</v>
       </c>
       <c r="F90">
-        <v>7.085494140635608</v>
+        <v>6.975575603735324</v>
       </c>
       <c r="G90">
-        <v>0.0008965241764252403</v>
+        <v>0.0008215072648725893</v>
       </c>
       <c r="H90">
         <v>0.006468277148910681</v>
@@ -2746,16 +2746,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D91">
-        <v>3383205.284246971</v>
+        <v>3302287.034570989</v>
       </c>
       <c r="E91">
-        <v>369.9545272338868</v>
+        <v>370.5417782268955</v>
       </c>
       <c r="F91">
-        <v>7.124122917356727</v>
+        <v>7.014123600103362</v>
       </c>
       <c r="G91">
-        <v>0.0008915879300941788</v>
+        <v>0.0008169197686234737</v>
       </c>
       <c r="H91">
         <v>0.006468277148910681</v>
@@ -2772,16 +2772,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D92">
-        <v>3381988.591091713</v>
+        <v>3300998.406609982</v>
       </c>
       <c r="E92">
-        <v>370.6606534749201</v>
+        <v>371.255266849016</v>
       </c>
       <c r="F92">
-        <v>7.163176870153943</v>
+        <v>7.053102076778969</v>
       </c>
       <c r="G92">
-        <v>0.0008866510806200444</v>
+        <v>0.0008123316426962404</v>
       </c>
       <c r="H92">
         <v>0.006468277148910681</v>
@@ -2798,16 +2798,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D93">
-        <v>3380751.84340146</v>
+        <v>3299688.20342202</v>
       </c>
       <c r="E93">
-        <v>371.3668912575199</v>
+        <v>371.9688718141004</v>
       </c>
       <c r="F93">
-        <v>7.202663135799162</v>
+        <v>7.092518365688933</v>
       </c>
       <c r="G93">
-        <v>0.0008817136118330531</v>
+        <v>0.0008077428713065531</v>
       </c>
       <c r="H93">
         <v>0.006468277148910681</v>

</xml_diff>

<commit_message>
Look into Gas Solving
</commit_message>
<xml_diff>
--- a/TheEngine/Regen Solver/enginefiles/solverdata.xlsx
+++ b/TheEngine/Regen Solver/enginefiles/solverdata.xlsx
@@ -438,13 +438,13 @@
         <v>300</v>
       </c>
       <c r="F2">
-        <v>4.905011801081626</v>
+        <v>0.3595125535138668</v>
       </c>
       <c r="G2">
-        <v>0.002849206603787273</v>
+        <v>0.03887316834614297</v>
       </c>
       <c r="H2">
-        <v>0.006542436735388365</v>
+        <v>0.02149279952187255</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -458,19 +458,19 @@
         <v>0.03093226317788614</v>
       </c>
       <c r="D3">
-        <v>3999776.610203336</v>
+        <v>3999999.654129643</v>
       </c>
       <c r="E3">
-        <v>300.3344679217842</v>
+        <v>300.181816659766</v>
       </c>
       <c r="F3">
-        <v>5.48904777647008</v>
+        <v>0.4298500468976093</v>
       </c>
       <c r="G3">
-        <v>0.002637155852782424</v>
+        <v>0.03367618519429238</v>
       </c>
       <c r="H3">
-        <v>0.005942060430261161</v>
+        <v>0.01878828933167205</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -484,19 +484,19 @@
         <v>0.03010170940624797</v>
       </c>
       <c r="D4">
-        <v>3999477.250081811</v>
+        <v>3999999.130534794</v>
       </c>
       <c r="E4">
-        <v>300.6909813421665</v>
+        <v>300.3797948111934</v>
       </c>
       <c r="F4">
-        <v>6.155198255148112</v>
+        <v>0.5127715153461251</v>
       </c>
       <c r="G4">
-        <v>0.002439013086187956</v>
+        <v>0.02927849863974034</v>
       </c>
       <c r="H4">
-        <v>0.005386125297889534</v>
+        <v>0.01642716045187816</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -510,19 +510,19 @@
         <v>0.02927115563460979</v>
       </c>
       <c r="D5">
-        <v>3999073.958072922</v>
+        <v>3999998.339840178</v>
       </c>
       <c r="E5">
-        <v>301.071570713086</v>
+        <v>300.5955607451178</v>
       </c>
       <c r="F5">
-        <v>6.91781991444688</v>
+        <v>0.6106515516813362</v>
       </c>
       <c r="G5">
-        <v>0.002253751992788962</v>
+        <v>0.02553354816920755</v>
       </c>
       <c r="H5">
-        <v>0.00487171151677468</v>
+        <v>0.01435985195672173</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -536,19 +536,19 @@
         <v>0.02844060186297162</v>
       </c>
       <c r="D6">
-        <v>3998527.480723054</v>
+        <v>3999997.147254071</v>
       </c>
       <c r="E6">
-        <v>301.4785320338666</v>
+        <v>300.830962196557</v>
       </c>
       <c r="F6">
-        <v>7.794417485639511</v>
+        <v>0.7264070173137478</v>
       </c>
       <c r="G6">
-        <v>0.00208042772103773</v>
+        <v>0.02232558157041539</v>
       </c>
       <c r="H6">
-        <v>0.004396092827715485</v>
+        <v>0.01254527433391712</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -562,19 +562,19 @@
         <v>0.02761004809133344</v>
       </c>
       <c r="D7">
-        <v>3997782.213071322</v>
+        <v>3999995.348498659</v>
       </c>
       <c r="E7">
-        <v>301.9144757798911</v>
+        <v>301.0881095611132</v>
       </c>
       <c r="F7">
-        <v>8.806511995106687</v>
+        <v>0.8636520522055269</v>
       </c>
       <c r="G7">
-        <v>0.001918165903864194</v>
+        <v>0.01956236391239931</v>
       </c>
       <c r="H7">
-        <v>0.00395671747536446</v>
+        <v>0.01094911233655031</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -588,19 +588,19 @@
         <v>0.02677949431969527</v>
       </c>
       <c r="D8">
-        <v>3996758.597779526</v>
+        <v>3999992.632061699</v>
       </c>
       <c r="E8">
-        <v>302.3823886517101</v>
+        <v>301.3694277199661</v>
       </c>
       <c r="F8">
-        <v>9.980814614497675</v>
+        <v>1.026909258277378</v>
       </c>
       <c r="G8">
-        <v>0.001766151593049934</v>
+        <v>0.01716976095127516</v>
       </c>
       <c r="H8">
-        <v>0.003551189604397998</v>
+        <v>0.009542504753872378</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -614,19 +614,19 @@
         <v>0.02594894054805708</v>
       </c>
       <c r="D9">
-        <v>3995341.535888504</v>
+        <v>3999988.519233504</v>
       </c>
       <c r="E9">
-        <v>302.8857129513292</v>
+        <v>301.677722309512</v>
       </c>
       <c r="F9">
-        <v>11.35084714915075</v>
+        <v>1.221903788643046</v>
       </c>
       <c r="G9">
-        <v>0.001623617318988921</v>
+        <v>0.01508766384157421</v>
       </c>
       <c r="H9">
-        <v>0.003177250208647025</v>
+        <v>0.008301005280092064</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -640,19 +640,19 @@
         <v>0.02511838677641891</v>
       </c>
       <c r="D10">
-        <v>3993362.41360171</v>
+        <v>3999982.267409943</v>
       </c>
       <c r="E10">
-        <v>303.4284509301681</v>
+        <v>302.016266230618</v>
       </c>
       <c r="F10">
-        <v>12.95923830117153</v>
+        <v>1.455984292642696</v>
       </c>
       <c r="G10">
-        <v>0.001489828972181673</v>
+        <v>0.01326687623441971</v>
       </c>
       <c r="H10">
-        <v>0.002832756114070572</v>
+        <v>0.00720375245234082</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -666,19 +666,19 @@
         <v>0.02428783300478073</v>
       </c>
       <c r="D11">
-        <v>3990570.669999055</v>
+        <v>3999972.711324879</v>
       </c>
       <c r="E11">
-        <v>304.0153058213451</v>
+        <v>302.3889155468186</v>
       </c>
       <c r="F11">
-        <v>14.86108918561069</v>
+        <v>1.738747175644569</v>
       </c>
       <c r="G11">
-        <v>0.001364067122881179</v>
+        <v>0.01166668366864363</v>
       </c>
       <c r="H11">
-        <v>0.002515654229479245</v>
+        <v>0.006232791435052959</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -692,19 +692,19 @@
         <v>0.02345727923314256</v>
       </c>
       <c r="D12">
-        <v>3986587.737230955</v>
+        <v>3999957.996571675</v>
       </c>
       <c r="E12">
-        <v>304.651879230879</v>
+        <v>302.8002700300441</v>
       </c>
       <c r="F12">
-        <v>17.12913436781196</v>
+        <v>2.083007241228094</v>
       </c>
       <c r="G12">
-        <v>0.001245598966604661</v>
+        <v>0.01025287903886758</v>
       </c>
       <c r="H12">
-        <v>0.002223945332654902</v>
+        <v>0.005372496120557248</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -718,19 +718,19 @@
         <v>0.02262672546150438</v>
       </c>
       <c r="D13">
-        <v>3980830.190098177</v>
+        <v>3999935.119760852</v>
       </c>
       <c r="E13">
-        <v>305.344960142939</v>
+        <v>303.2559056249376</v>
       </c>
       <c r="F13">
-        <v>19.86217358022127</v>
+        <v>2.506409377429537</v>
       </c>
       <c r="G13">
-        <v>0.001133630102095071</v>
+        <v>0.008996018808124383</v>
       </c>
       <c r="H13">
-        <v>0.00195562434030411</v>
+        <v>0.004609031209556679</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -744,19 +744,19 @@
         <v>0.0217961716898662</v>
       </c>
       <c r="D14">
-        <v>3972376.499475443</v>
+        <v>3999899.10540364</v>
       </c>
       <c r="E14">
-        <v>306.102974195615</v>
+        <v>303.7627321449904</v>
       </c>
       <c r="F14">
-        <v>23.2001899087946</v>
+        <v>3.034372544175556</v>
       </c>
       <c r="G14">
-        <v>0.001027208451763175</v>
+        <v>0.007869576213013095</v>
       </c>
       <c r="H14">
-        <v>0.001708562832462672</v>
+        <v>0.003929748438516379</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -770,19 +770,19 @@
         <v>0.02096561791822803</v>
       </c>
       <c r="D15">
-        <v>3959723.300935372</v>
+        <v>3999841.454402229</v>
       </c>
       <c r="E15">
-        <v>306.9367428490476</v>
+        <v>304.3295937697877</v>
       </c>
       <c r="F15">
-        <v>27.35569291313612</v>
+        <v>3.706318104315457</v>
       </c>
       <c r="G15">
-        <v>0.0009249950203275085</v>
+        <v>0.006847185036648109</v>
       </c>
       <c r="H15">
-        <v>0.001480226068461778</v>
+        <v>0.003322233670035768</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -796,19 +796,19 @@
         <v>0.02013506414658983</v>
       </c>
       <c r="D16">
-        <v>3940301.324010564</v>
+        <v>3999746.974622111</v>
       </c>
       <c r="E16">
-        <v>307.8609362505192</v>
+        <v>304.9684201480636</v>
       </c>
       <c r="F16">
-        <v>32.69700460986854</v>
+        <v>4.592551858886265</v>
       </c>
       <c r="G16">
-        <v>0.0008245508884374054</v>
+        <v>0.005895873631485016</v>
       </c>
       <c r="H16">
-        <v>0.001266772068834776</v>
+        <v>0.002771866874350751</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -822,19 +822,19 @@
         <v>0.01930451037495166</v>
       </c>
       <c r="D17">
-        <v>3909360.812148617</v>
+        <v>3999586.286627384</v>
       </c>
       <c r="E17">
-        <v>308.8975018887731</v>
+        <v>305.6969853262441</v>
       </c>
       <c r="F17">
-        <v>40.12263077154041</v>
+        <v>5.871379235921951</v>
       </c>
       <c r="G17">
-        <v>0.0007185636239751408</v>
+        <v>0.004942645032172242</v>
       </c>
       <c r="H17">
-        <v>0.001058130323103295</v>
+        <v>0.002249377538339802</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -848,19 +848,19 @@
         <v>0.01956298682688029</v>
       </c>
       <c r="D18">
-        <v>3856291.151585984</v>
+        <v>3999290.409933297</v>
       </c>
       <c r="E18">
-        <v>310.0884696275555</v>
+        <v>306.5495764486077</v>
       </c>
       <c r="F18">
-        <v>50.37010396659633</v>
+        <v>8.041819784835484</v>
       </c>
       <c r="G18">
-        <v>0.0005577303174063409</v>
+        <v>0.003529735288234876</v>
       </c>
       <c r="H18">
-        <v>0.0008541012114779965</v>
+        <v>0.001718296431349822</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -874,19 +874,19 @@
         <v>0.02135258148578198</v>
       </c>
       <c r="D19">
-        <v>3739606.498871365</v>
+        <v>3998559.64840577</v>
       </c>
       <c r="E19">
-        <v>311.5879780933276</v>
+        <v>307.6658191627608</v>
       </c>
       <c r="F19">
-        <v>44.62441060095711</v>
+        <v>7.258313218371503</v>
       </c>
       <c r="G19">
-        <v>0.000542265367818076</v>
+        <v>0.003396730212395858</v>
       </c>
       <c r="H19">
-        <v>0.0009463339455950721</v>
+        <v>0.001884574648725151</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -900,19 +900,19 @@
         <v>0.0231421761446837</v>
       </c>
       <c r="D20">
-        <v>3646202.960067133</v>
+        <v>3997984.838218637</v>
       </c>
       <c r="E20">
-        <v>313.0917013012407</v>
+        <v>308.777029361549</v>
       </c>
       <c r="F20">
-        <v>38.82946300048378</v>
+        <v>6.354541416379149</v>
       </c>
       <c r="G20">
-        <v>0.0005471647209861363</v>
+        <v>0.003429106194693121</v>
       </c>
       <c r="H20">
-        <v>0.001069404477373927</v>
+        <v>0.00212230701173971</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -926,19 +926,19 @@
         <v>0.02493177080358538</v>
       </c>
       <c r="D21">
-        <v>3576350.577169761</v>
+        <v>3997566.661092702</v>
       </c>
       <c r="E21">
-        <v>314.5547995954685</v>
+        <v>309.8482829730763</v>
       </c>
       <c r="F21">
-        <v>33.86687367475206</v>
+        <v>5.551557945546983</v>
       </c>
       <c r="G21">
-        <v>0.0005592877113105684</v>
+        <v>0.003516582592013947</v>
       </c>
       <c r="H21">
-        <v>0.001208072179267094</v>
+        <v>0.002394196471601855</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -952,19 +952,19 @@
         <v>0.0267213654624871</v>
       </c>
       <c r="D22">
-        <v>3524470.394304341</v>
+        <v>3997264.561917908</v>
       </c>
       <c r="E22">
-        <v>315.9653647690192</v>
+        <v>310.8734390895015</v>
       </c>
       <c r="F22">
-        <v>29.71775728473478</v>
+        <v>4.868043952367922</v>
       </c>
       <c r="G22">
-        <v>0.0005751899114771566</v>
+        <v>0.003632310065098838</v>
       </c>
       <c r="H22">
-        <v>0.001358867032755786</v>
+        <v>0.002691945911565041</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -978,19 +978,19 @@
         <v>0.02851096012138879</v>
       </c>
       <c r="D23">
-        <v>3485689.213575249</v>
+        <v>3997044.630402612</v>
       </c>
       <c r="E23">
-        <v>317.3205769244773</v>
+        <v>311.8528303725915</v>
       </c>
       <c r="F23">
-        <v>26.25397418616662</v>
+        <v>4.291641986023308</v>
       </c>
       <c r="G23">
-        <v>0.0005933740930978196</v>
+        <v>0.003765241389449442</v>
       </c>
       <c r="H23">
-        <v>0.001520395727963033</v>
+        <v>0.00301230754052626</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1004,19 +1004,19 @@
         <v>0.03030055478029048</v>
       </c>
       <c r="D24">
-        <v>3456389.216803909</v>
+        <v>3996882.575244343</v>
       </c>
       <c r="E24">
-        <v>318.6212618077764</v>
+        <v>312.7888281275833</v>
       </c>
       <c r="F24">
-        <v>23.34808244128254</v>
+        <v>3.805235132307799</v>
       </c>
       <c r="G24">
-        <v>0.00061304773703215</v>
+        <v>0.003909750903114328</v>
       </c>
       <c r="H24">
-        <v>0.001691941174899729</v>
+        <v>0.003353661375196944</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1030,19 +1030,19 @@
         <v>0.03209014943919218</v>
       </c>
       <c r="D25">
-        <v>3433987.903630811</v>
+        <v>3996761.583054078</v>
       </c>
       <c r="E25">
-        <v>319.8698074957406</v>
+        <v>313.6844128053844</v>
       </c>
       <c r="F25">
-        <v>20.89323199552232</v>
+        <v>3.392979261908903</v>
       </c>
       <c r="G25">
-        <v>0.0006337430556593427</v>
+        <v>0.004062603627360651</v>
       </c>
       <c r="H25">
-        <v>0.001873074068597041</v>
+        <v>0.003715073683693255</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1056,19 +1056,19 @@
         <v>0.03387974409809387</v>
       </c>
       <c r="D26">
-        <v>3416655.380971263</v>
+        <v>3996670.061190699</v>
       </c>
       <c r="E26">
-        <v>321.0692225956166</v>
+        <v>314.5426329824169</v>
       </c>
       <c r="F26">
-        <v>18.80392174771049</v>
+        <v>3.041558984983036</v>
       </c>
       <c r="G26">
-        <v>0.0006551638035196973</v>
+        <v>0.004221784877926677</v>
       </c>
       <c r="H26">
-        <v>0.002063509283295386</v>
+        <v>0.004095951231654739</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1082,19 +1082,19 @@
         <v>0.03566933875699557</v>
       </c>
       <c r="D27">
-        <v>3403089.676003241</v>
+        <v>3996599.96234468</v>
       </c>
       <c r="E27">
-        <v>322.2226820445551</v>
+        <v>315.3663920926822</v>
       </c>
       <c r="F27">
-        <v>17.0126280416103</v>
+        <v>2.740145256869806</v>
       </c>
       <c r="G27">
-        <v>0.0006771127808027774</v>
+        <v>0.004385966503927788</v>
       </c>
       <c r="H27">
-        <v>0.002263042612275085</v>
+        <v>0.004495889934875418</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1108,19 +1108,19 @@
         <v>0.03745893341589727</v>
       </c>
       <c r="D28">
-        <v>3392356.229944909</v>
+        <v>3996545.639272689</v>
       </c>
       <c r="E28">
-        <v>323.333305095259</v>
+        <v>316.1583704049423</v>
       </c>
       <c r="F28">
-        <v>15.46607156678846</v>
+        <v>2.480026581653641</v>
       </c>
       <c r="G28">
-        <v>0.0006994537009999353</v>
+        <v>0.00455423456395242</v>
       </c>
       <c r="H28">
-        <v>0.0024715192954805</v>
+        <v>0.004914600034618646</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1134,19 +1134,19 @@
         <v>0.03924852807479898</v>
       </c>
       <c r="D29">
-        <v>3383776.991143041</v>
+        <v>3996503.079819684</v>
       </c>
       <c r="E29">
-        <v>324.4040503517729</v>
+        <v>316.9210058642029</v>
       </c>
       <c r="F29">
-        <v>14.12203395015133</v>
+        <v>2.254206623996952</v>
       </c>
       <c r="G29">
-        <v>0.0007220895634491635</v>
+        <v>0.004725938612298529</v>
       </c>
       <c r="H29">
-        <v>0.002688816871064464</v>
+        <v>0.005351865587895499</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1160,19 +1160,19 @@
         <v>0.04103812273370067</v>
       </c>
       <c r="D30">
-        <v>3376854.409963838</v>
+        <v>3996469.397256505</v>
       </c>
       <c r="E30">
-        <v>325.4376715317665</v>
+        <v>317.6565007007844</v>
       </c>
       <c r="F30">
-        <v>12.94684529119103</v>
+        <v>2.057051723045936</v>
       </c>
       <c r="G30">
-        <v>0.0007449496695258027</v>
+        <v>0.004900602957629519</v>
       </c>
       <c r="H30">
-        <v>0.00291483514110167</v>
+        <v>0.005807520921206261</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1186,19 +1186,19 @@
         <v>0.04282771739260237</v>
       </c>
       <c r="D31">
-        <v>3371219.234501278</v>
+        <v>3996442.488691099</v>
       </c>
       <c r="E31">
-        <v>326.4367049772629</v>
+        <v>318.3668386856566</v>
       </c>
       <c r="F31">
-        <v>11.91345590160809</v>
+        <v>1.884004074180033</v>
       </c>
       <c r="G31">
-        <v>0.0007679814720056848</v>
+        <v>0.005077871792012867</v>
       </c>
       <c r="H31">
-        <v>0.003149489950879344</v>
+        <v>0.006281436135074914</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1212,19 +1212,19 @@
         <v>0.04461731205150407</v>
       </c>
       <c r="D32">
-        <v>3366594.398878599</v>
+        <v>3996420.803893499</v>
       </c>
       <c r="E32">
-        <v>327.4034735212522</v>
+        <v>319.053805943536</v>
       </c>
       <c r="F32">
-        <v>10.99996968058679</v>
+        <v>1.731355230666959</v>
       </c>
       <c r="G32">
-        <v>0.0007911452699057156</v>
+        <v>0.005257473888627332</v>
       </c>
       <c r="H32">
-        <v>0.003392709143079871</v>
+        <v>0.006773507745786641</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1238,19 +1238,19 @@
         <v>0.04640690671040576</v>
       </c>
       <c r="D33">
-        <v>3362769.808796308</v>
+        <v>3996403.187065701</v>
       </c>
       <c r="E33">
-        <v>328.3400983788061</v>
+        <v>319.7190120083605</v>
       </c>
       <c r="F33">
-        <v>10.18852916063212</v>
+        <v>1.596069371238073</v>
       </c>
       <c r="G33">
-        <v>0.0008144106499937629</v>
+        <v>0.005439199128021792</v>
       </c>
       <c r="H33">
-        <v>0.003644429817577348</v>
+        <v>0.007283652396122215</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1264,19 +1264,19 @@
         <v>0.04819650136930748</v>
       </c>
       <c r="D34">
-        <v>3359584.553136025</v>
+        <v>3996388.767248153</v>
       </c>
       <c r="E34">
-        <v>329.2485145205685</v>
+        <v>320.3639096350985</v>
       </c>
       <c r="F34">
-        <v>9.464464807376389</v>
+        <v>1.475645870323757</v>
       </c>
       <c r="G34">
-        <v>0.0008377540383665035</v>
+        <v>0.005622882448787852</v>
       </c>
       <c r="H34">
-        <v>0.003904596410081231</v>
+        <v>0.007811802481217228</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1290,19 +1290,19 @@
         <v>0.04998609602820916</v>
       </c>
       <c r="D35">
-        <v>3356914.220354675</v>
+        <v>3996376.881507758</v>
       </c>
       <c r="E35">
-        <v>330.1304870661394</v>
+        <v>320.9898127820843</v>
       </c>
       <c r="F35">
-        <v>8.815642231719297</v>
+        <v>1.368012322141343</v>
       </c>
       <c r="G35">
-        <v>0.0008611569784819222</v>
+        <v>0.005808392608728408</v>
       </c>
       <c r="H35">
-        <v>0.004173159303741212</v>
+        <v>0.008357903014476736</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1316,19 +1316,19 @@
         <v>0.05177569068711085</v>
       </c>
       <c r="D36">
-        <v>3354661.758579374</v>
+        <v>3996367.020474973</v>
       </c>
       <c r="E36">
-        <v>330.9876273933657</v>
+        <v>321.5979126194209</v>
       </c>
       <c r="F36">
-        <v>8.231957904509787</v>
+        <v>1.271440985321571</v>
       </c>
       <c r="G36">
-        <v>0.0008846048967679329</v>
+        <v>0.005995624149395092</v>
       </c>
       <c r="H36">
-        <v>0.004450073799171029</v>
+        <v>0.008921909322942382</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1342,19 +1342,19 @@
         <v>0.05356528534601257</v>
       </c>
       <c r="D37">
-        <v>3352750.821016089</v>
+        <v>3996358.789294279</v>
       </c>
       <c r="E37">
-        <v>331.8214083096973</v>
+        <v>322.189291628655</v>
       </c>
       <c r="F37">
-        <v>7.704946808533583</v>
+        <v>1.184483211531989</v>
       </c>
       <c r="G37">
-        <v>0.0009080862027412731</v>
+        <v>0.00618449154501355</v>
       </c>
       <c r="H37">
-        <v>0.004735299332450548</v>
+        <v>0.009503785313331379</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1368,19 +1368,19 @@
         <v>0.05535488000491426</v>
       </c>
       <c r="D38">
-        <v>3351120.872404031</v>
+        <v>3996351.879325792</v>
       </c>
       <c r="E38">
-        <v>332.6331779963685</v>
+        <v>322.764935950496</v>
       </c>
       <c r="F38">
-        <v>7.227474970243511</v>
+        <v>1.105917707850127</v>
       </c>
       <c r="G38">
-        <v>0.00093159162311481</v>
+        <v>0.006374924872415757</v>
       </c>
       <c r="H38">
-        <v>0.005028798869115337</v>
+        <v>0.01010350214072404</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1394,19 +1394,19 @@
         <v>0.05714447466381595</v>
       </c>
       <c r="D39">
-        <v>3349723.555996133</v>
+        <v>3996346.047428864</v>
       </c>
       <c r="E39">
-        <v>333.4241726383011</v>
+        <v>323.3257461689233</v>
       </c>
       <c r="F39">
-        <v>6.793496784176314</v>
+        <v>1.034709479145003</v>
       </c>
       <c r="G39">
-        <v>0.0009551137023758545</v>
+        <v>0.006566866559515084</v>
       </c>
       <c r="H39">
-        <v>0.005330538425664675</v>
+        <v>0.01072103716729345</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1420,19 +1420,19 @@
         <v>0.05893406932271766</v>
       </c>
       <c r="D40">
-        <v>3348519.971708253</v>
+        <v>3996341.100649453</v>
       </c>
       <c r="E40">
-        <v>334.1955277616438</v>
+        <v>323.8725467218601</v>
       </c>
       <c r="F40">
-        <v>6.397862140337804</v>
+        <v>0.9699770542585231</v>
       </c>
       <c r="G40">
-        <v>0.0009786464237734201</v>
+        <v>0.0067602689123495</v>
       </c>
       <c r="H40">
-        <v>0.00564048668604419</v>
+        <v>0.01135637313562076</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1446,19 +1446,19 @@
         <v>0.06072366398161935</v>
       </c>
       <c r="D41">
-        <v>3347478.619170708</v>
+        <v>3996336.884797886</v>
       </c>
       <c r="E41">
-        <v>334.9482883562499</v>
+        <v>324.4060941163971</v>
       </c>
       <c r="F41">
-        <v>6.036162103601146</v>
+        <v>0.9109661716982105</v>
       </c>
       <c r="G41">
-        <v>0.001002184918368445</v>
+        <v>0.006955092210672473</v>
       </c>
       <c r="H41">
-        <v>0.005958614688860019</v>
+        <v>0.01200949750094209</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1472,19 +1472,19 @@
         <v>0.06251325864052105</v>
       </c>
       <c r="D42">
-        <v>3346573.830401494</v>
+        <v>3996333.275854587</v>
       </c>
       <c r="E42">
-        <v>335.6834178854317</v>
+        <v>324.9270841088662</v>
       </c>
       <c r="F42">
-        <v>5.704604640569664</v>
+        <v>0.8570285299864135</v>
       </c>
       <c r="G42">
-        <v>0.001025725239597351</v>
+        <v>0.007151303226579883</v>
       </c>
       <c r="H42">
-        <v>0.006284895569669207</v>
+        <v>0.01268040188620993</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1498,19 +1498,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D43">
-        <v>3345784.566173799</v>
+        <v>3996330.173450393</v>
       </c>
       <c r="E43">
-        <v>336.401806292841</v>
+        <v>325.4361579907405</v>
       </c>
       <c r="F43">
-        <v>5.54436997722534</v>
+        <v>0.8299172231755227</v>
       </c>
       <c r="G43">
-        <v>0.001036638150099113</v>
+        <v>0.007254249327598167</v>
       </c>
       <c r="H43">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1524,19 +1524,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D44">
-        <v>3345145.874705372</v>
+        <v>3996327.691942479</v>
       </c>
       <c r="E44">
-        <v>337.1113512771659</v>
+        <v>325.9389179799066</v>
       </c>
       <c r="F44">
-        <v>5.568675918974766</v>
+        <v>0.8313953775547491</v>
       </c>
       <c r="G44">
-        <v>0.001032067158003627</v>
+        <v>0.00724135054417001</v>
       </c>
       <c r="H44">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1550,19 +1550,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D45">
-        <v>3344498.817383963</v>
+        <v>3996325.198254473</v>
       </c>
       <c r="E45">
-        <v>337.8209544012248</v>
+        <v>326.4416781711128</v>
       </c>
       <c r="F45">
-        <v>5.593195682262315</v>
+        <v>0.8328785718005356</v>
       </c>
       <c r="G45">
-        <v>0.00102749601242939</v>
+        <v>0.007228453798267891</v>
       </c>
       <c r="H45">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1576,19 +1576,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D46">
-        <v>3343843.246173757</v>
+        <v>3996322.692305175</v>
       </c>
       <c r="E46">
-        <v>338.5306164193937</v>
+        <v>326.9444385653504</v>
       </c>
       <c r="F46">
-        <v>5.617932122011637</v>
+        <v>0.8343668316105669</v>
       </c>
       <c r="G46">
-        <v>0.001022924706966759</v>
+        <v>0.00721555909045358</v>
       </c>
       <c r="H46">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1602,19 +1602,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D47">
-        <v>3343179.009727658</v>
+        <v>3996320.1740127</v>
       </c>
       <c r="E47">
-        <v>339.2403380992432</v>
+        <v>327.4471991636177</v>
       </c>
       <c r="F47">
-        <v>5.642888144558273</v>
+        <v>0.8358601828574513</v>
       </c>
       <c r="G47">
-        <v>0.001018353235094684</v>
+        <v>0.007202666421288944</v>
       </c>
       <c r="H47">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1628,19 +1628,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D48">
-        <v>3342505.95329748</v>
+        <v>3996317.643294476</v>
       </c>
       <c r="E48">
-        <v>339.9501202218298</v>
+        <v>327.9499599669196</v>
       </c>
       <c r="F48">
-        <v>5.668066708819723</v>
+        <v>0.8373586515902133</v>
       </c>
       <c r="G48">
-        <v>0.001013781590178275</v>
+        <v>0.007189775791335853</v>
       </c>
       <c r="H48">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1654,19 +1654,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D49">
-        <v>3341823.918641261</v>
+        <v>3996315.100067234</v>
       </c>
       <c r="E49">
-        <v>340.6599635819945</v>
+        <v>328.4527209762675</v>
       </c>
       <c r="F49">
-        <v>5.693470827497718</v>
+        <v>0.8388622640357988</v>
       </c>
       <c r="G49">
-        <v>0.001009209765466342</v>
+        <v>0.007176887201156289</v>
       </c>
       <c r="H49">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1680,19 +1680,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D50">
-        <v>3341132.7439276</v>
+        <v>3996312.544247</v>
       </c>
       <c r="E50">
-        <v>341.36986898867</v>
+        <v>328.9554821926799</v>
       </c>
       <c r="F50">
-        <v>5.719103568313937</v>
+        <v>0.8403710466005956</v>
       </c>
       <c r="G50">
-        <v>0.001004637754088823</v>
+        <v>0.007164000651312293</v>
       </c>
       <c r="H50">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -1706,19 +1706,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D51">
-        <v>3340432.263636915</v>
+        <v>3996309.975749088</v>
       </c>
       <c r="E51">
-        <v>342.0798372651959</v>
+        <v>329.4582436171818</v>
       </c>
       <c r="F51">
-        <v>5.744968055280063</v>
+        <v>0.8418850258719726</v>
       </c>
       <c r="G51">
-        <v>0.001000065549054182</v>
+        <v>0.00715111614236597</v>
       </c>
       <c r="H51">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1732,19 +1732,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D52">
-        <v>3339722.308459487</v>
+        <v>3996307.394488096</v>
       </c>
       <c r="E52">
-        <v>342.789869249642</v>
+        <v>329.9610052508054</v>
       </c>
       <c r="F52">
-        <v>5.771067470003406</v>
+        <v>0.843404228619832</v>
       </c>
       <c r="G52">
-        <v>0.0009954931432467218</v>
+        <v>0.007138233674879496</v>
       </c>
       <c r="H52">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -1758,19 +1758,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D53">
-        <v>3339002.705190194</v>
+        <v>3996304.800377897</v>
       </c>
       <c r="E53">
-        <v>343.4999657951416</v>
+        <v>330.4637670945897</v>
       </c>
       <c r="F53">
-        <v>5.797405053029354</v>
+        <v>0.8449286817981785</v>
       </c>
       <c r="G53">
-        <v>0.0009909205294238179</v>
+        <v>0.007125353249415083</v>
       </c>
       <c r="H53">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -1784,19 +1784,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D54">
-        <v>3338273.276619792</v>
+        <v>3996302.193331627</v>
       </c>
       <c r="E54">
-        <v>344.2101277702324</v>
+        <v>330.9665291495807</v>
       </c>
       <c r="F54">
-        <v>5.823984105221584</v>
+        <v>0.8464584125467058</v>
       </c>
       <c r="G54">
-        <v>0.0009863477002130957</v>
+        <v>0.00711247486653504</v>
       </c>
       <c r="H54">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -1810,19 +1810,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D55">
-        <v>3337533.841422617</v>
+        <v>3996299.573261685</v>
       </c>
       <c r="E55">
-        <v>344.9203560592078</v>
+        <v>331.4692914168315</v>
       </c>
       <c r="F55">
-        <v>5.850807989181658</v>
+        <v>0.847993448192398</v>
       </c>
       <c r="G55">
-        <v>0.0009817746481095202</v>
+        <v>0.007099598526801683</v>
       </c>
       <c r="H55">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -1836,19 +1836,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D56">
-        <v>3336784.214040587</v>
+        <v>3996296.94007972</v>
       </c>
       <c r="E56">
-        <v>345.6306515624777</v>
+        <v>331.9720538974022</v>
       </c>
       <c r="F56">
-        <v>5.877880130709041</v>
+        <v>0.8495338162511479</v>
       </c>
       <c r="G56">
-        <v>0.00097720136547241</v>
+        <v>0.007086724230777415</v>
       </c>
       <c r="H56">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -1862,19 +1862,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D57">
-        <v>3336024.204563329</v>
+        <v>3996294.293696627</v>
       </c>
       <c r="E57">
-        <v>346.3410151969389</v>
+        <v>332.4748165923605</v>
       </c>
       <c r="F57">
-        <v>5.905204020303027</v>
+        <v>0.8510795444293887</v>
       </c>
       <c r="G57">
-        <v>0.0009726278445223701</v>
+        <v>0.007073851979024736</v>
       </c>
       <c r="H57">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -1888,19 +1888,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D58">
-        <v>3335253.618604323</v>
+        <v>3996291.634022534</v>
       </c>
       <c r="E58">
-        <v>347.0514478963564</v>
+        <v>332.9775795027808</v>
       </c>
       <c r="F58">
-        <v>5.932783214707966</v>
+        <v>0.8526306606257552</v>
       </c>
       <c r="G58">
-        <v>0.0009680540773381412</v>
+        <v>0.007060981772106105</v>
       </c>
       <c r="H58">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -1914,19 +1914,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D59">
-        <v>3334472.257172881</v>
+        <v>3996288.960966801</v>
       </c>
       <c r="E59">
-        <v>347.7619506117549</v>
+        <v>333.4803426297452</v>
       </c>
       <c r="F59">
-        <v>5.960621338503279</v>
+        <v>0.8541871929327454</v>
       </c>
       <c r="G59">
-        <v>0.0009634800558533623</v>
+        <v>0.007048113610584088</v>
       </c>
       <c r="H59">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -1940,19 +1940,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D60">
-        <v>3333679.916541805</v>
+        <v>3996286.274438006</v>
       </c>
       <c r="E60">
-        <v>348.4725243118212</v>
+        <v>333.983105974343</v>
       </c>
       <c r="F60">
-        <v>5.988722085739762</v>
+        <v>0.855749169638408</v>
       </c>
       <c r="G60">
-        <v>0.0009589057718532379</v>
+        <v>0.007035247495021308</v>
       </c>
       <c r="H60">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -1966,19 +1966,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D61">
-        <v>3332876.388110569</v>
+        <v>3996283.57434394</v>
       </c>
       <c r="E61">
-        <v>349.1831699833191</v>
+        <v>334.4858695376711</v>
       </c>
       <c r="F61">
-        <v>6.017089221623735</v>
+        <v>0.8573166192280519</v>
       </c>
       <c r="G61">
-        <v>0.0009543312169711334</v>
+        <v>0.00702238342598042</v>
       </c>
       <c r="H61">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -1992,19 +1992,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D62">
-        <v>3332061.458263829</v>
+        <v>3996280.860591598</v>
       </c>
       <c r="E62">
-        <v>349.8938886315144</v>
+        <v>334.9886333208337</v>
       </c>
       <c r="F62">
-        <v>6.045726584250832</v>
+        <v>0.8588895703859656</v>
       </c>
       <c r="G62">
-        <v>0.0009497563826850454</v>
+        <v>0.007009521404024096</v>
       </c>
       <c r="H62">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2018,19 +2018,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D63">
-        <v>3331234.908225097</v>
+        <v>3996278.133087172</v>
       </c>
       <c r="E63">
-        <v>350.6046812806129</v>
+        <v>335.4913973249427</v>
       </c>
       <c r="F63">
-        <v>6.074638086390945</v>
+        <v>0.8604680519971559</v>
       </c>
       <c r="G63">
-        <v>0.0009451812603139994</v>
+        <v>0.006996661429715104</v>
       </c>
       <c r="H63">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2044,19 +2044,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D64">
-        <v>3330396.513905375</v>
+        <v>3996275.391736038</v>
       </c>
       <c r="E64">
-        <v>351.3155489742116</v>
+        <v>335.9941615511177</v>
       </c>
       <c r="F64">
-        <v>6.10382771732628</v>
+        <v>0.8620520931491125</v>
       </c>
       <c r="G64">
-        <v>0.0009406058410143347</v>
+        <v>0.006983803503616192</v>
       </c>
       <c r="H64">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2070,19 +2070,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D65">
-        <v>3329546.045746549</v>
+        <v>3996272.636442756</v>
       </c>
       <c r="E65">
-        <v>352.0264927757615</v>
+        <v>336.4969260004858</v>
       </c>
       <c r="F65">
-        <v>6.133299544744305</v>
+        <v>0.863641723133577</v>
       </c>
       <c r="G65">
-        <v>0.0009360301157758852</v>
+        <v>0.00697094762629021</v>
       </c>
       <c r="H65">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2096,19 +2096,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D66">
-        <v>3328683.268559345</v>
+        <v>3996269.867111051</v>
       </c>
       <c r="E66">
-        <v>352.7375137690448</v>
+        <v>336.999690674182</v>
       </c>
       <c r="F66">
-        <v>6.163057716687503</v>
+        <v>0.8652369714483471</v>
       </c>
       <c r="G66">
-        <v>0.0009314540754180523</v>
+        <v>0.00695809379830001</v>
       </c>
       <c r="H66">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -2122,19 +2122,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D67">
-        <v>3327807.941355614</v>
+        <v>3996267.083643815</v>
       </c>
       <c r="E67">
-        <v>353.4486130586656</v>
+        <v>337.5024555733492</v>
       </c>
       <c r="F67">
-        <v>6.193106463562032</v>
+        <v>0.8668378677990892</v>
       </c>
       <c r="G67">
-        <v>0.000926877710585768</v>
+        <v>0.006945242020208451</v>
       </c>
       <c r="H67">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2148,19 +2148,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D68">
-        <v>3326919.817174727</v>
+        <v>3996264.285943087</v>
       </c>
       <c r="E68">
-        <v>354.1597917705553</v>
+        <v>338.005220699138</v>
       </c>
       <c r="F68">
-        <v>6.223450100207266</v>
+        <v>0.8684444421011674</v>
       </c>
       <c r="G68">
-        <v>0.0009223010117453402</v>
+        <v>0.006932392292578514</v>
       </c>
       <c r="H68">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -2174,19 +2174,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D69">
-        <v>3326018.642903836</v>
+        <v>3996261.473910055</v>
       </c>
       <c r="E69">
-        <v>354.8710510524924</v>
+        <v>338.5079860527073</v>
       </c>
       <c r="F69">
-        <v>6.25409302802852</v>
+        <v>0.8700567244815086</v>
       </c>
       <c r="G69">
-        <v>0.0009177239691801812</v>
+        <v>0.006919544615973098</v>
       </c>
       <c r="H69">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2200,19 +2200,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D70">
-        <v>3325104.159091754</v>
+        <v>3996258.647445039</v>
       </c>
       <c r="E70">
-        <v>355.5823920746376</v>
+        <v>339.0107516352236</v>
       </c>
       <c r="F70">
-        <v>6.285039737195116</v>
+        <v>0.8716747452804625</v>
       </c>
       <c r="G70">
-        <v>0.0009131465729864106</v>
+        <v>0.006906698990955224</v>
       </c>
       <c r="H70">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2226,19 +2226,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D71">
-        <v>3324176.099756186</v>
+        <v>3996255.806447486</v>
       </c>
       <c r="E71">
-        <v>356.2938160300857</v>
+        <v>339.5135174478619</v>
       </c>
       <c r="F71">
-        <v>6.316294808906246</v>
+        <v>0.8732985350537077</v>
       </c>
       <c r="G71">
-        <v>0.0009085688130683294</v>
+        <v>0.006893855418087875</v>
       </c>
       <c r="H71">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -2252,19 +2252,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D72">
-        <v>3323234.192184047</v>
+        <v>3996252.950815959</v>
       </c>
       <c r="E72">
-        <v>357.0053241354327</v>
+        <v>340.0162834918053</v>
       </c>
       <c r="F72">
-        <v>6.347862917727046</v>
+        <v>0.8749281245741556</v>
       </c>
       <c r="G72">
-        <v>0.0009039906791337652</v>
+        <v>0.0068810138979341</v>
       </c>
       <c r="H72">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2278,19 +2278,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D73">
-        <v>3322278.156724571</v>
+        <v>3996250.080448127</v>
       </c>
       <c r="E73">
-        <v>357.716917631361</v>
+        <v>340.5190497682449</v>
       </c>
       <c r="F73">
-        <v>6.37974883399744</v>
+        <v>0.8765635448338897</v>
       </c>
       <c r="G73">
-        <v>0.000899412160689279</v>
+        <v>0.006868174431056967</v>
       </c>
       <c r="H73">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2304,19 +2304,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D74">
-        <v>3321307.706574913</v>
+        <v>3996247.195240759</v>
       </c>
       <c r="E74">
-        <v>358.4285977832414</v>
+        <v>341.0218162783804</v>
       </c>
       <c r="F74">
-        <v>6.411957426316483</v>
+        <v>0.8782048270461216</v>
       </c>
       <c r="G74">
-        <v>0.0008948332470352343</v>
+        <v>0.006855337018019528</v>
       </c>
       <c r="H74">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -2330,19 +2330,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D75">
-        <v>3320322.547557929</v>
+        <v>3996244.295089711</v>
       </c>
       <c r="E75">
-        <v>359.1403658817539</v>
+        <v>341.5245830234199</v>
       </c>
       <c r="F75">
-        <v>6.444493664104918</v>
+        <v>0.8798520026471612</v>
       </c>
       <c r="G75">
-        <v>0.0008902539272607106</v>
+        <v>0.006842501659384884</v>
       </c>
       <c r="H75">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -2356,19 +2356,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D76">
-        <v>3319322.377891812</v>
+        <v>3996241.379889915</v>
       </c>
       <c r="E76">
-        <v>359.8522232435273</v>
+        <v>342.0273500045798</v>
       </c>
       <c r="F76">
-        <v>6.477362620248942</v>
+        <v>0.8815051032984196</v>
       </c>
       <c r="G76">
-        <v>0.0008856741902382743</v>
+        <v>0.006829668355716145</v>
       </c>
       <c r="H76">
-        <v>0.006468277148910672</v>
+        <v>0.013057925765368</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -2382,19 +2382,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D77">
-        <v>3318306.887951222</v>
+        <v>3996238.449535376</v>
       </c>
       <c r="E77">
-        <v>360.5641712117983</v>
+        <v>342.5301172230853</v>
       </c>
       <c r="F77">
-        <v>6.510569473828069</v>
+        <v>0.883164160888423</v>
       </c>
       <c r="G77">
-        <v>0.0008810940246185995</v>
+        <v>0.006816837107576435</v>
       </c>
       <c r="H77">
-        <v>0.006468277148910681</v>
+        <v>0.01305792576536798</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -2408,19 +2408,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D78">
-        <v>3317275.760019564</v>
+        <v>3996235.503919153</v>
       </c>
       <c r="E78">
-        <v>361.2762111570909</v>
+        <v>343.0328846801698</v>
       </c>
       <c r="F78">
-        <v>6.544119512930488</v>
+        <v>0.8848292075348558</v>
       </c>
       <c r="G78">
-        <v>0.0008765134188249018</v>
+        <v>0.006804007915528881</v>
       </c>
       <c r="H78">
-        <v>0.006468277148910681</v>
+        <v>0.01305792576536798</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -2434,19 +2434,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D79">
-        <v>3316228.668032021</v>
+        <v>3996232.542933358</v>
       </c>
       <c r="E79">
-        <v>361.9883444779169</v>
+        <v>343.535652377076</v>
       </c>
       <c r="F79">
-        <v>6.578018137558922</v>
+        <v>0.8865002755866223</v>
       </c>
       <c r="G79">
-        <v>0.000871932361047239</v>
+        <v>0.006791180780136643</v>
       </c>
       <c r="H79">
-        <v>0.006468277148910681</v>
+        <v>0.01305792576536798</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -2460,19 +2460,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D80">
-        <v>3315165.277308962</v>
+        <v>3996229.566469136</v>
       </c>
       <c r="E80">
-        <v>362.700572601498</v>
+        <v>344.0384203150549</v>
       </c>
       <c r="F80">
-        <v>6.612270862630695</v>
+        <v>0.8881773976259308</v>
       </c>
       <c r="G80">
-        <v>0.0008673508392366054</v>
+        <v>0.006778355701962857</v>
       </c>
       <c r="H80">
-        <v>0.006468277148910681</v>
+        <v>0.01305792576536798</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -2486,19 +2486,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D81">
-        <v>3314085.244279277</v>
+        <v>3996226.574416664</v>
       </c>
       <c r="E81">
-        <v>363.4128969845111</v>
+        <v>344.5411884953666</v>
       </c>
       <c r="F81">
-        <v>6.646883321075436</v>
+        <v>0.8898606064704024</v>
       </c>
       <c r="G81">
-        <v>0.000862768841098868</v>
+        <v>0.006765532681570662</v>
       </c>
       <c r="H81">
-        <v>0.006468277148910681</v>
+        <v>0.01305792576536798</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -2512,19 +2512,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D82">
-        <v>3312988.216193237</v>
+        <v>3996223.566665135</v>
       </c>
       <c r="E82">
-        <v>364.125319113856</v>
+        <v>345.0439569192799</v>
       </c>
       <c r="F82">
-        <v>6.681861267034241</v>
+        <v>0.8915499351751962</v>
       </c>
       <c r="G82">
-        <v>0.0008581863540885112</v>
+        <v>0.006752711719523245</v>
       </c>
       <c r="H82">
-        <v>0.006468277148910681</v>
+        <v>0.01305792576536798</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -2538,19 +2538,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D83">
-        <v>3311873.830824388</v>
+        <v>3996220.543102748</v>
       </c>
       <c r="E83">
-        <v>364.8378405074485</v>
+        <v>345.5467255880729</v>
       </c>
       <c r="F83">
-        <v>6.717210579164193</v>
+        <v>0.8932454170351708</v>
       </c>
       <c r="G83">
-        <v>0.000853603365402178</v>
+        <v>0.006739892816383735</v>
       </c>
       <c r="H83">
-        <v>0.006468277148910681</v>
+        <v>0.01305792576536798</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -2564,19 +2564,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D84">
-        <v>3310741.71616001</v>
+        <v>3996217.503616699</v>
       </c>
       <c r="E84">
-        <v>365.5504627150381</v>
+        <v>346.0494945030327</v>
       </c>
       <c r="F84">
-        <v>6.752937264052361</v>
+        <v>0.8949470855870533</v>
       </c>
       <c r="G84">
-        <v>0.0008490198619720312</v>
+        <v>0.006727075972715289</v>
       </c>
       <c r="H84">
-        <v>0.006468277148910681</v>
+        <v>0.01305792576536798</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -2590,19 +2590,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D85">
-        <v>3309591.490079639</v>
+        <v>3996214.448093169</v>
       </c>
       <c r="E85">
-        <v>366.2631873190517</v>
+        <v>346.5522636654556</v>
       </c>
       <c r="F85">
-        <v>6.789047459743499</v>
+        <v>0.8966549746116455</v>
       </c>
       <c r="G85">
-        <v>0.0008444358304588856</v>
+        <v>0.006714261189081043</v>
       </c>
       <c r="H85">
-        <v>0.006468277148910681</v>
+        <v>0.01305792576536798</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -2616,19 +2616,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D86">
-        <v>3308422.7600211</v>
+        <v>3996211.376417313</v>
       </c>
       <c r="E86">
-        <v>366.976015935465</v>
+        <v>347.055033076647</v>
       </c>
       <c r="F86">
-        <v>6.825547439385984</v>
+        <v>0.8983691181360418</v>
       </c>
       <c r="G86">
-        <v>0.000839851257245142</v>
+        <v>0.006701448466044151</v>
       </c>
       <c r="H86">
-        <v>0.006468277148910681</v>
+        <v>0.01305792576536798</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -2642,19 +2642,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D87">
-        <v>3307235.122633511</v>
+        <v>3996208.288473248</v>
       </c>
       <c r="E87">
-        <v>367.6889502147018</v>
+        <v>347.5578027379219</v>
       </c>
       <c r="F87">
-        <v>6.862443615000607</v>
+        <v>0.900089550435887</v>
       </c>
       <c r="G87">
-        <v>0.0008352661284274916</v>
+        <v>0.00668863780416772</v>
       </c>
       <c r="H87">
-        <v>0.006468277148910681</v>
+        <v>0.01305792576536798</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -2668,19 +2668,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D88">
-        <v>3306028.163416653</v>
+        <v>3996205.184144045</v>
       </c>
       <c r="E88">
-        <v>368.4019918425624</v>
+        <v>348.0605726506045</v>
       </c>
       <c r="F88">
-        <v>6.899742541377174</v>
+        <v>0.9018163060376424</v>
       </c>
       <c r="G88">
-        <v>0.000830680429809386</v>
+        <v>0.006675829204014871</v>
       </c>
       <c r="H88">
-        <v>0.006468277148910681</v>
+        <v>0.01305792576536798</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -2694,19 +2694,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D89">
-        <v>3304801.456346103</v>
+        <v>3996202.063311712</v>
       </c>
       <c r="E89">
-        <v>369.1151425411824</v>
+        <v>348.5633428160287</v>
       </c>
       <c r="F89">
-        <v>6.937450920103951</v>
+        <v>0.903549419720889</v>
       </c>
       <c r="G89">
-        <v>0.0008260941468932742</v>
+        <v>0.006663022666148686</v>
       </c>
       <c r="H89">
-        <v>0.006468277148910681</v>
+        <v>0.01305792576536798</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -2720,19 +2720,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D90">
-        <v>3303554.563483458</v>
+        <v>3996198.92585719</v>
       </c>
       <c r="E90">
-        <v>369.8284040700232</v>
+        <v>349.0661132355379</v>
       </c>
       <c r="F90">
-        <v>6.975575603735324</v>
+        <v>0.9052889265206472</v>
       </c>
       <c r="G90">
-        <v>0.0008215072648725893</v>
+        <v>0.006650218191132272</v>
       </c>
       <c r="H90">
-        <v>0.006468277148910681</v>
+        <v>0.01305792576536798</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -2746,19 +2746,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D91">
-        <v>3302287.034570989</v>
+        <v>3996195.771660332</v>
       </c>
       <c r="E91">
-        <v>370.5417782268955</v>
+        <v>349.5688839104852</v>
       </c>
       <c r="F91">
-        <v>7.014123600103362</v>
+        <v>0.9070348617297326</v>
       </c>
       <c r="G91">
-        <v>0.0008169197686234737</v>
+        <v>0.006637415779528645</v>
       </c>
       <c r="H91">
-        <v>0.006468277148910681</v>
+        <v>0.01305792576536798</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -2772,19 +2772,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D92">
-        <v>3300998.406609982</v>
+        <v>3996192.6005999</v>
       </c>
       <c r="E92">
-        <v>371.255266849016</v>
+        <v>350.0716548422336</v>
       </c>
       <c r="F92">
-        <v>7.053102076778969</v>
+        <v>0.9087872609011252</v>
       </c>
       <c r="G92">
-        <v>0.0008123316426962404</v>
+        <v>0.006624615431900864</v>
       </c>
       <c r="H92">
-        <v>0.006468277148910681</v>
+        <v>0.01305792576536798</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -2798,19 +2798,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D93">
-        <v>3299688.20342202</v>
+        <v>3996189.412553546</v>
       </c>
       <c r="E93">
-        <v>371.9688718141004</v>
+        <v>350.5744260321557</v>
       </c>
       <c r="F93">
-        <v>7.092518365688933</v>
+        <v>0.9105461598503737</v>
       </c>
       <c r="G93">
-        <v>0.0008077428713065531</v>
+        <v>0.00661181714881193</v>
       </c>
       <c r="H93">
-        <v>0.006468277148910681</v>
+        <v>0.01305792576536798</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Tapered Pipe Pressure Drop
</commit_message>
<xml_diff>
--- a/TheEngine/Regen Solver/enginefiles/solverdata.xlsx
+++ b/TheEngine/Regen Solver/enginefiles/solverdata.xlsx
@@ -438,13 +438,13 @@
         <v>283.1374920971622</v>
       </c>
       <c r="F2">
-        <v>6.574894124418069</v>
+        <v>2.127364833503945</v>
       </c>
       <c r="G2">
-        <v>0.002125569134778001</v>
+        <v>0.006569344286977639</v>
       </c>
       <c r="H2">
-        <v>0.003400523745523518</v>
+        <v>0.01343119089470079</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -458,19 +458,19 @@
         <v>0.03093226317788614</v>
       </c>
       <c r="D3">
-        <v>3999493.656343908</v>
+        <v>3999976.256447726</v>
       </c>
       <c r="E3">
-        <v>283.1322222689139</v>
+        <v>283.1372449945611</v>
       </c>
       <c r="F3">
-        <v>7.292518926382241</v>
+        <v>2.446224249311697</v>
       </c>
       <c r="G3">
-        <v>0.001994361680556717</v>
+        <v>0.005933571181356647</v>
       </c>
       <c r="H3">
-        <v>0.003117014327055604</v>
+        <v>0.01200398052498067</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -484,19 +484,19 @@
         <v>0.03010170940624797</v>
       </c>
       <c r="D4">
-        <v>3998836.30079556</v>
+        <v>3999279.550752181</v>
       </c>
       <c r="E4">
-        <v>283.1253800280105</v>
+        <v>283.1299937919079</v>
       </c>
       <c r="F4">
-        <v>8.110020875883675</v>
+        <v>2.815538254827025</v>
       </c>
       <c r="G4">
-        <v>0.001869249896793794</v>
+        <v>0.005362386487542141</v>
       </c>
       <c r="H4">
-        <v>0.002850996294776099</v>
+        <v>0.01071425895107017</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -510,19 +510,19 @@
         <v>0.02927115563460979</v>
       </c>
       <c r="D5">
-        <v>3997977.55116158</v>
+        <v>3998350.248801796</v>
       </c>
       <c r="E5">
-        <v>283.1164402701226</v>
+        <v>283.1203203033534</v>
       </c>
       <c r="F5">
-        <v>9.045188106139113</v>
+        <v>3.244638571444561</v>
       </c>
       <c r="G5">
-        <v>0.001749949695515622</v>
+        <v>0.004848018063129506</v>
       </c>
       <c r="H5">
-        <v>0.002601654519005404</v>
+        <v>0.009548313517041759</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -536,19 +536,19 @@
         <v>0.02844060186297162</v>
       </c>
       <c r="D6">
-        <v>3996848.118999828</v>
+        <v>3997105.292131567</v>
       </c>
       <c r="E6">
-        <v>283.1046804800845</v>
+        <v>283.1073584161916</v>
       </c>
       <c r="F6">
-        <v>10.11982003615402</v>
+        <v>3.74511681032471</v>
       </c>
       <c r="G6">
-        <v>0.001636186558824927</v>
+        <v>0.004383682879079729</v>
       </c>
       <c r="H6">
-        <v>0.002368202693164735</v>
+        <v>0.008493994991080374</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -562,19 +562,19 @@
         <v>0.02761004809133344</v>
       </c>
       <c r="D7">
-        <v>3995351.793248411</v>
+        <v>3995428.503951395</v>
       </c>
       <c r="E7">
-        <v>283.089096745351</v>
+        <v>283.0898957672214</v>
       </c>
       <c r="F7">
-        <v>11.36086916836467</v>
+        <v>4.331387284077963</v>
       </c>
       <c r="G7">
-        <v>0.001527692803328674</v>
+        <v>0.003963521784677563</v>
       </c>
       <c r="H7">
-        <v>0.002149880354605342</v>
+        <v>0.007540499733811276</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -588,19 +588,19 @@
         <v>0.02677949431969527</v>
       </c>
       <c r="D8">
-        <v>3993353.562282624</v>
+        <v>3993155.980822924</v>
       </c>
       <c r="E8">
-        <v>283.0682790726366</v>
+        <v>283.066220238503</v>
       </c>
       <c r="F8">
-        <v>12.80199694933094</v>
+        <v>5.021561298400524</v>
       </c>
       <c r="G8">
-        <v>0.001424204012315278</v>
+        <v>0.003582443795933155</v>
       </c>
       <c r="H8">
-        <v>0.001945949372032706</v>
+        <v>0.006678182677868835</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -614,19 +614,19 @@
         <v>0.02594894054805708</v>
       </c>
       <c r="D9">
-        <v>3990661.743703191</v>
+        <v>3990053.722027511</v>
       </c>
       <c r="E9">
-        <v>283.0402233325322</v>
+        <v>283.0338842216633</v>
       </c>
       <c r="F9">
-        <v>14.48573865055291</v>
+        <v>5.838673374988801</v>
       </c>
       <c r="G9">
-        <v>0.001325454090211187</v>
+        <v>0.003235993341741126</v>
       </c>
       <c r="H9">
-        <v>0.001755689485580121</v>
+        <v>0.005898394166925096</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -640,19 +640,19 @@
         <v>0.02511838677641891</v>
       </c>
       <c r="D10">
-        <v>3987000.627102743</v>
+        <v>3985783.054539075</v>
       </c>
       <c r="E10">
-        <v>283.0020424213474</v>
+        <v>282.9893388778659</v>
       </c>
       <c r="F10">
-        <v>16.46659477451381</v>
+        <v>6.812448653519233</v>
       </c>
       <c r="G10">
-        <v>0.001231167910179601</v>
+        <v>0.002920233066833746</v>
       </c>
       <c r="H10">
-        <v>0.001578392143770472</v>
+        <v>0.005193333628574868</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -666,19 +666,19 @@
         <v>0.02428783300478073</v>
       </c>
       <c r="D11">
-        <v>3981967.737246613</v>
+        <v>3979845.919344942</v>
       </c>
       <c r="E11">
-        <v>282.9495130907549</v>
+        <v>282.9273524554824</v>
       </c>
       <c r="F11">
-        <v>18.81559267017348</v>
+        <v>7.981940225141827</v>
       </c>
       <c r="G11">
-        <v>0.001141049639992707</v>
+        <v>0.002631633666434023</v>
       </c>
       <c r="H11">
-        <v>0.001413351167241513</v>
+        <v>0.004555911539060774</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -692,19 +692,19 @@
         <v>0.02345727923314256</v>
       </c>
       <c r="D12">
-        <v>3974965.439767879</v>
+        <v>3971495.743555272</v>
       </c>
       <c r="E12">
-        <v>282.8763465614558</v>
+        <v>282.8400564792742</v>
       </c>
       <c r="F12">
-        <v>21.62731445396437</v>
+        <v>9.399647648636927</v>
       </c>
       <c r="G12">
-        <v>0.001054762764290714</v>
+        <v>0.002366958263891961</v>
       </c>
       <c r="H12">
-        <v>0.001259847151208023</v>
+        <v>0.00397960646604165</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -718,19 +718,19 @@
         <v>0.02262672546150438</v>
       </c>
       <c r="D13">
-        <v>3965088.170521055</v>
+        <v>3959586.798240114</v>
       </c>
       <c r="E13">
-        <v>282.7729767806148</v>
+        <v>282.7153197019022</v>
       </c>
       <c r="F13">
-        <v>25.03138506060043</v>
+        <v>11.13835967854074</v>
       </c>
       <c r="G13">
-        <v>0.0009718927961491105</v>
+        <v>0.002123117687450535</v>
       </c>
       <c r="H13">
-        <v>0.00111711846337556</v>
+        <v>0.00345829109325282</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -744,19 +744,19 @@
         <v>0.0217961716898662</v>
       </c>
       <c r="D14">
-        <v>3950929.168513061</v>
+        <v>3942306.748092168</v>
       </c>
       <c r="E14">
-        <v>282.6244629807855</v>
+        <v>282.5338288137144</v>
       </c>
       <c r="F14">
-        <v>29.21293173385055</v>
+        <v>13.30357828515761</v>
       </c>
       <c r="G14">
-        <v>0.0008918695006466142</v>
+        <v>0.00189694021125416</v>
       </c>
       <c r="H14">
-        <v>0.0009843000606588144</v>
+        <v>0.002985962964365312</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -770,19 +770,19 @@
         <v>0.02096561791822803</v>
       </c>
       <c r="D15">
-        <v>3930231.046664037</v>
+        <v>3916667.442647102</v>
       </c>
       <c r="E15">
-        <v>282.406648131928</v>
+        <v>282.2634509079583</v>
       </c>
       <c r="F15">
-        <v>34.45421950396137</v>
+        <v>16.05936348205446</v>
       </c>
       <c r="G15">
-        <v>0.0008137771672714324</v>
+        <v>0.001684685981576166</v>
       </c>
       <c r="H15">
-        <v>0.0008602709751461863</v>
+        <v>0.00255618169108828</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -796,19 +796,19 @@
         <v>0.02013506414658983</v>
       </c>
       <c r="D16">
-        <v>3899200.234144766</v>
+        <v>3877424.310176328</v>
       </c>
       <c r="E16">
-        <v>282.0784989522069</v>
+        <v>281.8470622538139</v>
       </c>
       <c r="F16">
-        <v>41.24143186857295</v>
+        <v>19.69614079985747</v>
       </c>
       <c r="G16">
-        <v>0.0007357595752693622</v>
+        <v>0.001480612543273258</v>
       </c>
       <c r="H16">
-        <v>0.0007431623901165254</v>
+        <v>0.002160383916993799</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -822,19 +822,19 @@
         <v>0.01930451037495166</v>
       </c>
       <c r="D17">
-        <v>3850950.829786114</v>
+        <v>3814295.662641164</v>
       </c>
       <c r="E17">
-        <v>281.5643992634711</v>
+        <v>281.1706401463467</v>
       </c>
       <c r="F17">
-        <v>50.7189556787887</v>
+        <v>24.92456096204876</v>
       </c>
       <c r="G17">
-        <v>0.000651868269835041</v>
+        <v>0.001269493351929316</v>
       </c>
       <c r="H17">
-        <v>0.0006276640903579544</v>
+        <v>0.00177883627040231</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -848,19 +848,19 @@
         <v>0.01956298682688029</v>
       </c>
       <c r="D18">
-        <v>3770468.760120213</v>
+        <v>3700764.998925004</v>
       </c>
       <c r="E18">
-        <v>280.6961499015744</v>
+        <v>279.9330414980626</v>
       </c>
       <c r="F18">
-        <v>63.28562037000471</v>
+        <v>33.01764785494194</v>
       </c>
       <c r="G18">
-        <v>0.000521293643369279</v>
+        <v>0.0009523521120393344</v>
       </c>
       <c r="H18">
-        <v>0.0005180459157867701</v>
+        <v>0.001396757235427562</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -874,19 +874,19 @@
         <v>0.02135258148578198</v>
       </c>
       <c r="D19">
-        <v>3603829.296381239</v>
+        <v>3466954.706184031</v>
       </c>
       <c r="E19">
-        <v>278.853975077268</v>
+        <v>277.2933201147379</v>
       </c>
       <c r="F19">
-        <v>57.47054083405503</v>
+        <v>30.31540904837559</v>
       </c>
       <c r="G19">
-        <v>0.0005125076409397112</v>
+        <v>0.0009228364819717596</v>
       </c>
       <c r="H19">
-        <v>0.0005764673330330602</v>
+        <v>0.001539886770165541</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -900,19 +900,19 @@
         <v>0.0231421761446837</v>
       </c>
       <c r="D20">
-        <v>3469843.184926076</v>
+        <v>3505162.453342678</v>
       </c>
       <c r="E20">
-        <v>277.3267186024111</v>
+        <v>277.7334605013237</v>
       </c>
       <c r="F20">
-        <v>51.32907186594354</v>
+        <v>26.68400815008156</v>
       </c>
       <c r="G20">
-        <v>0.0005208486253160574</v>
+        <v>0.0009397028794474608</v>
       </c>
       <c r="H20">
-        <v>0.0006524110166420991</v>
+        <v>0.001737377960813831</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -926,19 +926,19 @@
         <v>0.02493177080358538</v>
       </c>
       <c r="D21">
-        <v>3368344.38913317</v>
+        <v>3559694.465464081</v>
       </c>
       <c r="E21">
-        <v>276.1406656787618</v>
+        <v>278.3555822246578</v>
       </c>
       <c r="F21">
-        <v>45.889662824079</v>
+        <v>23.46412802573349</v>
       </c>
       <c r="G21">
-        <v>0.0005352112837323898</v>
+        <v>0.0009699714967923297</v>
       </c>
       <c r="H21">
-        <v>0.0007374596967945444</v>
+        <v>0.00196160194440404</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -952,19 +952,19 @@
         <v>0.0267213654624871</v>
       </c>
       <c r="D22">
-        <v>3291832.450887121</v>
+        <v>3602313.314814168</v>
       </c>
       <c r="E22">
-        <v>275.2291440770709</v>
+        <v>278.8369305761914</v>
       </c>
       <c r="F22">
-        <v>41.21182997937813</v>
+        <v>20.74667419975187</v>
       </c>
       <c r="G22">
-        <v>0.000552704849366414</v>
+        <v>0.00100661298573191</v>
       </c>
       <c r="H22">
-        <v>0.0008296764663261318</v>
+        <v>0.002206349654550542</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -978,19 +978,19 @@
         <v>0.02851096012138879</v>
       </c>
       <c r="D23">
-        <v>3233749.937251182</v>
+        <v>3633688.423332382</v>
       </c>
       <c r="E23">
-        <v>274.5267600881633</v>
+        <v>279.1886162891869</v>
       </c>
       <c r="F23">
-        <v>37.21100458326078</v>
+        <v>18.46523064899552</v>
       </c>
       <c r="G23">
-        <v>0.000572085038842507</v>
+        <v>0.001047032973949546</v>
       </c>
       <c r="H23">
-        <v>0.0009282740391306178</v>
+        <v>0.002469165328848003</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1004,19 +1004,19 @@
         <v>0.03030055478029048</v>
       </c>
       <c r="D24">
-        <v>3189182.021084434</v>
+        <v>3656740.71218102</v>
       </c>
       <c r="E24">
-        <v>273.9815175024336</v>
+        <v>279.4455878225033</v>
       </c>
       <c r="F24">
-        <v>33.78288903930657</v>
+        <v>16.54169419159196</v>
       </c>
       <c r="G24">
-        <v>0.0005926983561732853</v>
+        <v>0.001089968282580739</v>
       </c>
       <c r="H24">
-        <v>0.001032841123254559</v>
+        <v>0.002748808877020657</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1030,19 +1030,19 @@
         <v>0.03209014943919218</v>
       </c>
       <c r="D25">
-        <v>3154579.59833112</v>
+        <v>3673848.288034938</v>
       </c>
       <c r="E25">
-        <v>273.5543351662209</v>
+        <v>279.6355208396503</v>
       </c>
       <c r="F25">
-        <v>30.83209608467783</v>
+        <v>14.90877374077251</v>
       </c>
       <c r="G25">
-        <v>0.0006141608344280608</v>
+        <v>0.001134707801445363</v>
       </c>
       <c r="H25">
-        <v>0.001143127153835261</v>
+        <v>0.00304455491867066</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1056,19 +1056,19 @@
         <v>0.03387974409809387</v>
       </c>
       <c r="D26">
-        <v>3127397.264588523</v>
+        <v>3686710.39242345</v>
       </c>
       <c r="E26">
-        <v>273.2163473326287</v>
+        <v>279.7778904426137</v>
       </c>
       <c r="F26">
-        <v>28.27802769280106</v>
+        <v>13.51220610111882</v>
       </c>
       <c r="G26">
-        <v>0.0006362296304661173</v>
+        <v>0.001180813719333998</v>
       </c>
       <c r="H26">
-        <v>0.001258962469789997</v>
+        <v>0.003355934555318804</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1082,19 +1082,19 @@
         <v>0.03566933875699557</v>
       </c>
       <c r="D27">
-        <v>3105801.847238913</v>
+        <v>3696511.209669871</v>
       </c>
       <c r="E27">
-        <v>272.9462935175671</v>
+        <v>279.8861291731661</v>
       </c>
       <c r="F27">
-        <v>26.05444539416503</v>
+        <v>12.30899416776944</v>
       </c>
       <c r="G27">
-        <v>0.0006587428379885813</v>
+        <v>0.001227999132375576</v>
       </c>
       <c r="H27">
-        <v>0.001380223053273553</v>
+        <v>0.003682622002950303</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1108,19 +1108,19 @@
         <v>0.03745893341589727</v>
       </c>
       <c r="D28">
-        <v>3088461.637448158</v>
+        <v>3704076.577554698</v>
       </c>
       <c r="E28">
-        <v>272.7284564755211</v>
+        <v>279.9695352504052</v>
       </c>
       <c r="F28">
-        <v>24.10741572017071</v>
+        <v>11.26513139962166</v>
       </c>
       <c r="G28">
-        <v>0.0006815881115221059</v>
+        <v>0.001276067090568407</v>
       </c>
       <c r="H28">
-        <v>0.001506812936309283</v>
+        <v>0.004024378382460721</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1134,19 +1134,19 @@
         <v>0.03924852807479898</v>
       </c>
       <c r="D29">
-        <v>3074399.031964082</v>
+        <v>3709987.748274246</v>
       </c>
       <c r="E29">
-        <v>272.5511371870148</v>
+        <v>280.034616836658</v>
       </c>
       <c r="F29">
-        <v>22.39308175738487</v>
+        <v>10.35360961192639</v>
       </c>
       <c r="G29">
-        <v>0.0007046850029242986</v>
+        <v>0.001324877433560469</v>
       </c>
       <c r="H29">
-        <v>0.00163865458552784</v>
+        <v>0.004381021200659751</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1160,19 +1160,19 @@
         <v>0.04103812273370067</v>
       </c>
       <c r="D30">
-        <v>3062888.396573951</v>
+        <v>3714658.825351367</v>
       </c>
       <c r="E30">
-        <v>272.4055548092173</v>
+        <v>280.0859909746891</v>
       </c>
       <c r="F30">
-        <v>20.87569134448964</v>
+        <v>9.552836555596853</v>
       </c>
       <c r="G30">
-        <v>0.0007279744169477189</v>
+        <v>0.001374327498536356</v>
       </c>
       <c r="H30">
-        <v>0.001775683257435125</v>
+        <v>0.00475240655845208</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1186,19 +1186,19 @@
         <v>0.04282771739260237</v>
       </c>
       <c r="D31">
-        <v>3053385.142026707</v>
+        <v>3718388.676611534</v>
       </c>
       <c r="E31">
-        <v>272.2850595413605</v>
+        <v>280.1269789600093</v>
       </c>
       <c r="F31">
-        <v>19.52597140831083</v>
+        <v>8.845419594571592</v>
       </c>
       <c r="G31">
-        <v>0.0007514120171848434</v>
+        <v>0.001424340291473215</v>
       </c>
       <c r="H31">
-        <v>0.001917843486908414</v>
+        <v>0.005138418164278358</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1212,19 +1212,19 @@
         <v>0.04461731205150407</v>
       </c>
       <c r="D32">
-        <v>3045476.142610251</v>
+        <v>3721395.793713924</v>
       </c>
       <c r="E32">
-        <v>272.18456937714</v>
+        <v>280.1600026052305</v>
       </c>
       <c r="F32">
-        <v>18.31982663944789</v>
+        <v>8.21724022927661</v>
       </c>
       <c r="G32">
-        <v>0.0007749639432299351</v>
+        <v>0.001474856919302278</v>
       </c>
       <c r="H32">
-        <v>0.00206508679493743</v>
+        <v>0.005538960218507878</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1238,19 +1238,19 @@
         <v>0.04640690671040576</v>
       </c>
       <c r="D33">
-        <v>3038844.761885709</v>
+        <v>3723841.897653683</v>
       </c>
       <c r="E33">
-        <v>272.1001653588997</v>
+        <v>280.1868507759367</v>
       </c>
       <c r="F33">
-        <v>17.23731056038683</v>
+        <v>7.656750295506229</v>
       </c>
       <c r="G33">
-        <v>0.000798603939764653</v>
+        <v>0.0015258315749364</v>
       </c>
       <c r="H33">
-        <v>0.002217370129991288</v>
+        <v>0.005953952615388959</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1264,19 +1264,19 @@
         <v>0.04819650136930748</v>
       </c>
       <c r="D34">
-        <v>3033245.934332494</v>
+        <v>3725848.102718037</v>
       </c>
       <c r="E34">
-        <v>272.0287988473288</v>
+        <v>280.2088609495695</v>
       </c>
       <c r="F34">
-        <v>16.26181522526103</v>
+        <v>7.154434636436086</v>
       </c>
       <c r="G34">
-        <v>0.0008223113799565662</v>
+        <v>0.001577228114498745</v>
       </c>
       <c r="H34">
-        <v>0.002374654770624517</v>
+        <v>0.00638332759444184</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1290,19 +1290,19 @@
         <v>0.04998609602820916</v>
       </c>
       <c r="D35">
-        <v>3028488.227280665</v>
+        <v>3727506.12004255</v>
       </c>
       <c r="E35">
-        <v>271.9680781854831</v>
+        <v>280.2270445368591</v>
       </c>
       <c r="F35">
-        <v>15.37943286156799</v>
+        <v>6.702398383383314</v>
       </c>
       <c r="G35">
-        <v>0.0008460698729149681</v>
+        <v>0.001629017661683631</v>
       </c>
       <c r="H35">
-        <v>0.002536905529055699</v>
+        <v>0.006827027332510341</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1316,19 +1316,19 @@
         <v>0.05177569068711085</v>
       </c>
       <c r="D36">
-        <v>3024420.79414542</v>
+        <v>3728886.119125864</v>
       </c>
       <c r="E36">
-        <v>271.9161119454005</v>
+        <v>280.2421745271858</v>
       </c>
       <c r="F36">
-        <v>14.57845156773946</v>
+        <v>6.294047716243674</v>
       </c>
       <c r="G36">
-        <v>0.000869866262807917</v>
+        <v>0.001681176894207134</v>
       </c>
       <c r="H36">
-        <v>0.002704090157697462</v>
+        <v>0.00728500216648724</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1342,19 +1342,19 @@
         <v>0.05356528534601257</v>
       </c>
       <c r="D37">
-        <v>3020923.789271637</v>
+        <v>3730042.311123099</v>
       </c>
       <c r="E37">
-        <v>271.8713927791278</v>
+        <v>280.2548475664669</v>
       </c>
       <c r="F37">
-        <v>13.84895526484518</v>
+        <v>5.923841100981178</v>
       </c>
       <c r="G37">
-        <v>0.0008936898967259904</v>
+        <v>0.001733686794674878</v>
       </c>
       <c r="H37">
-        <v>0.002876178896497673</v>
+        <v>0.007757209251000137</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1368,19 +1368,19 @@
         <v>0.05535488000491426</v>
       </c>
       <c r="D38">
-        <v>3017901.257173637</v>
+        <v>3731016.960422047</v>
       </c>
       <c r="E38">
-        <v>271.8327106317425</v>
+        <v>280.2655284608042</v>
       </c>
       <c r="F38">
-        <v>13.18250479852524</v>
+        <v>5.587094000205509</v>
       </c>
       <c r="G38">
-        <v>0.0009175320807288851</v>
+        <v>0.001786531724662545</v>
       </c>
       <c r="H38">
-        <v>0.003053144120508089</v>
+        <v>0.008243611523762929</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1394,19 +1394,19 @@
         <v>0.05714447466381595</v>
       </c>
       <c r="D39">
-        <v>3015275.808000973</v>
+        <v>3731843.299040137</v>
       </c>
       <c r="E39">
-        <v>271.7990873571715</v>
+        <v>280.2745824487235</v>
       </c>
       <c r="F39">
-        <v>12.57188238977447</v>
+        <v>5.279824440156543</v>
       </c>
       <c r="G39">
-        <v>0.00094138567000895</v>
+        <v>0.001839698728029017</v>
       </c>
       <c r="H39">
-        <v>0.003234960060294455</v>
+        <v>0.008744176893104621</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1420,19 +1420,19 @@
         <v>0.05893406932271766</v>
       </c>
       <c r="D40">
-        <v>3012984.594866702</v>
+        <v>3732547.666296029</v>
       </c>
       <c r="E40">
-        <v>271.7697270619443</v>
+        <v>280.2822988581634</v>
       </c>
       <c r="F40">
-        <v>12.01088573590646</v>
+        <v>4.998630019494733</v>
       </c>
       <c r="G40">
-        <v>0.0009652447563134582</v>
+        <v>0.001893176999888423</v>
       </c>
       <c r="H40">
-        <v>0.003421602576784161</v>
+        <v>0.009258877590354167</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1446,19 +1446,19 @@
         <v>0.06072366398161935</v>
       </c>
       <c r="D41">
-        <v>3010976.248835387</v>
+        <v>3733151.095409825</v>
       </c>
       <c r="E41">
-        <v>271.7439781000184</v>
+        <v>280.2889086258325</v>
       </c>
       <c r="F41">
-        <v>11.4941612117957</v>
+        <v>4.740589291591262</v>
       </c>
       <c r="G41">
-        <v>0.0009891044266852481</v>
+        <v>0.001946957476645398</v>
       </c>
       <c r="H41">
-        <v>0.003613048976768559</v>
+        <v>0.00978768964459311</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1472,19 +1472,19 @@
         <v>0.06251325864052105</v>
       </c>
       <c r="D42">
-        <v>3009208.524657483</v>
+        <v>3733670.501109144</v>
       </c>
       <c r="E42">
-        <v>271.7213037669655</v>
+        <v>280.2945973964998</v>
       </c>
       <c r="F42">
-        <v>11.01706801491969</v>
+        <v>4.503182173424716</v>
       </c>
       <c r="G42">
-        <v>0.001012960575465256</v>
+        <v>0.002001032516321014</v>
       </c>
       <c r="H42">
-        <v>0.003809277860186856</v>
+        <v>0.01033059245229232</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1498,19 +1498,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D43">
-        <v>3007646.478505011</v>
+        <v>3734119.576520678</v>
       </c>
       <c r="E43">
-        <v>271.7012595397246</v>
+        <v>280.2995154064951</v>
       </c>
       <c r="F43">
-        <v>10.85441598434371</v>
+        <v>4.401351606676412</v>
       </c>
       <c r="G43">
-        <v>0.001024717080907827</v>
+        <v>0.002029501490233691</v>
       </c>
       <c r="H43">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1524,19 +1524,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D44">
-        <v>3006367.491835956</v>
+        <v>3734239.079031678</v>
       </c>
       <c r="E44">
-        <v>271.6848418805948</v>
+        <v>280.3008240542054</v>
       </c>
       <c r="F44">
-        <v>11.0466238948618</v>
+        <v>4.448764840990412</v>
       </c>
       <c r="G44">
-        <v>0.001021625939910644</v>
+        <v>0.002026204804352636</v>
       </c>
       <c r="H44">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1550,19 +1550,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D45">
-        <v>3005058.145044861</v>
+        <v>3733979.054884622</v>
       </c>
       <c r="E45">
-        <v>271.668029221526</v>
+        <v>280.2979765430619</v>
       </c>
       <c r="F45">
-        <v>11.24494721938051</v>
+        <v>4.497257376938184</v>
       </c>
       <c r="G45">
-        <v>0.001018517734222024</v>
+        <v>0.002022858129765588</v>
       </c>
       <c r="H45">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1576,19 +1576,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D46">
-        <v>3003717.325663697</v>
+        <v>3733714.119876452</v>
       </c>
       <c r="E46">
-        <v>271.6508068950135</v>
+        <v>280.295075102754</v>
       </c>
       <c r="F46">
-        <v>11.44967360610583</v>
+        <v>4.546693280801645</v>
       </c>
       <c r="G46">
-        <v>0.001015392062861266</v>
+        <v>0.00201950501547831</v>
       </c>
       <c r="H46">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1602,19 +1602,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D47">
-        <v>3002343.86447444</v>
+        <v>3733444.566687003</v>
       </c>
       <c r="E47">
-        <v>271.6331594759914</v>
+        <v>280.2921229303549</v>
       </c>
       <c r="F47">
-        <v>11.66110883139712</v>
+        <v>4.597099342657454</v>
       </c>
       <c r="G47">
-        <v>0.001012248508322918</v>
+        <v>0.002016145479740292</v>
       </c>
       <c r="H47">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1628,19 +1628,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D48">
-        <v>3000936.531737396</v>
+        <v>3733170.274159531</v>
       </c>
       <c r="E48">
-        <v>271.6150707309127</v>
+        <v>280.2891186907302</v>
       </c>
       <c r="F48">
-        <v>11.87957824407382</v>
+        <v>4.648503561197308</v>
       </c>
       <c r="G48">
-        <v>0.00100908663558558</v>
+        <v>0.002012779493067179</v>
       </c>
       <c r="H48">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1654,19 +1654,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D49">
-        <v>2999494.033107269</v>
+        <v>3732891.116318146</v>
       </c>
       <c r="E49">
-        <v>271.5965235625706</v>
+        <v>280.2860609955256</v>
       </c>
       <c r="F49">
-        <v>12.10542834976442</v>
+        <v>4.700935012781206</v>
       </c>
       <c r="G49">
-        <v>0.001005905991041858</v>
+        <v>0.002009407026336452</v>
       </c>
       <c r="H49">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1680,19 +1680,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D50">
-        <v>2998015.005205786</v>
+        <v>3732606.962625397</v>
       </c>
       <c r="E50">
-        <v>271.5774999502302</v>
+        <v>280.2829484059595</v>
       </c>
       <c r="F50">
-        <v>12.3390285513874</v>
+        <v>4.754423903403302</v>
       </c>
       <c r="G50">
-        <v>0.001002706101341645</v>
+        <v>0.002006028050879204</v>
       </c>
       <c r="H50">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -1706,19 +1706,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D51">
-        <v>2996498.010815988</v>
+        <v>3732317.677771894</v>
       </c>
       <c r="E51">
-        <v>271.5579808845932</v>
+        <v>280.2797794304925</v>
       </c>
       <c r="F51">
-        <v>12.58077306400043</v>
+        <v>4.809001623922494</v>
       </c>
       <c r="G51">
-        <v>0.0009994864721399939</v>
+        <v>0.002002642538519672</v>
       </c>
       <c r="H51">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1732,19 +1732,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D52">
-        <v>2994941.533659165</v>
+        <v>3732023.121453457</v>
       </c>
       <c r="E52">
-        <v>271.5379462970541</v>
+        <v>280.2765525223543</v>
       </c>
       <c r="F52">
-        <v>12.8310830247315</v>
+        <v>4.864700808564451</v>
       </c>
       <c r="G52">
-        <v>0.0009962465867397346</v>
+        <v>0.001999250461616892</v>
       </c>
       <c r="H52">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -1758,19 +1758,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D53">
-        <v>2993343.972710631</v>
+        <v>3731723.148135537</v>
       </c>
       <c r="E53">
-        <v>271.517374982644</v>
+        <v>280.2732660769324</v>
       </c>
       <c r="F53">
-        <v>13.09040882136357</v>
+        <v>4.921555396923318</v>
       </c>
       <c r="G53">
-        <v>0.0009929859046178284</v>
+        <v>0.001995851793108493</v>
       </c>
       <c r="H53">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -1784,19 +1784,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D54">
-        <v>2991703.636005115</v>
+        <v>3731417.606804025</v>
       </c>
       <c r="E54">
-        <v>271.496244515985</v>
+        <v>280.2699184290066</v>
       </c>
       <c r="F54">
-        <v>13.35923266645779</v>
+        <v>4.979600699709806</v>
       </c>
       <c r="G54">
-        <v>0.0009897038598230285</v>
+        <v>0.001992446506556835</v>
       </c>
       <c r="H54">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -1810,19 +1810,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D55">
-        <v>2990018.73387635</v>
+        <v>3731106.34070152</v>
       </c>
       <c r="E55">
-        <v>271.4745311594837</v>
+        <v>280.2665078498244</v>
       </c>
       <c r="F55">
-        <v>13.63807144774615</v>
+        <v>5.038873468512932</v>
       </c>
       <c r="G55">
-        <v>0.0009863998592308809</v>
+        <v>0.00198903457619755</v>
       </c>
       <c r="H55">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -1836,19 +1836,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D56">
-        <v>2988287.371568334</v>
+        <v>3730789.187048049</v>
       </c>
       <c r="E56">
-        <v>271.4522097629024</v>
+        <v>280.2630325440015</v>
       </c>
       <c r="F56">
-        <v>13.92747988999834</v>
+        <v>5.099411969864311</v>
       </c>
       <c r="G56">
-        <v>0.0009830732806402141</v>
+        <v>0.001985615976990604</v>
       </c>
       <c r="H56">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -1862,19 +1862,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D57">
-        <v>2986507.541147554</v>
+        <v>3730465.976745162</v>
       </c>
       <c r="E57">
-        <v>271.4292536533265</v>
+        <v>280.2594906462376</v>
       </c>
       <c r="F57">
-        <v>14.2280540687917</v>
+        <v>5.161256063918075</v>
       </c>
       <c r="G57">
-        <v>0.0009797234706932247</v>
+        <v>0.00198219068467399</v>
       </c>
       <c r="H57">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -1888,19 +1888,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D58">
-        <v>2984677.112636096</v>
+        <v>3730136.53406219</v>
       </c>
       <c r="E58">
-        <v>271.4056345144172</v>
+        <v>280.2558802178352</v>
       </c>
       <c r="F58">
-        <v>14.54043532272332</v>
+        <v>5.224447288085892</v>
       </c>
       <c r="G58">
-        <v>0.0009763497425988166</v>
+        <v>0.001978758675820171</v>
       </c>
       <c r="H58">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -1914,19 +1914,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D59">
-        <v>2982793.824274667</v>
+        <v>3729800.676303431</v>
       </c>
       <c r="E59">
-        <v>271.3813222536859</v>
+        <v>280.2521992430023</v>
       </c>
       <c r="F59">
-        <v>14.86531461777422</v>
+        <v>5.289028945995463</v>
       </c>
       <c r="G59">
-        <v>0.0009729513736360609</v>
+        <v>0.001975319927895411</v>
       </c>
       <c r="H59">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -1940,19 +1940,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D60">
-        <v>2980855.271812024</v>
+        <v>3729458.21345485</v>
       </c>
       <c r="E60">
-        <v>271.3562848563552</v>
+        <v>280.2484456249331</v>
       </c>
       <c r="F60">
-        <v>15.2034374259729</v>
+        <v>5.355046202172292</v>
       </c>
       <c r="G60">
-        <v>0.0009695276024113563</v>
+        <v>0.001971874419322056</v>
       </c>
       <c r="H60">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -1966,19 +1966,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D61">
-        <v>2978858.896702721</v>
+        <v>3729108.947808814</v>
       </c>
       <c r="E61">
-        <v>271.3304882241559</v>
+        <v>280.2446171816371</v>
       </c>
       <c r="F61">
-        <v>15.55560919046717</v>
+        <v>5.42254618287968</v>
       </c>
       <c r="G61">
-        <v>0.0009660776258391803</v>
+        <v>0.001968422129543956</v>
       </c>
       <c r="H61">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -1992,19 +1992,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D62">
-        <v>2976801.973078101</v>
+        <v>3728752.673565234</v>
       </c>
       <c r="E62">
-        <v>271.3038959971875</v>
+        <v>280.2407116415114</v>
       </c>
       <c r="F62">
-        <v>15.92270146090498</v>
+        <v>5.491578083589776</v>
       </c>
       <c r="G62">
-        <v>0.0009626005958117581</v>
+        <v>0.001964963039095095</v>
       </c>
       <c r="H62">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2018,19 +2018,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D63">
-        <v>2974681.593335681</v>
+        <v>3728389.176407333</v>
       </c>
       <c r="E63">
-        <v>271.2764693566738</v>
+        <v>280.2367266386254</v>
       </c>
       <c r="F63">
-        <v>16.30565879703578</v>
+        <v>5.562193283600706</v>
       </c>
       <c r="G63">
-        <v>0.0009590956155179716</v>
+        <v>0.001961497129671587</v>
       </c>
       <c r="H63">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2044,19 +2044,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D64">
-        <v>2972494.652168879</v>
+        <v>3728018.233050141</v>
       </c>
       <c r="E64">
-        <v>271.2481668061347</v>
+        <v>280.2326597077061</v>
       </c>
       <c r="F64">
-        <v>16.70550655514231</v>
+        <v>5.634445468361042</v>
       </c>
       <c r="G64">
-        <v>0.0009555617353656243</v>
+        <v>0.00195802438420713</v>
       </c>
       <c r="H64">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2070,19 +2070,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D65">
-        <v>2970237.828831851</v>
+        <v>3727639.610759623</v>
       </c>
       <c r="E65">
-        <v>271.2189439281009</v>
+        <v>280.2285082787923</v>
       </c>
       <c r="F65">
-        <v>17.12335969188705</v>
+        <v>5.708390760113994</v>
       </c>
       <c r="G65">
-        <v>0.0009519979484541235</v>
+        <v>0.001954544786952078</v>
       </c>
       <c r="H65">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2096,19 +2096,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D66">
-        <v>2967907.567402083</v>
+        <v>3727253.066840154</v>
       </c>
       <c r="E66">
-        <v>271.18875311305</v>
+        <v>280.224269671538</v>
       </c>
       <c r="F66">
-        <v>17.56043274413826</v>
+        <v>5.784087857529938</v>
       </c>
       <c r="G66">
-        <v>0.0009484031855361735</v>
+        <v>0.001951058323556169</v>
       </c>
       <c r="H66">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -2122,19 +2122,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D67">
-        <v>2965500.054765551</v>
+        <v>3726858.348087872</v>
       </c>
       <c r="E67">
-        <v>271.1575432567103</v>
+        <v>280.2199410891344</v>
       </c>
       <c r="F67">
-        <v>18.01805117223959</v>
+        <v>5.861598185058092</v>
       </c>
       <c r="G67">
-        <v>0.0009447763093970257</v>
+        <v>0.001947564981155134</v>
       </c>
       <c r="H67">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2148,19 +2148,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D68">
-        <v>2963011.196004239</v>
+        <v>3726455.190207209</v>
       </c>
       <c r="E68">
-        <v>271.1252594212356</v>
+        <v>280.2155196118221</v>
       </c>
       <c r="F68">
-        <v>18.49766428915454</v>
+        <v>5.940986052797192</v>
       </c>
       <c r="G68">
-        <v>0.0009411161085680125</v>
+        <v>0.001944064748461171</v>
       </c>
       <c r="H68">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -2174,19 +2174,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D69">
-        <v>2960436.586812333</v>
+        <v>3726043.317187624</v>
       </c>
       <c r="E69">
-        <v>271.0918424550039</v>
+        <v>280.2110021899583</v>
       </c>
       <c r="F69">
-        <v>19.00086004040275</v>
+        <v>6.022318827760974</v>
       </c>
       <c r="G69">
-        <v>0.0009374212902767614</v>
+        <v>0.001940557615857449</v>
       </c>
       <c r="H69">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2200,19 +2200,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D70">
-        <v>2957771.482503382</v>
+        <v>3725622.44063733</v>
       </c>
       <c r="E70">
-        <v>271.0572285648802</v>
+        <v>280.2063856366051</v>
       </c>
       <c r="F70">
-        <v>19.52938195154887</v>
+        <v>6.105667117498966</v>
       </c>
       <c r="G70">
-        <v>0.0009336904725195305</v>
+        <v>0.001937043575496697</v>
       </c>
       <c r="H70">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2226,19 +2226,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D71">
-        <v>2955010.763093985</v>
+        <v>3725192.259070456</v>
       </c>
       <c r="E71">
-        <v>271.0213488336978</v>
+        <v>280.2016666195969</v>
       </c>
       <c r="F71">
-        <v>20.08514862355839</v>
+        <v>6.191104967126884</v>
       </c>
       <c r="G71">
-        <v>0.0009299221751205248</v>
+        <v>0.001933522621403948</v>
       </c>
       <c r="H71">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -2252,19 +2252,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D72">
-        <v>2952148.893857015</v>
+        <v>3724752.457143782</v>
       </c>
       <c r="E72">
-        <v>270.9841286743925</v>
+        <v>280.1968416530461</v>
       </c>
       <c r="F72">
-        <v>20.6702762346162</v>
+        <v>6.278710070925126</v>
       </c>
       <c r="G72">
-        <v>0.0009261148096182787</v>
+        <v>0.00192999474958346</v>
       </c>
       <c r="H72">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2278,19 +2278,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D73">
-        <v>2949179.880625444</v>
+        <v>3724302.704838779</v>
       </c>
       <c r="E73">
-        <v>270.9454872106351</v>
+        <v>280.1919070882365</v>
       </c>
       <c r="F73">
-        <v>21.28710460390163</v>
+        <v>6.368563999779979</v>
       </c>
       <c r="G73">
-        <v>0.0009222666677890458</v>
+        <v>0.001926459958129861</v>
       </c>
       <c r="H73">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2304,19 +2304,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D74">
-        <v>2946097.218991623</v>
+        <v>3723842.656584304</v>
       </c>
       <c r="E74">
-        <v>270.9053365718612</v>
+        <v>280.1868591038561</v>
       </c>
       <c r="F74">
-        <v>21.93822749339761</v>
+        <v>6.460752445871282</v>
       </c>
       <c r="G74">
-        <v>0.0009183759085804296</v>
+        <v>0.001922918247343459</v>
       </c>
       <c r="H74">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -2330,19 +2330,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D75">
-        <v>2942893.836380548</v>
+        <v>3723371.950314788</v>
       </c>
       <c r="E75">
-        <v>270.8635810882235</v>
+        <v>280.1816936955072</v>
       </c>
       <c r="F75">
-        <v>22.62652797468794</v>
+        <v>6.555365486154924</v>
       </c>
       <c r="G75">
-        <v>0.000914440543183445</v>
+        <v>0.001919369619849704</v>
       </c>
       <c r="H75">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -2356,19 +2356,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D76">
-        <v>2939562.025771231</v>
+        <v>3722890.206458276</v>
       </c>
       <c r="E76">
-        <v>270.8201163680678</v>
+        <v>280.1764066644328</v>
       </c>
       <c r="F76">
-        <v>23.35521987757994</v>
+        <v>6.65249786634936</v>
       </c>
       <c r="G76">
-        <v>0.0009104584179157337</v>
+        <v>0.001915814080722673</v>
       </c>
       <c r="H76">
-        <v>0.003919512004382912</v>
+        <v>0.01063595663842262</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -2382,19 +2382,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D77">
-        <v>2936093.369588038</v>
+        <v>3722397.026848084</v>
       </c>
       <c r="E77">
-        <v>270.774828236919</v>
+        <v>280.1709936053903</v>
       </c>
       <c r="F77">
-        <v>24.12789657782614</v>
+        <v>6.752249307315781</v>
       </c>
       <c r="G77">
-        <v>0.0009064271945200075</v>
+        <v>0.001912251637612436</v>
       </c>
       <c r="H77">
-        <v>0.003919512004382911</v>
+        <v>0.01063595663842261</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -2408,19 +2408,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D78">
-        <v>2932478.65197048</v>
+        <v>3721891.99355119</v>
       </c>
       <c r="E78">
-        <v>270.7275915124675</v>
+        <v>280.1654498935935</v>
       </c>
       <c r="F78">
-        <v>24.94858868763642</v>
+        <v>6.854724835924101</v>
       </c>
       <c r="G78">
-        <v>0.000902344327396169</v>
+        <v>0.001908682300876028</v>
       </c>
       <c r="H78">
-        <v>0.003919512004382911</v>
+        <v>0.01063595663842261</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -2434,19 +2434,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D79">
-        <v>2928707.757238563</v>
+        <v>3721374.667605753</v>
       </c>
       <c r="E79">
-        <v>270.6782685844161</v>
+        <v>280.1597706706381</v>
       </c>
       <c r="F79">
-        <v>25.82183260584078</v>
+        <v>6.96003514272302</v>
       </c>
       <c r="G79">
-        <v>0.0008982070371784944</v>
+        <v>0.001905106083711803</v>
       </c>
       <c r="H79">
-        <v>0.003919512004382911</v>
+        <v>0.01063595663842261</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -2460,19 +2460,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D80">
-        <v>2924769.5518787</v>
+        <v>3720844.587659353</v>
       </c>
       <c r="E80">
-        <v>270.6267077609637</v>
+        <v>280.1539508293164</v>
       </c>
       <c r="F80">
-        <v>26.75275239270056</v>
+        <v>7.068296968987964</v>
       </c>
       <c r="G80">
-        <v>0.0008940122799340515</v>
+        <v>0.001901523002296673</v>
       </c>
       <c r="H80">
-        <v>0.003919512004382911</v>
+        <v>0.01063595663842261</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -2486,19 +2486,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D81">
-        <v>2920651.746752434</v>
+        <v>3720301.268498627</v>
       </c>
       <c r="E81">
-        <v>270.5727413347152</v>
+        <v>280.1479849972175</v>
       </c>
       <c r="F81">
-        <v>27.74715809612069</v>
+        <v>7.179633526007199</v>
       </c>
       <c r="G81">
-        <v>0.0008897567110871321</v>
+        <v>0.001897933075925768</v>
       </c>
       <c r="H81">
-        <v>0.003919512004382911</v>
+        <v>0.01063595663842261</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -2512,19 +2512,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D82">
-        <v>2916340.735436427</v>
+        <v>3719744.199459947</v>
       </c>
       <c r="E82">
-        <v>270.5161833093298</v>
+        <v>280.141867518995</v>
       </c>
       <c r="F82">
-        <v>28.81166452485623</v>
+        <v>7.294174949790245</v>
       </c>
       <c r="G82">
-        <v>0.0008854366429553391</v>
+        <v>0.001894336327153817</v>
       </c>
       <c r="H82">
-        <v>0.003919512004382911</v>
+        <v>0.01063595663842261</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -2538,19 +2538,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D83">
-        <v>2911821.403582694</v>
+        <v>3719172.842709655</v>
       </c>
       <c r="E83">
-        <v>270.4568267134555</v>
+        <v>280.1355924371741</v>
       </c>
       <c r="F83">
-        <v>29.95383561493277</v>
+        <v>7.412058794747818</v>
       </c>
       <c r="G83">
-        <v>0.0008810479945008352</v>
+        <v>0.001890732781937441</v>
       </c>
       <c r="H83">
-        <v>0.003919512004382911</v>
+        <v>0.01063595663842261</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -2564,19 +2564,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D84">
-        <v>2907076.902868274</v>
+        <v>3718586.631381061</v>
       </c>
       <c r="E84">
-        <v>270.3944404093383</v>
+        <v>280.1291534713552</v>
       </c>
       <c r="F84">
-        <v>31.18236107340593</v>
+        <v>7.533430570305858</v>
       </c>
       <c r="G84">
-        <v>0.0008765862315341512</v>
+        <v>0.00188712246977732</v>
       </c>
       <c r="H84">
-        <v>0.003919512004382911</v>
+        <v>0.01063595663842261</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -2590,19 +2590,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D85">
-        <v>2902088.381380053</v>
+        <v>3717984.967553932</v>
       </c>
       <c r="E85">
-        <v>270.3287652784298</v>
+        <v>280.1225439956513</v>
       </c>
       <c r="F85">
-        <v>32.50727405945555</v>
+        <v>7.658444324884626</v>
       </c>
       <c r="G85">
-        <v>0.0008720462951287421</v>
+        <v>0.001883505423858979</v>
       </c>
       <c r="H85">
-        <v>0.003919512004382911</v>
+        <v>0.01063595663842261</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -2616,19 +2616,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D86">
-        <v>2896834.660009325</v>
+        <v>3717367.220060566</v>
       </c>
       <c r="E86">
-        <v>270.2595096332057</v>
+        <v>280.1157570141831</v>
       </c>
       <c r="F86">
-        <v>33.94022149455659</v>
+        <v>7.787263282205383</v>
       </c>
       <c r="G86">
-        <v>0.0008674225153716213</v>
+        <v>0.001879881681190653</v>
       </c>
       <c r="H86">
-        <v>0.003919512004382911</v>
+        <v>0.01063595663842261</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -2642,19 +2642,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D87">
-        <v>2891291.841408041</v>
+        <v>3716732.722100646</v>
       </c>
       <c r="E87">
-        <v>270.1863436602457</v>
+        <v>280.1087851344296</v>
       </c>
       <c r="F87">
-        <v>35.49480250031544</v>
+        <v>7.920060535491983</v>
       </c>
       <c r="G87">
-        <v>0.0008627085067314475</v>
+        <v>0.001876251282736349</v>
       </c>
       <c r="H87">
-        <v>0.003919512004382911</v>
+        <v>0.01063595663842261</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -2668,19 +2668,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D88">
-        <v>2885432.833993386</v>
+        <v>3716080.768644941</v>
       </c>
       <c r="E88">
-        <v>270.1088926400891</v>
+        <v>280.1016205382091</v>
       </c>
       <c r="F88">
-        <v>37.18699591889232</v>
+        <v>8.057019805823542</v>
       </c>
       <c r="G88">
-        <v>0.000857897040188158</v>
+        <v>0.001872614273541893</v>
       </c>
       <c r="H88">
-        <v>0.003919512004382911</v>
+        <v>0.01063595663842261</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -2694,19 +2694,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D89">
-        <v>2879226.767956797</v>
+        <v>3715410.613605483</v>
       </c>
       <c r="E89">
-        <v>270.0267286081749</v>
+        <v>280.0942549500435</v>
       </c>
       <c r="F89">
-        <v>39.03570559238089</v>
+        <v>8.198336271681208</v>
       </c>
       <c r="G89">
-        <v>0.0008529798857184115</v>
+        <v>0.001868970702851164</v>
       </c>
       <c r="H89">
-        <v>0.003919512004382911</v>
+        <v>0.01063595663842261</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -2720,19 +2720,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D90">
-        <v>2872638.272616707</v>
+        <v>3714721.466747091</v>
       </c>
       <c r="E90">
-        <v>269.9393600090564</v>
+        <v>280.0866796026153</v>
       </c>
       <c r="F90">
-        <v>41.06346316164488</v>
+        <v>8.344217477631908</v>
       </c>
       <c r="G90">
-        <v>0.0008479476165932123</v>
+        <v>0.001865320624209335</v>
       </c>
       <c r="H90">
-        <v>0.003919512004382911</v>
+        <v>0.01063595663842261</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -2746,19 +2746,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D91">
-        <v>2865626.573822938</v>
+        <v>3714012.490311938</v>
       </c>
       <c r="E91">
-        <v>269.8462187391565</v>
+        <v>280.0788851990071</v>
       </c>
       <c r="F91">
-        <v>43.29734430552509</v>
+        <v>8.49488433112365</v>
       </c>
       <c r="G91">
-        <v>0.0008427893639557141</v>
+        <v>0.001861664095549075</v>
       </c>
       <c r="H91">
-        <v>0.003919512004382911</v>
+        <v>0.01063595663842261</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -2772,19 +2772,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D92">
-        <v>2858144.355064607</v>
+        <v>3713282.795325227</v>
       </c>
       <c r="E92">
-        <v>269.7466437504593</v>
+        <v>280.0708618713545</v>
       </c>
       <c r="F92">
-        <v>45.77017830588406</v>
+        <v>8.650572197552655</v>
       </c>
       <c r="G92">
-        <v>0.0008374925059097553</v>
+        <v>0.001858001179255168</v>
       </c>
       <c r="H92">
-        <v>0.003919512004382911</v>
+        <v>0.01063595663842261</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -2798,19 +2798,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D93">
-        <v>2850136.304269683</v>
+        <v>3712531.437545901</v>
       </c>
       <c r="E93">
-        <v>269.6398600658896</v>
+        <v>280.0625991355155</v>
       </c>
       <c r="F93">
-        <v>48.52216702848546</v>
+        <v>8.811532105126679</v>
       </c>
       <c r="G93">
-        <v>0.0008320422692453582</v>
+        <v>0.001854331942201728</v>
       </c>
       <c r="H93">
-        <v>0.003919512004382911</v>
+        <v>0.01063595663842261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Init Solver in Script Form
</commit_message>
<xml_diff>
--- a/TheEngine/Regen Solver/enginefiles/solverdata.xlsx
+++ b/TheEngine/Regen Solver/enginefiles/solverdata.xlsx
@@ -438,13 +438,13 @@
         <v>283.1374920971622</v>
       </c>
       <c r="F2">
-        <v>2.127364833503945</v>
+        <v>2.416999125376964</v>
       </c>
       <c r="G2">
-        <v>0.006569344286977639</v>
+        <v>0.005782125392005105</v>
       </c>
       <c r="H2">
-        <v>0.01343119089470079</v>
+        <v>0.008418753658892325</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -458,19 +458,19 @@
         <v>0.03093226317788614</v>
       </c>
       <c r="D3">
-        <v>3999976.256447726</v>
+        <v>3999966.890974297</v>
       </c>
       <c r="E3">
-        <v>283.1372449945611</v>
+        <v>283.1371475264175</v>
       </c>
       <c r="F3">
-        <v>2.446224249311697</v>
+        <v>2.753444843879728</v>
       </c>
       <c r="G3">
-        <v>0.005933571181356647</v>
+        <v>0.00527152387053591</v>
       </c>
       <c r="H3">
-        <v>0.01200398052498067</v>
+        <v>0.007558211210771029</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -484,19 +484,19 @@
         <v>0.03010170940624797</v>
       </c>
       <c r="D4">
-        <v>3999279.550752181</v>
+        <v>3999133.507116746</v>
       </c>
       <c r="E4">
-        <v>283.1299937919079</v>
+        <v>283.1284736738772</v>
       </c>
       <c r="F4">
-        <v>2.815538254827025</v>
+        <v>3.141448231192683</v>
       </c>
       <c r="G4">
-        <v>0.005362386487542141</v>
+        <v>0.004806088289894771</v>
       </c>
       <c r="H4">
-        <v>0.01071425895107017</v>
+        <v>0.006774855225354175</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -510,19 +510,19 @@
         <v>0.02927115563460979</v>
       </c>
       <c r="D5">
-        <v>3998350.248801796</v>
+        <v>3998036.367530147</v>
       </c>
       <c r="E5">
-        <v>283.1203203033534</v>
+        <v>283.1170526059545</v>
       </c>
       <c r="F5">
-        <v>3.244638571444561</v>
+        <v>3.590441347065426</v>
       </c>
       <c r="G5">
-        <v>0.004848018063129506</v>
+        <v>0.004381141240389579</v>
       </c>
       <c r="H5">
-        <v>0.009548313517041759</v>
+        <v>0.006061776921326648</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -536,19 +536,19 @@
         <v>0.02844060186297162</v>
       </c>
       <c r="D6">
-        <v>3997105.292131567</v>
+        <v>3996584.583766553</v>
       </c>
       <c r="E6">
-        <v>283.1073584161916</v>
+        <v>283.101936162808</v>
       </c>
       <c r="F6">
-        <v>3.74511681032471</v>
+        <v>4.112165934184568</v>
       </c>
       <c r="G6">
-        <v>0.004383682879079729</v>
+        <v>0.003992467591471663</v>
       </c>
       <c r="H6">
-        <v>0.008493994991080374</v>
+        <v>0.005412762554745912</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -562,19 +562,19 @@
         <v>0.02761004809133344</v>
       </c>
       <c r="D7">
-        <v>3995428.503951395</v>
+        <v>3994651.715313523</v>
       </c>
       <c r="E7">
-        <v>283.0898957672214</v>
+        <v>283.0818041778556</v>
       </c>
       <c r="F7">
-        <v>4.331387284077963</v>
+        <v>4.721214888791004</v>
       </c>
       <c r="G7">
-        <v>0.003963521784677563</v>
+        <v>0.003636350641302023</v>
       </c>
       <c r="H7">
-        <v>0.007540499733811276</v>
+        <v>0.004822204939748323</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -588,19 +588,19 @@
         <v>0.02677949431969527</v>
       </c>
       <c r="D8">
-        <v>3993155.980822924</v>
+        <v>3992060.414545513</v>
       </c>
       <c r="E8">
-        <v>283.066220238503</v>
+        <v>283.0548028687699</v>
       </c>
       <c r="F8">
-        <v>5.021561298400524</v>
+        <v>5.435914416709728</v>
       </c>
       <c r="G8">
-        <v>0.003582443795933155</v>
+        <v>0.003309492839352324</v>
       </c>
       <c r="H8">
-        <v>0.006678182677868835</v>
+        <v>0.004285025632101453</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -614,19 +614,19 @@
         <v>0.02594894054805708</v>
       </c>
       <c r="D9">
-        <v>3990053.722027511</v>
+        <v>3988558.873639854</v>
       </c>
       <c r="E9">
-        <v>283.0338842216633</v>
+        <v>283.0182961841772</v>
       </c>
       <c r="F9">
-        <v>5.838673374988801</v>
+        <v>6.279561384435706</v>
       </c>
       <c r="G9">
-        <v>0.003235993341741126</v>
+        <v>0.003008944877084452</v>
       </c>
       <c r="H9">
-        <v>0.005898394166925096</v>
+        <v>0.003796605003955727</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -640,19 +640,19 @@
         <v>0.02511838677641891</v>
       </c>
       <c r="D10">
-        <v>3985783.054539075</v>
+        <v>3983784.529203111</v>
       </c>
       <c r="E10">
-        <v>282.9893388778659</v>
+        <v>282.9684810145089</v>
       </c>
       <c r="F10">
-        <v>6.812448653519233</v>
+        <v>7.282206919339303</v>
       </c>
       <c r="G10">
-        <v>0.002920233066833746</v>
+        <v>0.002732038892357837</v>
       </c>
       <c r="H10">
-        <v>0.005193333628574868</v>
+        <v>0.003352717069395958</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -666,19 +666,19 @@
         <v>0.02428783300478073</v>
       </c>
       <c r="D11">
-        <v>3979845.919344942</v>
+        <v>3977206.783573049</v>
       </c>
       <c r="E11">
-        <v>282.9273524554824</v>
+        <v>282.8997766168991</v>
       </c>
       <c r="F11">
-        <v>7.981940225141827</v>
+        <v>8.483318187221073</v>
       </c>
       <c r="G11">
-        <v>0.002631633666434023</v>
+        <v>0.002476319813695583</v>
       </c>
       <c r="H11">
-        <v>0.004555911539060774</v>
+        <v>0.002949464620111497</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -692,19 +692,19 @@
         <v>0.02345727923314256</v>
       </c>
       <c r="D12">
-        <v>3971495.743555272</v>
+        <v>3968033.934469568</v>
       </c>
       <c r="E12">
-        <v>282.8400564792742</v>
+        <v>282.8038254250035</v>
       </c>
       <c r="F12">
-        <v>9.399647648636927</v>
+        <v>9.935935397890876</v>
       </c>
       <c r="G12">
-        <v>0.002366958263891961</v>
+        <v>0.002239464597771144</v>
       </c>
       <c r="H12">
-        <v>0.00397960646604165</v>
+        <v>0.002583206962112573</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -718,19 +718,19 @@
         <v>0.02262672546150438</v>
       </c>
       <c r="D13">
-        <v>3959586.798240114</v>
+        <v>3955056.233563002</v>
       </c>
       <c r="E13">
-        <v>282.7153197019022</v>
+        <v>282.6677925042071</v>
       </c>
       <c r="F13">
-        <v>11.13835967854074</v>
+        <v>11.71357833549839</v>
       </c>
       <c r="G13">
-        <v>0.002123117687450535</v>
+        <v>0.002019168077601863</v>
       </c>
       <c r="H13">
-        <v>0.00345829109325282</v>
+        <v>0.002250463993749165</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -744,19 +744,19 @@
         <v>0.0217961716898662</v>
       </c>
       <c r="D14">
-        <v>3942306.748092168</v>
+        <v>3936367.839641637</v>
       </c>
       <c r="E14">
-        <v>282.5338288137144</v>
+        <v>282.4713166923112</v>
       </c>
       <c r="F14">
-        <v>13.30357828515761</v>
+        <v>13.9227833766442</v>
       </c>
       <c r="G14">
-        <v>0.00189694021125416</v>
+        <v>0.001812942513807413</v>
       </c>
       <c r="H14">
-        <v>0.002985962964365312</v>
+        <v>0.00194775530799274</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -770,19 +770,19 @@
         <v>0.02096561791822803</v>
       </c>
       <c r="D15">
-        <v>3916667.442647102</v>
+        <v>3908838.452826834</v>
       </c>
       <c r="E15">
-        <v>282.2634509079583</v>
+        <v>282.180629223353</v>
       </c>
       <c r="F15">
-        <v>16.05936348205446</v>
+        <v>16.72916794277586</v>
       </c>
       <c r="G15">
-        <v>0.001684685981576166</v>
+        <v>0.001617669508666068</v>
       </c>
       <c r="H15">
-        <v>0.00255618169108828</v>
+        <v>0.00167124561884963</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -796,19 +796,19 @@
         <v>0.02013506414658983</v>
       </c>
       <c r="D16">
-        <v>3877424.310176328</v>
+        <v>3866994.07801601</v>
       </c>
       <c r="E16">
-        <v>281.8470622538139</v>
+        <v>281.7358675518466</v>
       </c>
       <c r="F16">
-        <v>19.69614079985747</v>
+        <v>20.42573573199484</v>
       </c>
       <c r="G16">
-        <v>0.001480612543273258</v>
+        <v>0.001428243165208343</v>
       </c>
       <c r="H16">
-        <v>0.002160383916993799</v>
+        <v>0.001415657074335822</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -822,19 +822,19 @@
         <v>0.01930451037495166</v>
       </c>
       <c r="D17">
-        <v>3814295.662641164</v>
+        <v>3800142.227998723</v>
       </c>
       <c r="E17">
-        <v>281.1706401463467</v>
+        <v>281.017851194172</v>
       </c>
       <c r="F17">
-        <v>24.92456096204876</v>
+        <v>25.72833718617417</v>
       </c>
       <c r="G17">
-        <v>0.001269493351929316</v>
+        <v>0.00123044732863197</v>
       </c>
       <c r="H17">
-        <v>0.00177883627040231</v>
+        <v>0.001168386392635802</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -848,19 +848,19 @@
         <v>0.01956298682688029</v>
       </c>
       <c r="D18">
-        <v>3700764.998925004</v>
+        <v>3680821.340662758</v>
       </c>
       <c r="E18">
-        <v>279.9330414980626</v>
+        <v>279.7127505384358</v>
       </c>
       <c r="F18">
-        <v>33.01764785494194</v>
+        <v>33.8613104020351</v>
       </c>
       <c r="G18">
-        <v>0.0009523521120393344</v>
+        <v>0.0009292951340225016</v>
       </c>
       <c r="H18">
-        <v>0.001396757235427562</v>
+        <v>0.0009204285007092687</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -874,19 +874,19 @@
         <v>0.02135258148578198</v>
       </c>
       <c r="D19">
-        <v>3466954.706184031</v>
+        <v>3438821.799887272</v>
       </c>
       <c r="E19">
-        <v>277.2933201147379</v>
+        <v>276.9669552337208</v>
       </c>
       <c r="F19">
-        <v>30.31540904837559</v>
+        <v>31.11123086214137</v>
       </c>
       <c r="G19">
-        <v>0.0009228364819717596</v>
+        <v>0.0009001990583854634</v>
       </c>
       <c r="H19">
-        <v>0.001539886770165541</v>
+        <v>0.00101463166339805</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -900,19 +900,19 @@
         <v>0.0231421761446837</v>
       </c>
       <c r="D20">
-        <v>3505162.453342678</v>
+        <v>3477953.148823767</v>
       </c>
       <c r="E20">
-        <v>277.7334605013237</v>
+        <v>277.4203822782536</v>
       </c>
       <c r="F20">
-        <v>26.68400815008156</v>
+        <v>27.40796143645796</v>
       </c>
       <c r="G20">
-        <v>0.0009397028794474608</v>
+        <v>0.000915833576679839</v>
       </c>
       <c r="H20">
-        <v>0.001737377960813831</v>
+        <v>0.001144222908442949</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -926,19 +926,19 @@
         <v>0.02493177080358538</v>
       </c>
       <c r="D21">
-        <v>3559694.465464081</v>
+        <v>3534473.954313901</v>
       </c>
       <c r="E21">
-        <v>278.3555822246578</v>
+        <v>278.0687347578817</v>
       </c>
       <c r="F21">
-        <v>23.46412802573349</v>
+        <v>24.12476733161485</v>
       </c>
       <c r="G21">
-        <v>0.0009699714967923297</v>
+        <v>0.0009443149095766275</v>
       </c>
       <c r="H21">
-        <v>0.00196160194440404</v>
+        <v>0.001291159629170041</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -952,19 +952,19 @@
         <v>0.0267213654624871</v>
       </c>
       <c r="D22">
-        <v>3602313.314814168</v>
+        <v>3578684.772585359</v>
       </c>
       <c r="E22">
-        <v>278.8369305761914</v>
+        <v>278.5705847143697</v>
       </c>
       <c r="F22">
-        <v>20.74667419975187</v>
+        <v>21.35455315480892</v>
       </c>
       <c r="G22">
-        <v>0.00100661298573191</v>
+        <v>0.000978835680405053</v>
       </c>
       <c r="H22">
-        <v>0.002206349654550542</v>
+        <v>0.001451366940826274</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -978,19 +978,19 @@
         <v>0.02851096012138879</v>
       </c>
       <c r="D23">
-        <v>3633688.423332382</v>
+        <v>3611235.477743314</v>
       </c>
       <c r="E23">
-        <v>279.1886162891869</v>
+        <v>278.9371685171066</v>
       </c>
       <c r="F23">
-        <v>18.46523064899552</v>
+        <v>19.02877636150933</v>
       </c>
       <c r="G23">
-        <v>0.001047032973949546</v>
+        <v>0.001016889951884487</v>
       </c>
       <c r="H23">
-        <v>0.002469165328848003</v>
+        <v>0.001623221091195757</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1004,19 +1004,19 @@
         <v>0.03030055478029048</v>
       </c>
       <c r="D24">
-        <v>3656740.71218102</v>
+        <v>3635158.792832683</v>
       </c>
       <c r="E24">
-        <v>279.4455878225033</v>
+        <v>279.2050428004576</v>
       </c>
       <c r="F24">
-        <v>16.54169419159196</v>
+        <v>17.06743915406703</v>
       </c>
       <c r="G24">
-        <v>0.001089968282580739</v>
+        <v>0.001057258652838027</v>
       </c>
       <c r="H24">
-        <v>0.002748808877020657</v>
+        <v>0.001805893214995846</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1030,19 +1030,19 @@
         <v>0.03209014943919218</v>
       </c>
       <c r="D25">
-        <v>3673848.288034938</v>
+        <v>3652921.750887206</v>
       </c>
       <c r="E25">
-        <v>279.6355208396503</v>
+        <v>279.40309926111</v>
       </c>
       <c r="F25">
-        <v>14.90877374077251</v>
+        <v>15.40185511746498</v>
       </c>
       <c r="G25">
-        <v>0.001134707801445363</v>
+        <v>0.001099255464596894</v>
       </c>
       <c r="H25">
-        <v>0.00304455491867066</v>
+        <v>0.001998891438855599</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1056,19 +1056,19 @@
         <v>0.03387974409809387</v>
       </c>
       <c r="D26">
-        <v>3686710.39242345</v>
+        <v>3666285.208475661</v>
       </c>
       <c r="E26">
-        <v>279.7778904426137</v>
+        <v>279.551634037035</v>
       </c>
       <c r="F26">
-        <v>13.51220610111882</v>
+        <v>13.97673991870708</v>
       </c>
       <c r="G26">
-        <v>0.001180813719333998</v>
+        <v>0.001142457787263048</v>
       </c>
       <c r="H26">
-        <v>0.003355934555318804</v>
+        <v>0.002201892063888259</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1082,19 +1082,19 @@
         <v>0.03566933875699557</v>
       </c>
       <c r="D27">
-        <v>3696511.209669871</v>
+        <v>3676475.573611133</v>
       </c>
       <c r="E27">
-        <v>279.8861291731661</v>
+        <v>279.6646318916831</v>
       </c>
       <c r="F27">
-        <v>12.30899416776944</v>
+        <v>12.74833570804737</v>
       </c>
       <c r="G27">
-        <v>0.001227999132375576</v>
+        <v>0.001186588683405454</v>
       </c>
       <c r="H27">
-        <v>0.003682622002950303</v>
+        <v>0.002414665391775768</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1108,19 +1108,19 @@
         <v>0.03745893341589727</v>
       </c>
       <c r="D28">
-        <v>3704076.577554698</v>
+        <v>3684347.94665918</v>
       </c>
       <c r="E28">
-        <v>279.9695352504052</v>
+        <v>279.7517682120496</v>
       </c>
       <c r="F28">
-        <v>11.26513139962166</v>
+        <v>11.68205732378545</v>
       </c>
       <c r="G28">
-        <v>0.001276067090568407</v>
+        <v>0.001231458068666923</v>
       </c>
       <c r="H28">
-        <v>0.004024378382460721</v>
+        <v>0.002637038916530709</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1134,19 +1134,19 @@
         <v>0.03924852807479898</v>
       </c>
       <c r="D29">
-        <v>3709987.748274246</v>
+        <v>3690504.193431249</v>
       </c>
       <c r="E29">
-        <v>280.034616836658</v>
+        <v>279.8198137514893</v>
       </c>
       <c r="F29">
-        <v>10.35360961192639</v>
+        <v>10.7504478214012</v>
       </c>
       <c r="G29">
-        <v>0.001324877433560469</v>
+        <v>0.00127693070153804</v>
       </c>
       <c r="H29">
-        <v>0.004381021200659751</v>
+        <v>0.00286887732034062</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1160,19 +1160,19 @@
         <v>0.04103812273370067</v>
       </c>
       <c r="D30">
-        <v>3714658.825351367</v>
+        <v>3695373.187169108</v>
       </c>
       <c r="E30">
-        <v>280.0859909746891</v>
+        <v>279.8735718976351</v>
       </c>
       <c r="F30">
-        <v>9.552836555596853</v>
+        <v>9.931560795933757</v>
       </c>
       <c r="G30">
-        <v>0.001374327498536356</v>
+        <v>0.001322907555395936</v>
       </c>
       <c r="H30">
-        <v>0.00475240655845208</v>
+        <v>0.003110070799408331</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1186,19 +1186,19 @@
         <v>0.04282771739260237</v>
       </c>
       <c r="D31">
-        <v>3718388.676611534</v>
+        <v>3699264.552039064</v>
       </c>
       <c r="E31">
-        <v>280.1269789600093</v>
+        <v>279.9164985711252</v>
       </c>
       <c r="F31">
-        <v>8.845419594571592</v>
+        <v>9.20771980230905</v>
       </c>
       <c r="G31">
-        <v>0.001424340291473215</v>
+        <v>0.001369314393150187</v>
       </c>
       <c r="H31">
-        <v>0.005138418164278358</v>
+        <v>0.003360527846630797</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1212,19 +1212,19 @@
         <v>0.04461731205150407</v>
       </c>
       <c r="D32">
-        <v>3721395.793713924</v>
+        <v>3702404.733001877</v>
       </c>
       <c r="E32">
-        <v>280.1600026052305</v>
+        <v>279.9511144548483</v>
       </c>
       <c r="F32">
-        <v>8.21724022927661</v>
+        <v>8.564575827987568</v>
       </c>
       <c r="G32">
-        <v>0.001474856919302278</v>
+        <v>0.001416094455497791</v>
       </c>
       <c r="H32">
-        <v>0.005538960218507878</v>
+        <v>0.003620170571146016</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1238,19 +1238,19 @@
         <v>0.04640690671040576</v>
       </c>
       <c r="D33">
-        <v>3723841.897653683</v>
+        <v>3704961.414588493</v>
       </c>
       <c r="E33">
-        <v>280.1868507759367</v>
+        <v>279.9792821206078</v>
       </c>
       <c r="F33">
-        <v>7.656750295506229</v>
+        <v>7.99039125536421</v>
       </c>
       <c r="G33">
-        <v>0.0015258315749364</v>
+        <v>0.001463203614674394</v>
       </c>
       <c r="H33">
-        <v>0.005953952615388959</v>
+        <v>0.003888931537829059</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1264,19 +1264,19 @@
         <v>0.04819650136930748</v>
       </c>
       <c r="D34">
-        <v>3725848.102718037</v>
+        <v>3707060.240457775</v>
       </c>
       <c r="E34">
-        <v>280.2088609495695</v>
+        <v>280.0023947463697</v>
       </c>
       <c r="F34">
-        <v>7.154434636436086</v>
+        <v>7.475493582023844</v>
       </c>
       <c r="G34">
-        <v>0.001577228114498745</v>
+        <v>0.001510607066402515</v>
       </c>
       <c r="H34">
-        <v>0.00638332759444184</v>
+        <v>0.00416675155813668</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1290,19 +1290,19 @@
         <v>0.04998609602820916</v>
       </c>
       <c r="D35">
-        <v>3727506.12004255</v>
+        <v>3708796.402666658</v>
       </c>
       <c r="E35">
-        <v>280.2270445368591</v>
+        <v>280.0215063625298</v>
       </c>
       <c r="F35">
-        <v>6.702398383383314</v>
+        <v>7.011856037269017</v>
       </c>
       <c r="G35">
-        <v>0.001629017661683631</v>
+        <v>0.001558277014407872</v>
       </c>
       <c r="H35">
-        <v>0.006827027332510341</v>
+        <v>0.004453578098880204</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1316,19 +1316,19 @@
         <v>0.05177569068711085</v>
       </c>
       <c r="D36">
-        <v>3728886.119125864</v>
+        <v>3710242.775054051</v>
       </c>
       <c r="E36">
-        <v>280.2421745271858</v>
+        <v>280.0374229418105</v>
       </c>
       <c r="F36">
-        <v>6.294047716243674</v>
+        <v>6.592773302325279</v>
       </c>
       <c r="G36">
-        <v>0.001681176894207134</v>
+        <v>0.001606191014222449</v>
       </c>
       <c r="H36">
-        <v>0.00728500216648724</v>
+        <v>0.004749364105667555</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1342,19 +1342,19 @@
         <v>0.05356528534601257</v>
       </c>
       <c r="D37">
-        <v>3730042.311123099</v>
+        <v>3711455.690899428</v>
       </c>
       <c r="E37">
-        <v>280.2548475664669</v>
+        <v>280.0507669233389</v>
       </c>
       <c r="F37">
-        <v>5.923841100981178</v>
+        <v>6.212608881169804</v>
       </c>
       <c r="G37">
-        <v>0.001733686794674878</v>
+        <v>0.001654330765959965</v>
       </c>
       <c r="H37">
-        <v>0.007757209251000137</v>
+        <v>0.005054067112608431</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1368,19 +1368,19 @@
         <v>0.05535488000491426</v>
       </c>
       <c r="D38">
-        <v>3731016.960422047</v>
+        <v>3712479.095302435</v>
       </c>
       <c r="E38">
-        <v>280.2655284608042</v>
+        <v>280.0620234781014</v>
       </c>
       <c r="F38">
-        <v>5.587094000205509</v>
+        <v>5.866596806391183</v>
       </c>
       <c r="G38">
-        <v>0.001786531724662545</v>
+        <v>0.001702681219596101</v>
       </c>
       <c r="H38">
-        <v>0.008243611523762929</v>
+        <v>0.00536764855471179</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1394,19 +1394,19 @@
         <v>0.05714447466381595</v>
       </c>
       <c r="D39">
-        <v>3731843.299040137</v>
+        <v>3713347.562841374</v>
       </c>
       <c r="E39">
-        <v>280.2745824487235</v>
+        <v>280.0715740666502</v>
       </c>
       <c r="F39">
-        <v>5.279824440156543</v>
+        <v>5.550684843957569</v>
       </c>
       <c r="G39">
-        <v>0.001839698728029017</v>
+        <v>0.001751229901909925</v>
       </c>
       <c r="H39">
-        <v>0.008744176893104621</v>
+        <v>0.005690073226822238</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1420,19 +1420,19 @@
         <v>0.05893406932271766</v>
       </c>
       <c r="D40">
-        <v>3732547.666296029</v>
+        <v>3714088.513843047</v>
       </c>
       <c r="E40">
-        <v>280.2822988581634</v>
+        <v>280.0797210453296</v>
       </c>
       <c r="F40">
-        <v>4.998630019494733</v>
+        <v>5.261409625212047</v>
       </c>
       <c r="G40">
-        <v>0.001893176999888423</v>
+        <v>0.001799966403607323</v>
       </c>
       <c r="H40">
-        <v>0.009258877590354167</v>
+        <v>0.006021308851391838</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1446,19 +1446,19 @@
         <v>0.06072366398161935</v>
       </c>
       <c r="D41">
-        <v>3733151.095409825</v>
+        <v>3714723.858409338</v>
       </c>
       <c r="E41">
-        <v>280.2889086258325</v>
+        <v>280.086705894411</v>
       </c>
       <c r="F41">
-        <v>4.740589291591262</v>
+        <v>4.995796523660102</v>
       </c>
       <c r="G41">
-        <v>0.001946957476645398</v>
+        <v>0.001848881983522731</v>
       </c>
       <c r="H41">
-        <v>0.00978768964459311</v>
+        <v>0.006361325727171394</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1472,19 +1472,19 @@
         <v>0.06251325864052105</v>
       </c>
       <c r="D42">
-        <v>3733670.501109144</v>
+        <v>3715271.227504424</v>
       </c>
       <c r="E42">
-        <v>280.2945973964998</v>
+        <v>280.0927228520969</v>
       </c>
       <c r="F42">
-        <v>4.503182173424716</v>
+        <v>4.751278845557027</v>
       </c>
       <c r="G42">
-        <v>0.002001032516321014</v>
+        <v>0.001897969260117312</v>
       </c>
       <c r="H42">
-        <v>0.01033059245229232</v>
+        <v>0.006710096440690721</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1498,19 +1498,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D43">
-        <v>3734119.576520678</v>
+        <v>3715744.903074514</v>
       </c>
       <c r="E43">
-        <v>280.2995154064951</v>
+        <v>280.0979292053099</v>
       </c>
       <c r="F43">
-        <v>4.401351606676412</v>
+        <v>4.646909304972931</v>
       </c>
       <c r="G43">
-        <v>0.002029501490233691</v>
+        <v>0.00192370389247722</v>
       </c>
       <c r="H43">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1524,19 +1524,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D44">
-        <v>3734239.079031678</v>
+        <v>3715861.891260651</v>
       </c>
       <c r="E44">
-        <v>280.3008240542054</v>
+        <v>280.0992149927341</v>
       </c>
       <c r="F44">
-        <v>4.448764840990412</v>
+        <v>4.697035651409338</v>
       </c>
       <c r="G44">
-        <v>0.002026204804352636</v>
+        <v>0.001920557800191829</v>
       </c>
       <c r="H44">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1550,19 +1550,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D45">
-        <v>3733979.054884622</v>
+        <v>3715564.227003922</v>
       </c>
       <c r="E45">
-        <v>280.2979765430619</v>
+        <v>280.095943381831</v>
       </c>
       <c r="F45">
-        <v>4.497257376938184</v>
+        <v>4.748320015452982</v>
       </c>
       <c r="G45">
-        <v>0.002022858129765588</v>
+        <v>0.00191736056935197</v>
       </c>
       <c r="H45">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1576,19 +1576,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D46">
-        <v>3733714.119876452</v>
+        <v>3715260.922073649</v>
       </c>
       <c r="E46">
-        <v>280.295075102754</v>
+        <v>280.0926095756372</v>
       </c>
       <c r="F46">
-        <v>4.546693280801645</v>
+        <v>4.800603838009845</v>
       </c>
       <c r="G46">
-        <v>0.00201950501547831</v>
+        <v>0.001914156904972485</v>
       </c>
       <c r="H46">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1602,19 +1602,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D47">
-        <v>3733444.566687003</v>
+        <v>3714952.339777606</v>
       </c>
       <c r="E47">
-        <v>280.2921229303549</v>
+        <v>280.0892175566181</v>
       </c>
       <c r="F47">
-        <v>4.597099342657454</v>
+        <v>4.853915513313679</v>
       </c>
       <c r="G47">
-        <v>0.002016145479740292</v>
+        <v>0.001910946825357876</v>
       </c>
       <c r="H47">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1628,19 +1628,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D48">
-        <v>3733170.274159531</v>
+        <v>3714638.341885189</v>
       </c>
       <c r="E48">
-        <v>280.2891186907302</v>
+        <v>280.0857657944684</v>
       </c>
       <c r="F48">
-        <v>4.648503561197308</v>
+        <v>4.908284759261321</v>
       </c>
       <c r="G48">
-        <v>0.002012779493067179</v>
+        <v>0.001907730294012336</v>
       </c>
       <c r="H48">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1654,19 +1654,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D49">
-        <v>3732891.116318146</v>
+        <v>3714318.784570079</v>
       </c>
       <c r="E49">
-        <v>280.2860609955256</v>
+        <v>280.0822526967918</v>
       </c>
       <c r="F49">
-        <v>4.700935012781206</v>
+        <v>4.963742439823391</v>
       </c>
       <c r="G49">
-        <v>0.002009407026336452</v>
+        <v>0.001904507274456263</v>
       </c>
       <c r="H49">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1680,19 +1680,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D50">
-        <v>3732606.962625397</v>
+        <v>3713993.518798046</v>
       </c>
       <c r="E50">
-        <v>280.2829484059595</v>
+        <v>280.078676613329</v>
       </c>
       <c r="F50">
-        <v>4.754423903403302</v>
+        <v>5.020320620339588</v>
       </c>
       <c r="G50">
-        <v>0.002006028050879204</v>
+        <v>0.001901277730316289</v>
       </c>
       <c r="H50">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -1706,19 +1706,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D51">
-        <v>3732317.677771894</v>
+        <v>3713662.390086808</v>
       </c>
       <c r="E51">
-        <v>280.2797794304925</v>
+        <v>280.07503583328</v>
       </c>
       <c r="F51">
-        <v>4.809001623922494</v>
+        <v>5.078052626371312</v>
       </c>
       <c r="G51">
-        <v>0.002002642538519672</v>
+        <v>0.001898041625347823</v>
       </c>
       <c r="H51">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1732,19 +1732,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D52">
-        <v>3732023.121453457</v>
+        <v>3713325.238251453</v>
       </c>
       <c r="E52">
-        <v>280.2765525223543</v>
+        <v>280.071328582466</v>
       </c>
       <c r="F52">
-        <v>4.864700808564451</v>
+        <v>5.136973106047253</v>
       </c>
       <c r="G52">
-        <v>0.001999250461616892</v>
+        <v>0.001894798923458606</v>
       </c>
       <c r="H52">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -1758,19 +1758,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D53">
-        <v>3731723.148135537</v>
+        <v>3712981.897135293</v>
       </c>
       <c r="E53">
-        <v>280.2732660769324</v>
+        <v>280.0675530203269</v>
       </c>
       <c r="F53">
-        <v>4.921555396923318</v>
+        <v>5.197118096146147</v>
       </c>
       <c r="G53">
-        <v>0.001995851793108493</v>
+        <v>0.001891549588733515</v>
       </c>
       <c r="H53">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -1784,19 +1784,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D54">
-        <v>3731417.606804025</v>
+        <v>3712632.194325158</v>
       </c>
       <c r="E54">
-        <v>280.2699184290066</v>
+        <v>280.0637072367472</v>
       </c>
       <c r="F54">
-        <v>4.979600699709806</v>
+        <v>5.258525092180667</v>
       </c>
       <c r="G54">
-        <v>0.001992446506556835</v>
+        <v>0.001888293585460526</v>
       </c>
       <c r="H54">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -1810,19 +1810,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D55">
-        <v>3731106.34070152</v>
+        <v>3712275.950850059</v>
       </c>
       <c r="E55">
-        <v>280.2665078498244</v>
+        <v>280.0597892486923</v>
       </c>
       <c r="F55">
-        <v>5.038873468512932</v>
+        <v>5.321233122768517</v>
       </c>
       <c r="G55">
-        <v>0.00198903457619755</v>
+        <v>0.001885030878157963</v>
       </c>
       <c r="H55">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -1836,19 +1836,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D56">
-        <v>3730789.187048049</v>
+        <v>3711912.980862061</v>
       </c>
       <c r="E56">
-        <v>280.2630325440015</v>
+        <v>280.0557969966492</v>
       </c>
       <c r="F56">
-        <v>5.099411969864311</v>
+        <v>5.385282828599801</v>
       </c>
       <c r="G56">
-        <v>0.001985615976990604</v>
+        <v>0.00188176143160304</v>
       </c>
       <c r="H56">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -1862,19 +1862,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D57">
-        <v>3730465.976745162</v>
+        <v>3711543.091298127</v>
       </c>
       <c r="E57">
-        <v>280.2594906462376</v>
+        <v>280.0517283408516</v>
       </c>
       <c r="F57">
-        <v>5.161256063918075</v>
+        <v>5.450716546336061</v>
       </c>
       <c r="G57">
-        <v>0.00198219068467399</v>
+        <v>0.001878485210861681</v>
       </c>
       <c r="H57">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -1888,19 +1888,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D58">
-        <v>3730136.53406219</v>
+        <v>3711166.081521574</v>
       </c>
       <c r="E58">
-        <v>280.2558802178352</v>
+        <v>280.0475810572783</v>
       </c>
       <c r="F58">
-        <v>5.224447288085892</v>
+        <v>5.517578397804365</v>
       </c>
       <c r="G58">
-        <v>0.001978758675820171</v>
+        <v>0.001875202181319721</v>
       </c>
       <c r="H58">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -1914,19 +1914,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D59">
-        <v>3729800.676303431</v>
+        <v>3710781.742941686</v>
       </c>
       <c r="E59">
-        <v>280.2521992430023</v>
+        <v>280.0433528334056</v>
       </c>
       <c r="F59">
-        <v>5.289028945995463</v>
+        <v>5.585914384880861</v>
       </c>
       <c r="G59">
-        <v>0.001975319927895411</v>
+        <v>0.00187191230871545</v>
       </c>
       <c r="H59">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -1940,19 +1940,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D60">
-        <v>3729458.21345485</v>
+        <v>3710389.858609891</v>
       </c>
       <c r="E60">
-        <v>280.2484456249331</v>
+        <v>280.0390412636988</v>
       </c>
       <c r="F60">
-        <v>5.355046202172292</v>
+        <v>5.655772490492311</v>
       </c>
       <c r="G60">
-        <v>0.001971874419322056</v>
+        <v>0.001868615559173516</v>
       </c>
       <c r="H60">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -1966,19 +1966,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D61">
-        <v>3729108.947808814</v>
+        <v>3709990.2027908</v>
       </c>
       <c r="E61">
-        <v>280.2446171816371</v>
+        <v>280.0346438448198</v>
       </c>
       <c r="F61">
-        <v>5.42254618287968</v>
+        <v>5.727202786201185</v>
       </c>
       <c r="G61">
-        <v>0.001968422129543956</v>
+        <v>0.001865311899240267</v>
       </c>
       <c r="H61">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -1992,19 +1992,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D62">
-        <v>3728752.673565234</v>
+        <v>3709582.540506224</v>
       </c>
       <c r="E62">
-        <v>280.2407116415114</v>
+        <v>280.0301579705344</v>
       </c>
       <c r="F62">
-        <v>5.491578083589776</v>
+        <v>5.800257546881339</v>
       </c>
       <c r="G62">
-        <v>0.001964963039095095</v>
+        <v>0.00186200129592041</v>
       </c>
       <c r="H62">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2018,19 +2018,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D63">
-        <v>3728389.176407333</v>
+        <v>3709166.627050163</v>
       </c>
       <c r="E63">
-        <v>280.2367266386254</v>
+        <v>280.0255809262922</v>
       </c>
       <c r="F63">
-        <v>5.562193283600706</v>
+        <v>5.874991373035946</v>
       </c>
       <c r="G63">
-        <v>0.001961497129671587</v>
+        <v>0.001858683716715111</v>
       </c>
       <c r="H63">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2044,19 +2044,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D64">
-        <v>3728018.233050141</v>
+        <v>3708742.207472559</v>
       </c>
       <c r="E64">
-        <v>280.2326597077061</v>
+        <v>280.0209098834563</v>
       </c>
       <c r="F64">
-        <v>5.634445468361042</v>
+        <v>5.95146132135956</v>
       </c>
       <c r="G64">
-        <v>0.00195802438420713</v>
+        <v>0.0018553591296614</v>
       </c>
       <c r="H64">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2070,19 +2070,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D65">
-        <v>3727639.610759623</v>
+        <v>3708309.01602941</v>
       </c>
       <c r="E65">
-        <v>280.2285082787923</v>
+        <v>280.0161418931582</v>
       </c>
       <c r="F65">
-        <v>5.708390760113994</v>
+        <v>6.029727044200615</v>
       </c>
       <c r="G65">
-        <v>0.001954544786952078</v>
+        <v>0.00185202750337293</v>
       </c>
       <c r="H65">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2096,19 +2096,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D66">
-        <v>3727253.066840154</v>
+        <v>3707866.775596646</v>
       </c>
       <c r="E66">
-        <v>280.224269671538</v>
+        <v>280.0112738797422</v>
       </c>
       <c r="F66">
-        <v>5.784087857529938</v>
+        <v>6.109850938641539</v>
       </c>
       <c r="G66">
-        <v>0.001951058323556169</v>
+        <v>0.001848688807082</v>
       </c>
       <c r="H66">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -2122,19 +2122,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D67">
-        <v>3726858.348087872</v>
+        <v>3707415.197044921</v>
       </c>
       <c r="E67">
-        <v>280.2199410891344</v>
+        <v>280.0063026337749</v>
       </c>
       <c r="F67">
-        <v>5.861598185058092</v>
+        <v>6.19189830598033</v>
       </c>
       <c r="G67">
-        <v>0.001947564981155134</v>
+        <v>0.001845343010682744</v>
       </c>
       <c r="H67">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2148,19 +2148,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D68">
-        <v>3726455.190207209</v>
+        <v>3706953.978572207</v>
       </c>
       <c r="E68">
-        <v>280.2155196118221</v>
+        <v>280.0012248045785</v>
       </c>
       <c r="F68">
-        <v>5.940986052797192</v>
+        <v>6.275937522471513</v>
       </c>
       <c r="G68">
-        <v>0.001944064748461171</v>
+        <v>0.00184199008477547</v>
       </c>
       <c r="H68">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -2174,19 +2174,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D69">
-        <v>3726043.317187624</v>
+        <v>3706482.804990805</v>
       </c>
       <c r="E69">
-        <v>280.2110021899583</v>
+        <v>279.9960368922532</v>
       </c>
       <c r="F69">
-        <v>6.022318827760974</v>
+        <v>6.362040222266482</v>
       </c>
       <c r="G69">
-        <v>0.001940557615857449</v>
+        <v>0.00183863000071195</v>
       </c>
       <c r="H69">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2200,19 +2200,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D70">
-        <v>3725622.44063733</v>
+        <v>3706001.346965061</v>
       </c>
       <c r="E70">
-        <v>280.2063856366051</v>
+        <v>279.9907352391476</v>
       </c>
       <c r="F70">
-        <v>6.105667117498966</v>
+        <v>6.450281493583919</v>
       </c>
       <c r="G70">
-        <v>0.001937043575496697</v>
+        <v>0.001835262730641523</v>
       </c>
       <c r="H70">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2226,19 +2226,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D71">
-        <v>3725192.259070456</v>
+        <v>3705509.260195718</v>
       </c>
       <c r="E71">
-        <v>280.2016666195969</v>
+        <v>279.985316020726</v>
       </c>
       <c r="F71">
-        <v>6.191104967126884</v>
+        <v>6.540740089242234</v>
       </c>
       <c r="G71">
-        <v>0.001933522621403948</v>
+        <v>0.001831888247557879</v>
       </c>
       <c r="H71">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -2252,19 +2252,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D72">
-        <v>3724752.457143782</v>
+        <v>3705006.184546465</v>
       </c>
       <c r="E72">
-        <v>280.1968416530461</v>
+        <v>279.9797752357901</v>
       </c>
       <c r="F72">
-        <v>6.278710070925126</v>
+        <v>6.633498652797905</v>
       </c>
       <c r="G72">
-        <v>0.00192999474958346</v>
+        <v>0.001828506525346191</v>
       </c>
       <c r="H72">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2278,19 +2278,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D73">
-        <v>3724302.704838779</v>
+        <v>3704491.743107776</v>
       </c>
       <c r="E73">
-        <v>280.1919070882365</v>
+        <v>279.974108695993</v>
       </c>
       <c r="F73">
-        <v>6.368563999779979</v>
+        <v>6.728643961658727</v>
       </c>
       <c r="G73">
-        <v>0.001926459958129861</v>
+        <v>0.001825117538830401</v>
       </c>
       <c r="H73">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2304,19 +2304,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D74">
-        <v>3723842.656584304</v>
+        <v>3703965.541192687</v>
       </c>
       <c r="E74">
-        <v>280.1868591038561</v>
+        <v>279.9683120145903</v>
       </c>
       <c r="F74">
-        <v>6.460752445871282</v>
+        <v>6.826267188680104</v>
       </c>
       <c r="G74">
-        <v>0.001922918247343459</v>
+        <v>0.001821721263820244</v>
       </c>
       <c r="H74">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -2330,19 +2330,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D75">
-        <v>3723371.950314788</v>
+        <v>3703427.165258605</v>
       </c>
       <c r="E75">
-        <v>280.1816936955072</v>
+        <v>279.9623805943566</v>
       </c>
       <c r="F75">
-        <v>6.555365486154924</v>
+        <v>6.926464183908084</v>
       </c>
       <c r="G75">
-        <v>0.001919369619849704</v>
+        <v>0.001818317677157648</v>
       </c>
       <c r="H75">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -2356,19 +2356,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D76">
-        <v>3722890.206458276</v>
+        <v>3702876.181748638</v>
       </c>
       <c r="E76">
-        <v>280.1764066644328</v>
+        <v>279.9563096145998</v>
       </c>
       <c r="F76">
-        <v>6.65249786634936</v>
+        <v>7.029335778306255</v>
       </c>
       <c r="G76">
-        <v>0.001915814080722673</v>
+        <v>0.001814906756761973</v>
       </c>
       <c r="H76">
-        <v>0.01063595663842262</v>
+        <v>0.006906135279788459</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -2382,19 +2382,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D77">
-        <v>3722397.026848084</v>
+        <v>3702312.135845284</v>
       </c>
       <c r="E77">
-        <v>280.1709936053903</v>
+        <v>279.9500940171871</v>
       </c>
       <c r="F77">
-        <v>6.752249307315781</v>
+        <v>7.134988111498464</v>
       </c>
       <c r="G77">
-        <v>0.001912251637612436</v>
+        <v>0.001811488481673517</v>
       </c>
       <c r="H77">
-        <v>0.01063595663842261</v>
+        <v>0.006906135279788454</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -2408,19 +2408,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D78">
-        <v>3721891.99355119</v>
+        <v>3701734.550128568</v>
       </c>
       <c r="E78">
-        <v>280.1654498935935</v>
+        <v>279.9437284914957</v>
       </c>
       <c r="F78">
-        <v>6.854724835924101</v>
+        <v>7.243532985776826</v>
       </c>
       <c r="G78">
-        <v>0.001908682300876028</v>
+        <v>0.001808062832094587</v>
       </c>
       <c r="H78">
-        <v>0.01063595663842261</v>
+        <v>0.006906135279788454</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -2434,19 +2434,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D79">
-        <v>3721374.667605753</v>
+        <v>3701142.923129879</v>
       </c>
       <c r="E79">
-        <v>280.1597706706381</v>
+        <v>279.9372074581898</v>
       </c>
       <c r="F79">
-        <v>6.96003514272302</v>
+        <v>7.355088248869329</v>
       </c>
       <c r="G79">
-        <v>0.001905106083711803</v>
+        <v>0.001804629789427305</v>
       </c>
       <c r="H79">
-        <v>0.01063595663842261</v>
+        <v>0.006906135279788454</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -2460,19 +2460,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D80">
-        <v>3720844.587659353</v>
+        <v>3700536.727771814</v>
       </c>
       <c r="E80">
-        <v>280.1539508293164</v>
+        <v>279.9305250517131</v>
       </c>
       <c r="F80">
-        <v>7.068296968987964</v>
+        <v>7.469778208236372</v>
       </c>
       <c r="G80">
-        <v>0.001901523002296673</v>
+        <v>0.001801189336307156</v>
       </c>
       <c r="H80">
-        <v>0.01063595663842261</v>
+        <v>0.006906135279788454</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -2486,19 +2486,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D81">
-        <v>3720301.268498627</v>
+        <v>3699915.409683313</v>
       </c>
       <c r="E81">
-        <v>280.1479849972175</v>
+        <v>279.9236751013767</v>
       </c>
       <c r="F81">
-        <v>7.179633526007199</v>
+        <v>7.587734079975194</v>
       </c>
       <c r="G81">
-        <v>0.001897933075925768</v>
+        <v>0.001797741456631125</v>
       </c>
       <c r="H81">
-        <v>0.01063595663842261</v>
+        <v>0.006906135279788454</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -2512,19 +2512,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D82">
-        <v>3719744.199459947</v>
+        <v>3699278.385378158</v>
       </c>
       <c r="E82">
-        <v>280.141867518995</v>
+        <v>279.9166511109059</v>
       </c>
       <c r="F82">
-        <v>7.294174949790245</v>
+        <v>7.709094475760401</v>
       </c>
       <c r="G82">
-        <v>0.001894336327153817</v>
+        <v>0.001794286135579086</v>
       </c>
       <c r="H82">
-        <v>0.01063595663842261</v>
+        <v>0.006906135279788454</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -2538,19 +2538,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D83">
-        <v>3719172.842709655</v>
+        <v>3698625.040283615</v>
       </c>
       <c r="E83">
-        <v>280.1355924371741</v>
+        <v>279.9094462362994</v>
       </c>
       <c r="F83">
-        <v>7.412058794747818</v>
+        <v>7.83400593164343</v>
       </c>
       <c r="G83">
-        <v>0.001890732781937441</v>
+        <v>0.001790823359626825</v>
       </c>
       <c r="H83">
-        <v>0.01063595663842261</v>
+        <v>0.006906135279788454</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -2564,19 +2564,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D84">
-        <v>3718586.631381061</v>
+        <v>3697954.726604453</v>
       </c>
       <c r="E84">
-        <v>280.1291534713552</v>
+        <v>279.9020532618289</v>
       </c>
       <c r="F84">
-        <v>7.533430570305858</v>
+        <v>7.96262348298042</v>
       </c>
       <c r="G84">
-        <v>0.00188712246977732</v>
+        <v>0.001787353116548795</v>
       </c>
       <c r="H84">
-        <v>0.01063595663842261</v>
+        <v>0.006906135279788454</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -2590,19 +2590,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D85">
-        <v>3717984.967553932</v>
+        <v>3697266.761005926</v>
       </c>
       <c r="E85">
-        <v>280.1225439956513</v>
+        <v>279.8944645739989</v>
       </c>
       <c r="F85">
-        <v>7.658444324884626</v>
+        <v>8.095111290263914</v>
       </c>
       <c r="G85">
-        <v>0.001883505423858979</v>
+        <v>0.001783875395408463</v>
       </c>
       <c r="H85">
-        <v>0.01063595663842261</v>
+        <v>0.006906135279788454</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -2616,19 +2616,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D86">
-        <v>3717367.220060566</v>
+        <v>3696560.422097359</v>
       </c>
       <c r="E86">
-        <v>280.1157570141831</v>
+        <v>279.8866721332541</v>
       </c>
       <c r="F86">
-        <v>7.787263282205383</v>
+        <v>8.23164332120901</v>
       </c>
       <c r="G86">
-        <v>0.001879881681190653</v>
+        <v>0.00178039018653361</v>
       </c>
       <c r="H86">
-        <v>0.01063595663842261</v>
+        <v>0.006906135279788454</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -2642,19 +2642,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D87">
-        <v>3716732.722100646</v>
+        <v>3695834.947695811</v>
       </c>
       <c r="E87">
-        <v>280.1087851344296</v>
+        <v>279.878667443204</v>
       </c>
       <c r="F87">
-        <v>7.920060535491983</v>
+        <v>8.372404095098409</v>
       </c>
       <c r="G87">
-        <v>0.001876251282736349</v>
+        <v>0.001776897481473593</v>
       </c>
       <c r="H87">
-        <v>0.01063595663842261</v>
+        <v>0.006906135279788454</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -2668,19 +2668,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D88">
-        <v>3716080.768644941</v>
+        <v>3695089.531846811</v>
       </c>
       <c r="E88">
-        <v>280.1016205382091</v>
+        <v>279.8704415171039</v>
       </c>
       <c r="F88">
-        <v>8.057019805823542</v>
+        <v>8.51758949613679</v>
       </c>
       <c r="G88">
-        <v>0.001872614273541893</v>
+        <v>0.001773397272934979</v>
       </c>
       <c r="H88">
-        <v>0.01063595663842261</v>
+        <v>0.006906135279788454</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -2694,19 +2694,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D89">
-        <v>3715410.613605483</v>
+        <v>3694323.321576368</v>
       </c>
       <c r="E89">
-        <v>280.0942549500435</v>
+        <v>279.8619848412983</v>
       </c>
       <c r="F89">
-        <v>8.198336271681208</v>
+        <v>8.667407663416389</v>
       </c>
       <c r="G89">
-        <v>0.001868970702851164</v>
+        <v>0.001769889554691437</v>
       </c>
       <c r="H89">
-        <v>0.01063595663842261</v>
+        <v>0.006906135279788454</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -2720,19 +2720,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D90">
-        <v>3714721.466747091</v>
+        <v>3693535.413345215</v>
       </c>
       <c r="E90">
-        <v>280.0866796026153</v>
+        <v>279.8532873352992</v>
       </c>
       <c r="F90">
-        <v>8.344217477631908</v>
+        <v>8.822079966070536</v>
       </c>
       <c r="G90">
-        <v>0.001865320624209335</v>
+        <v>0.00176637432146298</v>
       </c>
       <c r="H90">
-        <v>0.01063595663842261</v>
+        <v>0.006906135279788454</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -2746,19 +2746,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D91">
-        <v>3714012.490311938</v>
+        <v>3692724.849172624</v>
       </c>
       <c r="E91">
-        <v>280.0788851990071</v>
+        <v>279.8443383081264</v>
       </c>
       <c r="F91">
-        <v>8.49488433112365</v>
+        <v>8.981842073310537</v>
       </c>
       <c r="G91">
-        <v>0.001861664095549075</v>
+        <v>0.001762851568758814</v>
       </c>
       <c r="H91">
-        <v>0.01063595663842261</v>
+        <v>0.006906135279788454</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -2772,19 +2772,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D92">
-        <v>3713282.795325227</v>
+        <v>3691890.612392864</v>
       </c>
       <c r="E92">
-        <v>280.0708618713545</v>
+        <v>279.8351264104909</v>
       </c>
       <c r="F92">
-        <v>8.650572197552655</v>
+        <v>9.146945130325376</v>
       </c>
       <c r="G92">
-        <v>0.001858001179255168</v>
+        <v>0.00175932129267714</v>
       </c>
       <c r="H92">
-        <v>0.01063595663842261</v>
+        <v>0.006906135279788454</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -2798,19 +2798,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D93">
-        <v>3712531.437545901</v>
+        <v>3691031.623002633</v>
       </c>
       <c r="E93">
-        <v>280.0625991355155</v>
+        <v>279.8256395823508</v>
       </c>
       <c r="F93">
-        <v>8.811532105126679</v>
+        <v>9.317657052505581</v>
       </c>
       <c r="G93">
-        <v>0.001854331942201728</v>
+        <v>0.001755783489653913</v>
       </c>
       <c r="H93">
-        <v>0.01063595663842261</v>
+        <v>0.006906135279788454</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement Coolant Property Plotting
</commit_message>
<xml_diff>
--- a/TheEngine/Regen Solver/enginefiles/solverdata.xlsx
+++ b/TheEngine/Regen Solver/enginefiles/solverdata.xlsx
@@ -438,10 +438,10 @@
         <v>296.9248108308197</v>
       </c>
       <c r="F2">
-        <v>0.6836473894599429</v>
+        <v>1.259972168161066</v>
       </c>
       <c r="G2">
-        <v>0.02155842923748961</v>
+        <v>0.02152231782969481</v>
       </c>
       <c r="H2">
         <v>0.02020324814687743</v>
@@ -458,16 +458,16 @@
         <v>0.03029842497054849</v>
       </c>
       <c r="D3">
-        <v>5499998.702701763</v>
+        <v>5499997.603848021</v>
       </c>
       <c r="E3">
-        <v>296.9248002449296</v>
+        <v>296.9247912783351</v>
       </c>
       <c r="F3">
-        <v>0.8415077455509717</v>
+        <v>1.553360443562011</v>
       </c>
       <c r="G3">
-        <v>0.01819334419168741</v>
+        <v>0.01816623890213394</v>
       </c>
       <c r="H3">
         <v>0.0172623622910289</v>
@@ -484,16 +484,16 @@
         <v>0.029472504198055</v>
       </c>
       <c r="D4">
-        <v>5499896.618040415</v>
+        <v>5499807.618161806</v>
       </c>
       <c r="E4">
-        <v>296.9239672328284</v>
+        <v>296.9232409826439</v>
       </c>
       <c r="F4">
-        <v>1.03029077675371</v>
+        <v>1.905261076788692</v>
       </c>
       <c r="G4">
-        <v>0.01546028081687251</v>
+        <v>0.01543992564234681</v>
       </c>
       <c r="H4">
         <v>0.01477864358738224</v>
@@ -510,16 +510,16 @@
         <v>0.02864658342556152</v>
       </c>
       <c r="D5">
-        <v>5499747.158695379</v>
+        <v>5499528.69941133</v>
       </c>
       <c r="E5">
-        <v>296.9227476204543</v>
+        <v>296.920964909837</v>
       </c>
       <c r="F5">
-        <v>1.256217104954766</v>
+        <v>2.327757902124035</v>
       </c>
       <c r="G5">
-        <v>0.01321479369161234</v>
+        <v>0.01319977009156505</v>
       </c>
       <c r="H5">
         <v>0.01266810802241308</v>
@@ -536,16 +536,16 @@
         <v>0.02782066265306801</v>
       </c>
       <c r="D6">
-        <v>5499529.104279474</v>
+        <v>5499120.549530844</v>
       </c>
       <c r="E6">
-        <v>296.920968213767</v>
+        <v>296.9176341005143</v>
       </c>
       <c r="F6">
-        <v>1.527082109751978</v>
+        <v>2.836132519516152</v>
       </c>
       <c r="G6">
-        <v>0.01135053521384319</v>
+        <v>0.01133970503886501</v>
       </c>
       <c r="H6">
         <v>0.01086523569947432</v>
@@ -562,16 +562,16 @@
         <v>0.02699474188057452</v>
       </c>
       <c r="D7">
-        <v>5499211.393426839</v>
+        <v>5498523.850354813</v>
       </c>
       <c r="E7">
-        <v>296.9183754719548</v>
+        <v>296.9127642322449</v>
       </c>
       <c r="F7">
-        <v>1.852741411093201</v>
+        <v>3.449854618179286</v>
       </c>
       <c r="G7">
-        <v>0.009788054337672488</v>
+        <v>0.009780474216800205</v>
       </c>
       <c r="H7">
         <v>0.009318242253421361</v>
@@ -588,16 +588,16 @@
         <v>0.02616882110808103</v>
       </c>
       <c r="D8">
-        <v>5498748.143734373</v>
+        <v>5497650.466395412</v>
       </c>
       <c r="E8">
-        <v>296.9145948175445</v>
+        <v>296.9056354830771</v>
       </c>
       <c r="F8">
-        <v>2.245802556736555</v>
+        <v>4.194046322517058</v>
       </c>
       <c r="G8">
-        <v>0.008467092545497873</v>
+        <v>0.008461947983695392</v>
       </c>
       <c r="H8">
         <v>0.007985701757026981</v>
@@ -614,16 +614,16 @@
         <v>0.02534290033558753</v>
       </c>
       <c r="D9">
-        <v>5498070.801389691</v>
+        <v>5496367.834005219</v>
       </c>
       <c r="E9">
-        <v>296.9090664612397</v>
+        <v>296.8951647206952</v>
       </c>
       <c r="F9">
-        <v>2.722620103068041</v>
+        <v>5.101615986322027</v>
       </c>
       <c r="G9">
-        <v>0.007341278443160073</v>
+        <v>0.007337829090730687</v>
       </c>
       <c r="H9">
         <v>0.006834091180837826</v>
@@ -640,16 +640,16 @@
         <v>0.02451697956309404</v>
       </c>
       <c r="D10">
-        <v>5497075.502209187</v>
+        <v>5494473.565100662</v>
       </c>
       <c r="E10">
-        <v>296.9009420072986</v>
+        <v>296.8796972994979</v>
       </c>
       <c r="F10">
-        <v>3.304775164056951</v>
+        <v>6.216474544480375</v>
       </c>
       <c r="G10">
-        <v>0.006374395174157256</v>
+        <v>0.006371924515706349</v>
       </c>
       <c r="H10">
         <v>0.005835970092700017</v>
@@ -666,16 +666,16 @@
         <v>0.02369105879060053</v>
       </c>
       <c r="D11">
-        <v>5495602.161115331</v>
+        <v>5491652.919295067</v>
       </c>
       <c r="E11">
-        <v>296.8889132246661</v>
+        <v>296.856657773095</v>
       </c>
       <c r="F11">
-        <v>4.021371494528567</v>
+        <v>7.598598031341215</v>
       </c>
       <c r="G11">
-        <v>0.005537682882460314</v>
+        <v>0.005535445932675241</v>
       </c>
       <c r="H11">
         <v>0.004968596761149266</v>
@@ -692,16 +692,16 @@
         <v>0.02286513801810705</v>
       </c>
       <c r="D12">
-        <v>5493398.65782952</v>
+        <v>5487404.931690759</v>
       </c>
       <c r="E12">
-        <v>296.8709183828676</v>
+        <v>296.8219416474126</v>
       </c>
       <c r="F12">
-        <v>4.912810633177799</v>
+        <v>9.332465738698026</v>
       </c>
       <c r="G12">
-        <v>0.004807800343710525</v>
+        <v>0.004804961938795594</v>
       </c>
       <c r="H12">
         <v>0.00421282920879272</v>
@@ -718,16 +718,16 @@
         <v>0.02203921724561356</v>
       </c>
       <c r="D13">
-        <v>5490056.613802218</v>
+        <v>5480907.764206424</v>
       </c>
       <c r="E13">
-        <v>296.8436146876091</v>
+        <v>296.7688029081597</v>
       </c>
       <c r="F13">
-        <v>6.037527169608092</v>
+        <v>11.54228525166799</v>
       </c>
       <c r="G13">
-        <v>0.004165128421075618</v>
+        <v>0.004160682001944716</v>
       </c>
       <c r="H13">
         <v>0.003552164476049919</v>
@@ -744,16 +744,16 @@
         <v>0.02121329647312005</v>
       </c>
       <c r="D14">
-        <v>5484888.558368316</v>
+        <v>5470756.37802972</v>
       </c>
       <c r="E14">
-        <v>296.8013668028606</v>
+        <v>296.6856766115824</v>
       </c>
       <c r="F14">
-        <v>7.485573325886913</v>
+        <v>14.42286337312631</v>
       </c>
       <c r="G14">
-        <v>0.003591990189389377</v>
+        <v>0.003584642066983163</v>
       </c>
       <c r="H14">
         <v>0.002971681366204205</v>
@@ -770,16 +770,16 @@
         <v>0.02038737570062656</v>
       </c>
       <c r="D15">
-        <v>5476668.853859019</v>
+        <v>5454398.366317432</v>
       </c>
       <c r="E15">
-        <v>296.7341068244857</v>
+        <v>296.5514675122005</v>
       </c>
       <c r="F15">
-        <v>9.412129923544473</v>
+        <v>18.31525138320045</v>
       </c>
       <c r="G15">
-        <v>0.003069650663354039</v>
+        <v>0.003057649938999656</v>
       </c>
       <c r="H15">
         <v>0.002456181111012695</v>
@@ -796,16 +796,16 @@
         <v>0.01956145492813306</v>
       </c>
       <c r="D16">
-        <v>5462988.266798217</v>
+        <v>5426704.926498219</v>
       </c>
       <c r="E16">
-        <v>296.6219831286496</v>
+        <v>296.3235255856723</v>
       </c>
       <c r="F16">
-        <v>12.16011662798496</v>
+        <v>23.97583315808031</v>
       </c>
       <c r="G16">
-        <v>0.002567864130713002</v>
+        <v>0.002548802320326104</v>
       </c>
       <c r="H16">
         <v>0.001983469182924385</v>
@@ -822,16 +822,16 @@
         <v>0.01911027116091851</v>
       </c>
       <c r="D17">
-        <v>5437976.330688057</v>
+        <v>5374915.838027439</v>
       </c>
       <c r="E17">
-        <v>296.4164106712943</v>
+        <v>295.8947666204836</v>
       </c>
       <c r="F17">
-        <v>18.58664114488482</v>
+        <v>37.34683576855249</v>
       </c>
       <c r="G17">
-        <v>0.001768345742272758</v>
+        <v>0.001743046571665849</v>
       </c>
       <c r="H17">
         <v>0.001375818895597124</v>
@@ -848,16 +848,16 @@
         <v>0.02088988309406883</v>
       </c>
       <c r="D18">
-        <v>5349923.159843042</v>
+        <v>5189309.81327923</v>
       </c>
       <c r="E18">
-        <v>295.6866832508403</v>
+        <v>294.3308859613708</v>
       </c>
       <c r="F18">
-        <v>18.01372911891912</v>
+        <v>37.85497441977891</v>
       </c>
       <c r="G18">
-        <v>0.001607909656058838</v>
+        <v>0.001544826706557237</v>
       </c>
       <c r="H18">
         <v>0.001442167468283976</v>
@@ -874,16 +874,16 @@
         <v>0.02266949502721918</v>
       </c>
       <c r="D19">
-        <v>5352189.797854902</v>
+        <v>5172043.945375251</v>
       </c>
       <c r="E19">
-        <v>295.7055863850083</v>
+        <v>294.1831900426246</v>
       </c>
       <c r="F19">
-        <v>16.08531615342682</v>
+        <v>34.52333685584968</v>
       </c>
       <c r="G19">
-        <v>0.001613902923215904</v>
+        <v>0.001546548153195768</v>
       </c>
       <c r="H19">
         <v>0.001610289899490365</v>
@@ -900,16 +900,16 @@
         <v>0.02444910696036953</v>
       </c>
       <c r="D20">
-        <v>5369362.107155268</v>
+        <v>5201143.326950083</v>
       </c>
       <c r="E20">
-        <v>295.8485936877221</v>
+        <v>294.4318909240425</v>
       </c>
       <c r="F20">
-        <v>14.23266442466431</v>
+        <v>30.95196944053182</v>
       </c>
       <c r="G20">
-        <v>0.001657343572779781</v>
+        <v>0.001595781538908876</v>
       </c>
       <c r="H20">
         <v>0.001810478945500592</v>
@@ -926,16 +926,16 @@
         <v>0.02622871889351988</v>
       </c>
       <c r="D21">
-        <v>5384077.888665413</v>
+        <v>5229734.998231443</v>
       </c>
       <c r="E21">
-        <v>295.9708562192955</v>
+        <v>294.6751958583532</v>
       </c>
       <c r="F21">
-        <v>12.62473779067948</v>
+        <v>27.8120555056158</v>
       </c>
       <c r="G21">
-        <v>0.001716633876875941</v>
+        <v>0.001661512407817518</v>
       </c>
       <c r="H21">
         <v>0.002032465414512359</v>
@@ -952,16 +952,16 @@
         <v>0.0280083308266702</v>
       </c>
       <c r="D22">
-        <v>5395274.777311618</v>
+        <v>5251696.151926484</v>
       </c>
       <c r="E22">
-        <v>296.0637058792036</v>
+        <v>294.8613714209106</v>
       </c>
       <c r="F22">
-        <v>11.25630094082822</v>
+        <v>25.14447753493641</v>
       </c>
       <c r="G22">
-        <v>0.001784810219588252</v>
+        <v>0.001735275096531332</v>
       </c>
       <c r="H22">
         <v>0.002272623224529434</v>
@@ -978,16 +978,16 @@
         <v>0.02978794275982054</v>
       </c>
       <c r="D23">
-        <v>5403638.922639515</v>
+        <v>5267958.622750903</v>
       </c>
       <c r="E23">
-        <v>296.1329656372595</v>
+        <v>294.9988435318352</v>
       </c>
       <c r="F23">
-        <v>10.09381367877184</v>
+        <v>22.88413047959628</v>
       </c>
       <c r="G23">
-        <v>0.001858727434209209</v>
+        <v>0.001814023674314247</v>
       </c>
       <c r="H23">
         <v>0.002529237197972135</v>
@@ -1004,16 +1004,16 @@
         <v>0.03156755469297089</v>
       </c>
       <c r="D24">
-        <v>5409904.913654497</v>
+        <v>5280024.561107883</v>
       </c>
       <c r="E24">
-        <v>296.1847958800383</v>
+        <v>295.1006258896663</v>
       </c>
       <c r="F24">
-        <v>9.102566461239769</v>
+        <v>20.95962758281495</v>
       </c>
       <c r="G24">
-        <v>0.001936699597169171</v>
+        <v>0.001896342173178979</v>
       </c>
       <c r="H24">
         <v>0.002801349237103969</v>
@@ -1030,16 +1030,16 @@
         <v>0.03334716662612121</v>
       </c>
       <c r="D25">
-        <v>5414642.735470098</v>
+        <v>5289072.176067227</v>
       </c>
       <c r="E25">
-        <v>296.2239540162203</v>
+        <v>295.1768273619546</v>
       </c>
       <c r="F25">
-        <v>8.25250916498068</v>
+        <v>19.31017728111308</v>
       </c>
       <c r="G25">
-        <v>0.002017724203462729</v>
+        <v>0.001981453772511028</v>
       </c>
       <c r="H25">
         <v>0.00308836156752128</v>
@@ -1056,16 +1056,16 @@
         <v>0.03512677855927156</v>
       </c>
       <c r="D26">
-        <v>5418265.516548609</v>
+        <v>5295941.02113464</v>
       </c>
       <c r="E26">
-        <v>296.2538780030267</v>
+        <v>295.2346102599749</v>
       </c>
       <c r="F26">
-        <v>7.518945184261105</v>
+        <v>17.8867564531081</v>
       </c>
       <c r="G26">
-        <v>0.002101161028957978</v>
+        <v>0.002068888033076004</v>
       </c>
       <c r="H26">
         <v>0.003389870449412019</v>
@@ -1082,16 +1082,16 @@
         <v>0.03690639049242189</v>
       </c>
       <c r="D27">
-        <v>5421067.884588552</v>
+        <v>5301219.989768418</v>
       </c>
       <c r="E27">
-        <v>296.277014534627</v>
+        <v>295.278978580018</v>
       </c>
       <c r="F27">
-        <v>6.881918018617308</v>
+        <v>16.6503386342496</v>
       </c>
       <c r="G27">
-        <v>0.00218657916517405</v>
+        <v>0.002158341379528108</v>
       </c>
       <c r="H27">
         <v>0.003705586539372037</v>
@@ -1108,16 +1108,16 @@
         <v>0.03868600242557224</v>
       </c>
       <c r="D28">
-        <v>5423260.130983153</v>
+        <v>5305323.928629476</v>
       </c>
       <c r="E28">
-        <v>296.2951072478307</v>
+        <v>295.3134470844773</v>
       </c>
       <c r="F28">
-        <v>6.325360383656647</v>
+        <v>15.56984897767723</v>
       </c>
       <c r="G28">
-        <v>0.002273676651257643</v>
+        <v>0.002249609362372226</v>
       </c>
       <c r="H28">
         <v>0.004035292833437207</v>
@@ -1134,16 +1134,16 @@
         <v>0.04046561435872258</v>
       </c>
       <c r="D29">
-        <v>5424993.468762037</v>
+        <v>5308548.177246572</v>
       </c>
       <c r="E29">
-        <v>296.3094084582738</v>
+        <v>295.3405124604239</v>
       </c>
       <c r="F29">
-        <v>5.836309450260463</v>
+        <v>14.62041824195017</v>
       </c>
       <c r="G29">
-        <v>0.00236223501961497</v>
+        <v>0.002342550368120514</v>
       </c>
       <c r="H29">
         <v>0.004378820712803174</v>
@@ -1160,16 +1160,16 @@
         <v>0.04224522629187291</v>
       </c>
       <c r="D30">
-        <v>5426377.726978139</v>
+        <v>5311105.637268392</v>
       </c>
       <c r="E30">
-        <v>296.3208269215223</v>
+        <v>295.3619714001243</v>
       </c>
       <c r="F30">
-        <v>5.404257858161249</v>
+        <v>13.78200578963464</v>
       </c>
       <c r="G30">
-        <v>0.002452092061246507</v>
+        <v>0.002437064711475275</v>
       </c>
       <c r="H30">
         <v>0.004736035447923758</v>
@@ -1186,16 +1186,16 @@
         <v>0.04402483822502326</v>
       </c>
       <c r="D31">
-        <v>5427493.555365231</v>
+        <v>5313151.759302224</v>
       </c>
       <c r="E31">
-        <v>296.3300294790017</v>
+        <v>295.3791339881188</v>
       </c>
       <c r="F31">
-        <v>5.020638460818896</v>
+        <v>13.0383415174207</v>
       </c>
       <c r="G31">
-        <v>0.002543124731862501</v>
+        <v>0.002533081884805252</v>
       </c>
       <c r="H31">
         <v>0.005106826977759883</v>
@@ -1212,16 +1212,16 @@
         <v>0.04580445015817358</v>
       </c>
       <c r="D32">
-        <v>5428400.836237681</v>
+        <v>5314801.466206121</v>
       </c>
       <c r="E32">
-        <v>296.3375109781622</v>
+        <v>295.3929677125503</v>
       </c>
       <c r="F32">
-        <v>4.678421680333652</v>
+        <v>12.37611845085486</v>
       </c>
       <c r="G32">
-        <v>0.002635238004947057</v>
+        <v>0.002630552418606046</v>
       </c>
       <c r="H32">
         <v>0.005491103793679444</v>
@@ -1238,16 +1238,16 @@
         <v>0.04758406209132393</v>
       </c>
       <c r="D33">
-        <v>5429144.515633345</v>
+        <v>5316140.72850976</v>
       </c>
       <c r="E33">
-        <v>296.3436426682219</v>
+        <v>295.4041956974494</v>
       </c>
       <c r="F33">
-        <v>4.371802364411597</v>
+        <v>11.78437589804371</v>
       </c>
       <c r="G33">
-        <v>0.002728357366638765</v>
+        <v>0.002729442488249003</v>
       </c>
       <c r="H33">
         <v>0.005888788735379971</v>
@@ -1264,16 +1264,16 @@
         <v>0.04936367402447427</v>
       </c>
       <c r="D34">
-        <v>5429758.680740672</v>
+        <v>5317234.575669116</v>
       </c>
       <c r="E34">
-        <v>296.3487060009287</v>
+        <v>295.4133645409352</v>
       </c>
       <c r="F34">
-        <v>4.095956091246893</v>
+        <v>11.25402591303511</v>
       </c>
       <c r="G34">
-        <v>0.002822423623361268</v>
+        <v>0.002829730229293787</v>
       </c>
       <c r="H34">
         <v>0.006299816010575412</v>
@@ -1290,16 +1290,16 @@
         <v>0.05114328595762462</v>
       </c>
       <c r="D35">
-        <v>5430269.439620107</v>
+        <v>5318132.709238175</v>
       </c>
       <c r="E35">
-        <v>296.3529164801812</v>
+        <v>295.4208917639444</v>
       </c>
       <c r="F35">
-        <v>3.846848860610553</v>
+        <v>10.77748742787503</v>
       </c>
       <c r="G35">
-        <v>0.002917389224563415</v>
+        <v>0.002931403155950268</v>
       </c>
       <c r="H35">
         <v>0.00672412902473772</v>
@@ -1316,16 +1316,16 @@
         <v>0.05292289789077495</v>
       </c>
       <c r="D36">
-        <v>5430696.976339962</v>
+        <v>5318873.484068974</v>
       </c>
       <c r="E36">
-        <v>296.356440669534</v>
+        <v>295.4270994160586</v>
       </c>
       <c r="F36">
-        <v>3.621087738427608</v>
+        <v>10.34840157666648</v>
       </c>
       <c r="G36">
-        <v>0.003013215604924833</v>
+        <v>0.003034456314805123</v>
       </c>
       <c r="H36">
         <v>0.007161678762882656</v>
@@ -1342,16 +1342,16 @@
         <v>0.05470250982392529</v>
       </c>
       <c r="D37">
-        <v>5431057.033012887</v>
+        <v>5319486.765510894</v>
       </c>
       <c r="E37">
-        <v>296.3594084493158</v>
+        <v>295.4322381654423</v>
       </c>
       <c r="F37">
-        <v>3.415802972044199</v>
+        <v>9.961408617581677</v>
       </c>
       <c r="G37">
-        <v>0.003109871228734736</v>
+        <v>0.003138890942407212</v>
       </c>
       <c r="H37">
         <v>0.007612422557416451</v>
@@ -1368,16 +1368,16 @@
         <v>0.05648212175707563</v>
       </c>
       <c r="D38">
-        <v>5431361.989504386</v>
+        <v>5319996.003141358</v>
       </c>
       <c r="E38">
-        <v>296.3619219417183</v>
+        <v>295.4365047662669</v>
       </c>
       <c r="F38">
-        <v>3.228554381921683</v>
+        <v>9.611971927926962</v>
       </c>
       <c r="G38">
-        <v>0.003207330127930173</v>
+        <v>0.003244713476697272</v>
       </c>
       <c r="H38">
         <v>0.008076323132214198</v>
@@ -1394,16 +1394,16 @@
         <v>0.05826173369022596</v>
       </c>
       <c r="D39">
-        <v>5431621.657818756</v>
+        <v>5320419.751983259</v>
       </c>
       <c r="E39">
-        <v>296.36406207454</v>
+        <v>295.897657991236</v>
       </c>
       <c r="F39">
-        <v>3.057256573530843</v>
+        <v>9.286683155768383</v>
       </c>
       <c r="G39">
-        <v>0.003305570793560902</v>
+        <v>0.003279678191635957</v>
       </c>
       <c r="H39">
         <v>0.008553347848405078</v>
@@ -1420,16 +1420,16 @@
         <v>0.0600413456233763</v>
       </c>
       <c r="D40">
-        <v>5431843.872105212</v>
+        <v>5320793.173792223</v>
       </c>
       <c r="E40">
-        <v>296.365893454457</v>
+        <v>296.3676124108536</v>
       </c>
       <c r="F40">
-        <v>2.900118821016879</v>
+        <v>8.974335705253397</v>
       </c>
       <c r="G40">
-        <v>0.003404575324570047</v>
+        <v>0.003316601154591095</v>
       </c>
       <c r="H40">
         <v>0.009043468100516717</v>
@@ -1446,16 +1446,16 @@
         <v>0.06182095755652664</v>
       </c>
       <c r="D41">
-        <v>5432034.930832908</v>
+        <v>5321136.697293273</v>
       </c>
       <c r="E41">
-        <v>296.3674680181466</v>
+        <v>296.8454770643189</v>
       </c>
       <c r="F41">
-        <v>2.755596456299814</v>
+        <v>8.675647714232436</v>
       </c>
       <c r="G41">
-        <v>0.003504328766174295</v>
+        <v>0.003355404721589744</v>
       </c>
       <c r="H41">
         <v>0.009546658825384711</v>
@@ -1472,16 +1472,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D42">
-        <v>5432199.931028659</v>
+        <v>5321451.144076061</v>
       </c>
       <c r="E42">
-        <v>296.3688277914393</v>
+        <v>297.3304269947514</v>
       </c>
       <c r="F42">
-        <v>2.631236079486683</v>
+        <v>8.418594958573827</v>
       </c>
       <c r="G42">
-        <v>0.003599125265811534</v>
+        <v>0.003390502677704885</v>
       </c>
       <c r="H42">
         <v>0.01003337684633662</v>
@@ -1498,16 +1498,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D43">
-        <v>5432335.760710913</v>
+        <v>5321714.291417698</v>
       </c>
       <c r="E43">
-        <v>296.3699471447355</v>
+        <v>297.8223271327865</v>
       </c>
       <c r="F43">
-        <v>2.66018461787659</v>
+        <v>8.640557542866725</v>
       </c>
       <c r="G43">
-        <v>0.003599223528243177</v>
+        <v>0.003338612075891804</v>
       </c>
       <c r="H43">
         <v>0.01003337684633662</v>
@@ -1524,16 +1524,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D44">
-        <v>5432272.738035896</v>
+        <v>5321308.974492349</v>
       </c>
       <c r="E44">
-        <v>296.3694277865036</v>
+        <v>298.3309668814039</v>
       </c>
       <c r="F44">
-        <v>2.689861508022588</v>
+        <v>8.867831258913856</v>
       </c>
       <c r="G44">
-        <v>0.003599230817925349</v>
+        <v>0.00328837468714456</v>
       </c>
       <c r="H44">
         <v>0.01003337684633662</v>
@@ -1550,16 +1550,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D45">
-        <v>5432208.487364517</v>
+        <v>5320886.071337334</v>
       </c>
       <c r="E45">
-        <v>296.368898303655</v>
+        <v>298.8565122200457</v>
       </c>
       <c r="F45">
-        <v>2.720177749286444</v>
+        <v>9.095920371797364</v>
       </c>
       <c r="G45">
-        <v>0.003599278288524407</v>
+        <v>0.003240432182242853</v>
       </c>
       <c r="H45">
         <v>0.01003337684633662</v>
@@ -1576,16 +1576,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D46">
-        <v>5432143.118824018</v>
+        <v>5320451.761352854</v>
       </c>
       <c r="E46">
-        <v>296.3683596034635</v>
+        <v>299.3988242580751</v>
       </c>
       <c r="F46">
-        <v>2.751154184772889</v>
+        <v>9.32481277206205</v>
       </c>
       <c r="G46">
-        <v>0.003599367296863611</v>
+        <v>0.003194620484015525</v>
       </c>
       <c r="H46">
         <v>0.01003337684633662</v>
@@ -1602,16 +1602,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D47">
-        <v>5432076.600148802</v>
+        <v>5320005.961904661</v>
       </c>
       <c r="E47">
-        <v>296.3678114197615</v>
+        <v>299.9577515912276</v>
       </c>
       <c r="F47">
-        <v>2.782812669171545</v>
+        <v>9.554535680751886</v>
       </c>
       <c r="G47">
-        <v>0.003599499152917536</v>
+        <v>0.003150785335715752</v>
       </c>
       <c r="H47">
         <v>0.01003337684633662</v>
@@ -1628,16 +1628,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D48">
-        <v>5432008.897637835</v>
+        <v>5319548.52941865</v>
       </c>
       <c r="E48">
-        <v>296.3672534745363</v>
+        <v>300.5331334773247</v>
       </c>
       <c r="F48">
-        <v>2.815176042641838</v>
+        <v>9.785113820720367</v>
       </c>
       <c r="G48">
-        <v>0.00359967521531815</v>
+        <v>0.00310878740725311</v>
       </c>
       <c r="H48">
         <v>0.01003337684633662</v>
@@ -1654,16 +1654,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D49">
-        <v>5431939.976185316</v>
+        <v>5319079.319084472</v>
       </c>
       <c r="E49">
-        <v>296.3666854781823</v>
+        <v>301.1248003106082</v>
       </c>
       <c r="F49">
-        <v>2.84826818749012</v>
+        <v>10.01656946601496</v>
       </c>
       <c r="G49">
-        <v>0.003599896893639757</v>
+        <v>0.003068500503088111</v>
       </c>
       <c r="H49">
         <v>0.01003337684633662</v>
@@ -1680,16 +1680,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D50">
-        <v>5431869.799204085</v>
+        <v>5318598.185160685</v>
       </c>
       <c r="E50">
-        <v>296.3661071288687</v>
+        <v>301.7325740792267</v>
       </c>
       <c r="F50">
-        <v>2.882114088902484</v>
+        <v>10.24892284337339</v>
       </c>
       <c r="G50">
-        <v>0.003600165650736703</v>
+        <v>0.003029809978512314</v>
       </c>
       <c r="H50">
         <v>0.01003337684633662</v>
@@ -1706,16 +1706,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D51">
-        <v>5431798.328543745</v>
+        <v>5318104.980698022</v>
       </c>
       <c r="E51">
-        <v>296.3655181118633</v>
+        <v>302.3562688307819</v>
       </c>
       <c r="F51">
-        <v>2.916739900009322</v>
+        <v>10.48219248594043</v>
       </c>
       <c r="G51">
-        <v>0.003600483005209568</v>
+        <v>0.002992611385558168</v>
       </c>
       <c r="H51">
         <v>0.01003337684633662</v>
@@ -1732,16 +1732,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D52">
-        <v>5431725.524403168</v>
+        <v>5317599.557266882</v>
       </c>
       <c r="E52">
-        <v>296.3649180988101</v>
+        <v>302.9956911439513</v>
       </c>
       <c r="F52">
-        <v>2.952173011648398</v>
+        <v>10.71639561158416</v>
       </c>
       <c r="G52">
-        <v>0.003600850534008457</v>
+        <v>0.002956809291473403</v>
       </c>
       <c r="H52">
         <v>0.01003337684633662</v>
@@ -1758,16 +1758,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D53">
-        <v>5431651.345236907</v>
+        <v>5317081.764579857</v>
       </c>
       <c r="E53">
-        <v>296.3643067469571</v>
+        <v>303.6506406143278</v>
       </c>
       <c r="F53">
-        <v>2.988442127229649</v>
+        <v>10.95154834299726</v>
       </c>
       <c r="G53">
-        <v>0.003601269875182006</v>
+        <v>0.002922316293770902</v>
       </c>
       <c r="H53">
         <v>0.01003337684633662</v>
@@ -1784,16 +1784,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D54">
-        <v>5431575.74765501</v>
+        <v>5316551.450310919</v>
       </c>
       <c r="E54">
-        <v>296.3636836983286</v>
+        <v>304.3209103342317</v>
       </c>
       <c r="F54">
-        <v>3.02557734314463</v>
+        <v>11.18766603382409</v>
       </c>
       <c r="G54">
-        <v>0.003601742730782057</v>
+        <v>0.002889052130259958</v>
       </c>
       <c r="H54">
         <v>0.01003337684633662</v>
@@ -1810,16 +1810,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D55">
-        <v>5431498.686315686</v>
+        <v>5316008.459695411</v>
       </c>
       <c r="E55">
-        <v>296.3630485788399</v>
+        <v>305.0062873855798</v>
       </c>
       <c r="F55">
-        <v>3.063610235208777</v>
+        <v>11.42476349732839</v>
       </c>
       <c r="G55">
-        <v>0.003602270869933981</v>
+        <v>0.002856942924967937</v>
       </c>
       <c r="H55">
         <v>0.01003337684633662</v>
@@ -1836,16 +1836,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D56">
-        <v>5431420.113810195</v>
+        <v>5315452.635239011</v>
       </c>
       <c r="E56">
-        <v>296.3624009973458</v>
+        <v>305.7065533332124</v>
       </c>
       <c r="F56">
-        <v>3.102573951674102</v>
+        <v>11.66285522668682</v>
       </c>
       <c r="G56">
-        <v>0.003602856132084051</v>
+        <v>0.002825920526585479</v>
       </c>
       <c r="H56">
         <v>0.01003337684633662</v>
@@ -1862,16 +1862,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D57">
-        <v>5431339.980539303</v>
+        <v>5314883.816400476</v>
       </c>
       <c r="E57">
-        <v>296.3617405446212</v>
+        <v>306.4214847193604</v>
       </c>
       <c r="F57">
-        <v>3.14250331340599</v>
+        <v>11.90195559367504</v>
       </c>
       <c r="G57">
-        <v>0.003603500430435606</v>
+        <v>0.002795921930008415</v>
       </c>
       <c r="H57">
         <v>0.01003337684633662</v>
@@ -1888,16 +1888,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D58">
-        <v>5431258.23458055</v>
+        <v>5314301.839273054</v>
       </c>
       <c r="E58">
-        <v>296.3610667922648</v>
+        <v>307.1508535574325</v>
       </c>
       <c r="F58">
-        <v>3.183434921879934</v>
+        <v>12.1420790272273</v>
       </c>
       <c r="G58">
-        <v>0.003604205755586952</v>
+        <v>0.00276688876912453</v>
       </c>
       <c r="H58">
         <v>0.01003337684633662</v>
@@ -1914,16 +1914,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D59">
-        <v>5431174.82154551</v>
+        <v>5313706.53626611</v>
       </c>
       <c r="E59">
-        <v>296.360379291521</v>
+        <v>307.8944278232319</v>
       </c>
       <c r="F59">
-        <v>3.225407275723776</v>
+        <v>12.38324017330717</v>
       </c>
       <c r="G59">
-        <v>0.003604974179384996</v>
+        <v>0.002738766870866099</v>
       </c>
       <c r="H59">
         <v>0.01003337684633662</v>
@@ -1940,16 +1940,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D60">
-        <v>5431089.684426145</v>
+        <v>5313097.735788202</v>
       </c>
       <c r="E60">
-        <v>296.3596775720108</v>
+        <v>308.6519719416885</v>
       </c>
       <c r="F60">
-        <v>3.268460896609587</v>
+        <v>12.62545403738776</v>
       </c>
       <c r="G60">
-        <v>0.003605807859009492</v>
+        <v>0.002711505862102082</v>
       </c>
       <c r="H60">
         <v>0.01003337684633662</v>
@@ -1966,16 +1966,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D61">
-        <v>5431002.763429251</v>
+        <v>5312475.261932719</v>
       </c>
       <c r="E61">
-        <v>296.358961140365</v>
+        <v>309.4232472672026</v>
       </c>
       <c r="F61">
-        <v>3.312638465386973</v>
+        <v>12.86873611073721</v>
       </c>
       <c r="G61">
-        <v>0.003606709041304156</v>
+        <v>0.002685058822227869</v>
       </c>
       <c r="H61">
         <v>0.01003337684633662</v>
@@ -1992,16 +1992,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D62">
-        <v>5430913.995797884</v>
+        <v>5311838.934167053</v>
       </c>
       <c r="E62">
-        <v>296.3582294787489</v>
+        <v>310.2080125557435</v>
       </c>
       <c r="F62">
-        <v>3.357984969448656</v>
+        <v>13.11310248162869</v>
       </c>
       <c r="G62">
-        <v>0.003607680067372271</v>
+        <v>0.002659381975377083</v>
       </c>
       <c r="H62">
         <v>0.01003337684633662</v>
@@ -2018,16 +2018,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D63">
-        <v>5430823.315618539</v>
+        <v>5311188.567026115</v>
       </c>
       <c r="E63">
-        <v>296.3574820432711</v>
+        <v>311.0060244269217</v>
       </c>
       <c r="F63">
-        <v>3.404547862430942</v>
+        <v>13.3585699325375</v>
       </c>
       <c r="G63">
-        <v>0.003608723377455402</v>
+        <v>0.002634434417070125</v>
       </c>
       <c r="H63">
         <v>0.01003337684633662</v>
@@ -2044,16 +2044,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D64">
-        <v>5430730.653612722</v>
+        <v>5310523.969810876</v>
       </c>
       <c r="E64">
-        <v>296.3567182622618</v>
+        <v>311.8170378143535</v>
       </c>
       <c r="F64">
-        <v>3.45237723747713</v>
+        <v>13.60515602434482</v>
       </c>
       <c r="G64">
-        <v>0.003609841516116027</v>
+        <v>0.002610177870860088</v>
       </c>
       <c r="H64">
         <v>0.01003337684633662</v>
@@ -2070,16 +2070,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D65">
-        <v>5430635.936911387</v>
+        <v>5309844.946292405</v>
       </c>
       <c r="E65">
-        <v>296.3559375344101</v>
+        <v>312.6408064027602</v>
       </c>
       <c r="F65">
-        <v>3.501526015434477</v>
+        <v>13.85287916853467</v>
       </c>
       <c r="G65">
-        <v>0.003611037137746317</v>
+        <v>0.002586576471164544</v>
       </c>
       <c r="H65">
         <v>0.01003337684633662</v>
@@ -2096,16 +2096,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D66">
-        <v>5430539.08881057</v>
+        <v>5309151.294421748</v>
       </c>
       <c r="E66">
-        <v>296.3551392267456</v>
+        <v>313.4770830503858</v>
       </c>
       <c r="F66">
-        <v>3.552050149516687</v>
+        <v>14.10175868834147</v>
       </c>
       <c r="G66">
-        <v>0.003612313012426694</v>
+        <v>0.002563596569002222</v>
       </c>
       <c r="H66">
         <v>0.01003337684633662</v>
@@ -2122,16 +2122,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D67">
-        <v>5430440.0285063</v>
+        <v>5308442.806045805</v>
       </c>
       <c r="E67">
-        <v>296.3543226724495</v>
+        <v>314.3256201954661</v>
       </c>
       <c r="F67">
-        <v>3.604008848146284</v>
+        <v>14.35181486978126</v>
       </c>
       <c r="G67">
-        <v>0.003613672032160909</v>
+        <v>0.002541206557803442</v>
       </c>
       <c r="H67">
         <v>0.01003337684633662</v>
@@ -2148,16 +2148,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D68">
-        <v>5430338.670806727</v>
+        <v>5307719.266629213</v>
       </c>
       <c r="E68">
-        <v>296.353487168477</v>
+        <v>315.1861702456525</v>
       </c>
       <c r="F68">
-        <v>3.657464817899802</v>
+        <v>14.6030690034745</v>
       </c>
       <c r="G68">
-        <v>0.003615117217515274</v>
+        <v>0.002519376716846038</v>
       </c>
       <c r="H68">
         <v>0.01003337684633662</v>
@@ -2174,16 +2174,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D69">
-        <v>5430234.925819065</v>
+        <v>5306980.45498211</v>
       </c>
       <c r="E69">
-        <v>296.352631972972</v>
+        <v>316.0584859494544</v>
       </c>
       <c r="F69">
-        <v>3.712484528714702</v>
+        <v>14.85554341814237</v>
       </c>
       <c r="G69">
-        <v>0.003616651724693363</v>
+        <v>0.002498079070195466</v>
       </c>
       <c r="H69">
         <v>0.01003337684633662</v>
@@ -2200,16 +2200,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D70">
-        <v>5430128.698608744</v>
+        <v>5306226.142993493</v>
       </c>
       <c r="E70">
-        <v>296.3517563024513</v>
+        <v>316.9423207489422</v>
       </c>
       <c r="F70">
-        <v>3.769138503787551</v>
+        <v>15.10926150663207</v>
       </c>
       <c r="G70">
-        <v>0.003618278853079547</v>
+        <v>0.002477287259307603</v>
       </c>
       <c r="H70">
         <v>0.01003337684633662</v>
@@ -2226,16 +2226,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D71">
-        <v>5430019.888827779</v>
+        <v>5305456.095369785</v>
       </c>
       <c r="E71">
-        <v>296.3508593287355</v>
+        <v>317.8374291131187</v>
       </c>
       <c r="F71">
-        <v>3.827501636901852</v>
+        <v>15.36424774529622</v>
       </c>
       <c r="G71">
-        <v>0.003620002053287435</v>
+        <v>0.002456976427693247</v>
       </c>
       <c r="H71">
         <v>0.01003337684633662</v>
@@ -2252,16 +2252,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D72">
-        <v>5429908.390309046</v>
+        <v>5304670.069378096</v>
       </c>
       <c r="E72">
-        <v>296.3499401755981</v>
+        <v>318.7435668515346</v>
       </c>
       <c r="F72">
-        <v>3.887653540277206</v>
+        <v>15.62052770751926</v>
       </c>
       <c r="G72">
-        <v>0.003621824935753227</v>
+        <v>0.002437123116250169</v>
       </c>
       <c r="H72">
         <v>0.01003337684633662</v>
@@ -2278,16 +2278,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D73">
-        <v>5429794.090622672</v>
+        <v>5303867.814593573</v>
       </c>
       <c r="E73">
-        <v>296.3489979151003</v>
+        <v>319.6604914078857</v>
       </c>
       <c r="F73">
-        <v>3.949678926438166</v>
+        <v>15.87812807214916</v>
       </c>
       <c r="G73">
-        <v>0.003623751279917224</v>
+        <v>0.002417705168047126</v>
       </c>
       <c r="H73">
         <v>0.01003337684633662</v>
@@ -2304,16 +2304,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D74">
-        <v>5429676.870590323</v>
+        <v>5303049.072650169</v>
       </c>
       <c r="E74">
-        <v>296.3480315635799</v>
+        <v>320.5879621334798</v>
       </c>
       <c r="F74">
-        <v>4.013668028068305</v>
+        <v>16.13707662755472</v>
       </c>
       <c r="G74">
-        <v>0.003625785044040077</v>
+        <v>0.002398701641498593</v>
       </c>
       <c r="H74">
         <v>0.01003337684633662</v>
@@ -2330,16 +2330,16 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D75">
-        <v>5429556.603752571</v>
+        <v>5302213.576994042</v>
       </c>
       <c r="E75">
-        <v>296.347040077251</v>
+        <v>321.5257405406048</v>
       </c>
       <c r="F75">
-        <v>4.079717060353706</v>
+        <v>16.39740227198975</v>
       </c>
       <c r="G75">
-        <v>0.003627930375705978</v>
+        <v>0.002380092731002606</v>
       </c>
       <c r="H75">
         <v>0.01003337684633662</v>
@@ -2356,16 +2356,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D76">
-        <v>5429433.155783895</v>
+        <v>5301361.052638805</v>
       </c>
       <c r="E76">
-        <v>296.346022347371</v>
+        <v>322.4735905359636</v>
       </c>
       <c r="F76">
-        <v>4.147928730943187</v>
+        <v>16.65913501090406</v>
       </c>
       <c r="G76">
-        <v>0.003630191623068341</v>
+        <v>0.00236185969422999</v>
       </c>
       <c r="H76">
         <v>0.01003337684633661</v>
@@ -2382,16 +2382,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D77">
-        <v>5429306.383849133</v>
+        <v>5300491.215921746</v>
       </c>
       <c r="E77">
-        <v>296.3449771949251</v>
+        <v>323.4312786344587</v>
       </c>
       <c r="F77">
-        <v>4.218412803374157</v>
+        <v>16.92230595179869</v>
       </c>
       <c r="G77">
-        <v>0.003632573346899733</v>
+        <v>0.00234398478535398</v>
       </c>
       <c r="H77">
         <v>0.01003337684633661</v>
@@ -2408,16 +2408,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D78">
-        <v>5429176.135894339</v>
+        <v>5299603.774260125</v>
       </c>
       <c r="E78">
-        <v>296.3439033647666</v>
+        <v>324.398574153718</v>
       </c>
       <c r="F78">
-        <v>4.291286720651002</v>
+        <v>17.18694729718009</v>
       </c>
       <c r="G78">
-        <v>0.00363508033351316</v>
+        <v>0.002326451193596637</v>
       </c>
       <c r="H78">
         <v>0.01003337684633661</v>
@@ -2434,16 +2434,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D79">
-        <v>5429042.249864013</v>
+        <v>5298698.425906655</v>
       </c>
       <c r="E79">
-        <v>296.3427995191507</v>
+        <v>325.3752493898515</v>
       </c>
       <c r="F79">
-        <v>4.366676296639106</v>
+        <v>17.4530923361244</v>
       </c>
       <c r="G79">
-        <v>0.003637717608628223</v>
+        <v>0.002309242986544712</v>
       </c>
       <c r="H79">
         <v>0.01003337684633661</v>
@@ -2460,16 +2460,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D80">
-        <v>5428904.552835506</v>
+        <v>5297774.859703201</v>
       </c>
       <c r="E80">
-        <v>296.3416642305829</v>
+        <v>326.3610797750057</v>
       </c>
       <c r="F80">
-        <v>4.444716484077001</v>
+        <v>17.72077543492022</v>
       </c>
       <c r="G80">
-        <v>0.003640490452262972</v>
+        <v>0.002292345057753836</v>
       </c>
       <c r="H80">
         <v>0.01003337684633661</v>
@@ -2486,16 +2486,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D81">
-        <v>5428762.86006007</v>
+        <v>5296832.754831783</v>
       </c>
       <c r="E81">
-        <v>296.3404959738952</v>
+        <v>327.3558440173575</v>
       </c>
       <c r="F81">
-        <v>4.525552229343234</v>
+        <v>17.99003202721635</v>
       </c>
       <c r="G81">
-        <v>0.003643404414739635</v>
+        <v>0.00227574307821772</v>
       </c>
       <c r="H81">
         <v>0.01003337684633661</v>
@@ -2512,16 +2512,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D82">
-        <v>5428616.973898434</v>
+        <v>5295871.780561941</v>
       </c>
       <c r="E82">
-        <v>296.3392931174515</v>
+        <v>328.3593242242444</v>
       </c>
       <c r="F82">
-        <v>4.609339425680751</v>
+        <v>18.26089860405959</v>
       </c>
       <c r="G82">
-        <v>0.003646465333901592</v>
+        <v>0.002259423451329393</v>
       </c>
       <c r="H82">
         <v>0.01003337684633661</v>
@@ -2538,16 +2538,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D83">
-        <v>5428466.682636973</v>
+        <v>5294891.59599351</v>
       </c>
       <c r="E83">
-        <v>296.338053913366</v>
+        <v>329.3713060091758</v>
       </c>
       <c r="F83">
-        <v>4.696245978426418</v>
+        <v>18.53341270416858</v>
       </c>
       <c r="G83">
-        <v>0.003649679353647602</v>
+        <v>0.002243373271005464</v>
       </c>
       <c r="H83">
         <v>0.01003337684633661</v>
@@ -2564,16 +2564,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D84">
-        <v>5428311.759168323</v>
+        <v>5293891.849793899</v>
       </c>
       <c r="E84">
-        <v>296.3367764865998</v>
+        <v>330.3915785835034</v>
       </c>
       <c r="F84">
-        <v>4.786452997970896</v>
+        <v>18.80761290475194</v>
       </c>
       <c r="G84">
-        <v>0.003653052943901238</v>
+        <v>0.002227580282682644</v>
       </c>
       <c r="H84">
         <v>0.01003337684633661</v>
@@ -2590,16 +2590,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D85">
-        <v>5428151.959517805</v>
+        <v>5292872.179928931</v>
       </c>
       <c r="E85">
-        <v>296.335458822784</v>
+        <v>331.4199348335572</v>
       </c>
       <c r="F85">
-        <v>4.880156138756451</v>
+        <v>19.08353881314379</v>
       </c>
       <c r="G85">
-        <v>0.003656592922143409</v>
+        <v>0.002212032846929281</v>
       </c>
       <c r="H85">
         <v>0.01003337684633661</v>
@@ -2616,16 +2616,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D86">
-        <v>5427987.021193928</v>
+        <v>5291832.213386369</v>
       </c>
       <c r="E86">
-        <v>296.3340987545889</v>
+        <v>332.4561713840665</v>
       </c>
       <c r="F86">
-        <v>4.977567105687738</v>
+        <v>19.3612310594954</v>
       </c>
       <c r="G86">
-        <v>0.003660306476650242</v>
+        <v>0.00219671990544381</v>
       </c>
       <c r="H86">
         <v>0.01003337684633661</v>
@@ -2642,16 +2642,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D87">
-        <v>5427816.661337729</v>
+        <v>5290771.565891213</v>
       </c>
       <c r="E87">
-        <v>296.3326939464276</v>
+        <v>333.5000886486944</v>
       </c>
       <c r="F87">
-        <v>5.078915352992053</v>
+        <v>19.64073129073227</v>
       </c>
       <c r="G87">
-        <v>0.003664201191592089</v>
+        <v>0.002181630949237533</v>
       </c>
       <c r="H87">
         <v>0.01003337684633661</v>
@@ -2668,16 +2668,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D88">
-        <v>5427640.574641378</v>
+        <v>5289689.841611905</v>
       </c>
       <c r="E88">
-        <v>296.3312418772551</v>
+        <v>334.5514908685142</v>
       </c>
       <c r="F88">
-        <v>5.184450004946343</v>
+        <v>19.92208216595627</v>
       </c>
       <c r="G88">
-        <v>0.003668285074165264</v>
+        <v>0.002166755988821394</v>
       </c>
       <c r="H88">
         <v>0.01003337684633661</v>
@@ -2694,16 +2694,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D89">
-        <v>5427458.431001428</v>
+        <v>5288586.632856574</v>
       </c>
       <c r="E89">
-        <v>296.3297398211712</v>
+        <v>335.6101861392485</v>
       </c>
       <c r="F89">
-        <v>5.294442033154296</v>
+        <v>20.20532735344718</v>
       </c>
       <c r="G89">
-        <v>0.003672566583945874</v>
+        <v>0.002152085526235923</v>
       </c>
       <c r="H89">
         <v>0.01003337684633661</v>
@@ -2720,16 +2720,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D90">
-        <v>5427269.872865927</v>
+        <v>5287461.519758469</v>
       </c>
       <c r="E90">
-        <v>296.3281848254926</v>
+        <v>336.6759864280795</v>
       </c>
       <c r="F90">
-        <v>5.409186731407411</v>
+        <v>20.4905115293942</v>
       </c>
       <c r="G90">
-        <v>0.00367705466467366</v>
+        <v>0.002137610528780489</v>
       </c>
       <c r="H90">
         <v>0.01003337684633661</v>
@@ -2746,16 +2746,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D91">
-        <v>5427074.512227296</v>
+        <v>5286314.069949751</v>
       </c>
       <c r="E91">
-        <v>296.3265736858953</v>
+        <v>337.7487075808214</v>
       </c>
       <c r="F91">
-        <v>5.529006536854544</v>
+        <v>20.77768037846709</v>
       </c>
       <c r="G91">
-        <v>0.003681758778695989</v>
+        <v>0.002123322404312971</v>
       </c>
       <c r="H91">
         <v>0.01003337684633661</v>
@@ -2772,16 +2772,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D92">
-        <v>5426871.927203918</v>
+        <v>5285143.838222789</v>
       </c>
       <c r="E92">
-        <v>296.3249029181566</v>
+        <v>338.8281693202242</v>
       </c>
       <c r="F92">
-        <v>5.65425425555932</v>
+        <v>21.06688059631835</v>
       </c>
       <c r="G92">
-        <v>0.003686688944323826</v>
+        <v>0.002109212978003902</v>
       </c>
       <c r="H92">
         <v>0.01003337684633661</v>
@@ -2798,16 +2798,16 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D93">
-        <v>5426661.658142647</v>
+        <v>5283950.366178161</v>
       </c>
       <c r="E93">
-        <v>296.3231687259336</v>
+        <v>339.9141952361504</v>
       </c>
       <c r="F93">
-        <v>5.785316761949177</v>
+        <v>21.35815989409046</v>
       </c>
       <c r="G93">
-        <v>0.003691855776378694</v>
+        <v>0.00209527447044072</v>
       </c>
       <c r="H93">
         <v>0.01003337684633661</v>

</xml_diff>

<commit_message>
Look into Different Effects of Vapor Quality
</commit_message>
<xml_diff>
--- a/TheEngine/Regen Solver/enginefiles/solverdata.xlsx
+++ b/TheEngine/Regen Solver/enginefiles/solverdata.xlsx
@@ -432,19 +432,19 @@
         <v>0.03112434574304199</v>
       </c>
       <c r="D2">
-        <v>5500000</v>
+        <v>4500000</v>
       </c>
       <c r="E2">
-        <v>296.9248108308197</v>
+        <v>288.1145796254294</v>
       </c>
       <c r="F2">
-        <v>1.259972168161066</v>
+        <v>3.349692346136131</v>
       </c>
       <c r="G2">
-        <v>0.02152231782969481</v>
+        <v>0.006074750479563442</v>
       </c>
       <c r="H2">
-        <v>0.02020324814687743</v>
+        <v>0.008530521636098382</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -458,19 +458,19 @@
         <v>0.03029842497054849</v>
       </c>
       <c r="D3">
-        <v>5499997.603848021</v>
+        <v>4499960.262608993</v>
       </c>
       <c r="E3">
-        <v>296.9247912783351</v>
+        <v>288.1142009647439</v>
       </c>
       <c r="F3">
-        <v>1.553360443562011</v>
+        <v>3.865934636053684</v>
       </c>
       <c r="G3">
-        <v>0.01816623890213394</v>
+        <v>0.005481161521578688</v>
       </c>
       <c r="H3">
-        <v>0.0172623622910289</v>
+        <v>0.007589521581316231</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -484,19 +484,19 @@
         <v>0.029472504198055</v>
       </c>
       <c r="D4">
-        <v>5499807.618161806</v>
+        <v>4498818.281160072</v>
       </c>
       <c r="E4">
-        <v>296.9232409826439</v>
+        <v>288.1033178561757</v>
       </c>
       <c r="F4">
-        <v>1.905261076788692</v>
+        <v>4.468385712901691</v>
       </c>
       <c r="G4">
-        <v>0.01543992564234681</v>
+        <v>0.004947036497531111</v>
       </c>
       <c r="H4">
-        <v>0.01477864358738224</v>
+        <v>0.006742239127465475</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -510,19 +510,19 @@
         <v>0.02864658342556152</v>
       </c>
       <c r="D5">
-        <v>5499528.69941133</v>
+        <v>4497280.200171695</v>
       </c>
       <c r="E5">
-        <v>296.920964909837</v>
+        <v>288.0886566143727</v>
       </c>
       <c r="F5">
-        <v>2.327757902124035</v>
+        <v>5.173952587271874</v>
       </c>
       <c r="G5">
-        <v>0.01319977009156505</v>
+        <v>0.004465511087367863</v>
       </c>
       <c r="H5">
-        <v>0.01266810802241308</v>
+        <v>0.005979047183212387</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -536,19 +536,19 @@
         <v>0.02782066265306801</v>
       </c>
       <c r="D6">
-        <v>5499120.549530844</v>
+        <v>4495198.036170444</v>
       </c>
       <c r="E6">
-        <v>296.9176341005143</v>
+        <v>288.068803053241</v>
       </c>
       <c r="F6">
-        <v>2.836132519516152</v>
+        <v>6.004294460760488</v>
       </c>
       <c r="G6">
-        <v>0.01133970503886501</v>
+        <v>0.004030273586652404</v>
       </c>
       <c r="H6">
-        <v>0.01086523569947432</v>
+        <v>0.005291448978508987</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -562,19 +562,19 @@
         <v>0.02699474188057452</v>
       </c>
       <c r="D7">
-        <v>5498523.850354813</v>
+        <v>4492360.290640308</v>
       </c>
       <c r="E7">
-        <v>296.9127642322449</v>
+        <v>288.0417337985366</v>
       </c>
       <c r="F7">
-        <v>3.449854618179286</v>
+        <v>6.986877802192705</v>
       </c>
       <c r="G7">
-        <v>0.009780474216800205</v>
+        <v>0.003635869862519236</v>
       </c>
       <c r="H7">
-        <v>0.009318242253421361</v>
+        <v>0.004671912717276756</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -588,19 +588,19 @@
         <v>0.02616882110808103</v>
       </c>
       <c r="D8">
-        <v>5497650.466395412</v>
+        <v>4488462.390620776</v>
       </c>
       <c r="E8">
-        <v>296.9056354830771</v>
+        <v>288.0045306887867</v>
       </c>
       <c r="F8">
-        <v>4.194046322517058</v>
+        <v>8.156992743570859</v>
       </c>
       <c r="G8">
-        <v>0.008461947983695392</v>
+        <v>0.003277548262118485</v>
       </c>
       <c r="H8">
-        <v>0.007985701757026981</v>
+        <v>0.00411373041885352</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -614,19 +614,19 @@
         <v>0.02534290033558753</v>
       </c>
       <c r="D9">
-        <v>5496367.834005219</v>
+        <v>4483059.238755435</v>
       </c>
       <c r="E9">
-        <v>296.8951647206952</v>
+        <v>287.9529205228297</v>
       </c>
       <c r="F9">
-        <v>5.101615986322027</v>
+        <v>9.560697839132526</v>
       </c>
       <c r="G9">
-        <v>0.007337829090730687</v>
+        <v>0.00295112475928577</v>
       </c>
       <c r="H9">
-        <v>0.006834091180837826</v>
+        <v>0.003610894780251724</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -640,19 +640,19 @@
         <v>0.02451697956309404</v>
       </c>
       <c r="D10">
-        <v>5494473.565100662</v>
+        <v>4475489.087198098</v>
       </c>
       <c r="E10">
-        <v>296.8796972994979</v>
+        <v>287.8805324953544</v>
       </c>
       <c r="F10">
-        <v>6.216474544480375</v>
+        <v>11.25927036147207</v>
       </c>
       <c r="G10">
-        <v>0.006371924515706349</v>
+        <v>0.002652859158594914</v>
       </c>
       <c r="H10">
-        <v>0.005835970092700017</v>
+        <v>0.003157987494308005</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -666,19 +666,19 @@
         <v>0.02369105879060053</v>
       </c>
       <c r="D11">
-        <v>5491652.919295067</v>
+        <v>4464747.631958731</v>
       </c>
       <c r="E11">
-        <v>296.856657773095</v>
+        <v>287.7776609054353</v>
       </c>
       <c r="F11">
-        <v>7.598598031341215</v>
+        <v>13.33623228207553</v>
       </c>
       <c r="G11">
-        <v>0.005535445932675241</v>
+        <v>0.002379329830746681</v>
       </c>
       <c r="H11">
-        <v>0.004968596761149266</v>
+        <v>0.002750070310526011</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -692,19 +692,19 @@
         <v>0.02286513801810705</v>
       </c>
       <c r="D12">
-        <v>5487404.931690759</v>
+        <v>4449271.682480261</v>
       </c>
       <c r="E12">
-        <v>296.8219416474126</v>
+        <v>287.6291182548196</v>
       </c>
       <c r="F12">
-        <v>9.332465738698026</v>
+        <v>15.90909559368732</v>
       </c>
       <c r="G12">
-        <v>0.004804961938795594</v>
+        <v>0.00212728573582415</v>
       </c>
       <c r="H12">
-        <v>0.00421282920879272</v>
+        <v>0.002382563601653842</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -718,19 +718,19 @@
         <v>0.02203921724561356</v>
       </c>
       <c r="D13">
-        <v>5480907.764206424</v>
+        <v>4426548.59700731</v>
       </c>
       <c r="E13">
-        <v>296.7688029081597</v>
+        <v>287.4103085950457</v>
       </c>
       <c r="F13">
-        <v>11.54228525166799</v>
+        <v>19.15059021915603</v>
       </c>
       <c r="G13">
-        <v>0.004160682001944716</v>
+        <v>0.001893429684077908</v>
       </c>
       <c r="H13">
-        <v>0.003552164476049919</v>
+        <v>0.002051078017466962</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -744,19 +744,19 @@
         <v>0.02121329647312005</v>
       </c>
       <c r="D14">
-        <v>5470756.37802972</v>
+        <v>4392361.968365735</v>
       </c>
       <c r="E14">
-        <v>296.6856766115824</v>
+        <v>287.0795136450456</v>
       </c>
       <c r="F14">
-        <v>14.42286337312631</v>
+        <v>23.33162766656755</v>
       </c>
       <c r="G14">
-        <v>0.003584642066983163</v>
+        <v>0.001674006760113059</v>
       </c>
       <c r="H14">
-        <v>0.002971681366204205</v>
+        <v>0.001751100804445475</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -770,19 +770,19 @@
         <v>0.02038737570062656</v>
       </c>
       <c r="D15">
-        <v>5454398.366317432</v>
+        <v>4339184.345684472</v>
       </c>
       <c r="E15">
-        <v>296.5514675122005</v>
+        <v>286.5610912729446</v>
       </c>
       <c r="F15">
-        <v>18.31525138320045</v>
+        <v>28.92558841164883</v>
       </c>
       <c r="G15">
-        <v>0.003057649938999656</v>
+        <v>0.001463740750923743</v>
       </c>
       <c r="H15">
-        <v>0.002456181111012695</v>
+        <v>0.001477164413625231</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -796,19 +796,19 @@
         <v>0.01956145492813306</v>
       </c>
       <c r="D16">
-        <v>5426704.926498219</v>
+        <v>4252159.852511225</v>
       </c>
       <c r="E16">
-        <v>296.3235255856723</v>
+        <v>285.7023220665164</v>
       </c>
       <c r="F16">
-        <v>23.97583315808031</v>
+        <v>36.97038531803609</v>
       </c>
       <c r="G16">
-        <v>0.002548802320326104</v>
+        <v>0.001251460209737155</v>
       </c>
       <c r="H16">
-        <v>0.001983469182924385</v>
+        <v>0.001219244632520123</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -822,19 +822,19 @@
         <v>0.01911027116091851</v>
       </c>
       <c r="D17">
-        <v>5374915.838027439</v>
+        <v>4095262.59465168</v>
       </c>
       <c r="E17">
-        <v>295.8947666204836</v>
+        <v>284.120242981877</v>
       </c>
       <c r="F17">
-        <v>37.34683576855249</v>
+        <v>54.76904278352885</v>
       </c>
       <c r="G17">
-        <v>0.001743046571665849</v>
+        <v>0.0009026882855329143</v>
       </c>
       <c r="H17">
-        <v>0.001375818895597124</v>
+        <v>0.0008831476150437592</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -848,19 +848,19 @@
         <v>0.02088988309406883</v>
       </c>
       <c r="D18">
-        <v>5189309.81327923</v>
+        <v>3595907.968480114</v>
       </c>
       <c r="E18">
-        <v>294.3308859613708</v>
+        <v>278.7648555561087</v>
       </c>
       <c r="F18">
-        <v>37.85497441977891</v>
+        <v>55.7080835775707</v>
       </c>
       <c r="G18">
-        <v>0.001544826706557237</v>
+        <v>0.000808078706736171</v>
       </c>
       <c r="H18">
-        <v>0.001442167468283976</v>
+        <v>0.0009374808838650569</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -874,19 +874,19 @@
         <v>0.02266949502721918</v>
       </c>
       <c r="D19">
-        <v>5172043.945375251</v>
+        <v>3521396.992918161</v>
       </c>
       <c r="E19">
-        <v>294.1831900426246</v>
+        <v>277.9194098824447</v>
       </c>
       <c r="F19">
-        <v>34.52333685584968</v>
+        <v>50.86179740875176</v>
       </c>
       <c r="G19">
-        <v>0.001546548153195768</v>
+        <v>0.0008072802668042239</v>
       </c>
       <c r="H19">
-        <v>0.001610289899490365</v>
+        <v>0.001050547342209339</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -900,19 +900,19 @@
         <v>0.02444910696036953</v>
       </c>
       <c r="D20">
-        <v>5201143.326950083</v>
+        <v>3585017.569644557</v>
       </c>
       <c r="E20">
-        <v>294.4318909240425</v>
+        <v>278.6420960077653</v>
       </c>
       <c r="F20">
-        <v>30.95196944053182</v>
+        <v>45.44232518224646</v>
       </c>
       <c r="G20">
-        <v>0.001595781538908876</v>
+        <v>0.0008302250795670451</v>
       </c>
       <c r="H20">
-        <v>0.001810478945500592</v>
+        <v>0.001183023833902614</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -926,19 +926,19 @@
         <v>0.02622871889351988</v>
       </c>
       <c r="D21">
-        <v>5229734.998231443</v>
+        <v>3655993.813292407</v>
       </c>
       <c r="E21">
-        <v>294.6751958583532</v>
+        <v>279.4372806343129</v>
       </c>
       <c r="F21">
-        <v>27.8120555056158</v>
+        <v>40.68419575785195</v>
       </c>
       <c r="G21">
-        <v>0.001661512407817518</v>
+        <v>0.0008611638364278003</v>
       </c>
       <c r="H21">
-        <v>0.002032465414512359</v>
+        <v>0.001329017192244146</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -952,19 +952,19 @@
         <v>0.0280083308266702</v>
       </c>
       <c r="D22">
-        <v>5251696.151926484</v>
+        <v>3710846.040142818</v>
       </c>
       <c r="E22">
-        <v>294.8613714209106</v>
+        <v>280.0440602086887</v>
       </c>
       <c r="F22">
-        <v>25.14447753493641</v>
+        <v>36.68409008650473</v>
       </c>
       <c r="G22">
-        <v>0.001735275096531332</v>
+        <v>0.000895505504198118</v>
       </c>
       <c r="H22">
-        <v>0.002272623224529434</v>
+        <v>0.001486416363517067</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -978,19 +978,19 @@
         <v>0.02978794275982054</v>
       </c>
       <c r="D23">
-        <v>5267958.622750903</v>
+        <v>3750865.136493647</v>
       </c>
       <c r="E23">
-        <v>294.9988435318352</v>
+        <v>280.4825919758777</v>
       </c>
       <c r="F23">
-        <v>22.88413047959628</v>
+        <v>33.32442031773935</v>
       </c>
       <c r="G23">
-        <v>0.001814023674314247</v>
+        <v>0.0009317179477039952</v>
       </c>
       <c r="H23">
-        <v>0.002529237197972135</v>
+        <v>0.001654206280056361</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1004,19 +1004,19 @@
         <v>0.03156755469297089</v>
       </c>
       <c r="D24">
-        <v>5280024.561107883</v>
+        <v>3780116.115117721</v>
       </c>
       <c r="E24">
-        <v>295.1006258896663</v>
+        <v>280.800945170599</v>
       </c>
       <c r="F24">
-        <v>20.95962758281495</v>
+        <v>30.48072137135674</v>
       </c>
       <c r="G24">
-        <v>0.001896342173178979</v>
+        <v>0.0009691509555716444</v>
       </c>
       <c r="H24">
-        <v>0.002801349237103969</v>
+        <v>0.001831808876105749</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1030,19 +1030,19 @@
         <v>0.03334716662612121</v>
       </c>
       <c r="D25">
-        <v>5289072.176067227</v>
+        <v>3801791.000338648</v>
       </c>
       <c r="E25">
-        <v>295.1768273619546</v>
+        <v>281.0356716289462</v>
       </c>
       <c r="F25">
-        <v>19.31017728111308</v>
+        <v>28.05226324892948</v>
       </c>
       <c r="G25">
-        <v>0.001981453772511028</v>
+        <v>0.00100745816504008</v>
       </c>
       <c r="H25">
-        <v>0.00308836156752128</v>
+        <v>0.002018855361594545</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1056,19 +1056,19 @@
         <v>0.03512677855927156</v>
       </c>
       <c r="D26">
-        <v>5295941.02113464</v>
+        <v>3818095.162496113</v>
       </c>
       <c r="E26">
-        <v>295.2346102599749</v>
+        <v>281.2115850530347</v>
       </c>
       <c r="F26">
-        <v>17.8867564531081</v>
+        <v>25.96079953440488</v>
       </c>
       <c r="G26">
-        <v>0.002068888033076004</v>
+        <v>0.001046428131601754</v>
       </c>
       <c r="H26">
-        <v>0.003389870449412019</v>
+        <v>0.002215090354079881</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1082,19 +1082,19 @@
         <v>0.03690639049242189</v>
       </c>
       <c r="D27">
-        <v>5301219.989768418</v>
+        <v>3830534.276838058</v>
       </c>
       <c r="E27">
-        <v>295.278978580018</v>
+        <v>281.345423342885</v>
       </c>
       <c r="F27">
-        <v>16.6503386342496</v>
+        <v>24.1456059232269</v>
       </c>
       <c r="G27">
-        <v>0.002158341379528108</v>
+        <v>0.001085921468673947</v>
       </c>
       <c r="H27">
-        <v>0.003705586539372037</v>
+        <v>0.002420325773370507</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1108,19 +1108,19 @@
         <v>0.03868600242557224</v>
       </c>
       <c r="D28">
-        <v>5305323.928629476</v>
+        <v>3840147.549326329</v>
       </c>
       <c r="E28">
-        <v>295.3134470844773</v>
+        <v>281.4486369620874</v>
       </c>
       <c r="F28">
-        <v>15.56984897767723</v>
+        <v>22.55917450909869</v>
       </c>
       <c r="G28">
-        <v>0.002249609362372226</v>
+        <v>0.001125841635559042</v>
       </c>
       <c r="H28">
-        <v>0.004035292833437207</v>
+        <v>0.002634416392570845</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1134,19 +1134,19 @@
         <v>0.04046561435872258</v>
       </c>
       <c r="D29">
-        <v>5308548.177246572</v>
+        <v>3847663.430098201</v>
       </c>
       <c r="E29">
-        <v>295.3405124604239</v>
+        <v>281.5291986780579</v>
       </c>
       <c r="F29">
-        <v>14.62041824195017</v>
+        <v>21.16395675025579</v>
       </c>
       <c r="G29">
-        <v>0.002342550368120514</v>
+        <v>0.00116611937480909</v>
       </c>
       <c r="H29">
-        <v>0.004378820712803174</v>
+        <v>0.002857245854750486</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1160,19 +1160,19 @@
         <v>0.04224522629187291</v>
       </c>
       <c r="D30">
-        <v>5311105.637268392</v>
+        <v>3853600.74138019</v>
       </c>
       <c r="E30">
-        <v>295.3619714001243</v>
+        <v>281.5927576116209</v>
       </c>
       <c r="F30">
-        <v>13.78200578963464</v>
+        <v>19.92996602571818</v>
       </c>
       <c r="G30">
-        <v>0.002437064711475275</v>
+        <v>0.001206703690070255</v>
       </c>
       <c r="H30">
-        <v>0.004736035447923758</v>
+        <v>0.00308871817483182</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1186,19 +1186,19 @@
         <v>0.04402483822502326</v>
       </c>
       <c r="D31">
-        <v>5313151.759302224</v>
+        <v>3858334.678407589</v>
       </c>
       <c r="E31">
-        <v>295.3791339881188</v>
+        <v>281.6433825002633</v>
       </c>
       <c r="F31">
-        <v>13.0383415174207</v>
+        <v>18.83301552621097</v>
       </c>
       <c r="G31">
-        <v>0.002533081884805252</v>
+        <v>0.001247556291310992</v>
       </c>
       <c r="H31">
-        <v>0.005106826977759883</v>
+        <v>0.003328752310172847</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1212,19 +1212,19 @@
         <v>0.04580445015817358</v>
       </c>
       <c r="D32">
-        <v>5314801.466206121</v>
+        <v>3862140.458636379</v>
       </c>
       <c r="E32">
-        <v>295.3929677125503</v>
+        <v>281.6840483134277</v>
       </c>
       <c r="F32">
-        <v>12.37611845085486</v>
+        <v>17.85341433128506</v>
       </c>
       <c r="G32">
-        <v>0.002630552418606046</v>
+        <v>0.001288648011551859</v>
       </c>
       <c r="H32">
-        <v>0.005491103793679444</v>
+        <v>0.003577278542787549</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1238,19 +1238,19 @@
         <v>0.04758406209132393</v>
       </c>
       <c r="D33">
-        <v>5316140.72850976</v>
+        <v>3865222.637612782</v>
       </c>
       <c r="E33">
-        <v>295.4041956974494</v>
+        <v>281.7169605087356</v>
       </c>
       <c r="F33">
-        <v>11.78437589804371</v>
+        <v>16.97499319151688</v>
       </c>
       <c r="G33">
-        <v>0.002729442488249003</v>
+        <v>0.00132995640701751</v>
       </c>
       <c r="H33">
-        <v>0.005888788735379971</v>
+        <v>0.003834235980767893</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1264,19 +1264,19 @@
         <v>0.04936367402447427</v>
       </c>
       <c r="D34">
-        <v>5317234.575669116</v>
+        <v>3867735.108264371</v>
       </c>
       <c r="E34">
-        <v>295.4133645409352</v>
+        <v>281.7437748574241</v>
       </c>
       <c r="F34">
-        <v>11.25402591303511</v>
+        <v>16.18436897882165</v>
       </c>
       <c r="G34">
-        <v>0.002829730229293787</v>
+        <v>0.001371464099574782</v>
       </c>
       <c r="H34">
-        <v>0.006299816010575412</v>
+        <v>0.004099570778302695</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1290,19 +1290,19 @@
         <v>0.05114328595762462</v>
       </c>
       <c r="D35">
-        <v>5318132.709238175</v>
+        <v>3869794.951707656</v>
       </c>
       <c r="E35">
-        <v>295.4208917639444</v>
+        <v>281.7657489206854</v>
       </c>
       <c r="F35">
-        <v>10.77748742787503</v>
+        <v>15.47038348811119</v>
       </c>
       <c r="G35">
-        <v>0.002931403155950268</v>
+        <v>0.001413157602160399</v>
       </c>
       <c r="H35">
-        <v>0.00672412902473772</v>
+        <v>0.004373234832908403</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1316,19 +1316,19 @@
         <v>0.05292289789077495</v>
       </c>
       <c r="D36">
-        <v>5318873.484068974</v>
+        <v>3871492.167627157</v>
       </c>
       <c r="E36">
-        <v>295.4270994160586</v>
+        <v>281.7838480268501</v>
       </c>
       <c r="F36">
-        <v>10.34840157666648</v>
+        <v>14.82367091885915</v>
       </c>
       <c r="G36">
-        <v>0.003034456314805123</v>
+        <v>0.001455026468328097</v>
       </c>
       <c r="H36">
-        <v>0.007161678762882656</v>
+        <v>0.004655184808954336</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1342,19 +1342,19 @@
         <v>0.05470250982392529</v>
       </c>
       <c r="D37">
-        <v>5319486.765510894</v>
+        <v>3872896.602004613</v>
       </c>
       <c r="E37">
-        <v>295.4322381654423</v>
+        <v>281.7988204690107</v>
       </c>
       <c r="F37">
-        <v>9.961408617581677</v>
+        <v>14.23632132752274</v>
       </c>
       <c r="G37">
-        <v>0.003138890942407212</v>
+        <v>0.001497062665131647</v>
       </c>
       <c r="H37">
-        <v>0.007612422557416451</v>
+        <v>0.004945381390154049</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1368,19 +1368,19 @@
         <v>0.05648212175707563</v>
       </c>
       <c r="D38">
-        <v>5319996.003141358</v>
+        <v>3874062.941421865</v>
       </c>
       <c r="E38">
-        <v>295.4365047662669</v>
+        <v>281.8112515642875</v>
       </c>
       <c r="F38">
-        <v>9.611971927926962</v>
+        <v>13.70161639323721</v>
       </c>
       <c r="G38">
-        <v>0.003244713476697272</v>
+        <v>0.001539260103453166</v>
       </c>
       <c r="H38">
-        <v>0.008076323132214198</v>
+        <v>0.005243788696459604</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1394,19 +1394,19 @@
         <v>0.05826173369022596</v>
       </c>
       <c r="D39">
-        <v>5320419.751983259</v>
+        <v>3875034.355711815</v>
       </c>
       <c r="E39">
-        <v>295.897657991236</v>
+        <v>281.8216029903591</v>
       </c>
       <c r="F39">
-        <v>9.286683155768383</v>
+        <v>13.21382020992566</v>
       </c>
       <c r="G39">
-        <v>0.003279678191635957</v>
+        <v>0.00158161428155855</v>
       </c>
       <c r="H39">
-        <v>0.008553347848405078</v>
+        <v>0.005550373821435729</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1420,19 +1420,19 @@
         <v>0.0600413456233763</v>
       </c>
       <c r="D40">
-        <v>5320793.173792223</v>
+        <v>3875845.183799047</v>
       </c>
       <c r="E40">
-        <v>296.3676124108536</v>
+        <v>281.830241732518</v>
       </c>
       <c r="F40">
-        <v>8.974335705253397</v>
+        <v>12.76801234391833</v>
       </c>
       <c r="G40">
-        <v>0.003316601154591095</v>
+        <v>0.001624122011593456</v>
       </c>
       <c r="H40">
-        <v>0.009043468100516717</v>
+        <v>0.005865106459787318</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1446,19 +1446,19 @@
         <v>0.06182095755652664</v>
       </c>
       <c r="D41">
-        <v>5321136.697293273</v>
+        <v>3876522.934258359</v>
       </c>
       <c r="E41">
-        <v>296.8454770643189</v>
+        <v>281.8374616091806</v>
       </c>
       <c r="F41">
-        <v>8.675647714232436</v>
+        <v>12.35995364680829</v>
       </c>
       <c r="G41">
-        <v>0.003355404721589744</v>
+        <v>0.001666781207573764</v>
       </c>
       <c r="H41">
-        <v>0.009546658825384711</v>
+        <v>0.006187958602724221</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1472,19 +1472,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D42">
-        <v>5321451.144076061</v>
+        <v>3877089.789643451</v>
       </c>
       <c r="E42">
-        <v>297.3304269947514</v>
+        <v>281.8434994352384</v>
       </c>
       <c r="F42">
-        <v>8.418594958573827</v>
+        <v>12.02587319718006</v>
       </c>
       <c r="G42">
-        <v>0.003390502677704885</v>
+        <v>0.00170699198825568</v>
       </c>
       <c r="H42">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1498,19 +1498,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D43">
-        <v>5321714.291417698</v>
+        <v>3877527.188368597</v>
       </c>
       <c r="E43">
-        <v>297.8223271327865</v>
+        <v>281.8481579145759</v>
       </c>
       <c r="F43">
-        <v>8.640557542866725</v>
+        <v>12.37938520797392</v>
       </c>
       <c r="G43">
-        <v>0.003338612075891804</v>
+        <v>0.001703921011539139</v>
       </c>
       <c r="H43">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1524,19 +1524,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D44">
-        <v>5321308.974492349</v>
+        <v>3876069.347444586</v>
       </c>
       <c r="E44">
-        <v>298.3309668814039</v>
+        <v>281.8326297855052</v>
       </c>
       <c r="F44">
-        <v>8.867831258913856</v>
+        <v>12.75784281684561</v>
       </c>
       <c r="G44">
-        <v>0.00328837468714456</v>
+        <v>0.001700429970927155</v>
       </c>
       <c r="H44">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1550,19 +1550,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D45">
-        <v>5320886.071337334</v>
+        <v>3874524.127548253</v>
       </c>
       <c r="E45">
-        <v>298.8565122200457</v>
+        <v>281.8161662201084</v>
       </c>
       <c r="F45">
-        <v>9.095920371797364</v>
+        <v>13.15856675065528</v>
       </c>
       <c r="G45">
-        <v>0.003240432182242853</v>
+        <v>0.001696948645624376</v>
       </c>
       <c r="H45">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1576,19 +1576,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D46">
-        <v>5320451.761352854</v>
+        <v>3872897.590789796</v>
       </c>
       <c r="E46">
-        <v>299.3988242580751</v>
+        <v>281.7988310088691</v>
       </c>
       <c r="F46">
-        <v>9.32481277206205</v>
+        <v>13.58353845701165</v>
       </c>
       <c r="G46">
-        <v>0.003194620484015525</v>
+        <v>0.001693481001540403</v>
       </c>
       <c r="H46">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1602,19 +1602,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D47">
-        <v>5320005.961904661</v>
+        <v>3871182.928446277</v>
       </c>
       <c r="E47">
-        <v>299.9577515912276</v>
+        <v>281.7805507388572</v>
       </c>
       <c r="F47">
-        <v>9.554535680751886</v>
+        <v>14.03502283423567</v>
       </c>
       <c r="G47">
-        <v>0.003150785335715752</v>
+        <v>0.001690028099713938</v>
       </c>
       <c r="H47">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1628,19 +1628,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D48">
-        <v>5319548.52941865</v>
+        <v>3869372.414874882</v>
       </c>
       <c r="E48">
-        <v>300.5331334773247</v>
+        <v>281.7612420751139</v>
       </c>
       <c r="F48">
-        <v>9.785113820720367</v>
+        <v>14.51557810862474</v>
       </c>
       <c r="G48">
-        <v>0.00310878740725311</v>
+        <v>0.001686590969455263</v>
       </c>
       <c r="H48">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1654,19 +1654,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D49">
-        <v>5319079.319084472</v>
+        <v>3867457.360781424</v>
       </c>
       <c r="E49">
-        <v>301.1248003106082</v>
+        <v>281.7408112310166</v>
       </c>
       <c r="F49">
-        <v>10.01656946601496</v>
+        <v>15.02810491769607</v>
       </c>
       <c r="G49">
-        <v>0.003068500503088111</v>
+        <v>0.00168317060781279</v>
       </c>
       <c r="H49">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1680,19 +1680,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D50">
-        <v>5318598.185160685</v>
+        <v>3865427.955451748</v>
       </c>
       <c r="E50">
-        <v>301.7325740792267</v>
+        <v>281.7191522480081</v>
       </c>
       <c r="F50">
-        <v>10.24892284337339</v>
+        <v>15.57590598057785</v>
       </c>
       <c r="G50">
-        <v>0.003029809978512314</v>
+        <v>0.001679767951435033</v>
       </c>
       <c r="H50">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -1706,19 +1706,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D51">
-        <v>5318104.980698022</v>
+        <v>3863273.075540286</v>
       </c>
       <c r="E51">
-        <v>302.3562688307819</v>
+        <v>281.6961449090426</v>
       </c>
       <c r="F51">
-        <v>10.48219248594043</v>
+        <v>16.16275877045443</v>
       </c>
       <c r="G51">
-        <v>0.002992611385558168</v>
+        <v>0.001676383839012611</v>
       </c>
       <c r="H51">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1732,19 +1732,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D52">
-        <v>5317599.557266882</v>
+        <v>3860980.052739653</v>
       </c>
       <c r="E52">
-        <v>302.9956911439513</v>
+        <v>281.6716522009905</v>
       </c>
       <c r="F52">
-        <v>10.71639561158416</v>
+        <v>16.79300463100501</v>
       </c>
       <c r="G52">
-        <v>0.002956809291473403</v>
+        <v>0.0016730189615431</v>
       </c>
       <c r="H52">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -1758,19 +1758,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D53">
-        <v>5317081.764579857</v>
+        <v>3858534.389530085</v>
       </c>
       <c r="E53">
-        <v>303.6506406143278</v>
+        <v>281.6455172069106</v>
       </c>
       <c r="F53">
-        <v>10.95154834299726</v>
+        <v>17.47165886797425</v>
       </c>
       <c r="G53">
-        <v>0.002922316293770902</v>
+        <v>0.001669673796523514</v>
       </c>
       <c r="H53">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -1784,19 +1784,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D54">
-        <v>5316551.450310919</v>
+        <v>3855919.408805151</v>
       </c>
       <c r="E54">
-        <v>304.3209103342317</v>
+        <v>281.6175592713868</v>
       </c>
       <c r="F54">
-        <v>11.18766603382409</v>
+        <v>18.20454783795372</v>
       </c>
       <c r="G54">
-        <v>0.002889052130259958</v>
+        <v>0.001666348520814491</v>
       </c>
       <c r="H54">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -1810,19 +1810,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D55">
-        <v>5316008.459695411</v>
+        <v>3853115.818514598</v>
       </c>
       <c r="E55">
-        <v>305.0062873855798</v>
+        <v>281.5875692304689</v>
       </c>
       <c r="F55">
-        <v>11.42476349732839</v>
+        <v>18.99848112484769</v>
       </c>
       <c r="G55">
-        <v>0.002856942924967937</v>
+        <v>0.001663042895027914</v>
       </c>
       <c r="H55">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -1836,19 +1836,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D56">
-        <v>5315452.635239011</v>
+        <v>3850101.166009207</v>
       </c>
       <c r="E56">
-        <v>305.7065533332124</v>
+        <v>281.555303425993</v>
       </c>
       <c r="F56">
-        <v>11.66285522668682</v>
+        <v>19.86146980088597</v>
       </c>
       <c r="G56">
-        <v>0.002825920526585479</v>
+        <v>0.001659756109628464</v>
       </c>
       <c r="H56">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -1862,19 +1862,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D57">
-        <v>5314883.816400476</v>
+        <v>3846849.147703799</v>
       </c>
       <c r="E57">
-        <v>306.4214847193604</v>
+        <v>281.5204761231017</v>
       </c>
       <c r="F57">
-        <v>11.90195559367504</v>
+        <v>20.80300590972929</v>
       </c>
       <c r="G57">
-        <v>0.002795921930008415</v>
+        <v>0.001656486579152518</v>
       </c>
       <c r="H57">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -1888,19 +1888,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D58">
-        <v>5314301.839273054</v>
+        <v>3843328.726756925</v>
       </c>
       <c r="E58">
-        <v>307.1508535574325</v>
+        <v>281.4827498057358</v>
       </c>
       <c r="F58">
-        <v>12.1420790272273</v>
+        <v>21.83442429761702</v>
       </c>
       <c r="G58">
-        <v>0.00276688876912453</v>
+        <v>0.001653231665491275</v>
       </c>
       <c r="H58">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -1914,19 +1914,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D59">
-        <v>5313706.53626611</v>
+        <v>3839502.992784514</v>
       </c>
       <c r="E59">
-        <v>307.8944278232319</v>
+        <v>281.4417226161515</v>
       </c>
       <c r="F59">
-        <v>12.38324017330717</v>
+        <v>22.96937672216903</v>
       </c>
       <c r="G59">
-        <v>0.002738766870866099</v>
+        <v>0.001649987303212575</v>
       </c>
       <c r="H59">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -1940,19 +1940,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D60">
-        <v>5313097.735788202</v>
+        <v>3835327.670157767</v>
       </c>
       <c r="E60">
-        <v>308.6519719416885</v>
+        <v>281.3969118970421</v>
       </c>
       <c r="F60">
-        <v>12.62545403738776</v>
+        <v>24.22446134521689</v>
       </c>
       <c r="G60">
-        <v>0.002711505862102082</v>
+        <v>0.001646747488068812</v>
       </c>
       <c r="H60">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -1966,19 +1966,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D61">
-        <v>5312475.261932719</v>
+        <v>3830749.140312113</v>
       </c>
       <c r="E61">
-        <v>309.4232472672026</v>
+        <v>281.3477323334748</v>
       </c>
       <c r="F61">
-        <v>12.86873611073721</v>
+        <v>25.6200708316079</v>
       </c>
       <c r="G61">
-        <v>0.002685058822227869</v>
+        <v>0.001643503571994566</v>
       </c>
       <c r="H61">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -1992,19 +1992,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D62">
-        <v>5311838.934167053</v>
+        <v>3825701.780683127</v>
       </c>
       <c r="E62">
-        <v>310.2080125557435</v>
+        <v>282.1809691104066</v>
       </c>
       <c r="F62">
-        <v>13.11310248162869</v>
+        <v>26.90667079164783</v>
       </c>
       <c r="G62">
-        <v>0.002659381975377083</v>
+        <v>0.001615341811793374</v>
       </c>
       <c r="H62">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2018,19 +2018,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D63">
-        <v>5311188.567026115</v>
+        <v>3820806.536219803</v>
       </c>
       <c r="E63">
-        <v>311.0060244269217</v>
+        <v>283.0411091027392</v>
       </c>
       <c r="F63">
-        <v>13.3585699325375</v>
+        <v>27.71543588094902</v>
       </c>
       <c r="G63">
-        <v>0.002634434417070125</v>
+        <v>0.001590163433544918</v>
       </c>
       <c r="H63">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2044,19 +2044,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D64">
-        <v>5310523.969810876</v>
+        <v>3817180.304018879</v>
       </c>
       <c r="E64">
-        <v>311.8170378143535</v>
+        <v>283.9274855763807</v>
       </c>
       <c r="F64">
-        <v>13.60515602434482</v>
+        <v>28.50497998579237</v>
       </c>
       <c r="G64">
-        <v>0.002610177870860088</v>
+        <v>0.00156658783413678</v>
       </c>
       <c r="H64">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2070,19 +2070,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D65">
-        <v>5309844.946292405</v>
+        <v>3813502.017998157</v>
       </c>
       <c r="E65">
-        <v>312.6408064027602</v>
+        <v>284.838895614412</v>
       </c>
       <c r="F65">
-        <v>13.85287916853467</v>
+        <v>29.30031012306693</v>
       </c>
       <c r="G65">
-        <v>0.002586576471164544</v>
+        <v>0.001544027146741291</v>
       </c>
       <c r="H65">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2096,19 +2096,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D66">
-        <v>5309151.294421748</v>
+        <v>3809696.0037578</v>
       </c>
       <c r="E66">
-        <v>313.4770830503858</v>
+        <v>285.774787412447</v>
       </c>
       <c r="F66">
-        <v>14.10175868834147</v>
+        <v>30.10302075219266</v>
       </c>
       <c r="G66">
-        <v>0.002563596569002222</v>
+        <v>0.001522382946276478</v>
       </c>
       <c r="H66">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -2122,19 +2122,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D67">
-        <v>5308442.806045805</v>
+        <v>3805754.808411618</v>
       </c>
       <c r="E67">
-        <v>314.3256201954661</v>
+        <v>286.7346298392324</v>
       </c>
       <c r="F67">
-        <v>14.35181486978126</v>
+        <v>30.9134365452062</v>
       </c>
       <c r="G67">
-        <v>0.002541206557803442</v>
+        <v>0.001501587842726844</v>
       </c>
       <c r="H67">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2148,19 +2148,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D68">
-        <v>5307719.266629213</v>
+        <v>3801674.63537896</v>
       </c>
       <c r="E68">
-        <v>315.1861702456525</v>
+        <v>287.7178809977548</v>
       </c>
       <c r="F68">
-        <v>14.6030690034745</v>
+        <v>31.73181983499446</v>
       </c>
       <c r="G68">
-        <v>0.002519376716846038</v>
+        <v>0.001481581629407713</v>
       </c>
       <c r="H68">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -2174,19 +2174,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D69">
-        <v>5306980.45498211</v>
+        <v>3797451.766163342</v>
       </c>
       <c r="E69">
-        <v>316.0584859494544</v>
+        <v>288.723988360484</v>
       </c>
       <c r="F69">
-        <v>14.85554341814237</v>
+        <v>32.55843935900175</v>
       </c>
       <c r="G69">
-        <v>0.002498079070195466</v>
+        <v>0.001462309379936737</v>
       </c>
       <c r="H69">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2200,19 +2200,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D70">
-        <v>5306226.142993493</v>
+        <v>3793082.348403097</v>
       </c>
       <c r="E70">
-        <v>316.9423207489422</v>
+        <v>289.7523906157909</v>
       </c>
       <c r="F70">
-        <v>15.10926150663207</v>
+        <v>33.39357628497076</v>
       </c>
       <c r="G70">
-        <v>0.002477287259307603</v>
+        <v>0.001443720769670183</v>
       </c>
       <c r="H70">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2226,19 +2226,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D71">
-        <v>5305456.095369785</v>
+        <v>3788562.371000716</v>
       </c>
       <c r="E71">
-        <v>317.8374291131187</v>
+        <v>290.802519614598</v>
       </c>
       <c r="F71">
-        <v>15.36424774529622</v>
+        <v>34.23752651365065</v>
       </c>
       <c r="G71">
-        <v>0.002456976427693247</v>
+        <v>0.001425769550479232</v>
       </c>
       <c r="H71">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -2252,19 +2252,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D72">
-        <v>5304670.069378096</v>
+        <v>3783887.649555819</v>
       </c>
       <c r="E72">
-        <v>318.7435668515346</v>
+        <v>291.87380230736</v>
       </c>
       <c r="F72">
-        <v>15.62052770751926</v>
+        <v>35.09060269139733</v>
       </c>
       <c r="G72">
-        <v>0.002437123116250169</v>
+        <v>0.001408413102324841</v>
       </c>
       <c r="H72">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2278,19 +2278,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D73">
-        <v>5303867.814593573</v>
+        <v>3779053.81168098</v>
       </c>
       <c r="E73">
-        <v>319.6604914078857</v>
+        <v>292.9656626435658</v>
       </c>
       <c r="F73">
-        <v>15.87812807214916</v>
+        <v>35.9531357969458</v>
       </c>
       <c r="G73">
-        <v>0.002417705168047126</v>
+        <v>0.001391612060137868</v>
       </c>
       <c r="H73">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2304,19 +2304,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D74">
-        <v>5303049.072650169</v>
+        <v>3774056.282806724</v>
       </c>
       <c r="E74">
-        <v>320.5879621334798</v>
+        <v>294.0775234128725</v>
       </c>
       <c r="F74">
-        <v>16.13707662755472</v>
+        <v>36.82547679070569</v>
       </c>
       <c r="G74">
-        <v>0.002398701641498593</v>
+        <v>0.001375329984939636</v>
       </c>
       <c r="H74">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -2330,19 +2330,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D75">
-        <v>5302213.576994042</v>
+        <v>3768890.270883734</v>
       </c>
       <c r="E75">
-        <v>321.5257405406048</v>
+        <v>295.2088080094932</v>
       </c>
       <c r="F75">
-        <v>16.39740227198975</v>
+        <v>37.70799803273231</v>
       </c>
       <c r="G75">
-        <v>0.002380092731002606</v>
+        <v>0.001359533084768783</v>
       </c>
       <c r="H75">
-        <v>0.01003337684633662</v>
+        <v>0.00649998653025552</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -2356,19 +2356,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D76">
-        <v>5301361.052638805</v>
+        <v>3763550.751011967</v>
       </c>
       <c r="E76">
-        <v>322.4735905359636</v>
+        <v>296.3589421048729</v>
       </c>
       <c r="F76">
-        <v>16.65913501090406</v>
+        <v>38.60109461804244</v>
       </c>
       <c r="G76">
-        <v>0.00236185969422999</v>
+        <v>0.00134418997209665</v>
       </c>
       <c r="H76">
-        <v>0.01003337684633661</v>
+        <v>0.006499986530255529</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -2382,19 +2382,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D77">
-        <v>5300491.215921746</v>
+        <v>3758032.449534914</v>
       </c>
       <c r="E77">
-        <v>323.4312786344587</v>
+        <v>297.5273552162193</v>
       </c>
       <c r="F77">
-        <v>16.92230595179869</v>
+        <v>39.50518564222387</v>
       </c>
       <c r="G77">
-        <v>0.00234398478535398</v>
+        <v>0.001329271452458753</v>
       </c>
       <c r="H77">
-        <v>0.01003337684633661</v>
+        <v>0.006499986530255529</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -2408,19 +2408,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D78">
-        <v>5299603.774260125</v>
+        <v>3752329.827570149</v>
       </c>
       <c r="E78">
-        <v>324.398574153718</v>
+        <v>298.7134821614893</v>
       </c>
       <c r="F78">
-        <v>17.18694729718009</v>
+        <v>40.42071542506105</v>
       </c>
       <c r="G78">
-        <v>0.002326451193596637</v>
+        <v>0.00131475033920126</v>
       </c>
       <c r="H78">
-        <v>0.01003337684633661</v>
+        <v>0.006499986530255529</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -2434,19 +2434,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D79">
-        <v>5298698.425906655</v>
+        <v>3746437.063884491</v>
       </c>
       <c r="E79">
-        <v>325.3752493898515</v>
+        <v>299.9167643941873</v>
       </c>
       <c r="F79">
-        <v>17.4530923361244</v>
+        <v>41.34815472050116</v>
       </c>
       <c r="G79">
-        <v>0.002309242986544712</v>
+        <v>0.001300601290125855</v>
       </c>
       <c r="H79">
-        <v>0.01003337684633661</v>
+        <v>0.006499986530255529</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -2460,19 +2460,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D80">
-        <v>5297774.859703201</v>
+        <v>3740348.037005253</v>
       </c>
       <c r="E80">
-        <v>326.3610797750057</v>
+        <v>301.1366512139389</v>
       </c>
       <c r="F80">
-        <v>17.72077543492022</v>
+        <v>42.28800194097863</v>
       </c>
       <c r="G80">
-        <v>0.002292345057753836</v>
+        <v>0.001286800662553389</v>
       </c>
       <c r="H80">
-        <v>0.01003337684633661</v>
+        <v>0.006499986530255529</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -2486,19 +2486,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D81">
-        <v>5296832.754831783</v>
+        <v>3734056.306445044</v>
       </c>
       <c r="E81">
-        <v>327.3558440173575</v>
+        <v>302.3726008511767</v>
       </c>
       <c r="F81">
-        <v>17.99003202721635</v>
+        <v>43.24078442372005</v>
       </c>
       <c r="G81">
-        <v>0.00227574307821772</v>
+        <v>0.001273326383936207</v>
       </c>
       <c r="H81">
-        <v>0.01003337684633661</v>
+        <v>0.006499986530255529</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -2512,19 +2512,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D82">
-        <v>5295871.780561941</v>
+        <v>3727555.092903876</v>
       </c>
       <c r="E82">
-        <v>328.3593242242444</v>
+        <v>303.6240814264074</v>
       </c>
       <c r="F82">
-        <v>18.26089860405959</v>
+        <v>44.20705976628514</v>
       </c>
       <c r="G82">
-        <v>0.002259423451329393</v>
+        <v>0.001260157835652789</v>
       </c>
       <c r="H82">
-        <v>0.01003337684633661</v>
+        <v>0.006499986530255529</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -2538,19 +2538,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D83">
-        <v>5294891.59599351</v>
+        <v>3720837.257298253</v>
       </c>
       <c r="E83">
-        <v>329.3713060091758</v>
+        <v>304.8905717863662</v>
       </c>
       <c r="F83">
-        <v>18.53341270416858</v>
+        <v>45.18741725832371</v>
       </c>
       <c r="G83">
-        <v>0.002243373271005464</v>
+        <v>0.001247275748034673</v>
       </c>
       <c r="H83">
-        <v>0.01003337684633661</v>
+        <v>0.006499986530255529</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -2564,19 +2564,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D84">
-        <v>5293891.849793899</v>
+        <v>3713895.27845243</v>
       </c>
       <c r="E84">
-        <v>330.3915785835034</v>
+        <v>306.1715622209301</v>
       </c>
       <c r="F84">
-        <v>18.80761290475194</v>
+        <v>46.18247943641484</v>
       </c>
       <c r="G84">
-        <v>0.002227580282682644</v>
+        <v>0.001234662105019165</v>
       </c>
       <c r="H84">
-        <v>0.01003337684633661</v>
+        <v>0.006499986530255529</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -2590,19 +2590,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D85">
-        <v>5292872.179928931</v>
+        <v>3706721.229271477</v>
       </c>
       <c r="E85">
-        <v>331.4199348335572</v>
+        <v>307.4665550659378</v>
       </c>
       <c r="F85">
-        <v>19.08353881314379</v>
+        <v>47.19290378897324</v>
       </c>
       <c r="G85">
-        <v>0.002212032846929281</v>
+        <v>0.001222300057104403</v>
       </c>
       <c r="H85">
-        <v>0.01003337684633661</v>
+        <v>0.006499986530255529</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -2616,19 +2616,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D86">
-        <v>5291832.213386369</v>
+        <v>3699306.751198992</v>
       </c>
       <c r="E86">
-        <v>332.4561713840665</v>
+        <v>308.775065198068</v>
       </c>
       <c r="F86">
-        <v>19.3612310594954</v>
+        <v>48.21938463862927</v>
       </c>
       <c r="G86">
-        <v>0.00219671990544381</v>
+        <v>0.001210173841515886</v>
       </c>
       <c r="H86">
-        <v>0.01003337684633661</v>
+        <v>0.006499986530255529</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -2642,19 +2642,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D87">
-        <v>5290771.565891213</v>
+        <v>3691643.026743633</v>
       </c>
       <c r="E87">
-        <v>333.5000886486944</v>
+        <v>310.0966204286833</v>
       </c>
       <c r="F87">
-        <v>19.64073129073227</v>
+        <v>49.26265523028218</v>
       </c>
       <c r="G87">
-        <v>0.002181630949237533</v>
+        <v>0.001198268708684186</v>
       </c>
       <c r="H87">
-        <v>0.01003337684633661</v>
+        <v>0.006499986530255529</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -2668,19 +2668,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D88">
-        <v>5289689.841611905</v>
+        <v>3683720.749837643</v>
       </c>
       <c r="E88">
-        <v>334.5514908685142</v>
+        <v>311.4307618040625</v>
       </c>
       <c r="F88">
-        <v>19.92208216595627</v>
+        <v>50.32349005426204</v>
       </c>
       <c r="G88">
-        <v>0.002166755988821394</v>
+        <v>0.001186570854289219</v>
       </c>
       <c r="H88">
-        <v>0.01003337684633661</v>
+        <v>0.006499986530255529</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -2694,19 +2694,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D89">
-        <v>5288586.632856574</v>
+        <v>3675530.093766672</v>
       </c>
       <c r="E89">
-        <v>335.6101861392485</v>
+        <v>312.7770438197659</v>
       </c>
       <c r="F89">
-        <v>20.20532735344718</v>
+        <v>51.40270743579131</v>
       </c>
       <c r="G89">
-        <v>0.002152085526235923</v>
+        <v>0.001175067356253159</v>
       </c>
       <c r="H89">
-        <v>0.01003337684633661</v>
+        <v>0.006499986530255529</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -2720,19 +2720,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D90">
-        <v>5287461.519758469</v>
+        <v>3667060.67638274</v>
       </c>
       <c r="E90">
-        <v>336.6759864280795</v>
+        <v>314.1350345570069</v>
       </c>
       <c r="F90">
-        <v>20.4905115293942</v>
+        <v>52.50117242428558</v>
       </c>
       <c r="G90">
-        <v>0.002137610528780489</v>
+        <v>0.00116374611616686</v>
       </c>
       <c r="H90">
-        <v>0.01003337684633661</v>
+        <v>0.006499986530255529</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -2746,19 +2746,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D91">
-        <v>5286314.069949751</v>
+        <v>3658301.522280485</v>
       </c>
       <c r="E91">
-        <v>337.7487075808214</v>
+        <v>315.5043157488914</v>
       </c>
       <c r="F91">
-        <v>20.77768037846709</v>
+        <v>53.61980001907093</v>
       </c>
       <c r="G91">
-        <v>0.002123322404312971</v>
+        <v>0.001152595804717688</v>
       </c>
       <c r="H91">
-        <v>0.01003337684633661</v>
+        <v>0.006499986530255529</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -2772,19 +2772,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D92">
-        <v>5285143.838222789</v>
+        <v>3649241.021580027</v>
       </c>
       <c r="E92">
-        <v>338.8281693202242</v>
+        <v>316.8844827842465</v>
       </c>
       <c r="F92">
-        <v>21.06688059631835</v>
+        <v>54.75955877191128</v>
       </c>
       <c r="G92">
-        <v>0.002109212978003902</v>
+        <v>0.001141605810753614</v>
       </c>
       <c r="H92">
-        <v>0.01003337684633661</v>
+        <v>0.006499986530255529</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -2798,19 +2798,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D93">
-        <v>5283950.366178161</v>
+        <v>3639866.884916938</v>
       </c>
       <c r="E93">
-        <v>339.9141952361504</v>
+        <v>318.2751446565155</v>
       </c>
       <c r="F93">
-        <v>21.35815989409046</v>
+        <v>55.92147481146261</v>
       </c>
       <c r="G93">
-        <v>0.00209527447044072</v>
+        <v>0.001130766193672103</v>
       </c>
       <c r="H93">
-        <v>0.01003337684633661</v>
+        <v>0.006499986530255529</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Work on Script Version
</commit_message>
<xml_diff>
--- a/TheEngine/Regen Solver/enginefiles/solverdata.xlsx
+++ b/TheEngine/Regen Solver/enginefiles/solverdata.xlsx
@@ -438,13 +438,13 @@
         <v>288.1145796254294</v>
       </c>
       <c r="F2">
-        <v>3.349692346136131</v>
+        <v>3.656094375228009</v>
       </c>
       <c r="G2">
-        <v>0.006074750479563442</v>
+        <v>0.005565650964579227</v>
       </c>
       <c r="H2">
-        <v>0.008530521636098382</v>
+        <v>0.005454591059024392</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -458,19 +458,19 @@
         <v>0.03029842497054849</v>
       </c>
       <c r="D3">
-        <v>4499960.262608993</v>
+        <v>4499950.053907844</v>
       </c>
       <c r="E3">
-        <v>288.1142009647439</v>
+        <v>288.1141036848301</v>
       </c>
       <c r="F3">
-        <v>3.865934636053684</v>
+        <v>4.190076422036327</v>
       </c>
       <c r="G3">
-        <v>0.005481161521578688</v>
+        <v>0.005057143982657782</v>
       </c>
       <c r="H3">
-        <v>0.007589521581316231</v>
+        <v>0.00486901296120758</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -484,19 +484,19 @@
         <v>0.029472504198055</v>
       </c>
       <c r="D4">
-        <v>4498818.281160072</v>
+        <v>4498663.277085356</v>
       </c>
       <c r="E4">
-        <v>288.1033178561757</v>
+        <v>288.1018405031897</v>
       </c>
       <c r="F4">
-        <v>4.468385712901691</v>
+        <v>4.811548179781115</v>
       </c>
       <c r="G4">
-        <v>0.004947036497531111</v>
+        <v>0.004594235965509072</v>
       </c>
       <c r="H4">
-        <v>0.006742239127465475</v>
+        <v>0.004338854288853006</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -510,19 +510,19 @@
         <v>0.02864658342556152</v>
       </c>
       <c r="D5">
-        <v>4497280.200171695</v>
+        <v>4496946.202826858</v>
       </c>
       <c r="E5">
-        <v>288.0886566143727</v>
+        <v>288.0854723964588</v>
       </c>
       <c r="F5">
-        <v>5.173952587271874</v>
+        <v>5.537508284883274</v>
       </c>
       <c r="G5">
-        <v>0.004465511087367863</v>
+        <v>0.004172384655007708</v>
       </c>
       <c r="H5">
-        <v>0.005979047183212387</v>
+        <v>0.003858858283718739</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -536,19 +536,19 @@
         <v>0.02782066265306801</v>
       </c>
       <c r="D6">
-        <v>4495198.036170444</v>
+        <v>4494641.969103299</v>
       </c>
       <c r="E6">
-        <v>288.068803053241</v>
+        <v>288.0634997455525</v>
       </c>
       <c r="F6">
-        <v>6.004294460760488</v>
+        <v>6.389830916869052</v>
       </c>
       <c r="G6">
-        <v>0.004030273586652404</v>
+        <v>0.003787177639467792</v>
       </c>
       <c r="H6">
-        <v>0.005291448978508987</v>
+        <v>0.003424328670984899</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -562,19 +562,19 @@
         <v>0.02699474188057452</v>
       </c>
       <c r="D7">
-        <v>4492360.290640308</v>
+        <v>4491527.000071269</v>
       </c>
       <c r="E7">
-        <v>288.0417337985366</v>
+        <v>288.0337825890617</v>
       </c>
       <c r="F7">
-        <v>6.986877802192705</v>
+        <v>7.3962497060019</v>
       </c>
       <c r="G7">
-        <v>0.003635869862519236</v>
+        <v>0.003434731041445112</v>
       </c>
       <c r="H7">
-        <v>0.004671912717276756</v>
+        <v>0.003031053208107388</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -588,19 +588,19 @@
         <v>0.02616882110808103</v>
       </c>
       <c r="D8">
-        <v>4488462.390620776</v>
+        <v>4487280.545447507</v>
       </c>
       <c r="E8">
-        <v>288.0045306887867</v>
+        <v>287.9932458720727</v>
       </c>
       <c r="F8">
-        <v>8.156992743570859</v>
+        <v>8.592393623045998</v>
       </c>
       <c r="G8">
-        <v>0.003277548262118485</v>
+        <v>0.003111596358493659</v>
       </c>
       <c r="H8">
-        <v>0.00411373041885352</v>
+        <v>0.002675237058909835</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -614,19 +614,19 @@
         <v>0.02534290033558753</v>
       </c>
       <c r="D9">
-        <v>4483059.238755435</v>
+        <v>4481435.505081112</v>
       </c>
       <c r="E9">
-        <v>287.9529205228297</v>
+        <v>287.9374016723725</v>
       </c>
       <c r="F9">
-        <v>9.560697839132526</v>
+        <v>10.02476199976335</v>
       </c>
       <c r="G9">
-        <v>0.00295112475928577</v>
+        <v>0.002814675052937939</v>
       </c>
       <c r="H9">
-        <v>0.003610894780251724</v>
+        <v>0.002353443141982423</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -640,19 +640,19 @@
         <v>0.02451697956309404</v>
       </c>
       <c r="D10">
-        <v>4475489.087198098</v>
+        <v>4473299.652610684</v>
       </c>
       <c r="E10">
-        <v>287.8805324953544</v>
+        <v>287.859579260179</v>
       </c>
       <c r="F10">
-        <v>11.25927036147207</v>
+        <v>11.75522310748077</v>
       </c>
       <c r="G10">
-        <v>0.002652859158594914</v>
+        <v>0.002541134639348475</v>
       </c>
       <c r="H10">
-        <v>0.003157987494308005</v>
+        <v>0.002062536131775195</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -666,19 +666,19 @@
         <v>0.02369105879060053</v>
       </c>
       <c r="D11">
-        <v>4464747.631958731</v>
+        <v>4461825.512570077</v>
       </c>
       <c r="E11">
-        <v>287.7776609054353</v>
+        <v>287.749643305974</v>
       </c>
       <c r="F11">
-        <v>13.33623228207553</v>
+        <v>13.86812051426362</v>
       </c>
       <c r="G11">
-        <v>0.002379329830746681</v>
+        <v>0.00228831603480864</v>
       </c>
       <c r="H11">
-        <v>0.002750070310526011</v>
+        <v>0.001799625134479897</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -692,19 +692,19 @@
         <v>0.02286513801810705</v>
       </c>
       <c r="D12">
-        <v>4449271.682480261</v>
+        <v>4445387.015389714</v>
       </c>
       <c r="E12">
-        <v>287.6291182548196</v>
+        <v>287.5917709809168</v>
       </c>
       <c r="F12">
-        <v>15.90909559368732</v>
+        <v>16.48215909057802</v>
       </c>
       <c r="G12">
-        <v>0.00212728573582415</v>
+        <v>0.002053613004249776</v>
       </c>
       <c r="H12">
-        <v>0.002382563601653842</v>
+        <v>0.001561995621239777</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -718,19 +718,19 @@
         <v>0.02203921724561356</v>
       </c>
       <c r="D13">
-        <v>4426548.59700731</v>
+        <v>4421376.592046415</v>
       </c>
       <c r="E13">
-        <v>287.4103085950457</v>
+        <v>287.3603871884911</v>
       </c>
       <c r="F13">
-        <v>19.15059021915603</v>
+        <v>19.771894906541</v>
       </c>
       <c r="G13">
-        <v>0.001893429684077908</v>
+        <v>0.001834280090436213</v>
       </c>
       <c r="H13">
-        <v>0.002051078017466962</v>
+        <v>0.001347008483073192</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -744,19 +744,19 @@
         <v>0.02121329647312005</v>
       </c>
       <c r="D14">
-        <v>4392361.968365735</v>
+        <v>4385427.496948788</v>
       </c>
       <c r="E14">
-        <v>287.0795136450456</v>
+        <v>287.0121785989533</v>
       </c>
       <c r="F14">
-        <v>23.33162766656755</v>
+        <v>24.01122866914344</v>
       </c>
       <c r="G14">
-        <v>0.001674006760113059</v>
+        <v>0.001627047502569853</v>
       </c>
       <c r="H14">
-        <v>0.001751100804445475</v>
+        <v>0.001151901911954504</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -770,19 +770,19 @@
         <v>0.02038737570062656</v>
       </c>
       <c r="D15">
-        <v>4339184.345684472</v>
+        <v>4329757.60064327</v>
       </c>
       <c r="E15">
-        <v>286.5610912729446</v>
+        <v>286.4686939010593</v>
       </c>
       <c r="F15">
-        <v>28.92558841164883</v>
+        <v>29.67890357875835</v>
       </c>
       <c r="G15">
-        <v>0.001463740750923743</v>
+        <v>0.001427100329280454</v>
       </c>
       <c r="H15">
-        <v>0.001477164413625231</v>
+        <v>0.0009732518096418261</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -796,19 +796,19 @@
         <v>0.01956145492813306</v>
       </c>
       <c r="D16">
-        <v>4252159.852511225</v>
+        <v>4239032.554788486</v>
       </c>
       <c r="E16">
-        <v>285.7023220665164</v>
+        <v>285.5716403806056</v>
       </c>
       <c r="F16">
-        <v>36.97038531803609</v>
+        <v>37.82403060256069</v>
       </c>
       <c r="G16">
-        <v>0.001251460209737155</v>
+        <v>0.001223848157442328</v>
       </c>
       <c r="H16">
-        <v>0.001219244632520123</v>
+        <v>0.0008046116947123709</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -822,19 +822,19 @@
         <v>0.01911027116091851</v>
       </c>
       <c r="D17">
-        <v>4095262.59465168</v>
+        <v>4076134.661483259</v>
       </c>
       <c r="E17">
-        <v>284.120242981877</v>
+        <v>283.9242901044451</v>
       </c>
       <c r="F17">
-        <v>54.76904278352885</v>
+        <v>55.77140905355221</v>
       </c>
       <c r="G17">
-        <v>0.0009026882855329143</v>
+        <v>0.0008871695166148265</v>
       </c>
       <c r="H17">
-        <v>0.0008831476150437592</v>
+        <v>0.0005843209908022175</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -848,19 +848,19 @@
         <v>0.02088988309406883</v>
       </c>
       <c r="D18">
-        <v>3595907.968480114</v>
+        <v>3562569.479778449</v>
       </c>
       <c r="E18">
-        <v>278.7648555561087</v>
+        <v>278.3881863958325</v>
       </c>
       <c r="F18">
-        <v>55.7080835775707</v>
+        <v>56.79615966072861</v>
       </c>
       <c r="G18">
-        <v>0.000808078706736171</v>
+        <v>0.0007938931374026335</v>
       </c>
       <c r="H18">
-        <v>0.0009374808838650569</v>
+        <v>0.0006204035028902214</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -874,19 +874,19 @@
         <v>0.02266949502721918</v>
       </c>
       <c r="D19">
-        <v>3521396.992918161</v>
+        <v>3482742.448528838</v>
       </c>
       <c r="E19">
-        <v>277.9194098824447</v>
+        <v>277.475619567879</v>
       </c>
       <c r="F19">
-        <v>50.86179740875176</v>
+        <v>51.91856848074306</v>
       </c>
       <c r="G19">
-        <v>0.0008072802668042239</v>
+        <v>0.0007924114716662376</v>
       </c>
       <c r="H19">
-        <v>0.001050547342209339</v>
+        <v>0.0006950640136342677</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -900,19 +900,19 @@
         <v>0.02444910696036953</v>
       </c>
       <c r="D20">
-        <v>3585017.569644557</v>
+        <v>3546678.443232951</v>
       </c>
       <c r="E20">
-        <v>278.6420960077653</v>
+        <v>278.2077308270634</v>
       </c>
       <c r="F20">
-        <v>45.44232518224646</v>
+        <v>46.42029981017195</v>
       </c>
       <c r="G20">
-        <v>0.0008302250795670451</v>
+        <v>0.0008143243978610638</v>
       </c>
       <c r="H20">
-        <v>0.001183023833902614</v>
+        <v>0.0007824552404017434</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -926,19 +926,19 @@
         <v>0.02622871889351988</v>
       </c>
       <c r="D21">
-        <v>3655993.813292407</v>
+        <v>3619323.888773834</v>
       </c>
       <c r="E21">
-        <v>279.4372806343129</v>
+        <v>279.0278819958173</v>
       </c>
       <c r="F21">
-        <v>40.68419575785195</v>
+        <v>41.5857657890859</v>
       </c>
       <c r="G21">
-        <v>0.0008611638364278003</v>
+        <v>0.0008440631373143284</v>
       </c>
       <c r="H21">
-        <v>0.001329017192244146</v>
+        <v>0.0008786927366491308</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -952,19 +952,19 @@
         <v>0.0280083308266702</v>
       </c>
       <c r="D22">
-        <v>3710846.040142818</v>
+        <v>3675613.209737322</v>
       </c>
       <c r="E22">
-        <v>280.0440602086887</v>
+        <v>279.6550783527885</v>
       </c>
       <c r="F22">
-        <v>36.68409008650473</v>
+        <v>37.52266752408183</v>
       </c>
       <c r="G22">
-        <v>0.000895505504198118</v>
+        <v>0.0008770584150294723</v>
       </c>
       <c r="H22">
-        <v>0.001486416363517067</v>
+        <v>0.0009823798133846184</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -978,19 +978,19 @@
         <v>0.02978794275982054</v>
       </c>
       <c r="D23">
-        <v>3750865.136493647</v>
+        <v>3716651.472483592</v>
       </c>
       <c r="E23">
-        <v>280.4825919758777</v>
+        <v>280.1078922981255</v>
       </c>
       <c r="F23">
-        <v>33.32442031773935</v>
+        <v>34.1118175583627</v>
       </c>
       <c r="G23">
-        <v>0.0009317179477039952</v>
+        <v>0.0009117987632374035</v>
       </c>
       <c r="H23">
-        <v>0.001654206280056361</v>
+        <v>0.001092841279055025</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1004,19 +1004,19 @@
         <v>0.03156755469297089</v>
       </c>
       <c r="D24">
-        <v>3780116.115117721</v>
+        <v>3746609.679617418</v>
       </c>
       <c r="E24">
-        <v>280.800945170599</v>
+        <v>280.4361250285585</v>
       </c>
       <c r="F24">
-        <v>30.48072137135674</v>
+        <v>31.22582968515646</v>
       </c>
       <c r="G24">
-        <v>0.0009691509555716444</v>
+        <v>0.0009476526349606955</v>
       </c>
       <c r="H24">
-        <v>0.001831808876105749</v>
+        <v>0.001209689858688494</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1030,19 +1030,19 @@
         <v>0.03334716662612121</v>
       </c>
       <c r="D25">
-        <v>3801791.000338648</v>
+        <v>3768782.296430608</v>
       </c>
       <c r="E25">
-        <v>281.0356716289462</v>
+        <v>280.6778101975392</v>
       </c>
       <c r="F25">
-        <v>28.05226324892948</v>
+        <v>28.76178107687479</v>
       </c>
       <c r="G25">
-        <v>0.00100745816504008</v>
+        <v>0.0009842864842473352</v>
       </c>
       <c r="H25">
-        <v>0.002018855361594545</v>
+        <v>0.001332676285182604</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1056,19 +1056,19 @@
         <v>0.03512677855927156</v>
       </c>
       <c r="D26">
-        <v>3818095.162496113</v>
+        <v>3785442.729424576</v>
       </c>
       <c r="E26">
-        <v>281.2115850530347</v>
+        <v>280.8587213354973</v>
       </c>
       <c r="F26">
-        <v>25.96079953440488</v>
+        <v>26.63991377803996</v>
       </c>
       <c r="G26">
-        <v>0.001046428131601754</v>
+        <v>0.001021497185475097</v>
       </c>
       <c r="H26">
-        <v>0.002215090354079881</v>
+        <v>0.001461626159102144</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1082,19 +1082,19 @@
         <v>0.03690639049242189</v>
       </c>
       <c r="D27">
-        <v>3830534.276838058</v>
+        <v>3798140.291871773</v>
       </c>
       <c r="E27">
-        <v>281.345423342885</v>
+        <v>280.9962059713998</v>
       </c>
       <c r="F27">
-        <v>24.1456059232269</v>
+        <v>24.79844261846361</v>
       </c>
       <c r="G27">
-        <v>0.001085921468673947</v>
+        <v>0.001059150895445119</v>
       </c>
       <c r="H27">
-        <v>0.002420325773370507</v>
+        <v>0.001596409566505965</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1108,19 +1108,19 @@
         <v>0.03868600242557224</v>
       </c>
       <c r="D28">
-        <v>3840147.549326329</v>
+        <v>3807942.76857071</v>
       </c>
       <c r="E28">
-        <v>281.4486369620874</v>
+        <v>281.1021114239456</v>
       </c>
       <c r="F28">
-        <v>22.55917450909869</v>
+        <v>23.18909102407539</v>
       </c>
       <c r="G28">
-        <v>0.001125841635559042</v>
+        <v>0.00109715492488907</v>
       </c>
       <c r="H28">
-        <v>0.002634416392570845</v>
+        <v>0.001736924958617161</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1134,19 +1134,19 @@
         <v>0.04046561435872258</v>
       </c>
       <c r="D29">
-        <v>3847663.430098201</v>
+        <v>3815597.840414727</v>
       </c>
       <c r="E29">
-        <v>281.5291986780579</v>
+        <v>281.1846763231176</v>
       </c>
       <c r="F29">
-        <v>21.16395675025579</v>
+        <v>21.77373699138506</v>
       </c>
       <c r="G29">
-        <v>0.00116611937480909</v>
+        <v>0.001135442794613163</v>
       </c>
       <c r="H29">
-        <v>0.002857245854750486</v>
+        <v>0.001883089926146102</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1160,19 +1160,19 @@
         <v>0.04224522629187291</v>
       </c>
       <c r="D30">
-        <v>3853600.74138019</v>
+        <v>3821637.593499009</v>
       </c>
       <c r="E30">
-        <v>281.5927576116209</v>
+        <v>281.2497325456474</v>
       </c>
       <c r="F30">
-        <v>19.92996602571818</v>
+        <v>20.52195537477932</v>
       </c>
       <c r="G30">
-        <v>0.001206703690070255</v>
+        <v>0.001173965574321076</v>
       </c>
       <c r="H30">
-        <v>0.00308871817483182</v>
+        <v>0.002034835588647792</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1186,19 +1186,19 @@
         <v>0.04402483822502326</v>
       </c>
       <c r="D31">
-        <v>3858334.678407589</v>
+        <v>3826446.569635886</v>
       </c>
       <c r="E31">
-        <v>281.6433825002633</v>
+        <v>281.3014772900638</v>
       </c>
       <c r="F31">
-        <v>18.83301552621097</v>
+        <v>19.40921702547481</v>
       </c>
       <c r="G31">
-        <v>0.001247556291310992</v>
+        <v>0.001212686547634981</v>
       </c>
       <c r="H31">
-        <v>0.003328752310172847</v>
+        <v>0.002192103007144468</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1212,19 +1212,19 @@
         <v>0.04580445015817358</v>
       </c>
       <c r="D32">
-        <v>3862140.458636379</v>
+        <v>3830306.695807001</v>
       </c>
       <c r="E32">
-        <v>281.6840483134277</v>
+        <v>281.3429775809184</v>
       </c>
       <c r="F32">
-        <v>17.85341433128506</v>
+        <v>18.41555910060696</v>
       </c>
       <c r="G32">
-        <v>0.001288648011551859</v>
+        <v>0.00125157776826626</v>
       </c>
       <c r="H32">
-        <v>0.003577278542787549</v>
+        <v>0.002354840791735719</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1238,19 +1238,19 @@
         <v>0.04758406209132393</v>
       </c>
       <c r="D33">
-        <v>3865222.637612782</v>
+        <v>3833427.42238711</v>
       </c>
       <c r="E33">
-        <v>281.7169605087356</v>
+        <v>281.3765059582456</v>
       </c>
       <c r="F33">
-        <v>16.97499319151688</v>
+        <v>17.52459318869391</v>
       </c>
       <c r="G33">
-        <v>0.00132995640701751</v>
+        <v>0.00129061775184943</v>
       </c>
       <c r="H33">
-        <v>0.003834235980767893</v>
+        <v>0.002523003447802754</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1264,19 +1264,19 @@
         <v>0.04936367402447427</v>
       </c>
       <c r="D34">
-        <v>3867735.108264371</v>
+        <v>3835966.263983103</v>
       </c>
       <c r="E34">
-        <v>281.7437748574241</v>
+        <v>281.4037678004219</v>
       </c>
       <c r="F34">
-        <v>16.18436897882165</v>
+        <v>16.72275733780561</v>
       </c>
       <c r="G34">
-        <v>0.001371464099574782</v>
+        <v>0.001329789880540066</v>
       </c>
       <c r="H34">
-        <v>0.004099570778302695</v>
+        <v>0.00269655019667703</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1290,19 +1290,19 @@
         <v>0.05114328595762462</v>
       </c>
       <c r="D35">
-        <v>3869794.951707656</v>
+        <v>3838043.014808577</v>
       </c>
       <c r="E35">
-        <v>281.7657489206854</v>
+        <v>281.4260578298563</v>
       </c>
       <c r="F35">
-        <v>15.47038348811119</v>
+        <v>15.99874591350827</v>
       </c>
       <c r="G35">
-        <v>0.001413157602160399</v>
+        <v>0.001369081271709555</v>
       </c>
       <c r="H35">
-        <v>0.004373234832908403</v>
+        <v>0.002875444111564876</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1316,19 +1316,19 @@
         <v>0.05292289789077495</v>
       </c>
       <c r="D36">
-        <v>3871492.167627157</v>
+        <v>3839749.729326267</v>
       </c>
       <c r="E36">
-        <v>281.7838480268501</v>
+        <v>281.4443695324328</v>
       </c>
       <c r="F36">
-        <v>14.82367091885915</v>
+        <v>15.34307050942753</v>
       </c>
       <c r="G36">
-        <v>0.001455026468328097</v>
+        <v>0.00140848195829612</v>
       </c>
       <c r="H36">
-        <v>0.004655184808954336</v>
+        <v>0.0030596514691536</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1342,19 +1342,19 @@
         <v>0.05470250982392529</v>
       </c>
       <c r="D37">
-        <v>3872896.602004613</v>
+        <v>3841157.824789534</v>
       </c>
       <c r="E37">
-        <v>281.7988204690107</v>
+        <v>281.4594727536782</v>
       </c>
       <c r="F37">
-        <v>14.23632132752274</v>
+        <v>14.74771848545969</v>
       </c>
       <c r="G37">
-        <v>0.001497062665131647</v>
+        <v>0.001447984284044434</v>
       </c>
       <c r="H37">
-        <v>0.004945381390154049</v>
+        <v>0.003249141252657469</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1368,19 +1368,19 @@
         <v>0.05648212175707563</v>
       </c>
       <c r="D38">
-        <v>3874062.941421865</v>
+        <v>3842323.199571275</v>
       </c>
       <c r="E38">
-        <v>281.8112515642875</v>
+        <v>281.4719694563004</v>
       </c>
       <c r="F38">
-        <v>13.70161639323721</v>
+        <v>14.2058850007023</v>
       </c>
       <c r="G38">
-        <v>0.001539260103453166</v>
+        <v>0.001487582450324692</v>
       </c>
       <c r="H38">
-        <v>0.005243788696459604</v>
+        <v>0.003443884763671729</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1394,19 +1394,19 @@
         <v>0.05826173369022596</v>
       </c>
       <c r="D39">
-        <v>3875034.355711815</v>
+        <v>3843289.965051821</v>
       </c>
       <c r="E39">
-        <v>281.8216029903591</v>
+        <v>281.482334276614</v>
       </c>
       <c r="F39">
-        <v>13.21382020992566</v>
+        <v>13.71176093140745</v>
       </c>
       <c r="G39">
-        <v>0.00158161428155855</v>
+        <v>0.001527272172015383</v>
       </c>
       <c r="H39">
-        <v>0.005550373821435729</v>
+        <v>0.003643855313820268</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1420,19 +1420,19 @@
         <v>0.0600413456233763</v>
       </c>
       <c r="D40">
-        <v>3875845.183799047</v>
+        <v>3844093.196485154</v>
       </c>
       <c r="E40">
-        <v>281.830241732518</v>
+        <v>281.4909443593575</v>
       </c>
       <c r="F40">
-        <v>12.76801234391833</v>
+        <v>13.26036368927963</v>
       </c>
       <c r="G40">
-        <v>0.001624122011593456</v>
+        <v>0.001567050413307075</v>
       </c>
       <c r="H40">
-        <v>0.005865106459787318</v>
+        <v>0.003849027976152104</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1446,19 +1446,19 @@
         <v>0.06182095755652664</v>
       </c>
       <c r="D41">
-        <v>3876522.934258359</v>
+        <v>3844760.981489335</v>
       </c>
       <c r="E41">
-        <v>281.8374616091806</v>
+        <v>281.4981015369328</v>
       </c>
       <c r="F41">
-        <v>12.35995364680829</v>
+        <v>12.84740127189641</v>
       </c>
       <c r="G41">
-        <v>0.001666781207573764</v>
+        <v>0.001606915182783216</v>
       </c>
       <c r="H41">
-        <v>0.006187958602724221</v>
+        <v>0.004059379381541419</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1472,19 +1472,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D42">
-        <v>3877089.789643451</v>
+        <v>3845315.960079048</v>
       </c>
       <c r="E42">
-        <v>281.8434994352384</v>
+        <v>281.5040489793652</v>
       </c>
       <c r="F42">
-        <v>12.02587319718006</v>
+        <v>12.51014771145389</v>
       </c>
       <c r="G42">
-        <v>0.00170699198825568</v>
+        <v>0.001644430127214736</v>
       </c>
       <c r="H42">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1498,19 +1498,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D43">
-        <v>3877527.188368597</v>
+        <v>3845741.037443511</v>
       </c>
       <c r="E43">
-        <v>281.8481579145759</v>
+        <v>281.5086039023232</v>
       </c>
       <c r="F43">
-        <v>12.37938520797392</v>
+        <v>12.87928545862838</v>
       </c>
       <c r="G43">
-        <v>0.001703921011539139</v>
+        <v>0.001641360996549282</v>
       </c>
       <c r="H43">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1524,19 +1524,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D44">
-        <v>3876069.347444586</v>
+        <v>3844143.942569709</v>
       </c>
       <c r="E44">
-        <v>281.8326297855052</v>
+        <v>281.491488277398</v>
       </c>
       <c r="F44">
-        <v>12.75784281684561</v>
+        <v>13.27487037493452</v>
       </c>
       <c r="G44">
-        <v>0.001700429970927155</v>
+        <v>0.001637858351388118</v>
       </c>
       <c r="H44">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1550,19 +1550,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D45">
-        <v>3874524.127548253</v>
+        <v>3842450.14003476</v>
       </c>
       <c r="E45">
-        <v>281.8161662201084</v>
+        <v>281.4733305118277</v>
       </c>
       <c r="F45">
-        <v>13.15856675065528</v>
+        <v>13.69383769263286</v>
       </c>
       <c r="G45">
-        <v>0.001696948645624376</v>
+        <v>0.001634359746100847</v>
       </c>
       <c r="H45">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1576,19 +1576,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D46">
-        <v>3872897.590789796</v>
+        <v>3840666.886377125</v>
       </c>
       <c r="E46">
-        <v>281.7988310088691</v>
+        <v>281.4542074172937</v>
       </c>
       <c r="F46">
-        <v>13.58353845701165</v>
+        <v>14.13827244535902</v>
       </c>
       <c r="G46">
-        <v>0.001693481001540403</v>
+        <v>0.001630869040628448</v>
       </c>
       <c r="H46">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1602,19 +1602,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D47">
-        <v>3871182.928446277</v>
+        <v>3838786.674239528</v>
       </c>
       <c r="E47">
-        <v>281.7805507388572</v>
+        <v>281.4340374504714</v>
       </c>
       <c r="F47">
-        <v>14.03502283423567</v>
+        <v>14.61056420259522</v>
       </c>
       <c r="G47">
-        <v>0.001690028099713938</v>
+        <v>0.001627386860454491</v>
       </c>
       <c r="H47">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1628,19 +1628,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D48">
-        <v>3869372.414874882</v>
+        <v>3836800.967693379</v>
       </c>
       <c r="E48">
-        <v>281.7612420751139</v>
+        <v>281.4127278539858</v>
       </c>
       <c r="F48">
-        <v>14.51557810862474</v>
+        <v>15.11341351548282</v>
       </c>
       <c r="G48">
-        <v>0.001686590969455263</v>
+        <v>0.001623913750191648</v>
       </c>
       <c r="H48">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1654,19 +1654,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D49">
-        <v>3867457.360781424</v>
+        <v>3834700.160850705</v>
       </c>
       <c r="E49">
-        <v>281.7408112310166</v>
+        <v>281.3901741735068</v>
       </c>
       <c r="F49">
-        <v>15.02810491769607</v>
+        <v>15.64988414940617</v>
       </c>
       <c r="G49">
-        <v>0.00168317060781279</v>
+        <v>0.001620450170592717</v>
       </c>
       <c r="H49">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1680,19 +1680,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D50">
-        <v>3865427.955451748</v>
+        <v>3832473.401944818</v>
       </c>
       <c r="E50">
-        <v>281.7191522480081</v>
+        <v>281.36625832325</v>
       </c>
       <c r="F50">
-        <v>15.57590598057785</v>
+        <v>16.22346670349518</v>
       </c>
       <c r="G50">
-        <v>0.001679767951435033</v>
+        <v>0.001616996463008819</v>
       </c>
       <c r="H50">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -1706,19 +1706,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D51">
-        <v>3863273.075540286</v>
+        <v>3830108.379744311</v>
       </c>
       <c r="E51">
-        <v>281.6961449090426</v>
+        <v>281.3408462352944</v>
       </c>
       <c r="F51">
-        <v>16.16275877045443</v>
+        <v>16.83815617047246</v>
       </c>
       <c r="G51">
-        <v>0.001676383839012611</v>
+        <v>0.001613552802885284</v>
       </c>
       <c r="H51">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1732,19 +1732,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D52">
-        <v>3860980.052739653</v>
+        <v>3827591.063760823</v>
       </c>
       <c r="E52">
-        <v>281.6716522009905</v>
+        <v>281.3137849974523</v>
       </c>
       <c r="F52">
-        <v>16.79300463100501</v>
+        <v>17.49854714742868</v>
       </c>
       <c r="G52">
-        <v>0.0016730189615431</v>
+        <v>0.001610119139328258</v>
       </c>
       <c r="H52">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -1758,19 +1758,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D53">
-        <v>3858534.389530085</v>
+        <v>3824905.386040103</v>
       </c>
       <c r="E53">
-        <v>281.6455172069106</v>
+        <v>281.2848993437679</v>
       </c>
       <c r="F53">
-        <v>17.47165886797425</v>
+        <v>18.20995159239639</v>
       </c>
       <c r="G53">
-        <v>0.001669673796523514</v>
+        <v>0.001606695116330795</v>
       </c>
       <c r="H53">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -1784,19 +1784,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D54">
-        <v>3855919.408805151</v>
+        <v>3822032.848445782</v>
       </c>
       <c r="E54">
-        <v>281.6175592713868</v>
+        <v>281.2539873182859</v>
       </c>
       <c r="F54">
-        <v>18.20454783795372</v>
+        <v>18.97854564254785</v>
       </c>
       <c r="G54">
-        <v>0.001666348520814491</v>
+        <v>0.001603279969800154</v>
       </c>
       <c r="H54">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -1810,19 +1810,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D55">
-        <v>3853115.818514598</v>
+        <v>3818952.034034324</v>
       </c>
       <c r="E55">
-        <v>281.5875692304689</v>
+        <v>281.2208148731968</v>
       </c>
       <c r="F55">
-        <v>18.99848112484769</v>
+        <v>19.81155426420715</v>
       </c>
       <c r="G55">
-        <v>0.001663042895027914</v>
+        <v>0.001599872392418161</v>
       </c>
       <c r="H55">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -1836,19 +1836,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D56">
-        <v>3850101.166009207</v>
+        <v>3815637.993735922</v>
       </c>
       <c r="E56">
-        <v>281.555303425993</v>
+        <v>281.1851090795342</v>
       </c>
       <c r="F56">
-        <v>19.86146980088597</v>
+        <v>20.71748567970026</v>
       </c>
       <c r="G56">
-        <v>0.001659756109628464</v>
+        <v>0.001596470355413747</v>
       </c>
       <c r="H56">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -1862,19 +1862,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D57">
-        <v>3846849.147703799</v>
+        <v>3812061.469159165</v>
       </c>
       <c r="E57">
-        <v>281.5204761231017</v>
+        <v>281.1465495116441</v>
       </c>
       <c r="F57">
-        <v>20.80300590972929</v>
+        <v>21.70643205062357</v>
       </c>
       <c r="G57">
-        <v>0.001656486579152518</v>
+        <v>0.001593070872122944</v>
       </c>
       <c r="H57">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -1888,19 +1888,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D58">
-        <v>3843328.726756925</v>
+        <v>3808187.897487967</v>
       </c>
       <c r="E58">
-        <v>281.4827498057358</v>
+        <v>281.1047571992738</v>
       </c>
       <c r="F58">
-        <v>21.83442429761702</v>
+        <v>22.7904594734484</v>
       </c>
       <c r="G58">
-        <v>0.001653231665491275</v>
+        <v>0.001589669682149182</v>
       </c>
       <c r="H58">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -1914,19 +1914,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D59">
-        <v>3839502.992784514</v>
+        <v>3803976.12290054</v>
       </c>
       <c r="E59">
-        <v>281.4417226161515</v>
+        <v>281.0592802978697</v>
       </c>
       <c r="F59">
-        <v>22.96937672216903</v>
+        <v>23.98412004130211</v>
       </c>
       <c r="G59">
-        <v>0.001649987303212575</v>
+        <v>0.001586260826067106</v>
       </c>
       <c r="H59">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -1940,19 +1940,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D60">
-        <v>3835327.670157767</v>
+        <v>3799376.707167951</v>
       </c>
       <c r="E60">
-        <v>281.3969118970421</v>
+        <v>281.0095752680367</v>
       </c>
       <c r="F60">
-        <v>24.22446134521689</v>
+        <v>25.30513329116265</v>
       </c>
       <c r="G60">
-        <v>0.001646747488068812</v>
+        <v>0.001582836067432115</v>
       </c>
       <c r="H60">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -1966,19 +1966,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D61">
-        <v>3830749.140312113</v>
+        <v>3794329.684346064</v>
       </c>
       <c r="E61">
-        <v>281.3477323334748</v>
+        <v>280.9549818134206</v>
       </c>
       <c r="F61">
-        <v>25.6200708316079</v>
+        <v>26.77530667731174</v>
       </c>
       <c r="G61">
-        <v>0.001643503571994566</v>
+        <v>0.001579384098924639</v>
       </c>
       <c r="H61">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -1992,19 +1992,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D62">
-        <v>3825701.780683127</v>
+        <v>3788761.531253209</v>
       </c>
       <c r="E62">
-        <v>282.1809691104066</v>
+        <v>281.796250485005</v>
       </c>
       <c r="F62">
-        <v>26.90667079164783</v>
+        <v>28.34747705913678</v>
       </c>
       <c r="G62">
-        <v>0.001615341811793374</v>
+        <v>0.001551881604143266</v>
       </c>
       <c r="H62">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2018,19 +2018,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D63">
-        <v>3820806.536219803</v>
+        <v>3782692.995204248</v>
       </c>
       <c r="E63">
-        <v>283.0411091027392</v>
+        <v>282.6646644423092</v>
       </c>
       <c r="F63">
-        <v>27.71543588094902</v>
+        <v>29.21913380828811</v>
       </c>
       <c r="G63">
-        <v>0.001590163433544918</v>
+        <v>0.001527459794810484</v>
       </c>
       <c r="H63">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2044,19 +2044,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D64">
-        <v>3817180.304018879</v>
+        <v>3778602.335788406</v>
       </c>
       <c r="E64">
-        <v>283.9274855763807</v>
+        <v>283.5598583379592</v>
       </c>
       <c r="F64">
-        <v>28.50497998579237</v>
+        <v>30.05667667691423</v>
       </c>
       <c r="G64">
-        <v>0.00156658783413678</v>
+        <v>0.001504831898861178</v>
       </c>
       <c r="H64">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2070,19 +2070,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D65">
-        <v>3813502.017998157</v>
+        <v>3774493.2391426</v>
       </c>
       <c r="E65">
-        <v>284.838895614412</v>
+        <v>284.4802548834756</v>
       </c>
       <c r="F65">
-        <v>29.30031012306693</v>
+        <v>30.8997340083142</v>
       </c>
       <c r="G65">
-        <v>0.001544027146741291</v>
+        <v>0.001483192473640295</v>
       </c>
       <c r="H65">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2096,19 +2096,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D66">
-        <v>3809696.0037578</v>
+        <v>3770242.195641362</v>
       </c>
       <c r="E66">
-        <v>285.774787412447</v>
+        <v>285.4252677992795</v>
       </c>
       <c r="F66">
-        <v>30.10302075219266</v>
+        <v>31.75093261202746</v>
       </c>
       <c r="G66">
-        <v>0.001522382946276478</v>
+        <v>0.001462431731425706</v>
       </c>
       <c r="H66">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -2122,19 +2122,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D67">
-        <v>3805754.808411618</v>
+        <v>3765837.930797995</v>
       </c>
       <c r="E67">
-        <v>286.7346298392324</v>
+        <v>286.3943543072576</v>
       </c>
       <c r="F67">
-        <v>30.9134365452062</v>
+        <v>32.61070207641954</v>
       </c>
       <c r="G67">
-        <v>0.001501587842726844</v>
+        <v>0.001442484192970071</v>
       </c>
       <c r="H67">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2148,19 +2148,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D68">
-        <v>3801674.63537896</v>
+        <v>3761275.818786754</v>
       </c>
       <c r="E68">
-        <v>287.7178809977548</v>
+        <v>287.3869624045008</v>
       </c>
       <c r="F68">
-        <v>31.73181983499446</v>
+        <v>33.47934963302851</v>
       </c>
       <c r="G68">
-        <v>0.001481581629407713</v>
+        <v>0.001423292151482247</v>
       </c>
       <c r="H68">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -2174,19 +2174,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D69">
-        <v>3797451.766163342</v>
+        <v>3756551.487247796</v>
       </c>
       <c r="E69">
-        <v>288.723988360484</v>
+        <v>288.4025296592851</v>
       </c>
       <c r="F69">
-        <v>32.55843935900175</v>
+        <v>34.35718760613661</v>
       </c>
       <c r="G69">
-        <v>0.001462309379936737</v>
+        <v>0.001404802985312798</v>
       </c>
       <c r="H69">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2200,19 +2200,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D70">
-        <v>3793082.348403097</v>
+        <v>3751660.412022651</v>
       </c>
       <c r="E70">
-        <v>289.7523906157909</v>
+        <v>289.440485031562</v>
       </c>
       <c r="F70">
-        <v>33.39357628497076</v>
+        <v>35.24454346116372</v>
       </c>
       <c r="G70">
-        <v>0.001443720769670183</v>
+        <v>0.001386968465041448</v>
       </c>
       <c r="H70">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2226,19 +2226,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D71">
-        <v>3788562.371000716</v>
+        <v>3746597.877139918</v>
       </c>
       <c r="E71">
-        <v>290.802519614598</v>
+        <v>290.5002508762188</v>
       </c>
       <c r="F71">
-        <v>34.23752651365065</v>
+        <v>36.14176273495863</v>
       </c>
       <c r="G71">
-        <v>0.001425769550479232</v>
+        <v>0.001369744246799264</v>
       </c>
       <c r="H71">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -2252,19 +2252,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D72">
-        <v>3783887.649555819</v>
+        <v>3741358.956068951</v>
       </c>
       <c r="E72">
-        <v>291.87380230736</v>
+        <v>291.5812449378083</v>
       </c>
       <c r="F72">
-        <v>35.09060269139733</v>
+        <v>37.04921121595761</v>
       </c>
       <c r="G72">
-        <v>0.001408413102324841</v>
+        <v>0.00135308945136181</v>
       </c>
       <c r="H72">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2278,19 +2278,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D73">
-        <v>3779053.81168098</v>
+        <v>3735938.494240512</v>
       </c>
       <c r="E73">
-        <v>292.9656626435658</v>
+        <v>292.6828823032008</v>
       </c>
       <c r="F73">
-        <v>35.9531357969458</v>
+        <v>37.96727693000761</v>
       </c>
       <c r="G73">
-        <v>0.001391612060137868</v>
+        <v>0.001336966304616664</v>
       </c>
       <c r="H73">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2304,19 +2304,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D74">
-        <v>3774056.282806724</v>
+        <v>3730331.091106815</v>
       </c>
       <c r="E74">
-        <v>294.0775234128725</v>
+        <v>293.8045772900005</v>
       </c>
       <c r="F74">
-        <v>36.82547679070569</v>
+        <v>38.8963719749442</v>
       </c>
       <c r="G74">
-        <v>0.001375329984939636</v>
+        <v>0.001321339829360871</v>
       </c>
       <c r="H74">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -2330,19 +2330,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D75">
-        <v>3768890.270883734</v>
+        <v>3724531.08165183</v>
       </c>
       <c r="E75">
-        <v>295.2088080094932</v>
+        <v>294.9457452521855</v>
       </c>
       <c r="F75">
-        <v>37.70799803273231</v>
+        <v>39.83693423799075</v>
       </c>
       <c r="G75">
-        <v>0.001359533084768783</v>
+        <v>0.001306177579697346</v>
       </c>
       <c r="H75">
-        <v>0.00649998653025552</v>
+        <v>0.004262571633766798</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -2356,19 +2356,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D76">
-        <v>3763550.751011967</v>
+        <v>3718532.517274352</v>
       </c>
       <c r="E76">
-        <v>296.3589421048729</v>
+        <v>296.1058042875183</v>
       </c>
       <c r="F76">
-        <v>38.60109461804244</v>
+        <v>40.78942902975658</v>
       </c>
       <c r="G76">
-        <v>0.00134418997209665</v>
+        <v>0.001291449410859206</v>
       </c>
       <c r="H76">
-        <v>0.006499986530255529</v>
+        <v>0.004262571633766793</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -2382,19 +2382,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D77">
-        <v>3758032.449534914</v>
+        <v>3712329.145949263</v>
       </c>
       <c r="E77">
-        <v>297.5273552162193</v>
+        <v>297.2841768343802</v>
       </c>
       <c r="F77">
-        <v>39.50518564222387</v>
+        <v>41.75435066877403</v>
       </c>
       <c r="G77">
-        <v>0.001329271452458753</v>
+        <v>0.001277127278560003</v>
       </c>
       <c r="H77">
-        <v>0.006499986530255529</v>
+        <v>0.004262571633766793</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -2408,19 +2408,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D78">
-        <v>3752329.827570149</v>
+        <v>3705914.391553654</v>
       </c>
       <c r="E78">
-        <v>298.7134821614893</v>
+        <v>298.4802911487461</v>
       </c>
       <c r="F78">
-        <v>40.42071542506105</v>
+        <v>42.73222405060929</v>
       </c>
       <c r="G78">
-        <v>0.00131475033920126</v>
+        <v>0.00126318506300832</v>
       </c>
       <c r="H78">
-        <v>0.006499986530255529</v>
+        <v>0.004262571633766793</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -2434,19 +2434,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D79">
-        <v>3746437.063884491</v>
+        <v>3699281.332225536</v>
       </c>
       <c r="E79">
-        <v>299.9167643941873</v>
+        <v>299.6935826549305</v>
       </c>
       <c r="F79">
-        <v>41.34815472050116</v>
+        <v>43.7236062355973</v>
       </c>
       <c r="G79">
-        <v>0.001300601290125855</v>
+        <v>0.001249598413581471</v>
       </c>
       <c r="H79">
-        <v>0.006499986530255529</v>
+        <v>0.004262571633766793</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -2460,19 +2460,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D80">
-        <v>3740348.037005253</v>
+        <v>3692422.67760398</v>
       </c>
       <c r="E80">
-        <v>301.1366512139389</v>
+        <v>300.9234951664581</v>
       </c>
       <c r="F80">
-        <v>42.28800194097863</v>
+        <v>44.72908808923681</v>
       </c>
       <c r="G80">
-        <v>0.001286800662553389</v>
+        <v>0.001236344610859222</v>
       </c>
       <c r="H80">
-        <v>0.006499986530255529</v>
+        <v>0.004262571633766793</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -2486,19 +2486,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D81">
-        <v>3734056.306445044</v>
+        <v>3685330.74478032</v>
       </c>
       <c r="E81">
-        <v>302.3726008511767</v>
+        <v>302.16948197588</v>
       </c>
       <c r="F81">
-        <v>43.24078442372005</v>
+        <v>45.74929600930663</v>
       </c>
       <c r="G81">
-        <v>0.001273326383936207</v>
+        <v>0.001223402443301324</v>
       </c>
       <c r="H81">
-        <v>0.006499986530255529</v>
+        <v>0.004262571633766793</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -2512,19 +2512,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D82">
-        <v>3727555.092903876</v>
+        <v>3677997.432770327</v>
       </c>
       <c r="E82">
-        <v>303.6240814264074</v>
+        <v>303.4310068145433</v>
       </c>
       <c r="F82">
-        <v>44.20705976628514</v>
+        <v>46.78489377390964</v>
       </c>
       <c r="G82">
-        <v>0.001260157835652789</v>
+        <v>0.001210752096334052</v>
       </c>
       <c r="H82">
-        <v>0.006499986530255529</v>
+        <v>0.004262571633766793</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -2538,19 +2538,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D83">
-        <v>3720837.257298253</v>
+        <v>3670414.195296539</v>
       </c>
       <c r="E83">
-        <v>304.8905717863662</v>
+        <v>304.707544685206</v>
       </c>
       <c r="F83">
-        <v>45.18741725832371</v>
+        <v>47.8365845450049</v>
       </c>
       <c r="G83">
-        <v>0.001247275748034673</v>
+        <v>0.001198375052007949</v>
       </c>
       <c r="H83">
-        <v>0.006499986530255529</v>
+        <v>0.004262571633766793</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -2564,19 +2564,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D84">
-        <v>3713895.27845243</v>
+        <v>3662572.011647788</v>
       </c>
       <c r="E84">
-        <v>306.1715622209301</v>
+        <v>305.9985825719721</v>
       </c>
       <c r="F84">
-        <v>46.18247943641484</v>
+        <v>48.90511306264752</v>
       </c>
       <c r="G84">
-        <v>0.001234662105019165</v>
+        <v>0.001186253997716107</v>
       </c>
       <c r="H84">
-        <v>0.006499986530255529</v>
+        <v>0.004262571633766793</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -2590,19 +2590,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D85">
-        <v>3706721.229271477</v>
+        <v>3654461.355358742</v>
       </c>
       <c r="E85">
-        <v>307.4665550659378</v>
+        <v>307.3036200332972</v>
       </c>
       <c r="F85">
-        <v>47.19290378897324</v>
+        <v>49.99126806621826</v>
       </c>
       <c r="G85">
-        <v>0.001222300057104403</v>
+        <v>0.001174372742731111</v>
       </c>
       <c r="H85">
-        <v>0.006499986530255529</v>
+        <v>0.004262571633766793</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -2616,19 +2616,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D86">
-        <v>3699306.751198992</v>
+        <v>3646072.160425389</v>
       </c>
       <c r="E86">
-        <v>308.775065198068</v>
+        <v>308.622169684812</v>
       </c>
       <c r="F86">
-        <v>48.21938463862927</v>
+        <v>51.09588498049285</v>
       </c>
       <c r="G86">
-        <v>0.001210173841515886</v>
+        <v>0.001162716141539114</v>
       </c>
       <c r="H86">
-        <v>0.006499986530255529</v>
+        <v>0.004262571633766793</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -2642,19 +2642,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D87">
-        <v>3691643.026743633</v>
+        <v>3637393.784742016</v>
       </c>
       <c r="E87">
-        <v>310.0966204286833</v>
+        <v>309.9537575794361</v>
       </c>
       <c r="F87">
-        <v>49.26265523028218</v>
+        <v>52.2198489065836</v>
       </c>
       <c r="G87">
-        <v>0.001198268708684186</v>
+        <v>0.001151270023129454</v>
       </c>
       <c r="H87">
-        <v>0.006499986530255529</v>
+        <v>0.004262571633766793</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -2668,19 +2668,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D88">
-        <v>3683720.749837643</v>
+        <v>3628414.970410599</v>
       </c>
       <c r="E88">
-        <v>311.4307618040625</v>
+        <v>311.2979234927486</v>
       </c>
       <c r="F88">
-        <v>50.32349005426204</v>
+        <v>53.36409796069928</v>
       </c>
       <c r="G88">
-        <v>0.001186570854289219</v>
+        <v>0.001140021125544765</v>
       </c>
       <c r="H88">
-        <v>0.006499986530255529</v>
+        <v>0.004262571633766793</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -2694,19 +2694,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D89">
-        <v>3675530.093766672</v>
+        <v>3619123.800533542</v>
       </c>
       <c r="E89">
-        <v>312.7770438197659</v>
+        <v>312.6542211218552</v>
       </c>
       <c r="F89">
-        <v>51.40270743579131</v>
+        <v>54.52962700744058</v>
       </c>
       <c r="G89">
-        <v>0.001175067356253159</v>
+        <v>0.001128957035115267</v>
       </c>
       <c r="H89">
-        <v>0.006499986530255529</v>
+        <v>0.004262571633766793</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -2720,19 +2720,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D90">
-        <v>3667060.67638274</v>
+        <v>3609507.652054424</v>
       </c>
       <c r="E90">
-        <v>314.1350345570069</v>
+        <v>314.0222182060902</v>
       </c>
       <c r="F90">
-        <v>52.50117242428558</v>
+        <v>55.7174918391236</v>
       </c>
       <c r="G90">
-        <v>0.00116374611616686</v>
+        <v>0.001118066129896864</v>
       </c>
       <c r="H90">
-        <v>0.006499986530255529</v>
+        <v>0.004262571633766793</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -2746,19 +2746,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D91">
-        <v>3658301.522280485</v>
+        <v>3599553.144157321</v>
       </c>
       <c r="E91">
-        <v>315.5043157488914</v>
+        <v>315.4014965778363</v>
       </c>
       <c r="F91">
-        <v>53.61980001907093</v>
+        <v>56.92881385856984</v>
       </c>
       <c r="G91">
-        <v>0.001152595804717688</v>
+        <v>0.001107337526909807</v>
       </c>
       <c r="H91">
-        <v>0.006499986530255529</v>
+        <v>0.004262571633766793</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -2772,19 +2772,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D92">
-        <v>3649241.021580027</v>
+        <v>3589246.08167209</v>
       </c>
       <c r="E92">
-        <v>316.8844827842465</v>
+        <v>316.7916521515638</v>
       </c>
       <c r="F92">
-        <v>54.75955877191128</v>
+        <v>58.16478533011526</v>
       </c>
       <c r="G92">
-        <v>0.001141605810753614</v>
+        <v>0.001096761032836487</v>
       </c>
       <c r="H92">
-        <v>0.006499986530255529</v>
+        <v>0.004262571633766793</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -2798,19 +2798,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D93">
-        <v>3639866.884916938</v>
+        <v>3578571.392858681</v>
       </c>
       <c r="E93">
-        <v>318.2751446565155</v>
+        <v>318.1922948589142</v>
       </c>
       <c r="F93">
-        <v>55.92147481146261</v>
+        <v>59.42667527251594</v>
       </c>
       <c r="G93">
-        <v>0.001130766193672103</v>
+        <v>0.0010863270978862</v>
       </c>
       <c r="H93">
-        <v>0.006499986530255529</v>
+        <v>0.004262571633766793</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Linear Temperature Profile Definitions
</commit_message>
<xml_diff>
--- a/TheEngine/Regen Solver/enginefiles/solverdata.xlsx
+++ b/TheEngine/Regen Solver/enginefiles/solverdata.xlsx
@@ -438,13 +438,13 @@
         <v>288.1145796254294</v>
       </c>
       <c r="F2">
-        <v>3.656094375228009</v>
+        <v>3.651755013093158</v>
       </c>
       <c r="G2">
-        <v>0.005565650964579227</v>
+        <v>0.005572264599657401</v>
       </c>
       <c r="H2">
-        <v>0.005454591059024392</v>
+        <v>0.007615357616818812</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -458,19 +458,19 @@
         <v>0.03029842497054849</v>
       </c>
       <c r="D3">
-        <v>4499950.053907844</v>
+        <v>4499950.209224804</v>
       </c>
       <c r="E3">
-        <v>288.1141036848301</v>
+        <v>288.1141051648649</v>
       </c>
       <c r="F3">
-        <v>4.190076422036327</v>
+        <v>3.853902650776024</v>
       </c>
       <c r="G3">
-        <v>0.005057143982657782</v>
+        <v>0.005499567600562982</v>
       </c>
       <c r="H3">
-        <v>0.00486901296120758</v>
+        <v>0.007423287372138057</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -484,19 +484,19 @@
         <v>0.029472504198055</v>
       </c>
       <c r="D4">
-        <v>4498663.277085356</v>
+        <v>4499470.329730766</v>
       </c>
       <c r="E4">
-        <v>288.1018405031897</v>
+        <v>288.1095321488901</v>
       </c>
       <c r="F4">
-        <v>4.811548179781115</v>
+        <v>4.094194974781712</v>
       </c>
       <c r="G4">
-        <v>0.004594235965509072</v>
+        <v>0.005400488435281656</v>
       </c>
       <c r="H4">
-        <v>0.004338854288853006</v>
+        <v>0.007190997836826019</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -510,19 +510,19 @@
         <v>0.02864658342556152</v>
       </c>
       <c r="D5">
-        <v>4496946.202826858</v>
+        <v>4498873.259099169</v>
       </c>
       <c r="E5">
-        <v>288.0854723964588</v>
+        <v>288.1038418449287</v>
       </c>
       <c r="F5">
-        <v>5.537508284883274</v>
+        <v>4.379741655047277</v>
       </c>
       <c r="G5">
-        <v>0.004172384655007708</v>
+        <v>0.005275387456556131</v>
       </c>
       <c r="H5">
-        <v>0.003858858283718739</v>
+        <v>0.00692114894990719</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -536,19 +536,19 @@
         <v>0.02782066265306801</v>
       </c>
       <c r="D6">
-        <v>4494641.969103299</v>
+        <v>4498124.226081409</v>
       </c>
       <c r="E6">
-        <v>288.0634997455525</v>
+        <v>288.0967024771016</v>
       </c>
       <c r="F6">
-        <v>6.389830916869052</v>
+        <v>4.719721488883242</v>
       </c>
       <c r="G6">
-        <v>0.003787177639467792</v>
+        <v>0.005124862610490295</v>
       </c>
       <c r="H6">
-        <v>0.003424328670984899</v>
+        <v>0.006616945396397372</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -562,19 +562,19 @@
         <v>0.02699474188057452</v>
       </c>
       <c r="D7">
-        <v>4491527.000071269</v>
+        <v>4497174.706004631</v>
       </c>
       <c r="E7">
-        <v>288.0337825890617</v>
+        <v>288.0876508878874</v>
       </c>
       <c r="F7">
-        <v>7.3962497060019</v>
+        <v>5.125838090180885</v>
       </c>
       <c r="G7">
-        <v>0.003434731041445112</v>
+        <v>0.004949922385933965</v>
       </c>
       <c r="H7">
-        <v>0.003031053208107388</v>
+        <v>0.006282077221116508</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -588,19 +588,19 @@
         <v>0.02616882110808103</v>
       </c>
       <c r="D8">
-        <v>4487280.545447507</v>
+        <v>4495956.605246617</v>
       </c>
       <c r="E8">
-        <v>287.9932458720727</v>
+        <v>288.0760368592772</v>
       </c>
       <c r="F8">
-        <v>8.592393623045998</v>
+        <v>5.613202947475396</v>
       </c>
       <c r="G8">
-        <v>0.003111596358493659</v>
+        <v>0.004751945729213477</v>
       </c>
       <c r="H8">
-        <v>0.002675237058909835</v>
+        <v>0.005920634283267094</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -614,19 +614,19 @@
         <v>0.02534290033558753</v>
       </c>
       <c r="D9">
-        <v>4481435.505081112</v>
+        <v>4494372.68470552</v>
       </c>
       <c r="E9">
-        <v>287.9374016723725</v>
+        <v>288.0609313557791</v>
       </c>
       <c r="F9">
-        <v>10.02476199976335</v>
+        <v>6.201627251113021</v>
       </c>
       <c r="G9">
-        <v>0.002814675052937939</v>
+        <v>0.00453260907977424</v>
       </c>
       <c r="H9">
-        <v>0.002353443141982423</v>
+        <v>0.005536992342578199</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -640,19 +640,19 @@
         <v>0.02451697956309404</v>
       </c>
       <c r="D10">
-        <v>4473299.652610684</v>
+        <v>4492281.267137013</v>
       </c>
       <c r="E10">
-        <v>287.859579260179</v>
+        <v>288.0409798086959</v>
       </c>
       <c r="F10">
-        <v>11.75522310748077</v>
+        <v>6.917578341048428</v>
       </c>
       <c r="G10">
-        <v>0.002541134639348475</v>
+        <v>0.004293771910173346</v>
       </c>
       <c r="H10">
-        <v>0.002062536131775195</v>
+        <v>0.00513566622364592</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -666,19 +666,19 @@
         <v>0.02369105879060053</v>
       </c>
       <c r="D11">
-        <v>4461825.512570077</v>
+        <v>4489471.007782832</v>
       </c>
       <c r="E11">
-        <v>287.749643305974</v>
+        <v>288.0141596696402</v>
       </c>
       <c r="F11">
-        <v>13.86812051426362</v>
+        <v>7.797279292727093</v>
       </c>
       <c r="G11">
-        <v>0.00228831603480864</v>
+        <v>0.004037303300267244</v>
       </c>
       <c r="H11">
-        <v>0.001799625134479897</v>
+        <v>0.004721118644100829</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -692,19 +692,19 @@
         <v>0.02286513801810705</v>
       </c>
       <c r="D12">
-        <v>4445387.015389714</v>
+        <v>4485617.539580474</v>
       </c>
       <c r="E12">
-        <v>287.5917709809168</v>
+        <v>287.9773629073712</v>
       </c>
       <c r="F12">
-        <v>16.48215909057802</v>
+        <v>8.891924790998445</v>
       </c>
       <c r="G12">
-        <v>0.002053613004249776</v>
+        <v>0.003764809294105662</v>
       </c>
       <c r="H12">
-        <v>0.001561995621239777</v>
+        <v>0.004297494762274978</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -718,19 +718,19 @@
         <v>0.02203921724561356</v>
       </c>
       <c r="D13">
-        <v>4421376.592046415</v>
+        <v>4480204.904334273</v>
       </c>
       <c r="E13">
-        <v>287.3603871884911</v>
+        <v>287.9256373682554</v>
       </c>
       <c r="F13">
-        <v>19.771894906541</v>
+        <v>10.27722988670528</v>
       </c>
       <c r="G13">
-        <v>0.001834280090436213</v>
+        <v>0.003477156916449146</v>
       </c>
       <c r="H13">
-        <v>0.001347008483073192</v>
+        <v>0.003868199744364725</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -744,19 +744,19 @@
         <v>0.02121329647312005</v>
       </c>
       <c r="D14">
-        <v>4385427.496948788</v>
+        <v>4472372.355966241</v>
       </c>
       <c r="E14">
-        <v>287.0121785989533</v>
+        <v>287.8507025534057</v>
       </c>
       <c r="F14">
-        <v>24.01122866914344</v>
+        <v>12.07323589222351</v>
       </c>
       <c r="G14">
-        <v>0.001627047502569853</v>
+        <v>0.00317348383973878</v>
       </c>
       <c r="H14">
-        <v>0.001151901911954504</v>
+        <v>0.003435063160929314</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -770,19 +770,19 @@
         <v>0.02038737570062656</v>
       </c>
       <c r="D15">
-        <v>4329757.60064327</v>
+        <v>4460581.390224939</v>
       </c>
       <c r="E15">
-        <v>286.4686939010593</v>
+        <v>287.7377103273069</v>
       </c>
       <c r="F15">
-        <v>29.67890357875835</v>
+        <v>14.49460935743762</v>
       </c>
       <c r="G15">
-        <v>0.001427100329280454</v>
+        <v>0.002848522430674907</v>
       </c>
       <c r="H15">
-        <v>0.0009732518096418261</v>
+        <v>0.002996100228687672</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -796,19 +796,19 @@
         <v>0.01956145492813306</v>
       </c>
       <c r="D16">
-        <v>4239032.554788486</v>
+        <v>4441749.461918081</v>
       </c>
       <c r="E16">
-        <v>285.5716403806056</v>
+        <v>287.5567771678961</v>
       </c>
       <c r="F16">
-        <v>37.82403060256069</v>
+        <v>18.03989698115229</v>
       </c>
       <c r="G16">
-        <v>0.001223848157442328</v>
+        <v>0.002481338418105604</v>
       </c>
       <c r="H16">
-        <v>0.0008046116947123709</v>
+        <v>0.00253589845318474</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -822,19 +822,19 @@
         <v>0.01911027116091851</v>
       </c>
       <c r="D17">
-        <v>4076134.661483259</v>
+        <v>4408005.242785337</v>
       </c>
       <c r="E17">
-        <v>283.9242901044451</v>
+        <v>287.2311197987503</v>
       </c>
       <c r="F17">
-        <v>55.77140905355221</v>
+        <v>27.53723412267134</v>
       </c>
       <c r="G17">
-        <v>0.0008871695166148265</v>
+        <v>0.001717303259068159</v>
       </c>
       <c r="H17">
-        <v>0.0005843209908022175</v>
+        <v>0.001789287348877393</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -848,19 +848,19 @@
         <v>0.02088988309406883</v>
       </c>
       <c r="D18">
-        <v>3562569.479778449</v>
+        <v>4273827.444518375</v>
       </c>
       <c r="E18">
-        <v>278.3881863958325</v>
+        <v>285.9173630487176</v>
       </c>
       <c r="F18">
-        <v>56.79615966072861</v>
+        <v>27.85330976728616</v>
       </c>
       <c r="G18">
-        <v>0.0007938931374026335</v>
+        <v>0.001506940446398405</v>
       </c>
       <c r="H18">
-        <v>0.0006204035028902214</v>
+        <v>0.001835494154326826</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -874,19 +874,19 @@
         <v>0.02266949502721918</v>
       </c>
       <c r="D19">
-        <v>3482742.448528838</v>
+        <v>4261404.796375863</v>
       </c>
       <c r="E19">
-        <v>277.475619567879</v>
+        <v>285.7941740222304</v>
       </c>
       <c r="F19">
-        <v>51.91856848074306</v>
+        <v>25.71135512624252</v>
       </c>
       <c r="G19">
-        <v>0.0007924114716662376</v>
+        <v>0.001471603075520245</v>
       </c>
       <c r="H19">
-        <v>0.0006950640136342677</v>
+        <v>0.002017742692201473</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -900,19 +900,19 @@
         <v>0.02444910696036953</v>
       </c>
       <c r="D20">
-        <v>3546678.443232951</v>
+        <v>4279902.638579682</v>
       </c>
       <c r="E20">
-        <v>278.2077308270634</v>
+        <v>285.9775100254796</v>
       </c>
       <c r="F20">
-        <v>46.42029981017195</v>
+        <v>23.44200232991436</v>
       </c>
       <c r="G20">
-        <v>0.0008143243978610638</v>
+        <v>0.001474294155814378</v>
       </c>
       <c r="H20">
-        <v>0.0007824552404017434</v>
+        <v>0.002236372872411311</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -926,19 +926,19 @@
         <v>0.02622871889351988</v>
       </c>
       <c r="D21">
-        <v>3619323.888773834</v>
+        <v>4298409.896062412</v>
       </c>
       <c r="E21">
-        <v>279.0278819958173</v>
+        <v>286.1603463441003</v>
       </c>
       <c r="F21">
-        <v>41.5857657890859</v>
+        <v>21.41088366660772</v>
       </c>
       <c r="G21">
-        <v>0.0008440631373143284</v>
+        <v>0.001490944032910625</v>
       </c>
       <c r="H21">
-        <v>0.0008786927366491308</v>
+        <v>0.002476216162030311</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -952,19 +952,19 @@
         <v>0.0280083308266702</v>
       </c>
       <c r="D22">
-        <v>3675613.209737322</v>
+        <v>4313243.033166707</v>
       </c>
       <c r="E22">
-        <v>279.6550783527885</v>
+        <v>286.3064599682582</v>
       </c>
       <c r="F22">
-        <v>37.52266752408183</v>
+        <v>19.65568662501942</v>
       </c>
       <c r="G22">
-        <v>0.0008770584150294723</v>
+        <v>0.00151387701476662</v>
       </c>
       <c r="H22">
-        <v>0.0009823798133846184</v>
+        <v>0.002731560851983424</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -978,19 +978,19 @@
         <v>0.02978794275982054</v>
       </c>
       <c r="D23">
-        <v>3716651.472483592</v>
+        <v>4324648.0472227</v>
       </c>
       <c r="E23">
-        <v>280.1078922981255</v>
+        <v>286.4185489097594</v>
       </c>
       <c r="F23">
-        <v>34.1118175583627</v>
+        <v>18.15090074747606</v>
       </c>
       <c r="G23">
-        <v>0.0009117987632374035</v>
+        <v>0.00153970077030164</v>
       </c>
       <c r="H23">
-        <v>0.001092841279055025</v>
+        <v>0.002999428030635581</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1004,19 +1004,19 @@
         <v>0.03156755469297089</v>
       </c>
       <c r="D24">
-        <v>3746609.679617418</v>
+        <v>4333357.339203728</v>
       </c>
       <c r="E24">
-        <v>280.4361250285585</v>
+        <v>286.5039949684863</v>
       </c>
       <c r="F24">
-        <v>31.22582968515646</v>
+        <v>16.8603655124343</v>
       </c>
       <c r="G24">
-        <v>0.0009476526349606955</v>
+        <v>0.001566629745497767</v>
       </c>
       <c r="H24">
-        <v>0.001209689858688494</v>
+        <v>0.003277931595140243</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1030,19 +1030,19 @@
         <v>0.03334716662612121</v>
       </c>
       <c r="D25">
-        <v>3768782.296430608</v>
+        <v>4340029.324986956</v>
       </c>
       <c r="E25">
-        <v>280.6778101975392</v>
+        <v>286.5693660803273</v>
       </c>
       <c r="F25">
-        <v>28.76178107687479</v>
+        <v>15.74996597535596</v>
       </c>
       <c r="G25">
-        <v>0.0009842864842473352</v>
+        <v>0.00159362318683616</v>
       </c>
       <c r="H25">
-        <v>0.001332676285182604</v>
+        <v>0.003565713767135267</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1056,19 +1056,19 @@
         <v>0.03512677855927156</v>
       </c>
       <c r="D26">
-        <v>3785442.729424576</v>
+        <v>4345173.068839589</v>
       </c>
       <c r="E26">
-        <v>280.8587213354973</v>
+        <v>286.6197122406942</v>
       </c>
       <c r="F26">
-        <v>26.63991377803996</v>
+        <v>14.7905196355095</v>
       </c>
       <c r="G26">
-        <v>0.001021497185475097</v>
+        <v>0.001620032984955762</v>
       </c>
       <c r="H26">
-        <v>0.001461626159102144</v>
+        <v>0.00386170806267469</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1082,19 +1082,19 @@
         <v>0.03690639049242189</v>
       </c>
       <c r="D27">
-        <v>3798140.291871773</v>
+        <v>4349166.240868012</v>
       </c>
       <c r="E27">
-        <v>280.9962059713998</v>
+        <v>286.6587659476536</v>
       </c>
       <c r="F27">
-        <v>24.79844261846361</v>
+        <v>13.95788840411186</v>
       </c>
       <c r="G27">
-        <v>0.001059150895445119</v>
+        <v>0.001645437044121459</v>
       </c>
       <c r="H27">
-        <v>0.001596409566505965</v>
+        <v>0.004165025434192116</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1108,19 +1108,19 @@
         <v>0.03868600242557224</v>
       </c>
       <c r="D28">
-        <v>3807942.76857071</v>
+        <v>4352286.214290478</v>
       </c>
       <c r="E28">
-        <v>281.1021114239456</v>
+        <v>286.689260937791</v>
       </c>
       <c r="F28">
-        <v>23.18909102407539</v>
+        <v>13.2323364982597</v>
       </c>
       <c r="G28">
-        <v>0.00109715492488907</v>
+        <v>0.001669552089648645</v>
       </c>
       <c r="H28">
-        <v>0.001736924958617161</v>
+        <v>0.004474893879312136</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1134,19 +1134,19 @@
         <v>0.04046561435872258</v>
       </c>
       <c r="D29">
-        <v>3815597.840414727</v>
+        <v>4354737.027278671</v>
       </c>
       <c r="E29">
-        <v>281.1846763231176</v>
+        <v>286.7132039663194</v>
       </c>
       <c r="F29">
-        <v>21.77373699138506</v>
+        <v>12.59776592119353</v>
       </c>
       <c r="G29">
-        <v>0.001135442794613163</v>
+        <v>0.001692184496369246</v>
       </c>
       <c r="H29">
-        <v>0.001883089926146102</v>
+        <v>0.00479062383696469</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1160,19 +1160,19 @@
         <v>0.04224522629187291</v>
       </c>
       <c r="D30">
-        <v>3821637.593499009</v>
+        <v>4356669.748130793</v>
       </c>
       <c r="E30">
-        <v>281.2497325456474</v>
+        <v>286.7320783990012</v>
       </c>
       <c r="F30">
-        <v>20.52195537477932</v>
+        <v>12.04102200487696</v>
       </c>
       <c r="G30">
-        <v>0.001173965574321076</v>
+        <v>0.001713200892281765</v>
       </c>
       <c r="H30">
-        <v>0.002034835588647792</v>
+        <v>0.005111587080414901</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1186,19 +1186,19 @@
         <v>0.04402483822502326</v>
       </c>
       <c r="D31">
-        <v>3826446.569635886</v>
+        <v>4358197.18240021</v>
       </c>
       <c r="E31">
-        <v>281.3014772900638</v>
+        <v>286.7469904642047</v>
       </c>
       <c r="F31">
-        <v>19.40921702547481</v>
+        <v>11.55131466385689</v>
       </c>
       <c r="G31">
-        <v>0.001212686547634981</v>
+        <v>0.001732509740003881</v>
       </c>
       <c r="H31">
-        <v>0.002192103007144468</v>
+        <v>0.005437203154275915</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1212,19 +1212,19 @@
         <v>0.04580445015817358</v>
       </c>
       <c r="D32">
-        <v>3830306.695807001</v>
+        <v>4359404.343036837</v>
       </c>
       <c r="E32">
-        <v>281.3429775809184</v>
+        <v>286.7587729793574</v>
       </c>
       <c r="F32">
-        <v>18.41555910060696</v>
+        <v>11.11975257840805</v>
       </c>
       <c r="G32">
-        <v>0.00125157776826626</v>
+        <v>0.001750049341743204</v>
       </c>
       <c r="H32">
-        <v>0.002354840791735719</v>
+        <v>0.005766930263261304</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1238,19 +1238,19 @@
         <v>0.04758406209132393</v>
       </c>
       <c r="D33">
-        <v>3833427.42238711</v>
+        <v>4360355.892104086</v>
       </c>
       <c r="E33">
-        <v>281.3765059582456</v>
+        <v>286.7680588659395</v>
       </c>
       <c r="F33">
-        <v>17.52459318869391</v>
+        <v>10.73897365302902</v>
       </c>
       <c r="G33">
-        <v>0.00129061775184943</v>
+        <v>0.001765779770017693</v>
       </c>
       <c r="H33">
-        <v>0.002523003447802754</v>
+        <v>0.006100258911046111</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1264,19 +1264,19 @@
         <v>0.04936367402447427</v>
       </c>
       <c r="D34">
-        <v>3835966.263983103</v>
+        <v>4361101.452504632</v>
       </c>
       <c r="E34">
-        <v>281.4037678004219</v>
+        <v>286.7753335065947</v>
       </c>
       <c r="F34">
-        <v>16.72275733780561</v>
+        <v>10.40285330799668</v>
       </c>
       <c r="G34">
-        <v>0.001329789880540066</v>
+        <v>0.001779677286824377</v>
       </c>
       <c r="H34">
-        <v>0.00269655019667703</v>
+        <v>0.00643670730563572</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1290,19 +1290,19 @@
         <v>0.05114328595762462</v>
       </c>
       <c r="D35">
-        <v>3838043.014808577</v>
+        <v>4361679.426190006</v>
       </c>
       <c r="E35">
-        <v>281.4260578298563</v>
+        <v>286.7809723142838</v>
       </c>
       <c r="F35">
-        <v>15.99874591350827</v>
+        <v>10.10627425070433</v>
       </c>
       <c r="G35">
-        <v>0.001369081271709555</v>
+        <v>0.001791730390167778</v>
       </c>
       <c r="H35">
-        <v>0.002875444111564876</v>
+        <v>0.006775817938782938</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1316,19 +1316,19 @@
         <v>0.05292289789077495</v>
       </c>
       <c r="D36">
-        <v>3839749.729326267</v>
+        <v>4362119.761802351</v>
       </c>
       <c r="E36">
-        <v>281.4443695324328</v>
+        <v>286.7852679253423</v>
       </c>
       <c r="F36">
-        <v>15.34307050942753</v>
+        <v>9.844944344617202</v>
       </c>
       <c r="G36">
-        <v>0.00140848195829612</v>
+        <v>0.001801936953830545</v>
       </c>
       <c r="H36">
-        <v>0.0030596514691536</v>
+        <v>0.007117154969199271</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1342,19 +1342,19 @@
         <v>0.05470250982392529</v>
       </c>
       <c r="D37">
-        <v>3841157.824789534</v>
+        <v>4362445.978632754</v>
       </c>
       <c r="E37">
-        <v>281.4594727536782</v>
+        <v>286.7884500621317</v>
       </c>
       <c r="F37">
-        <v>14.74771848545969</v>
+        <v>9.615252006686804</v>
       </c>
       <c r="G37">
-        <v>0.001447984284044434</v>
+        <v>0.001810302119051188</v>
       </c>
       <c r="H37">
-        <v>0.003249141252657469</v>
+        <v>0.007460302170802551</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1368,19 +1368,19 @@
         <v>0.05648212175707563</v>
       </c>
       <c r="D38">
-        <v>3842323.199571275</v>
+        <v>4362676.659946618</v>
       </c>
       <c r="E38">
-        <v>281.4719694563004</v>
+        <v>286.7907001738268</v>
       </c>
       <c r="F38">
-        <v>14.2058850007023</v>
+        <v>9.414150922064326</v>
       </c>
       <c r="G38">
-        <v>0.001487582450324692</v>
+        <v>0.001816836714186145</v>
       </c>
       <c r="H38">
-        <v>0.003443884763671729</v>
+        <v>0.007804861287631722</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1394,19 +1394,19 @@
         <v>0.05826173369022596</v>
       </c>
       <c r="D39">
-        <v>3843289.965051821</v>
+        <v>4362826.564383106</v>
       </c>
       <c r="E39">
-        <v>281.482334276614</v>
+        <v>286.7921623237943</v>
       </c>
       <c r="F39">
-        <v>13.71176093140745</v>
+        <v>9.239067741693527</v>
       </c>
       <c r="G39">
-        <v>0.001527272172015383</v>
+        <v>0.001821556052028307</v>
       </c>
       <c r="H39">
-        <v>0.003643855313820268</v>
+        <v>0.008150450687705056</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1420,19 +1420,19 @@
         <v>0.0600413456233763</v>
       </c>
       <c r="D40">
-        <v>3844093.196485154</v>
+        <v>4362907.459967121</v>
       </c>
       <c r="E40">
-        <v>281.4909443593575</v>
+        <v>286.7929513539823</v>
       </c>
       <c r="F40">
-        <v>13.26036368927963</v>
+        <v>9.087827885657966</v>
       </c>
       <c r="G40">
-        <v>0.001567050413307075</v>
+        <v>0.001824479001852924</v>
       </c>
       <c r="H40">
-        <v>0.003849027976152104</v>
+        <v>0.008496704241232313</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1446,19 +1446,19 @@
         <v>0.06182095755652664</v>
       </c>
       <c r="D41">
-        <v>3844760.981489335</v>
+        <v>4362928.754811501</v>
       </c>
       <c r="E41">
-        <v>281.4981015369328</v>
+        <v>286.7931590553972</v>
       </c>
       <c r="F41">
-        <v>12.84740127189641</v>
+        <v>8.958595696278914</v>
       </c>
       <c r="G41">
-        <v>0.001606915182783216</v>
+        <v>0.001825627264072266</v>
       </c>
       <c r="H41">
-        <v>0.004059379381541419</v>
+        <v>0.008843270369061006</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1472,19 +1472,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D42">
-        <v>3845315.960079048</v>
+        <v>4362897.977433402</v>
       </c>
       <c r="E42">
-        <v>281.5040489793652</v>
+        <v>286.7928588648869</v>
       </c>
       <c r="F42">
-        <v>12.51014771145389</v>
+        <v>8.865928361464634</v>
       </c>
       <c r="G42">
-        <v>0.001644430127214736</v>
+        <v>0.001824995394933626</v>
       </c>
       <c r="H42">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1498,19 +1498,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D43">
-        <v>3845741.037443511</v>
+        <v>4362826.802878256</v>
       </c>
       <c r="E43">
-        <v>281.5086039023232</v>
+        <v>286.7921646500175</v>
       </c>
       <c r="F43">
-        <v>12.87928545862838</v>
+        <v>9.05381720473174</v>
       </c>
       <c r="G43">
-        <v>0.001641360996549282</v>
+        <v>0.001823082848665206</v>
       </c>
       <c r="H43">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1524,19 +1524,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D44">
-        <v>3844143.942569709</v>
+        <v>4362031.300221232</v>
       </c>
       <c r="E44">
-        <v>281.491488277398</v>
+        <v>286.7844049812059</v>
       </c>
       <c r="F44">
-        <v>13.27487037493452</v>
+        <v>9.25050901129317</v>
       </c>
       <c r="G44">
-        <v>0.001637858351388118</v>
+        <v>0.001821024651317835</v>
       </c>
       <c r="H44">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1550,19 +1550,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D45">
-        <v>3842450.14003476</v>
+        <v>4361205.174444675</v>
       </c>
       <c r="E45">
-        <v>281.4733305118277</v>
+        <v>286.776345476466</v>
       </c>
       <c r="F45">
-        <v>13.69383769263286</v>
+        <v>9.455355971228132</v>
       </c>
       <c r="G45">
-        <v>0.001634359746100847</v>
+        <v>0.001818993077116036</v>
       </c>
       <c r="H45">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1576,19 +1576,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D46">
-        <v>3840666.886377125</v>
+        <v>4360349.73340687</v>
       </c>
       <c r="E46">
-        <v>281.4542074172937</v>
+        <v>286.7679987699238</v>
       </c>
       <c r="F46">
-        <v>14.13827244535902</v>
+        <v>9.668869555621184</v>
       </c>
       <c r="G46">
-        <v>0.001630869040628448</v>
+        <v>0.001816990376354613</v>
       </c>
       <c r="H46">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1602,19 +1602,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D47">
-        <v>3838786.674239528</v>
+        <v>4359463.299231189</v>
       </c>
       <c r="E47">
-        <v>281.4340374504714</v>
+        <v>286.7593483596944</v>
       </c>
       <c r="F47">
-        <v>14.61056420259522</v>
+        <v>9.891610854289155</v>
       </c>
       <c r="G47">
-        <v>0.001627386860454491</v>
+        <v>0.001815018174982218</v>
       </c>
       <c r="H47">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1628,19 +1628,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D48">
-        <v>3836800.967693379</v>
+        <v>4358544.043322096</v>
       </c>
       <c r="E48">
-        <v>281.4127278539858</v>
+        <v>286.7503762579721</v>
       </c>
       <c r="F48">
-        <v>15.11341351548282</v>
+        <v>10.12419083307648</v>
       </c>
       <c r="G48">
-        <v>0.001623913750191648</v>
+        <v>0.001813078186820316</v>
       </c>
       <c r="H48">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1654,19 +1654,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D49">
-        <v>3834700.160850705</v>
+        <v>4357589.983626813</v>
       </c>
       <c r="E49">
-        <v>281.3901741735068</v>
+        <v>286.7410629621758</v>
       </c>
       <c r="F49">
-        <v>15.64988414940617</v>
+        <v>10.36727601478587</v>
       </c>
       <c r="G49">
-        <v>0.001620450170592717</v>
+        <v>0.001811172221842123</v>
       </c>
       <c r="H49">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1680,19 +1680,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D50">
-        <v>3832473.401944818</v>
+        <v>4356598.967779974</v>
       </c>
       <c r="E50">
-        <v>281.36625832325</v>
+        <v>286.7313872880327</v>
       </c>
       <c r="F50">
-        <v>16.22346670349518</v>
+        <v>10.62159498612822</v>
       </c>
       <c r="G50">
-        <v>0.001616996463008819</v>
+        <v>0.001809302191617581</v>
       </c>
       <c r="H50">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -1706,19 +1706,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D51">
-        <v>3830108.379744311</v>
+        <v>4355568.653865043</v>
       </c>
       <c r="E51">
-        <v>281.3408462352944</v>
+        <v>286.721326179003</v>
       </c>
       <c r="F51">
-        <v>16.83815617047246</v>
+        <v>10.88794584624938</v>
       </c>
       <c r="G51">
-        <v>0.001613552802885284</v>
+        <v>0.001807470114922459</v>
       </c>
       <c r="H51">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1732,19 +1732,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D52">
-        <v>3827591.063760823</v>
+        <v>4354496.488457861</v>
       </c>
       <c r="E52">
-        <v>281.3137849974523</v>
+        <v>286.7108544887</v>
       </c>
       <c r="F52">
-        <v>17.49854714742868</v>
+        <v>11.16720476020864</v>
       </c>
       <c r="G52">
-        <v>0.001610119139328258</v>
+        <v>0.001805678123484401</v>
       </c>
       <c r="H52">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -1758,19 +1758,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D53">
-        <v>3824905.386040103</v>
+        <v>4353379.681488375</v>
       </c>
       <c r="E53">
-        <v>281.2848993437679</v>
+        <v>286.699944731682</v>
       </c>
       <c r="F53">
-        <v>18.20995159239639</v>
+        <v>11.46033581422986</v>
       </c>
       <c r="G53">
-        <v>0.001606695116330795</v>
+        <v>0.00180392846780731</v>
       </c>
       <c r="H53">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -1784,19 +1784,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D54">
-        <v>3822032.848445782</v>
+        <v>4352215.177362773</v>
       </c>
       <c r="E54">
-        <v>281.2539873182859</v>
+        <v>286.688566797057</v>
       </c>
       <c r="F54">
-        <v>18.97854564254785</v>
+        <v>11.76840241077179</v>
       </c>
       <c r="G54">
-        <v>0.001603279969800154</v>
+        <v>0.001802223522991898</v>
       </c>
       <c r="H54">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -1810,19 +1810,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D55">
-        <v>3818952.034034324</v>
+        <v>4350999.621672702</v>
       </c>
       <c r="E55">
-        <v>281.2208148731968</v>
+        <v>286.6766876181819</v>
       </c>
       <c r="F55">
-        <v>19.81155426420715</v>
+        <v>12.09258049268191</v>
       </c>
       <c r="G55">
-        <v>0.001599872392418161</v>
+        <v>0.001800565794439567</v>
       </c>
       <c r="H55">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -1836,19 +1836,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D56">
-        <v>3815637.993735922</v>
+        <v>4349729.322674938</v>
       </c>
       <c r="E56">
-        <v>281.1851090795342</v>
+        <v>286.6642707903082</v>
       </c>
       <c r="F56">
-        <v>20.71748567970026</v>
+        <v>12.43417394968119</v>
       </c>
       <c r="G56">
-        <v>0.001596470355413747</v>
+        <v>0.001798957923285972</v>
       </c>
       <c r="H56">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -1862,19 +1862,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D57">
-        <v>3812061.469159165</v>
+        <v>4348400.206546118</v>
       </c>
       <c r="E57">
-        <v>281.1465495116441</v>
+        <v>286.6512761262346</v>
       </c>
       <c r="F57">
-        <v>21.70643205062357</v>
+        <v>12.79463264081792</v>
       </c>
       <c r="G57">
-        <v>0.001593070872122944</v>
+        <v>0.001797402691357539</v>
       </c>
       <c r="H57">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -1888,19 +1888,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D58">
-        <v>3808187.897487967</v>
+        <v>4347007.76519287</v>
       </c>
       <c r="E58">
-        <v>281.1047571992738</v>
+        <v>286.63765913778</v>
       </c>
       <c r="F58">
-        <v>22.7904594734484</v>
+        <v>13.17557356814211</v>
       </c>
       <c r="G58">
-        <v>0.001589669682149182</v>
+        <v>0.001795903025373916</v>
       </c>
       <c r="H58">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -1914,19 +1914,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D59">
-        <v>3803976.12290054</v>
+        <v>4345546.995114657</v>
       </c>
       <c r="E59">
-        <v>281.0592802978697</v>
+        <v>286.6233704280569</v>
       </c>
       <c r="F59">
-        <v>23.98412004130211</v>
+        <v>13.57880586611691</v>
       </c>
       <c r="G59">
-        <v>0.001586260826067106</v>
+        <v>0.001794462000026639</v>
       </c>
       <c r="H59">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -1940,19 +1940,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D60">
-        <v>3799376.707167951</v>
+        <v>4344012.325457009</v>
       </c>
       <c r="E60">
-        <v>281.0095752680367</v>
+        <v>286.6083549759144</v>
       </c>
       <c r="F60">
-        <v>25.30513329116265</v>
+        <v>14.00636043682867</v>
       </c>
       <c r="G60">
-        <v>0.001582836067432115</v>
+        <v>0.001793082839441538</v>
       </c>
       <c r="H60">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -1966,19 +1966,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D61">
-        <v>3794329.684346064</v>
+        <v>4342397.532933048</v>
       </c>
       <c r="E61">
-        <v>280.9549818134206</v>
+        <v>286.5925512893083</v>
       </c>
       <c r="F61">
-        <v>26.77530667731174</v>
+        <v>14.46052527458457</v>
       </c>
       <c r="G61">
-        <v>0.001579384098924639</v>
+        <v>0.001791768916369509</v>
       </c>
       <c r="H61">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -1992,19 +1992,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D62">
-        <v>3788761.531253209</v>
+        <v>4340695.640698818</v>
       </c>
       <c r="E62">
-        <v>281.796250485005</v>
+        <v>286.5758903984056</v>
       </c>
       <c r="F62">
-        <v>28.34747705913678</v>
+        <v>14.94388780098478</v>
       </c>
       <c r="G62">
-        <v>0.001551881604143266</v>
+        <v>0.001790523748232359</v>
       </c>
       <c r="H62">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2018,19 +2018,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D63">
-        <v>3782692.995204248</v>
+        <v>4338898.797499117</v>
       </c>
       <c r="E63">
-        <v>282.6646644423092</v>
+        <v>286.5582946515005</v>
       </c>
       <c r="F63">
-        <v>29.21913380828811</v>
+        <v>15.45938589508852</v>
       </c>
       <c r="G63">
-        <v>0.001527459794810484</v>
+        <v>0.001789350988858945</v>
       </c>
       <c r="H63">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2044,19 +2044,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D64">
-        <v>3778602.335788406</v>
+        <v>4336998.13239468</v>
       </c>
       <c r="E64">
-        <v>283.5598583379592</v>
+        <v>286.5396762667039</v>
       </c>
       <c r="F64">
-        <v>30.05667667691423</v>
+        <v>16.01036978360543</v>
       </c>
       <c r="G64">
-        <v>0.001504831898861178</v>
+        <v>0.001788254414353201</v>
       </c>
       <c r="H64">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2070,19 +2070,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D65">
-        <v>3774493.2391426</v>
+        <v>4334983.579054016</v>
       </c>
       <c r="E65">
-        <v>284.4802548834756</v>
+        <v>286.5199355789989</v>
       </c>
       <c r="F65">
-        <v>30.8997340083142</v>
+        <v>16.60067759643832</v>
       </c>
       <c r="G65">
-        <v>0.001483192473640295</v>
+        <v>0.001787237901002102</v>
       </c>
       <c r="H65">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2096,19 +2096,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D66">
-        <v>3770242.195641362</v>
+        <v>4332843.661825371</v>
       </c>
       <c r="E66">
-        <v>285.4252677992795</v>
+        <v>286.498958904438</v>
       </c>
       <c r="F66">
-        <v>31.75093261202746</v>
+        <v>17.23472825504001</v>
       </c>
       <c r="G66">
-        <v>0.001462431731425706</v>
+        <v>0.001786305392402683</v>
       </c>
       <c r="H66">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -2122,19 +2122,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D67">
-        <v>3765837.930797995</v>
+        <v>4330565.233426728</v>
       </c>
       <c r="E67">
-        <v>286.3943543072576</v>
+        <v>286.4766159192739</v>
       </c>
       <c r="F67">
-        <v>32.61070207641954</v>
+        <v>17.91763653382058</v>
       </c>
       <c r="G67">
-        <v>0.001442484192970071</v>
+        <v>0.00178546085198421</v>
       </c>
       <c r="H67">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2148,19 +2148,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D68">
-        <v>3761275.818786754</v>
+        <v>4328133.150860772</v>
       </c>
       <c r="E68">
-        <v>287.3869624045008</v>
+        <v>286.4527564191868</v>
       </c>
       <c r="F68">
-        <v>33.47934963302851</v>
+        <v>18.65535674804286</v>
       </c>
       <c r="G68">
-        <v>0.001423292151482247</v>
+        <v>0.001784708195709708</v>
       </c>
       <c r="H68">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -2174,19 +2174,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D69">
-        <v>3756551.487247796</v>
+        <v>4325529.871721403</v>
       </c>
       <c r="E69">
-        <v>288.4025296592851</v>
+        <v>286.4272062788764</v>
       </c>
       <c r="F69">
-        <v>34.35718760613661</v>
+        <v>19.45486376742619</v>
       </c>
       <c r="G69">
-        <v>0.001404802985312798</v>
+        <v>0.001784051197791725</v>
       </c>
       <c r="H69">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2200,19 +2200,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D70">
-        <v>3751660.412022651</v>
+        <v>4322734.946881829</v>
       </c>
       <c r="E70">
-        <v>289.440485031562</v>
+        <v>286.3997623697662</v>
       </c>
       <c r="F70">
-        <v>35.24454346116372</v>
+        <v>20.32438322182518</v>
       </c>
       <c r="G70">
-        <v>0.001386968465041448</v>
+        <v>0.001783493359499608</v>
       </c>
       <c r="H70">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2226,19 +2226,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D71">
-        <v>3746597.877139918</v>
+        <v>4319724.376849907</v>
       </c>
       <c r="E71">
-        <v>290.5002508762188</v>
+        <v>287.0676118382531</v>
       </c>
       <c r="F71">
-        <v>36.14176273495863</v>
+        <v>21.19492851419065</v>
       </c>
       <c r="G71">
-        <v>0.001369744246799264</v>
+        <v>0.001753751037074774</v>
       </c>
       <c r="H71">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -2252,19 +2252,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D72">
-        <v>3741358.956068951</v>
+        <v>4316615.617894707</v>
       </c>
       <c r="E72">
-        <v>291.5812449378083</v>
+        <v>287.7578361669448</v>
       </c>
       <c r="F72">
-        <v>37.04921121595761</v>
+        <v>21.81023084256069</v>
       </c>
       <c r="G72">
-        <v>0.00135308945136181</v>
+        <v>0.001725793008542144</v>
       </c>
       <c r="H72">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2278,19 +2278,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D73">
-        <v>3735938.494240512</v>
+        <v>4314110.072184375</v>
       </c>
       <c r="E73">
-        <v>292.6828823032008</v>
+        <v>288.4701254115243</v>
       </c>
       <c r="F73">
-        <v>37.96727693000761</v>
+        <v>22.41980637627957</v>
       </c>
       <c r="G73">
-        <v>0.001336966304616664</v>
+        <v>0.00169935845331911</v>
       </c>
       <c r="H73">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2304,19 +2304,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D74">
-        <v>3730331.091106815</v>
+        <v>4311544.625136264</v>
       </c>
       <c r="E74">
-        <v>293.8045772900005</v>
+        <v>289.2038324364225</v>
       </c>
       <c r="F74">
-        <v>38.8963719749442</v>
+        <v>23.03421294261776</v>
       </c>
       <c r="G74">
-        <v>0.001321339829360871</v>
+        <v>0.001674026061172838</v>
       </c>
       <c r="H74">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -2330,19 +2330,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D75">
-        <v>3724531.08165183</v>
+        <v>4308888.972564092</v>
       </c>
       <c r="E75">
-        <v>294.9457452521855</v>
+        <v>289.958618561601</v>
       </c>
       <c r="F75">
-        <v>39.83693423799075</v>
+        <v>23.65408832883999</v>
       </c>
       <c r="G75">
-        <v>0.001306177579697346</v>
+        <v>0.001649701278702568</v>
       </c>
       <c r="H75">
-        <v>0.004262571633766798</v>
+        <v>0.009170233837628798</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -2356,19 +2356,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D76">
-        <v>3718532.517274352</v>
+        <v>4306139.428236136</v>
       </c>
       <c r="E76">
-        <v>296.1058042875183</v>
+        <v>290.7341463717214</v>
       </c>
       <c r="F76">
-        <v>40.78942902975658</v>
+        <v>24.27965432702783</v>
       </c>
       <c r="G76">
-        <v>0.001291449410859206</v>
+        <v>0.001626309905593047</v>
       </c>
       <c r="H76">
-        <v>0.004262571633766793</v>
+        <v>0.00917023383762881</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -2382,19 +2382,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D77">
-        <v>3712329.145949263</v>
+        <v>4303293.358609101</v>
       </c>
       <c r="E77">
-        <v>297.2841768343802</v>
+        <v>291.5300680771124</v>
       </c>
       <c r="F77">
-        <v>41.75435066877403</v>
+        <v>24.91111444280907</v>
       </c>
       <c r="G77">
-        <v>0.001277127278560003</v>
+        <v>0.00160378524951626</v>
       </c>
       <c r="H77">
-        <v>0.004262571633766793</v>
+        <v>0.00917023383762881</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -2408,19 +2408,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D78">
-        <v>3705914.391553654</v>
+        <v>4300348.095064798</v>
       </c>
       <c r="E78">
-        <v>298.4802911487461</v>
+        <v>292.3460259083091</v>
       </c>
       <c r="F78">
-        <v>42.73222405060929</v>
+        <v>25.54867226370813</v>
       </c>
       <c r="G78">
-        <v>0.00126318506300832</v>
+        <v>0.001582066778963971</v>
       </c>
       <c r="H78">
-        <v>0.004262571633766793</v>
+        <v>0.00917023383762881</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -2434,19 +2434,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D79">
-        <v>3699281.332225536</v>
+        <v>4297300.881018923</v>
       </c>
       <c r="E79">
-        <v>299.6935826549305</v>
+        <v>293.1816530423749</v>
       </c>
       <c r="F79">
-        <v>43.7236062355973</v>
+        <v>26.19253385003498</v>
       </c>
       <c r="G79">
-        <v>0.001249598413581471</v>
+        <v>0.001561099350429316</v>
       </c>
       <c r="H79">
-        <v>0.004262571633766793</v>
+        <v>0.00917023383762881</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -2460,19 +2460,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D80">
-        <v>3692422.67760398</v>
+        <v>4294148.862576202</v>
       </c>
       <c r="E80">
-        <v>300.9234951664581</v>
+        <v>294.0365745870172</v>
       </c>
       <c r="F80">
-        <v>44.72908808923681</v>
+        <v>26.84290928152634</v>
       </c>
       <c r="G80">
-        <v>0.001236344610859222</v>
+        <v>0.001540832568380568</v>
       </c>
       <c r="H80">
-        <v>0.004262571633766793</v>
+        <v>0.00917023383762881</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -2486,19 +2486,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D81">
-        <v>3685330.74478032</v>
+        <v>4290889.080880358</v>
       </c>
       <c r="E81">
-        <v>302.16948197588</v>
+        <v>294.9104085903607</v>
       </c>
       <c r="F81">
-        <v>45.74929600930663</v>
+        <v>27.50001407087104</v>
       </c>
       <c r="G81">
-        <v>0.001223402443301324</v>
+        <v>0.00152122023849114</v>
       </c>
       <c r="H81">
-        <v>0.004262571633766793</v>
+        <v>0.00917023383762881</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -2512,19 +2512,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D82">
-        <v>3677997.432770327</v>
+        <v>4287518.464189363</v>
       </c>
       <c r="E82">
-        <v>303.4310068145433</v>
+        <v>295.8027670673696</v>
       </c>
       <c r="F82">
-        <v>46.78489377390964</v>
+        <v>28.16407046328581</v>
       </c>
       <c r="G82">
-        <v>0.001210752096334052</v>
+        <v>0.001502219899585149</v>
       </c>
       <c r="H82">
-        <v>0.004262571633766793</v>
+        <v>0.00917023383762881</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -2538,19 +2538,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D83">
-        <v>3670414.195296539</v>
+        <v>4284033.81965528</v>
       </c>
       <c r="E83">
-        <v>304.707544685206</v>
+        <v>296.7132570328204</v>
       </c>
       <c r="F83">
-        <v>47.8365845450049</v>
+        <v>28.83530863930292</v>
       </c>
       <c r="G83">
-        <v>0.001198375052007949</v>
+        <v>0.001483792421308333</v>
       </c>
       <c r="H83">
-        <v>0.004262571633766793</v>
+        <v>0.00917023383762881</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -2564,19 +2564,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D84">
-        <v>3662572.011647788</v>
+        <v>4280431.824784954</v>
       </c>
       <c r="E84">
-        <v>305.9985825719721</v>
+        <v>297.6414815313926</v>
       </c>
       <c r="F84">
-        <v>48.90511306264752</v>
+        <v>29.51396783302144</v>
       </c>
       <c r="G84">
-        <v>0.001186253997716107</v>
+        <v>0.001465901657057661</v>
       </c>
       <c r="H84">
-        <v>0.004262571633766793</v>
+        <v>0.00917023383762881</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -2590,19 +2590,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D85">
-        <v>3654461.355358742</v>
+        <v>4276709.018565874</v>
       </c>
       <c r="E85">
-        <v>307.3036200332972</v>
+        <v>298.587040655941</v>
       </c>
       <c r="F85">
-        <v>49.99126806621826</v>
+        <v>30.20029737738794</v>
       </c>
       <c r="G85">
-        <v>0.001174372742731111</v>
+        <v>0.001448514143511105</v>
       </c>
       <c r="H85">
-        <v>0.004262571633766793</v>
+        <v>0.00917023383762881</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -2616,19 +2616,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D86">
-        <v>3646072.160425389</v>
+        <v>4272861.792237624</v>
       </c>
       <c r="E86">
-        <v>308.622169684812</v>
+        <v>299.5495325456415</v>
       </c>
       <c r="F86">
-        <v>51.09588498049285</v>
+        <v>30.89455768776321</v>
       </c>
       <c r="G86">
-        <v>0.001162716141539114</v>
+        <v>0.00143159883956268</v>
       </c>
       <c r="H86">
-        <v>0.004262571633766793</v>
+        <v>0.00917023383762881</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -2642,19 +2642,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D87">
-        <v>3637393.784742016</v>
+        <v>4268886.379684529</v>
       </c>
       <c r="E87">
-        <v>309.9537575794361</v>
+        <v>300.5285543564523</v>
       </c>
       <c r="F87">
-        <v>52.2198489065836</v>
+        <v>31.59702119486484</v>
       </c>
       <c r="G87">
-        <v>0.001151270023129454</v>
+        <v>0.00141512689866226</v>
       </c>
       <c r="H87">
-        <v>0.004262571633766793</v>
+        <v>0.00917023383762881</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -2668,19 +2668,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D88">
-        <v>3628414.970410599</v>
+        <v>4264778.847419865</v>
       </c>
       <c r="E88">
-        <v>311.2979234927486</v>
+        <v>301.5237031971642</v>
       </c>
       <c r="F88">
-        <v>53.36409796069928</v>
+        <v>32.30797323810082</v>
       </c>
       <c r="G88">
-        <v>0.001140021125544765</v>
+        <v>0.001399071469539919</v>
       </c>
       <c r="H88">
-        <v>0.004262571633766793</v>
+        <v>0.00917023383762881</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -2694,19 +2694,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D89">
-        <v>3619123.800533542</v>
+        <v>4260535.084126486</v>
       </c>
       <c r="E89">
-        <v>312.6542211218552</v>
+        <v>302.5345770252043</v>
       </c>
       <c r="F89">
-        <v>54.52962700744058</v>
+        <v>33.02771293028721</v>
       </c>
       <c r="G89">
-        <v>0.001128957035115267</v>
+        <v>0.001383407521103372</v>
       </c>
       <c r="H89">
-        <v>0.004262571633766793</v>
+        <v>0.00917023383762881</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -2720,19 +2720,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D90">
-        <v>3609507.652054424</v>
+        <v>4256150.789712932</v>
       </c>
       <c r="E90">
-        <v>314.0222182060902</v>
+        <v>303.5607754972817</v>
       </c>
       <c r="F90">
-        <v>55.7174918391236</v>
+        <v>33.75655400475366</v>
       </c>
       <c r="G90">
-        <v>0.001118066129896864</v>
+        <v>0.001368111687967555</v>
       </c>
       <c r="H90">
-        <v>0.004262571633766793</v>
+        <v>0.00917023383762881</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -2746,19 +2746,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D91">
-        <v>3599553.144157321</v>
+        <v>4251621.463838059</v>
       </c>
       <c r="E91">
-        <v>315.4014965778363</v>
+        <v>304.6019007708916</v>
       </c>
       <c r="F91">
-        <v>56.92881385856984</v>
+        <v>34.49482565586715</v>
       </c>
       <c r="G91">
-        <v>0.001107337526909807</v>
+        <v>0.001353162133633578</v>
       </c>
       <c r="H91">
-        <v>0.004262571633766793</v>
+        <v>0.00917023383762881</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -2772,19 +2772,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D92">
-        <v>3589246.08167209</v>
+        <v>4246942.393850964</v>
       </c>
       <c r="E92">
-        <v>316.7916521515638</v>
+        <v>305.657558253612</v>
       </c>
       <c r="F92">
-        <v>58.16478533011526</v>
+        <v>35.24287338404872</v>
       </c>
       <c r="G92">
-        <v>0.001096761032836487</v>
+        <v>0.001338538428800535</v>
       </c>
       <c r="H92">
-        <v>0.004262571633766793</v>
+        <v>0.00917023383762881</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -2798,19 +2798,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D93">
-        <v>3578571.392858681</v>
+        <v>4242108.642086448</v>
       </c>
       <c r="E93">
-        <v>318.1922948589142</v>
+        <v>306.7273572980037</v>
       </c>
       <c r="F93">
-        <v>59.42667527251594</v>
+        <v>36.00105985641289</v>
       </c>
       <c r="G93">
-        <v>0.0010863270978862</v>
+        <v>0.001324221442684548</v>
       </c>
       <c r="H93">
-        <v>0.004262571633766793</v>
+        <v>0.00917023383762881</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Critical Mass Flow Rate Estimation
</commit_message>
<xml_diff>
--- a/TheEngine/Regen Solver/enginefiles/solverdata.xlsx
+++ b/TheEngine/Regen Solver/enginefiles/solverdata.xlsx
@@ -438,13 +438,13 @@
         <v>288.1145796254294</v>
       </c>
       <c r="F2">
-        <v>3.651755013093158</v>
+        <v>3.951000445503544</v>
       </c>
       <c r="G2">
-        <v>0.005572264599657401</v>
+        <v>0.005150225991302586</v>
       </c>
       <c r="H2">
-        <v>0.007615357616818812</v>
+        <v>0.004889619209503845</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -458,19 +458,19 @@
         <v>0.03029842497054849</v>
       </c>
       <c r="D3">
-        <v>4499950.209224804</v>
+        <v>4499938.741724721</v>
       </c>
       <c r="E3">
-        <v>288.1141051648649</v>
+        <v>288.1139958895124</v>
       </c>
       <c r="F3">
-        <v>3.853902650776024</v>
+        <v>4.17049484526296</v>
       </c>
       <c r="G3">
-        <v>0.005499567600562982</v>
+        <v>0.005082084374084406</v>
       </c>
       <c r="H3">
-        <v>0.007423287372138057</v>
+        <v>0.004766072315499016</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -484,19 +484,19 @@
         <v>0.029472504198055</v>
       </c>
       <c r="D4">
-        <v>4499470.329730766</v>
+        <v>4499371.753992386</v>
       </c>
       <c r="E4">
-        <v>288.1095321488901</v>
+        <v>288.1085927249239</v>
       </c>
       <c r="F4">
-        <v>4.094194974781712</v>
+        <v>4.429616803339078</v>
       </c>
       <c r="G4">
-        <v>0.005400488435281656</v>
+        <v>0.004991567043722514</v>
       </c>
       <c r="H4">
-        <v>0.007190997836826019</v>
+        <v>0.004617598523249564</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -510,19 +510,19 @@
         <v>0.02864658342556152</v>
       </c>
       <c r="D5">
-        <v>4498873.259099169</v>
+        <v>4498671.082200786</v>
       </c>
       <c r="E5">
-        <v>288.1038418449287</v>
+        <v>288.1019148951242</v>
       </c>
       <c r="F5">
-        <v>4.379741655047277</v>
+        <v>4.735641093493563</v>
       </c>
       <c r="G5">
-        <v>0.005275387456556131</v>
+        <v>0.004878959002764082</v>
       </c>
       <c r="H5">
-        <v>0.00692114894990719</v>
+        <v>0.004445826539184793</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -536,19 +536,19 @@
         <v>0.02782066265306801</v>
       </c>
       <c r="D6">
-        <v>4498124.226081409</v>
+        <v>4497797.915245974</v>
       </c>
       <c r="E6">
-        <v>288.0967024771016</v>
+        <v>288.0935919823681</v>
       </c>
       <c r="F6">
-        <v>4.719721488883242</v>
+        <v>5.09799019945835</v>
       </c>
       <c r="G6">
-        <v>0.005124862610490295</v>
+        <v>0.004744654626704549</v>
       </c>
       <c r="H6">
-        <v>0.006616945396397372</v>
+        <v>0.004252698601489258</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -562,19 +562,19 @@
         <v>0.02699474188057452</v>
       </c>
       <c r="D7">
-        <v>4497174.706004631</v>
+        <v>4496698.260228595</v>
       </c>
       <c r="E7">
-        <v>288.0876508878874</v>
+        <v>288.0831084800097</v>
       </c>
       <c r="F7">
-        <v>5.125838090180885</v>
+        <v>5.528652061859373</v>
       </c>
       <c r="G7">
-        <v>0.004949922385933965</v>
+        <v>0.00458935162565802</v>
       </c>
       <c r="H7">
-        <v>0.006282077221116508</v>
+        <v>0.004040437763912341</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -588,19 +588,19 @@
         <v>0.02616882110808103</v>
       </c>
       <c r="D8">
-        <v>4495956.605246617</v>
+        <v>4495296.765808728</v>
       </c>
       <c r="E8">
-        <v>288.0760368592772</v>
+        <v>288.0697446031033</v>
       </c>
       <c r="F8">
-        <v>5.613202947475396</v>
+        <v>6.043073763125285</v>
       </c>
       <c r="G8">
-        <v>0.004751945729213477</v>
+        <v>0.004414021882111358</v>
       </c>
       <c r="H8">
-        <v>0.005920634283267094</v>
+        <v>0.003811500253523136</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -614,19 +614,19 @@
         <v>0.02534290033558753</v>
       </c>
       <c r="D9">
-        <v>4494372.68470552</v>
+        <v>4493486.423048829</v>
       </c>
       <c r="E9">
-        <v>288.0609313557791</v>
+        <v>288.0524775194562</v>
       </c>
       <c r="F9">
-        <v>6.201627251113021</v>
+        <v>6.661468557920183</v>
       </c>
       <c r="G9">
-        <v>0.00453260907977424</v>
+        <v>0.004219855930684975</v>
       </c>
       <c r="H9">
-        <v>0.005536992342578199</v>
+        <v>0.003568511051010036</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -640,19 +640,19 @@
         <v>0.02451697956309404</v>
       </c>
       <c r="D10">
-        <v>4492281.267137013</v>
+        <v>4491112.186328761</v>
       </c>
       <c r="E10">
-        <v>288.0409798086959</v>
+        <v>288.0298240458173</v>
       </c>
       <c r="F10">
-        <v>6.917578341048428</v>
+        <v>7.410794714743556</v>
       </c>
       <c r="G10">
-        <v>0.004293771910173346</v>
+        <v>0.004008172231957837</v>
       </c>
       <c r="H10">
-        <v>0.00513566622364592</v>
+        <v>0.003314179163871476</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -666,19 +666,19 @@
         <v>0.02369105879060053</v>
       </c>
       <c r="D11">
-        <v>4489471.007782832</v>
+        <v>4487944.059974287</v>
       </c>
       <c r="E11">
-        <v>288.0141596696402</v>
+        <v>287.9995816986361</v>
       </c>
       <c r="F11">
-        <v>7.797279292727093</v>
+        <v>8.327889598298002</v>
       </c>
       <c r="G11">
-        <v>0.004037303300267244</v>
+        <v>0.003780273561572748</v>
       </c>
       <c r="H11">
-        <v>0.004721118644100829</v>
+        <v>0.003051184505410432</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -692,19 +692,19 @@
         <v>0.02286513801810705</v>
       </c>
       <c r="D12">
-        <v>4485617.539580474</v>
+        <v>4483631.028698791</v>
       </c>
       <c r="E12">
-        <v>287.9773629073712</v>
+        <v>287.9583844013953</v>
       </c>
       <c r="F12">
-        <v>8.891924790998445</v>
+        <v>9.464741728828674</v>
       </c>
       <c r="G12">
-        <v>0.003764809294105662</v>
+        <v>0.003537211056516205</v>
       </c>
       <c r="H12">
-        <v>0.004297494762274978</v>
+        <v>0.002782016241311469</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -718,19 +718,19 @@
         <v>0.02203921724561356</v>
       </c>
       <c r="D13">
-        <v>4480204.904334273</v>
+        <v>4477617.879274815</v>
       </c>
       <c r="E13">
-        <v>287.9256373682554</v>
+        <v>287.9008979616783</v>
       </c>
       <c r="F13">
-        <v>10.27722988670528</v>
+        <v>10.89813793118175</v>
       </c>
       <c r="G13">
-        <v>0.003477156916449146</v>
+        <v>0.003279356182438713</v>
       </c>
       <c r="H13">
-        <v>0.003868199744364725</v>
+        <v>0.00250870838128259</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -744,19 +744,19 @@
         <v>0.02121329647312005</v>
       </c>
       <c r="D14">
-        <v>4472372.355966241</v>
+        <v>4468983.592583368</v>
       </c>
       <c r="E14">
-        <v>287.8507025534057</v>
+        <v>287.818251225561</v>
       </c>
       <c r="F14">
-        <v>12.07323589222351</v>
+        <v>12.74965995401138</v>
       </c>
       <c r="G14">
-        <v>0.00317348383973878</v>
+        <v>0.003005486380406337</v>
       </c>
       <c r="H14">
-        <v>0.003435063160929314</v>
+        <v>0.002232306255318037</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -770,19 +770,19 @@
         <v>0.02038737570062656</v>
       </c>
       <c r="D15">
-        <v>4460581.390224939</v>
+        <v>4456091.290623012</v>
       </c>
       <c r="E15">
-        <v>287.7377103273069</v>
+        <v>287.6946227382366</v>
       </c>
       <c r="F15">
-        <v>14.49460935743762</v>
+        <v>15.23641694306266</v>
       </c>
       <c r="G15">
-        <v>0.002848522430674907</v>
+        <v>0.002710282523922772</v>
       </c>
       <c r="H15">
-        <v>0.002996100228687672</v>
+        <v>0.001951423350163182</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -796,19 +796,19 @@
         <v>0.01956145492813306</v>
       </c>
       <c r="D16">
-        <v>4441749.461918081</v>
+        <v>4435680.565209452</v>
       </c>
       <c r="E16">
-        <v>287.5567771678961</v>
+        <v>287.4983453907358</v>
       </c>
       <c r="F16">
-        <v>18.03989698115229</v>
+        <v>18.86164606616117</v>
       </c>
       <c r="G16">
-        <v>0.002481338418105604</v>
+        <v>0.002373765043902406</v>
       </c>
       <c r="H16">
-        <v>0.00253589845318474</v>
+        <v>0.001656029482811165</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -822,19 +822,19 @@
         <v>0.01911027116091851</v>
       </c>
       <c r="D17">
-        <v>4408005.242785337</v>
+        <v>4399479.825951125</v>
       </c>
       <c r="E17">
-        <v>287.2311197987503</v>
+        <v>287.1485463326395</v>
       </c>
       <c r="F17">
-        <v>27.53723412267134</v>
+        <v>28.45681500088225</v>
       </c>
       <c r="G17">
-        <v>0.001717303259068159</v>
+        <v>0.001662339609194077</v>
       </c>
       <c r="H17">
-        <v>0.001789287348877393</v>
+        <v>0.001174978530569183</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -848,19 +848,19 @@
         <v>0.02088988309406883</v>
       </c>
       <c r="D18">
-        <v>4273827.444518375</v>
+        <v>4259052.212008365</v>
       </c>
       <c r="E18">
-        <v>285.9173630487176</v>
+        <v>285.7708143805087</v>
       </c>
       <c r="F18">
-        <v>27.85330976728616</v>
+        <v>28.74624208756715</v>
       </c>
       <c r="G18">
-        <v>0.001506940446398405</v>
+        <v>0.001460978596209525</v>
       </c>
       <c r="H18">
-        <v>0.001835494154326826</v>
+        <v>0.001206409092976211</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -874,19 +874,19 @@
         <v>0.02266949502721918</v>
       </c>
       <c r="D19">
-        <v>4261404.796375863</v>
+        <v>4246110.789659574</v>
       </c>
       <c r="E19">
-        <v>285.7941740222304</v>
+        <v>285.6421414605923</v>
       </c>
       <c r="F19">
-        <v>25.71135512624252</v>
+        <v>26.54363188101098</v>
       </c>
       <c r="G19">
-        <v>0.001471603075520245</v>
+        <v>0.001426328783665248</v>
       </c>
       <c r="H19">
-        <v>0.002017742692201473</v>
+        <v>0.001325957687250003</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -900,19 +900,19 @@
         <v>0.02444910696036953</v>
       </c>
       <c r="D20">
-        <v>4279902.638579682</v>
+        <v>4265522.900215349</v>
       </c>
       <c r="E20">
-        <v>285.9775100254796</v>
+        <v>285.8350409016894</v>
       </c>
       <c r="F20">
-        <v>23.44200232991436</v>
+        <v>24.21461221557877</v>
       </c>
       <c r="G20">
-        <v>0.001474294155814378</v>
+        <v>0.001428074571813216</v>
       </c>
       <c r="H20">
-        <v>0.002236372872411311</v>
+        <v>0.001469063650235908</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -926,19 +926,19 @@
         <v>0.02622871889351988</v>
       </c>
       <c r="D21">
-        <v>4298409.896062412</v>
+        <v>4284941.024391057</v>
       </c>
       <c r="E21">
-        <v>286.1603463441003</v>
+        <v>286.0273436744911</v>
       </c>
       <c r="F21">
-        <v>21.41088366660772</v>
+        <v>22.13284682281619</v>
       </c>
       <c r="G21">
-        <v>0.001490944032910625</v>
+        <v>0.001443089656994752</v>
       </c>
       <c r="H21">
-        <v>0.002476216162030311</v>
+        <v>0.001625869071621931</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -952,19 +952,19 @@
         <v>0.0280083308266702</v>
       </c>
       <c r="D22">
-        <v>4313243.033166707</v>
+        <v>4300482.221840494</v>
       </c>
       <c r="E22">
-        <v>286.3064599682582</v>
+        <v>286.1807824532439</v>
       </c>
       <c r="F22">
-        <v>19.65568662501942</v>
+        <v>20.33531917584564</v>
       </c>
       <c r="G22">
-        <v>0.00151387701476662</v>
+        <v>0.001464034184377028</v>
       </c>
       <c r="H22">
-        <v>0.002731560851983424</v>
+        <v>0.001792655008752646</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -978,19 +978,19 @@
         <v>0.02978794275982054</v>
       </c>
       <c r="D23">
-        <v>4324648.0472227</v>
+        <v>4312416.591316001</v>
       </c>
       <c r="E23">
-        <v>286.4185489097594</v>
+        <v>286.29832903147</v>
       </c>
       <c r="F23">
-        <v>18.15090074747606</v>
+        <v>18.79490232157276</v>
       </c>
       <c r="G23">
-        <v>0.00153970077030164</v>
+        <v>0.001487680916718522</v>
       </c>
       <c r="H23">
-        <v>0.002999428030635581</v>
+        <v>0.001967479957400649</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1004,19 +1004,19 @@
         <v>0.03156755469297089</v>
       </c>
       <c r="D24">
-        <v>4333357.339203728</v>
+        <v>4321520.083741616</v>
       </c>
       <c r="E24">
-        <v>286.5039949684863</v>
+        <v>286.387829242878</v>
       </c>
       <c r="F24">
-        <v>16.8603655124343</v>
+        <v>17.47408022080733</v>
       </c>
       <c r="G24">
-        <v>0.001566629745497767</v>
+        <v>0.001512337740640048</v>
       </c>
       <c r="H24">
-        <v>0.003277931595140243</v>
+        <v>0.002149114661449114</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1030,19 +1030,19 @@
         <v>0.03334716662612121</v>
       </c>
       <c r="D25">
-        <v>4340029.324986956</v>
+        <v>4328486.434555272</v>
       </c>
       <c r="E25">
-        <v>286.5693660803273</v>
+        <v>286.4562228684182</v>
       </c>
       <c r="F25">
-        <v>15.74996597535596</v>
+        <v>16.33770561077392</v>
       </c>
       <c r="G25">
-        <v>0.00159362318683616</v>
+        <v>0.001537022325862672</v>
       </c>
       <c r="H25">
-        <v>0.003565713767135267</v>
+        <v>0.002336675025689555</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1056,19 +1056,19 @@
         <v>0.03512677855927156</v>
       </c>
       <c r="D26">
-        <v>4345173.068839589</v>
+        <v>4333850.588033762</v>
       </c>
       <c r="E26">
-        <v>286.6197122406942</v>
+        <v>286.5088303306525</v>
       </c>
       <c r="F26">
-        <v>14.7905196355095</v>
+        <v>15.35581625218083</v>
       </c>
       <c r="G26">
-        <v>0.001620032984955762</v>
+        <v>0.001561125936190083</v>
       </c>
       <c r="H26">
-        <v>0.00386170806267469</v>
+        <v>0.002529467770282997</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1082,19 +1082,19 @@
         <v>0.03690639049242189</v>
       </c>
       <c r="D27">
-        <v>4349166.240868012</v>
+        <v>4338008.828001891</v>
       </c>
       <c r="E27">
-        <v>286.6587659476536</v>
+        <v>286.549577520879</v>
       </c>
       <c r="F27">
-        <v>13.95788840411186</v>
+        <v>14.50367914218242</v>
       </c>
       <c r="G27">
-        <v>0.001645437044121459</v>
+        <v>0.001584254547500019</v>
       </c>
       <c r="H27">
-        <v>0.004165025434192116</v>
+        <v>0.002726916176392131</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1108,19 +1108,19 @@
         <v>0.03868600242557224</v>
       </c>
       <c r="D28">
-        <v>4352286.214290478</v>
+        <v>4341251.948542095</v>
       </c>
       <c r="E28">
-        <v>286.689260937791</v>
+        <v>286.5813369842197</v>
       </c>
       <c r="F28">
-        <v>13.2323364982597</v>
+        <v>13.76109811539021</v>
       </c>
       <c r="G28">
-        <v>0.001669552089648645</v>
+        <v>0.001606145761131376</v>
       </c>
       <c r="H28">
-        <v>0.004474893879312136</v>
+        <v>0.002928520627467398</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1134,19 +1134,19 @@
         <v>0.04046561435872258</v>
       </c>
       <c r="D29">
-        <v>4354737.027278671</v>
+        <v>4343793.753670502</v>
       </c>
       <c r="E29">
-        <v>286.7132039663194</v>
+        <v>286.6062161108559</v>
       </c>
       <c r="F29">
-        <v>12.59776592119353</v>
+        <v>13.11161376208007</v>
       </c>
       <c r="G29">
-        <v>0.001692184496369246</v>
+        <v>0.001626621969903978</v>
       </c>
       <c r="H29">
-        <v>0.00479062383696469</v>
+        <v>0.003133835948783437</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1160,19 +1160,19 @@
         <v>0.04224522629187291</v>
       </c>
       <c r="D30">
-        <v>4356669.748130793</v>
+        <v>4345792.497771563</v>
       </c>
       <c r="E30">
-        <v>286.7320783990012</v>
+        <v>286.6257720957922</v>
       </c>
       <c r="F30">
-        <v>12.04102200487696</v>
+        <v>12.54178393014717</v>
       </c>
       <c r="G30">
-        <v>0.001713200892281765</v>
+        <v>0.001645562373542862</v>
       </c>
       <c r="H30">
-        <v>0.005111587080414901</v>
+        <v>0.003342457548259067</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1186,19 +1186,19 @@
         <v>0.04402483822502326</v>
       </c>
       <c r="D31">
-        <v>4358197.18240021</v>
+        <v>4347366.334715841</v>
       </c>
       <c r="E31">
-        <v>286.7469904642047</v>
+        <v>286.6411659805414</v>
       </c>
       <c r="F31">
-        <v>11.55131466385689</v>
+        <v>12.04058717748817</v>
       </c>
       <c r="G31">
-        <v>0.001732509740003881</v>
+        <v>0.001662885456364279</v>
       </c>
       <c r="H31">
-        <v>0.005437203154275915</v>
+        <v>0.003554012482759693</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1212,19 +1212,19 @@
         <v>0.04580445015817358</v>
       </c>
       <c r="D32">
-        <v>4359404.343036837</v>
+        <v>4348604.301306475</v>
       </c>
       <c r="E32">
-        <v>286.7587729793574</v>
+        <v>286.6532717384537</v>
       </c>
       <c r="F32">
-        <v>11.11975257840805</v>
+        <v>11.59894412069569</v>
       </c>
       <c r="G32">
-        <v>0.001750049341743204</v>
+        <v>0.001678537586254865</v>
       </c>
       <c r="H32">
-        <v>0.005766930263261304</v>
+        <v>0.003768153435148493</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1238,19 +1238,19 @@
         <v>0.04758406209132393</v>
       </c>
       <c r="D33">
-        <v>4360355.892104086</v>
+        <v>4349574.117167798</v>
       </c>
       <c r="E33">
-        <v>286.7680588659395</v>
+        <v>286.6627535119822</v>
       </c>
       <c r="F33">
-        <v>10.73897365302902</v>
+        <v>11.20933849925048</v>
       </c>
       <c r="G33">
-        <v>0.001765779770017693</v>
+        <v>0.001692485354341924</v>
       </c>
       <c r="H33">
-        <v>0.006100258911046111</v>
+        <v>0.00398455449254227</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1264,19 +1264,19 @@
         <v>0.04936367402447427</v>
       </c>
       <c r="D34">
-        <v>4361101.452504632</v>
+        <v>4350327.749140552</v>
       </c>
       <c r="E34">
-        <v>286.7753335065947</v>
+        <v>286.6701205856821</v>
       </c>
       <c r="F34">
-        <v>10.40285330799668</v>
+        <v>10.86551848879606</v>
       </c>
       <c r="G34">
-        <v>0.001779677286824377</v>
+        <v>0.001704710285471294</v>
       </c>
       <c r="H34">
-        <v>0.00643670730563572</v>
+        <v>0.004202908083874748</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1290,19 +1290,19 @@
         <v>0.05114328595762462</v>
       </c>
       <c r="D35">
-        <v>4361679.426190006</v>
+        <v>4350905.409813343</v>
       </c>
       <c r="E35">
-        <v>286.7809723142838</v>
+        <v>286.6757668162787</v>
       </c>
       <c r="F35">
-        <v>10.10627425070433</v>
+        <v>10.56226121732258</v>
       </c>
       <c r="G35">
-        <v>0.001791730390167778</v>
+        <v>0.001715205098757368</v>
       </c>
       <c r="H35">
-        <v>0.006775817938782938</v>
+        <v>0.004422922689759432</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1316,19 +1316,19 @@
         <v>0.05292289789077495</v>
       </c>
       <c r="D36">
-        <v>4362119.761802351</v>
+        <v>4351338.455339114</v>
       </c>
       <c r="E36">
-        <v>286.7852679253423</v>
+        <v>286.6799991654826</v>
       </c>
       <c r="F36">
-        <v>9.844944344617202</v>
+        <v>10.29518662723297</v>
       </c>
       <c r="G36">
-        <v>0.001801936953830545</v>
+        <v>0.001723971009093573</v>
       </c>
       <c r="H36">
-        <v>0.007117154969199271</v>
+        <v>0.004644321082536211</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1342,19 +1342,19 @@
         <v>0.05470250982392529</v>
       </c>
       <c r="D37">
-        <v>4362445.978632754</v>
+        <v>4351651.504402515</v>
       </c>
       <c r="E37">
-        <v>286.7884500621317</v>
+        <v>286.6830585382196</v>
       </c>
       <c r="F37">
-        <v>9.615252006686804</v>
+        <v>10.0606097840184</v>
       </c>
       <c r="G37">
-        <v>0.001810302119051188</v>
+        <v>0.001731015744256085</v>
       </c>
       <c r="H37">
-        <v>0.007460302170802551</v>
+        <v>0.004866838940184393</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1368,19 +1368,19 @@
         <v>0.05648212175707563</v>
       </c>
       <c r="D38">
-        <v>4362676.659946618</v>
+        <v>4351864.00160152</v>
       </c>
       <c r="E38">
-        <v>286.7907001738268</v>
+        <v>286.6851351413467</v>
       </c>
       <c r="F38">
-        <v>9.414150922064326</v>
+        <v>9.855423187576802</v>
       </c>
       <c r="G38">
-        <v>0.001816836714186145</v>
+        <v>0.00173635206415255</v>
       </c>
       <c r="H38">
-        <v>0.007804861287631722</v>
+        <v>0.005090223730272982</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1394,19 +1394,19 @@
         <v>0.05826173369022596</v>
       </c>
       <c r="D39">
-        <v>4362826.564383106</v>
+        <v>4351991.38098955</v>
       </c>
       <c r="E39">
-        <v>286.7921623237943</v>
+        <v>286.6863799044852</v>
       </c>
       <c r="F39">
-        <v>9.239067741693527</v>
+        <v>9.677002585296568</v>
       </c>
       <c r="G39">
-        <v>0.001821556052028307</v>
+        <v>0.001739996638925434</v>
       </c>
       <c r="H39">
-        <v>0.008150450687705056</v>
+        <v>0.005314233793212711</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1420,19 +1420,19 @@
         <v>0.0600413456233763</v>
       </c>
       <c r="D40">
-        <v>4362907.459967121</v>
+        <v>4352045.939222693</v>
       </c>
       <c r="E40">
-        <v>286.7929513539823</v>
+        <v>286.6869130442088</v>
       </c>
       <c r="F40">
-        <v>9.087827885657966</v>
+        <v>9.523131289230353</v>
       </c>
       <c r="G40">
-        <v>0.001824479001852924</v>
+        <v>0.001741969187807049</v>
       </c>
       <c r="H40">
-        <v>0.008496704241232313</v>
+        <v>0.005538637575737033</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1446,19 +1446,19 @@
         <v>0.06182095755652664</v>
       </c>
       <c r="D41">
-        <v>4362928.754811501</v>
+        <v>4352037.495846447</v>
       </c>
       <c r="E41">
-        <v>286.7931590553972</v>
+        <v>286.6868305363797</v>
       </c>
       <c r="F41">
-        <v>8.958595696278914</v>
+        <v>9.391939153056438</v>
       </c>
       <c r="G41">
-        <v>0.001825627264072266</v>
+        <v>0.00174229181001052</v>
       </c>
       <c r="H41">
-        <v>0.008843270369061006</v>
+        <v>0.00576321297895854</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1472,19 +1472,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D42">
-        <v>4362897.977433402</v>
+        <v>4351973.896106312</v>
       </c>
       <c r="E42">
-        <v>286.7928588648869</v>
+        <v>286.6862090422119</v>
       </c>
       <c r="F42">
-        <v>8.865928361464634</v>
+        <v>9.298539256005199</v>
       </c>
       <c r="G42">
-        <v>0.001824995394933626</v>
+        <v>0.001740998303699879</v>
       </c>
       <c r="H42">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1498,19 +1498,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D43">
-        <v>4362826.802878256</v>
+        <v>4351870.426284381</v>
       </c>
       <c r="E43">
-        <v>286.7921646500175</v>
+        <v>286.6851979245957</v>
       </c>
       <c r="F43">
-        <v>9.05381720473174</v>
+        <v>9.495862408080013</v>
       </c>
       <c r="G43">
-        <v>0.001823082848665206</v>
+        <v>0.001739137161956372</v>
       </c>
       <c r="H43">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1524,19 +1524,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D44">
-        <v>4362031.300221232</v>
+        <v>4350979.6779093</v>
       </c>
       <c r="E44">
-        <v>286.7844049812059</v>
+        <v>286.6764926943393</v>
       </c>
       <c r="F44">
-        <v>9.25050901129317</v>
+        <v>9.702547272165845</v>
       </c>
       <c r="G44">
-        <v>0.001821024651317835</v>
+        <v>0.001737122200257145</v>
       </c>
       <c r="H44">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1550,19 +1550,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D45">
-        <v>4361205.174444675</v>
+        <v>4350054.490633124</v>
       </c>
       <c r="E45">
-        <v>286.776345476466</v>
+        <v>286.6674494780508</v>
       </c>
       <c r="F45">
-        <v>9.455355971228132</v>
+        <v>9.917819414423629</v>
       </c>
       <c r="G45">
-        <v>0.001818993077116036</v>
+        <v>0.001735130787834604</v>
       </c>
       <c r="H45">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1576,19 +1576,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D46">
-        <v>4360349.73340687</v>
+        <v>4349096.536407231</v>
       </c>
       <c r="E46">
-        <v>286.7679987699238</v>
+        <v>286.6580844604522</v>
       </c>
       <c r="F46">
-        <v>9.668869555621184</v>
+        <v>10.14221748562237</v>
       </c>
       <c r="G46">
-        <v>0.001816990376354613</v>
+        <v>0.001733165099313345</v>
       </c>
       <c r="H46">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1602,19 +1602,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D47">
-        <v>4359463.299231189</v>
+        <v>4348103.942625263</v>
       </c>
       <c r="E47">
-        <v>286.7593483596944</v>
+        <v>286.6483791707414</v>
       </c>
       <c r="F47">
-        <v>9.891610854289155</v>
+        <v>10.37633348400944</v>
       </c>
       <c r="G47">
-        <v>0.001815018174982218</v>
+        <v>0.001731226580621842</v>
       </c>
       <c r="H47">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1628,19 +1628,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D48">
-        <v>4358544.043322096</v>
+        <v>4347074.665827832</v>
       </c>
       <c r="E48">
-        <v>286.7503762579721</v>
+        <v>286.6383134485919</v>
       </c>
       <c r="F48">
-        <v>10.12419083307648</v>
+        <v>10.62081214309105</v>
       </c>
       <c r="G48">
-        <v>0.001813078186820316</v>
+        <v>0.001729316752009213</v>
       </c>
       <c r="H48">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1654,19 +1654,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D49">
-        <v>4357589.983626813</v>
+        <v>4346006.490889685</v>
       </c>
       <c r="E49">
-        <v>286.7410629621758</v>
+        <v>286.6278654335136</v>
       </c>
       <c r="F49">
-        <v>10.36727601478587</v>
+        <v>10.87635694310267</v>
       </c>
       <c r="G49">
-        <v>0.001811172221842123</v>
+        <v>0.001727437215898863</v>
       </c>
       <c r="H49">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1680,19 +1680,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D50">
-        <v>4356598.967779974</v>
+        <v>4344897.012154372</v>
       </c>
       <c r="E50">
-        <v>286.7313872880327</v>
+        <v>286.6170113773364</v>
       </c>
       <c r="F50">
-        <v>10.62159498612822</v>
+        <v>11.14373700565148</v>
       </c>
       <c r="G50">
-        <v>0.001809302191617581</v>
+        <v>0.001725589661050569</v>
       </c>
       <c r="H50">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -1706,19 +1706,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D51">
-        <v>4355568.653865043</v>
+        <v>4343743.611877549</v>
       </c>
       <c r="E51">
-        <v>286.721326179003</v>
+        <v>286.6057254298741</v>
       </c>
       <c r="F51">
-        <v>10.88794584624938</v>
+        <v>11.42379498819539</v>
       </c>
       <c r="G51">
-        <v>0.001807470114922459</v>
+        <v>0.001723775866732372</v>
       </c>
       <c r="H51">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1732,19 +1732,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D52">
-        <v>4354496.488457861</v>
+        <v>4342543.435618807</v>
       </c>
       <c r="E52">
-        <v>286.7108544887</v>
+        <v>286.5939793941415</v>
       </c>
       <c r="F52">
-        <v>11.16720476020864</v>
+        <v>11.71745615217667</v>
       </c>
       <c r="G52">
-        <v>0.001805678123484401</v>
+        <v>0.001721997706858604</v>
       </c>
       <c r="H52">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -1758,19 +1758,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D53">
-        <v>4353379.681488375</v>
+        <v>4341293.364060117</v>
       </c>
       <c r="E53">
-        <v>286.699944731682</v>
+        <v>286.581742445909</v>
       </c>
       <c r="F53">
-        <v>11.46033581422986</v>
+        <v>12.02573881434449</v>
       </c>
       <c r="G53">
-        <v>0.00180392846780731</v>
+        <v>0.001720257154010054</v>
       </c>
       <c r="H53">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -1784,19 +1784,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D54">
-        <v>4352215.177362773</v>
+        <v>4339989.980623025</v>
       </c>
       <c r="E54">
-        <v>286.688566797057</v>
+        <v>286.5689808112998</v>
       </c>
       <c r="F54">
-        <v>11.76840241077179</v>
+        <v>12.349766434796</v>
       </c>
       <c r="G54">
-        <v>0.001802223522991898</v>
+        <v>0.001718556283224599</v>
       </c>
       <c r="H54">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -1810,19 +1810,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D55">
-        <v>4350999.621672702</v>
+        <v>4338629.534126318</v>
       </c>
       <c r="E55">
-        <v>286.6766876181819</v>
+        <v>286.5556573948375</v>
       </c>
       <c r="F55">
-        <v>12.09258049268191</v>
+        <v>12.69078164994841</v>
       </c>
       <c r="G55">
-        <v>0.001800565794439567</v>
+        <v>0.001716897275409922</v>
       </c>
       <c r="H55">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -1836,19 +1836,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D56">
-        <v>4349729.322674938</v>
+        <v>4337207.895564079</v>
       </c>
       <c r="E56">
-        <v>286.6642707903082</v>
+        <v>286.5417313487157</v>
       </c>
       <c r="F56">
-        <v>12.43417394968119</v>
+        <v>13.05016262700768</v>
       </c>
       <c r="G56">
-        <v>0.001798957923285972</v>
+        <v>0.001715282420182874</v>
       </c>
       <c r="H56">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -1862,19 +1862,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D57">
-        <v>4348400.206546118</v>
+        <v>4335720.507882103</v>
       </c>
       <c r="E57">
-        <v>286.6512761262346</v>
+        <v>286.5271575720374</v>
       </c>
       <c r="F57">
-        <v>12.79463264081792</v>
+        <v>13.42944220242173</v>
       </c>
       <c r="G57">
-        <v>0.001797402691357539</v>
+        <v>0.001713714117878269</v>
       </c>
       <c r="H57">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -1888,19 +1888,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D58">
-        <v>4347007.76519287</v>
+        <v>4334162.327377089</v>
       </c>
       <c r="E58">
-        <v>286.63765913778</v>
+        <v>286.5118861262139</v>
       </c>
       <c r="F58">
-        <v>13.17557356814211</v>
+        <v>13.83033037548489</v>
       </c>
       <c r="G58">
-        <v>0.001795903025373916</v>
+        <v>0.001712194880389476</v>
       </c>
       <c r="H58">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -1914,19 +1914,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D59">
-        <v>4345546.995114657</v>
+        <v>4332527.75502286</v>
       </c>
       <c r="E59">
-        <v>286.6233704280569</v>
+        <v>286.4958615494914</v>
       </c>
       <c r="F59">
-        <v>13.57880586611691</v>
+        <v>14.254740866593</v>
       </c>
       <c r="G59">
-        <v>0.001794462000026639</v>
+        <v>0.001710727330397616</v>
       </c>
       <c r="H59">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -1940,19 +1940,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D60">
-        <v>4344012.325457009</v>
+        <v>4330810.555620828</v>
       </c>
       <c r="E60">
-        <v>286.6083549759144</v>
+        <v>286.4790220494679</v>
       </c>
       <c r="F60">
-        <v>14.00636043682867</v>
+        <v>14.70482262693316</v>
       </c>
       <c r="G60">
-        <v>0.001793082839441538</v>
+        <v>0.001709314198407353</v>
       </c>
       <c r="H60">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -1966,19 +1966,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D61">
-        <v>4342397.532933048</v>
+        <v>4329003.762150983</v>
       </c>
       <c r="E61">
-        <v>286.5925512893083</v>
+        <v>286.4612985472088</v>
       </c>
       <c r="F61">
-        <v>14.46052527458457</v>
+        <v>15.18299741522497</v>
       </c>
       <c r="G61">
-        <v>0.001791768916369509</v>
+        <v>0.001707958316823726</v>
       </c>
       <c r="H61">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -1992,19 +1992,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D62">
-        <v>4340695.640698818</v>
+        <v>4327099.562028161</v>
       </c>
       <c r="E62">
-        <v>286.5758903984056</v>
+        <v>286.4426135397907</v>
       </c>
       <c r="F62">
-        <v>14.94388780098478</v>
+        <v>15.69200485474936</v>
       </c>
       <c r="G62">
-        <v>0.001790523748232359</v>
+        <v>0.00170666261006087</v>
       </c>
       <c r="H62">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2018,19 +2018,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D63">
-        <v>4338898.797499117</v>
+        <v>4325089.16109598</v>
       </c>
       <c r="E63">
-        <v>286.5582946515005</v>
+        <v>286.422879739281</v>
       </c>
       <c r="F63">
-        <v>15.45938589508852</v>
+        <v>16.23495677412526</v>
       </c>
       <c r="G63">
-        <v>0.001789350988858945</v>
+        <v>0.00170543007934816</v>
       </c>
       <c r="H63">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2044,19 +2044,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D64">
-        <v>4336998.13239468</v>
+        <v>4322962.620048434</v>
       </c>
       <c r="E64">
-        <v>286.5396762667039</v>
+        <v>286.4019984346125</v>
       </c>
       <c r="F64">
-        <v>16.01036978360543</v>
+        <v>16.81540315133203</v>
       </c>
       <c r="G64">
-        <v>0.001788254414353201</v>
+        <v>0.001704263780462241</v>
       </c>
       <c r="H64">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2070,19 +2070,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D65">
-        <v>4334983.579054016</v>
+        <v>4320708.656460021</v>
       </c>
       <c r="E65">
-        <v>286.5199355789989</v>
+        <v>286.3798575075281</v>
       </c>
       <c r="F65">
-        <v>16.60067759643832</v>
+        <v>17.43741266917859</v>
       </c>
       <c r="G65">
-        <v>0.001787237901002102</v>
+        <v>0.001703166792022714</v>
       </c>
       <c r="H65">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2096,19 +2096,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D66">
-        <v>4332843.661825371</v>
+        <v>4318314.403593316</v>
       </c>
       <c r="E66">
-        <v>286.498958904438</v>
+        <v>286.3563290133789</v>
       </c>
       <c r="F66">
-        <v>17.23472825504001</v>
+        <v>18.10567181857212</v>
       </c>
       <c r="G66">
-        <v>0.001786305392402683</v>
+        <v>0.001702142171184506</v>
       </c>
       <c r="H66">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -2122,19 +2122,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D67">
-        <v>4330565.233426728</v>
+        <v>4315765.11444411</v>
       </c>
       <c r="E67">
-        <v>286.4766159192739</v>
+        <v>286.3312662100712</v>
       </c>
       <c r="F67">
-        <v>17.91763653382058</v>
+        <v>18.82560774996692</v>
       </c>
       <c r="G67">
-        <v>0.00178546085198421</v>
+        <v>0.001701192892455195</v>
       </c>
       <c r="H67">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2148,19 +2148,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D68">
-        <v>4328133.150860772</v>
+        <v>4313043.795798274</v>
       </c>
       <c r="E68">
-        <v>286.4527564191868</v>
+        <v>286.304499881019</v>
       </c>
       <c r="F68">
-        <v>18.65535674804286</v>
+        <v>19.60354181428021</v>
       </c>
       <c r="G68">
-        <v>0.001784708195709708</v>
+        <v>0.001700321763835517</v>
       </c>
       <c r="H68">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -2174,19 +2174,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D69">
-        <v>4325529.871721403</v>
+        <v>4310130.752002115</v>
       </c>
       <c r="E69">
-        <v>286.4272062788764</v>
+        <v>286.27583374636</v>
       </c>
       <c r="F69">
-        <v>19.45486376742619</v>
+        <v>20.44688316145358</v>
       </c>
       <c r="G69">
-        <v>0.001784051197791725</v>
+        <v>0.001699531312341948</v>
       </c>
       <c r="H69">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2200,19 +2200,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D70">
-        <v>4322734.946881829</v>
+        <v>4307003.011081595</v>
       </c>
       <c r="E70">
-        <v>286.3997623697662</v>
+        <v>286.245038684724</v>
       </c>
       <c r="F70">
-        <v>20.32438322182518</v>
+        <v>21.36437519256381</v>
       </c>
       <c r="G70">
-        <v>0.001783493359499608</v>
+        <v>0.001698823627947093</v>
       </c>
       <c r="H70">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2226,19 +2226,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D71">
-        <v>4319724.376849907</v>
+        <v>4303633.595870976</v>
       </c>
       <c r="E71">
-        <v>287.0676118382531</v>
+        <v>286.9161296718924</v>
       </c>
       <c r="F71">
-        <v>21.19492851419065</v>
+        <v>22.36394514119429</v>
       </c>
       <c r="G71">
-        <v>0.001753751037074774</v>
+        <v>0.001670370942140564</v>
       </c>
       <c r="H71">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -2252,19 +2252,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D72">
-        <v>4316615.617894707</v>
+        <v>4299922.856894268</v>
       </c>
       <c r="E72">
-        <v>287.7578361669448</v>
+        <v>287.6097688875745</v>
       </c>
       <c r="F72">
-        <v>21.81023084256069</v>
+        <v>23.02145109070572</v>
       </c>
       <c r="G72">
-        <v>0.001725793008542144</v>
+        <v>0.001643579191444813</v>
       </c>
       <c r="H72">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2278,19 +2278,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D73">
-        <v>4314110.072184375</v>
+        <v>4297079.746383652</v>
       </c>
       <c r="E73">
-        <v>288.4701254115243</v>
+        <v>288.325751218678</v>
       </c>
       <c r="F73">
-        <v>22.41980637627957</v>
+        <v>23.66859676631845</v>
       </c>
       <c r="G73">
-        <v>0.00169935845331911</v>
+        <v>0.00161836921907928</v>
       </c>
       <c r="H73">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2304,19 +2304,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D74">
-        <v>4311544.625136264</v>
+        <v>4294179.467432562</v>
       </c>
       <c r="E74">
-        <v>289.2038324364225</v>
+        <v>289.0632918455577</v>
       </c>
       <c r="F74">
-        <v>23.03421294261776</v>
+        <v>24.32081016359712</v>
       </c>
       <c r="G74">
-        <v>0.001674026061172838</v>
+        <v>0.001594217838295722</v>
       </c>
       <c r="H74">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -2330,19 +2330,19 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D75">
-        <v>4308888.972564092</v>
+        <v>4291176.201255948</v>
       </c>
       <c r="E75">
-        <v>289.958618561601</v>
+        <v>289.8220406967703</v>
       </c>
       <c r="F75">
-        <v>23.65408832883999</v>
+        <v>24.97902211172765</v>
       </c>
       <c r="G75">
-        <v>0.001649701278702568</v>
+        <v>0.00157102823451052</v>
       </c>
       <c r="H75">
-        <v>0.009170233837628798</v>
+        <v>0.005975062616975481</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -2356,19 +2356,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D76">
-        <v>4306139.428236136</v>
+        <v>4288064.985995948</v>
       </c>
       <c r="E76">
-        <v>290.7341463717214</v>
+        <v>290.6016559183944</v>
       </c>
       <c r="F76">
-        <v>24.27965432702783</v>
+        <v>25.64349404560835</v>
       </c>
       <c r="G76">
-        <v>0.001626309905593047</v>
+        <v>0.001548729145823301</v>
       </c>
       <c r="H76">
-        <v>0.00917023383762881</v>
+        <v>0.005975062616975487</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -2382,19 +2382,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D77">
-        <v>4303293.358609101</v>
+        <v>4284842.680617458</v>
       </c>
       <c r="E77">
-        <v>291.5300680771124</v>
+        <v>291.401785602836</v>
       </c>
       <c r="F77">
-        <v>24.91111444280907</v>
+        <v>26.31445620236355</v>
       </c>
       <c r="G77">
-        <v>0.00160378524951626</v>
+        <v>0.001527256807358545</v>
       </c>
       <c r="H77">
-        <v>0.00917023383762881</v>
+        <v>0.005975062616975487</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -2408,19 +2408,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D78">
-        <v>4300348.095064798</v>
+        <v>4281506.133331283</v>
       </c>
       <c r="E78">
-        <v>292.3460259083091</v>
+        <v>292.2220678446314</v>
       </c>
       <c r="F78">
-        <v>25.54867226370813</v>
+        <v>26.99213906768586</v>
       </c>
       <c r="G78">
-        <v>0.001582066778963971</v>
+        <v>0.001506553363313357</v>
       </c>
       <c r="H78">
-        <v>0.00917023383762881</v>
+        <v>0.005975062616975487</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -2434,19 +2434,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D79">
-        <v>4297300.881018923</v>
+        <v>4278052.087462561</v>
       </c>
       <c r="E79">
-        <v>293.1816530423749</v>
+        <v>293.0621316674073</v>
       </c>
       <c r="F79">
-        <v>26.19253385003498</v>
+        <v>27.67677657238193</v>
       </c>
       <c r="G79">
-        <v>0.001561099350429316</v>
+        <v>0.001486566113951195</v>
       </c>
       <c r="H79">
-        <v>0.00917023383762881</v>
+        <v>0.005975062616975487</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -2460,19 +2460,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D80">
-        <v>4294148.862576202</v>
+        <v>4274477.16864248</v>
       </c>
       <c r="E80">
-        <v>294.0365745870172</v>
+        <v>293.9215980235363</v>
       </c>
       <c r="F80">
-        <v>26.84290928152634</v>
+        <v>28.36860786399677</v>
       </c>
       <c r="G80">
-        <v>0.001540832568380568</v>
+        <v>0.001467246899919296</v>
       </c>
       <c r="H80">
-        <v>0.00917023383762881</v>
+        <v>0.005975062616975487</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -2486,19 +2486,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D81">
-        <v>4290889.080880358</v>
+        <v>4270777.875391199</v>
       </c>
       <c r="E81">
-        <v>294.9104085903607</v>
+        <v>294.800080822896</v>
       </c>
       <c r="F81">
-        <v>27.50001407087104</v>
+        <v>29.06787888454368</v>
       </c>
       <c r="G81">
-        <v>0.00152122023849114</v>
+        <v>0.001448551578555537</v>
       </c>
       <c r="H81">
-        <v>0.00917023383762881</v>
+        <v>0.005975062616975487</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -2512,19 +2512,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D82">
-        <v>4287518.464189363</v>
+        <v>4266950.569504418</v>
       </c>
       <c r="E82">
-        <v>295.8027670673696</v>
+        <v>295.6971879784436</v>
       </c>
       <c r="F82">
-        <v>28.16407046328581</v>
+        <v>29.77484381135711</v>
       </c>
       <c r="G82">
-        <v>0.001502219899585149</v>
+        <v>0.00143043957664683</v>
       </c>
       <c r="H82">
-        <v>0.00917023383762881</v>
+        <v>0.005975062616975487</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -2538,19 +2538,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D83">
-        <v>4284033.81965528</v>
+        <v>4262991.466116594</v>
       </c>
       <c r="E83">
-        <v>296.7132570328204</v>
+        <v>296.6125224584019</v>
       </c>
       <c r="F83">
-        <v>28.83530863930292</v>
+        <v>30.48976650151139</v>
       </c>
       <c r="G83">
-        <v>0.001483792421308333</v>
+        <v>0.001412873501341346</v>
       </c>
       <c r="H83">
-        <v>0.00917023383762881</v>
+        <v>0.005975062616975487</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -2564,19 +2564,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D84">
-        <v>4280431.824784954</v>
+        <v>4258896.622988237</v>
       </c>
       <c r="E84">
-        <v>297.6414815313926</v>
+        <v>297.5456833352644</v>
       </c>
       <c r="F84">
-        <v>29.51396783302144</v>
+        <v>31.21292165188228</v>
       </c>
       <c r="G84">
-        <v>0.001465901657057661</v>
+        <v>0.001395818814041393</v>
       </c>
       <c r="H84">
-        <v>0.00917023383762881</v>
+        <v>0.005975062616975487</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -2590,19 +2590,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D85">
-        <v>4276709.018565874</v>
+        <v>4254661.930025212</v>
       </c>
       <c r="E85">
-        <v>298.587040655941</v>
+        <v>298.4962668224942</v>
       </c>
       <c r="F85">
-        <v>30.20029737738794</v>
+        <v>31.94459608072658</v>
       </c>
       <c r="G85">
-        <v>0.001448514143511105</v>
+        <v>0.001379243539139381</v>
       </c>
       <c r="H85">
-        <v>0.00917023383762881</v>
+        <v>0.005975062616975487</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -2616,19 +2616,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D86">
-        <v>4272861.792237624</v>
+        <v>4250283.097674962</v>
       </c>
       <c r="E86">
-        <v>299.5495325456415</v>
+        <v>299.4638672901369</v>
       </c>
       <c r="F86">
-        <v>30.89455768776321</v>
+        <v>32.68508985967521</v>
       </c>
       <c r="G86">
-        <v>0.00143159883956268</v>
+        <v>0.001363118015403327</v>
       </c>
       <c r="H86">
-        <v>0.00917023383762881</v>
+        <v>0.005975062616975487</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -2642,19 +2642,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D87">
-        <v>4268886.379684529</v>
+        <v>4245755.645112409</v>
       </c>
       <c r="E87">
-        <v>300.5285543564523</v>
+        <v>300.4480782517883</v>
       </c>
       <c r="F87">
-        <v>31.59702119486484</v>
+        <v>33.43471741543139</v>
       </c>
       <c r="G87">
-        <v>0.00141512689866226</v>
+        <v>0.001347414678428394</v>
       </c>
       <c r="H87">
-        <v>0.00917023383762881</v>
+        <v>0.005975062616975487</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -2668,19 +2668,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D88">
-        <v>4264778.847419865</v>
+        <v>4241074.887823214</v>
       </c>
       <c r="E88">
-        <v>301.5237031971642</v>
+        <v>301.4484933159262</v>
       </c>
       <c r="F88">
-        <v>32.30797323810082</v>
+        <v>34.1938085993923</v>
       </c>
       <c r="G88">
-        <v>0.001399071469539919</v>
+        <v>0.001332107870254679</v>
       </c>
       <c r="H88">
-        <v>0.00917023383762881</v>
+        <v>0.005975062616975487</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -2694,19 +2694,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D89">
-        <v>4260535.084126486</v>
+        <v>4236235.924582827</v>
       </c>
       <c r="E89">
-        <v>302.5345770252043</v>
+        <v>302.4647070956676</v>
       </c>
       <c r="F89">
-        <v>33.02771293028721</v>
+        <v>34.96270973739635</v>
       </c>
       <c r="G89">
-        <v>0.001383407521103372</v>
+        <v>0.001317173672113212</v>
       </c>
       <c r="H89">
-        <v>0.00917023383762881</v>
+        <v>0.005975062616975487</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -2720,19 +2720,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D90">
-        <v>4256150.789712932</v>
+        <v>4231233.623777163</v>
       </c>
       <c r="E90">
-        <v>303.5607754972817</v>
+        <v>303.4963160719607</v>
       </c>
       <c r="F90">
-        <v>33.75655400475366</v>
+        <v>35.74178467261875</v>
       </c>
       <c r="G90">
-        <v>0.001368111687967555</v>
+        <v>0.001302589756899391</v>
       </c>
       <c r="H90">
-        <v>0.00917023383762881</v>
+        <v>0.005975062616975487</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -2746,19 +2746,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D91">
-        <v>4251621.463838059</v>
+        <v>4226062.60900035</v>
       </c>
       <c r="E91">
-        <v>304.6019007708916</v>
+        <v>304.5429194061869</v>
       </c>
       <c r="F91">
-        <v>34.49482565586715</v>
+        <v>36.53141581482861</v>
       </c>
       <c r="G91">
-        <v>0.001353162133633578</v>
+        <v>0.001288335258510794</v>
       </c>
       <c r="H91">
-        <v>0.00917023383762881</v>
+        <v>0.005975062616975487</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -2772,19 +2772,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D92">
-        <v>4246942.393850964</v>
+        <v>4220717.243856466</v>
       </c>
       <c r="E92">
-        <v>305.657558253612</v>
+        <v>305.6041196991026</v>
       </c>
       <c r="F92">
-        <v>35.24287338404872</v>
+        <v>37.33200520941668</v>
       </c>
       <c r="G92">
-        <v>0.001338538428800535</v>
+        <v>0.001274390655635652</v>
       </c>
       <c r="H92">
-        <v>0.00917023383762881</v>
+        <v>0.005975062616975487</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -2798,19 +2798,19 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D93">
-        <v>4242108.642086448</v>
+        <v>4215191.615883186</v>
       </c>
       <c r="E93">
-        <v>306.7273572980037</v>
+        <v>306.6795236939586</v>
       </c>
       <c r="F93">
-        <v>36.00105985641289</v>
+        <v>38.14397563983406</v>
       </c>
       <c r="G93">
-        <v>0.001324221442684548</v>
+        <v>0.001260737667954634</v>
       </c>
       <c r="H93">
-        <v>0.00917023383762881</v>
+        <v>0.005975062616975487</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Channel Width Exports
</commit_message>
<xml_diff>
--- a/TheEngine/Regen Solver/enginefiles/solverdata.xlsx
+++ b/TheEngine/Regen Solver/enginefiles/solverdata.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Axial Position of Node [m]</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>Channel Height [m]</t>
+  </si>
+  <si>
+    <t>Channel Width [m]</t>
   </si>
   <si>
     <t>Wall Thickness [m]</t>
@@ -392,13 +395,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H93"/>
+  <dimension ref="A1:I93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -420,8 +423,11 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -438,16 +444,19 @@
         <v>288.1145796254294</v>
       </c>
       <c r="F2">
-        <v>3.951000445503544</v>
+        <v>3.951000445885971</v>
       </c>
       <c r="G2">
-        <v>0.005150225991302586</v>
+        <v>0.005150225990804084</v>
       </c>
       <c r="H2">
+        <v>0.009185997400259802</v>
+      </c>
+      <c r="I2">
         <v>0.004889619209503845</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -458,22 +467,25 @@
         <v>0.03029842497054849</v>
       </c>
       <c r="D3">
-        <v>4499938.741724721</v>
+        <v>4499938.741724705</v>
       </c>
       <c r="E3">
-        <v>288.1139958895124</v>
+        <v>288.1139958895121</v>
       </c>
       <c r="F3">
-        <v>4.17049484526296</v>
+        <v>4.170494844911912</v>
       </c>
       <c r="G3">
-        <v>0.005082084374084406</v>
+        <v>0.005082084374512197</v>
       </c>
       <c r="H3">
+        <v>0.008861659071345705</v>
+      </c>
+      <c r="I3">
         <v>0.004766072315499016</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -484,22 +496,25 @@
         <v>0.029472504198055</v>
       </c>
       <c r="D4">
-        <v>4499371.753992386</v>
+        <v>4499371.75399409</v>
       </c>
       <c r="E4">
-        <v>288.1085927249239</v>
+        <v>288.10859272494</v>
       </c>
       <c r="F4">
-        <v>4.429616803339078</v>
+        <v>4.429616803020725</v>
       </c>
       <c r="G4">
-        <v>0.004991567043722514</v>
+        <v>0.004991567044080954</v>
       </c>
       <c r="H4">
+        <v>0.00853732074243161</v>
+      </c>
+      <c r="I4">
         <v>0.004617598523249564</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -510,22 +525,25 @@
         <v>0.02864658342556152</v>
       </c>
       <c r="D5">
-        <v>4498671.082200786</v>
+        <v>4498671.082202471</v>
       </c>
       <c r="E5">
-        <v>288.1019148951242</v>
+        <v>288.1019148951402</v>
       </c>
       <c r="F5">
-        <v>4.735641093493563</v>
+        <v>4.735641093206453</v>
       </c>
       <c r="G5">
-        <v>0.004878959002764082</v>
+        <v>0.004878959003059597</v>
       </c>
       <c r="H5">
+        <v>0.008212982413517519</v>
+      </c>
+      <c r="I5">
         <v>0.004445826539184793</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -536,22 +554,25 @@
         <v>0.02782066265306801</v>
       </c>
       <c r="D6">
-        <v>4497797.915245974</v>
+        <v>4497797.915247642</v>
       </c>
       <c r="E6">
-        <v>288.0935919823681</v>
+        <v>288.0935919823842</v>
       </c>
       <c r="F6">
-        <v>5.09799019945835</v>
+        <v>5.097990199196006</v>
       </c>
       <c r="G6">
-        <v>0.004744654626704549</v>
+        <v>0.004744654626948432</v>
       </c>
       <c r="H6">
+        <v>0.007888644084603418</v>
+      </c>
+      <c r="I6">
         <v>0.004252698601489258</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -562,22 +583,25 @@
         <v>0.02699474188057452</v>
       </c>
       <c r="D7">
-        <v>4496698.260228595</v>
+        <v>4496698.260230262</v>
       </c>
       <c r="E7">
-        <v>288.0831084800097</v>
+        <v>288.0831084800256</v>
       </c>
       <c r="F7">
-        <v>5.528652061859373</v>
+        <v>5.52865206160937</v>
       </c>
       <c r="G7">
-        <v>0.00458935162565802</v>
+        <v>0.004589351625865277</v>
       </c>
       <c r="H7">
+        <v>0.007564305755689323</v>
+      </c>
+      <c r="I7">
         <v>0.004040437763912341</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -588,22 +612,25 @@
         <v>0.02616882110808103</v>
       </c>
       <c r="D8">
-        <v>4495296.765808728</v>
+        <v>4495296.765810432</v>
       </c>
       <c r="E8">
-        <v>288.0697446031033</v>
+        <v>288.0697446031195</v>
       </c>
       <c r="F8">
-        <v>6.043073763125285</v>
+        <v>6.043073762866509</v>
       </c>
       <c r="G8">
-        <v>0.004414021882111358</v>
+        <v>0.004414021882300111</v>
       </c>
       <c r="H8">
+        <v>0.007239967426775229</v>
+      </c>
+      <c r="I8">
         <v>0.003811500253523136</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -614,22 +641,25 @@
         <v>0.02534290033558753</v>
       </c>
       <c r="D9">
-        <v>4493486.423048829</v>
+        <v>4493486.42305065</v>
       </c>
       <c r="E9">
-        <v>288.0524775194562</v>
+        <v>288.0524775194735</v>
       </c>
       <c r="F9">
-        <v>6.661468557920183</v>
+        <v>6.661468557618894</v>
       </c>
       <c r="G9">
-        <v>0.004219855930684975</v>
+        <v>0.00421985593087556</v>
       </c>
       <c r="H9">
+        <v>0.006915629097861133</v>
+      </c>
+      <c r="I9">
         <v>0.003568511051010036</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -640,22 +670,25 @@
         <v>0.02451697956309404</v>
       </c>
       <c r="D10">
-        <v>4491112.186328761</v>
+        <v>4491112.186330855</v>
       </c>
       <c r="E10">
-        <v>288.0298240458173</v>
+        <v>288.0298240458374</v>
       </c>
       <c r="F10">
-        <v>7.410794714743556</v>
+        <v>7.410794714347491</v>
       </c>
       <c r="G10">
-        <v>0.004008172231957837</v>
+        <v>0.004008172232171748</v>
       </c>
       <c r="H10">
+        <v>0.006591290768947037</v>
+      </c>
+      <c r="I10">
         <v>0.003314179163871476</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -666,22 +699,25 @@
         <v>0.02369105879060053</v>
       </c>
       <c r="D11">
-        <v>4487944.059974287</v>
+        <v>4487944.05997694</v>
       </c>
       <c r="E11">
-        <v>287.9995816986361</v>
+        <v>287.9995816986615</v>
       </c>
       <c r="F11">
-        <v>8.327889598298002</v>
+        <v>8.327889597727188</v>
       </c>
       <c r="G11">
-        <v>0.003780273561572748</v>
+        <v>0.003780273561831502</v>
       </c>
       <c r="H11">
+        <v>0.006266952440032936</v>
+      </c>
+      <c r="I11">
         <v>0.003051184505410432</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -692,22 +728,25 @@
         <v>0.02286513801810705</v>
       </c>
       <c r="D12">
-        <v>4483631.028698791</v>
+        <v>4483631.028702533</v>
       </c>
       <c r="E12">
-        <v>287.9583844013953</v>
+        <v>287.958384401431</v>
       </c>
       <c r="F12">
-        <v>9.464741728828674</v>
+        <v>9.464741727960076</v>
       </c>
       <c r="G12">
-        <v>0.003537211056516205</v>
+        <v>0.003537211056840347</v>
       </c>
       <c r="H12">
+        <v>0.005942614111118845</v>
+      </c>
+      <c r="I12">
         <v>0.002782016241311469</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -718,22 +757,25 @@
         <v>0.02203921724561356</v>
       </c>
       <c r="D13">
-        <v>4477617.879274815</v>
+        <v>4477617.87928063</v>
       </c>
       <c r="E13">
-        <v>287.9008979616783</v>
+        <v>287.900897961734</v>
       </c>
       <c r="F13">
-        <v>10.89813793118175</v>
+        <v>10.89813792982213</v>
       </c>
       <c r="G13">
-        <v>0.003279356182438713</v>
+        <v>0.003279356182847146</v>
       </c>
       <c r="H13">
+        <v>0.005618275782204749</v>
+      </c>
+      <c r="I13">
         <v>0.00250870838128259</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -744,22 +786,25 @@
         <v>0.02121329647312005</v>
       </c>
       <c r="D14">
-        <v>4468983.592583368</v>
+        <v>4468983.592593119</v>
       </c>
       <c r="E14">
-        <v>287.818251225561</v>
+        <v>287.8182512256545</v>
       </c>
       <c r="F14">
-        <v>12.74965995401138</v>
+        <v>12.74965995608624</v>
       </c>
       <c r="G14">
-        <v>0.003005486380406337</v>
+        <v>0.003005486379916164</v>
       </c>
       <c r="H14">
+        <v>0.005293937453290648</v>
+      </c>
+      <c r="I14">
         <v>0.002232306255318037</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -770,22 +815,25 @@
         <v>0.02038737570062656</v>
       </c>
       <c r="D15">
-        <v>4456091.290623012</v>
+        <v>4456091.290608353</v>
       </c>
       <c r="E15">
-        <v>287.6946227382366</v>
+        <v>287.6946227380959</v>
       </c>
       <c r="F15">
-        <v>15.23641694306266</v>
+        <v>15.23641694522129</v>
       </c>
       <c r="G15">
-        <v>0.002710282523922772</v>
+        <v>0.002710282523540246</v>
       </c>
       <c r="H15">
+        <v>0.004969599124376551</v>
+      </c>
+      <c r="I15">
         <v>0.001951423350163182</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -796,22 +844,25 @@
         <v>0.01956145492813306</v>
       </c>
       <c r="D16">
-        <v>4435680.565209452</v>
+        <v>4435680.565190914</v>
       </c>
       <c r="E16">
-        <v>287.4983453907358</v>
+        <v>287.4983453905572</v>
       </c>
       <c r="F16">
-        <v>18.86164606616117</v>
+        <v>18.86164606816268</v>
       </c>
       <c r="G16">
-        <v>0.002373765043902406</v>
+        <v>0.002373765043652138</v>
       </c>
       <c r="H16">
+        <v>0.004645260795462457</v>
+      </c>
+      <c r="I16">
         <v>0.001656029482811165</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:9">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -822,22 +873,25 @@
         <v>0.01911027116091851</v>
       </c>
       <c r="D17">
-        <v>4399479.825951125</v>
+        <v>4399479.82592976</v>
       </c>
       <c r="E17">
-        <v>287.1485463326395</v>
+        <v>287.1485463324324</v>
       </c>
       <c r="F17">
-        <v>28.45681500088225</v>
+        <v>28.45681500144963</v>
       </c>
       <c r="G17">
-        <v>0.001662339609194077</v>
+        <v>0.001662339609162266</v>
       </c>
       <c r="H17">
+        <v>0.004468081344399932</v>
+      </c>
+      <c r="I17">
         <v>0.001174978530569183</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:9">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -848,22 +902,25 @@
         <v>0.02088988309406883</v>
       </c>
       <c r="D18">
-        <v>4259052.212008365</v>
+        <v>4259052.212003737</v>
       </c>
       <c r="E18">
-        <v>285.7708143805087</v>
+        <v>285.7708143804628</v>
       </c>
       <c r="F18">
-        <v>28.74624208756715</v>
+        <v>28.74624208766015</v>
       </c>
       <c r="G18">
-        <v>0.001460978596209525</v>
+        <v>0.001460978596205065</v>
       </c>
       <c r="H18">
+        <v>0.005166933316328154</v>
+      </c>
+      <c r="I18">
         <v>0.001206409092976211</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:9">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -874,22 +931,25 @@
         <v>0.02266949502721918</v>
       </c>
       <c r="D19">
-        <v>4246110.789659574</v>
+        <v>4246110.789661271</v>
       </c>
       <c r="E19">
-        <v>285.6421414605923</v>
+        <v>285.6421414606092</v>
       </c>
       <c r="F19">
-        <v>26.54363188101098</v>
+        <v>26.54363188102617</v>
       </c>
       <c r="G19">
-        <v>0.001426328783665248</v>
+        <v>0.001426328783664336</v>
       </c>
       <c r="H19">
+        <v>0.005865785288256387</v>
+      </c>
+      <c r="I19">
         <v>0.001325957687250003</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:9">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -900,22 +960,25 @@
         <v>0.02444910696036953</v>
       </c>
       <c r="D20">
-        <v>4265522.900215349</v>
+        <v>4265522.900218</v>
       </c>
       <c r="E20">
-        <v>285.8350409016894</v>
+        <v>285.8350409017156</v>
       </c>
       <c r="F20">
-        <v>24.21461221557877</v>
+        <v>24.21461221761576</v>
       </c>
       <c r="G20">
-        <v>0.001428074571813216</v>
+        <v>0.001428074571692932</v>
       </c>
       <c r="H20">
+        <v>0.006564637260184621</v>
+      </c>
+      <c r="I20">
         <v>0.001469063650235908</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:9">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -926,22 +989,25 @@
         <v>0.02622871889351988</v>
       </c>
       <c r="D21">
-        <v>4284941.024391057</v>
+        <v>4284941.024372413</v>
       </c>
       <c r="E21">
-        <v>286.0273436744911</v>
+        <v>286.0273436743069</v>
       </c>
       <c r="F21">
-        <v>22.13284682281619</v>
+        <v>22.13284683045498</v>
       </c>
       <c r="G21">
-        <v>0.001443089656994752</v>
+        <v>0.001443089656497774</v>
       </c>
       <c r="H21">
+        <v>0.007263489232112854</v>
+      </c>
+      <c r="I21">
         <v>0.001625869071621931</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:9">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -952,22 +1018,25 @@
         <v>0.0280083308266702</v>
       </c>
       <c r="D22">
-        <v>4300482.221840494</v>
+        <v>4300482.221769645</v>
       </c>
       <c r="E22">
-        <v>286.1807824532439</v>
+        <v>286.1807824525452</v>
       </c>
       <c r="F22">
-        <v>20.33531917584564</v>
+        <v>20.33531917172927</v>
       </c>
       <c r="G22">
-        <v>0.001464034184377028</v>
+        <v>0.001464034184677575</v>
       </c>
       <c r="H22">
+        <v>0.007962341204041077</v>
+      </c>
+      <c r="I22">
         <v>0.001792655008752646</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:9">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -978,22 +1047,25 @@
         <v>0.02978794275982054</v>
       </c>
       <c r="D23">
-        <v>4312416.591316001</v>
+        <v>4312416.591347085</v>
       </c>
       <c r="E23">
-        <v>286.29832903147</v>
+        <v>286.2983290317757</v>
       </c>
       <c r="F23">
-        <v>18.79490232157276</v>
+        <v>18.79490231892169</v>
       </c>
       <c r="G23">
-        <v>0.001487680916718522</v>
+        <v>0.001487680916926486</v>
       </c>
       <c r="H23">
+        <v>0.008661193175969303</v>
+      </c>
+      <c r="I23">
         <v>0.001967479957400649</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:9">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1004,22 +1076,25 @@
         <v>0.03156755469297089</v>
       </c>
       <c r="D24">
-        <v>4321520.083741616</v>
+        <v>4321520.083760626</v>
       </c>
       <c r="E24">
-        <v>286.387829242878</v>
+        <v>286.3878292430649</v>
       </c>
       <c r="F24">
-        <v>17.47408022080733</v>
+        <v>17.47408021917708</v>
       </c>
       <c r="G24">
-        <v>0.001512337740640048</v>
+        <v>0.001512337740779966</v>
       </c>
       <c r="H24">
+        <v>0.009360045147897535</v>
+      </c>
+      <c r="I24">
         <v>0.002149114661449114</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:9">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1030,22 +1105,25 @@
         <v>0.03334716662612121</v>
       </c>
       <c r="D25">
-        <v>4328486.434555272</v>
+        <v>4328486.434566718</v>
       </c>
       <c r="E25">
-        <v>286.4562228684182</v>
+        <v>286.4562228685306</v>
       </c>
       <c r="F25">
-        <v>16.33770561077392</v>
+        <v>16.33770560973663</v>
       </c>
       <c r="G25">
-        <v>0.001537022325862672</v>
+        <v>0.001537022325959533</v>
       </c>
       <c r="H25">
+        <v>0.01005889711982576</v>
+      </c>
+      <c r="I25">
         <v>0.002336675025689555</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:9">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1056,22 +1134,25 @@
         <v>0.03512677855927156</v>
       </c>
       <c r="D26">
-        <v>4333850.588033762</v>
+        <v>4333850.588041208</v>
       </c>
       <c r="E26">
-        <v>286.5088303306525</v>
+        <v>286.5088303307253</v>
       </c>
       <c r="F26">
-        <v>15.35581625218083</v>
+        <v>15.3558162515</v>
       </c>
       <c r="G26">
-        <v>0.001561125936190083</v>
+        <v>0.001561125936258819</v>
       </c>
       <c r="H26">
+        <v>0.01075774909175399</v>
+      </c>
+      <c r="I26">
         <v>0.002529467770282997</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:9">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1082,22 +1163,25 @@
         <v>0.03690639049242189</v>
       </c>
       <c r="D27">
-        <v>4338008.828001891</v>
+        <v>4338008.828007137</v>
       </c>
       <c r="E27">
-        <v>286.549577520879</v>
+        <v>286.5495775209306</v>
       </c>
       <c r="F27">
-        <v>14.50367914218242</v>
+        <v>14.50367914172356</v>
       </c>
       <c r="G27">
-        <v>0.001584254547500019</v>
+        <v>0.00158425454754979</v>
       </c>
       <c r="H27">
+        <v>0.01145660106368222</v>
+      </c>
+      <c r="I27">
         <v>0.002726916176392131</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:9">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1108,22 +1192,25 @@
         <v>0.03868600242557224</v>
       </c>
       <c r="D28">
-        <v>4341251.948542095</v>
+        <v>4341251.948546082</v>
       </c>
       <c r="E28">
-        <v>286.5813369842197</v>
+        <v>286.5813369842587</v>
       </c>
       <c r="F28">
-        <v>13.76109811539021</v>
+        <v>13.76109811507385</v>
       </c>
       <c r="G28">
-        <v>0.001606145761131376</v>
+        <v>0.001606145761168032</v>
       </c>
       <c r="H28">
+        <v>0.01215545303561045</v>
+      </c>
+      <c r="I28">
         <v>0.002928520627467398</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:9">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1134,22 +1221,25 @@
         <v>0.04046561435872258</v>
       </c>
       <c r="D29">
-        <v>4343793.753670502</v>
+        <v>4343793.753673744</v>
       </c>
       <c r="E29">
-        <v>286.6062161108559</v>
+        <v>286.6062161108875</v>
       </c>
       <c r="F29">
-        <v>13.11161376208007</v>
+        <v>13.11161376185763</v>
       </c>
       <c r="G29">
-        <v>0.001626621969903978</v>
+        <v>0.001626621969931352</v>
       </c>
       <c r="H29">
+        <v>0.01285430500753868</v>
+      </c>
+      <c r="I29">
         <v>0.003133835948783437</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:9">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1160,22 +1250,25 @@
         <v>0.04224522629187291</v>
       </c>
       <c r="D30">
-        <v>4345792.497771563</v>
+        <v>4345792.49777435</v>
       </c>
       <c r="E30">
-        <v>286.6257720957922</v>
+        <v>286.6257720958195</v>
       </c>
       <c r="F30">
-        <v>12.54178393014717</v>
+        <v>12.54178392998792</v>
       </c>
       <c r="G30">
-        <v>0.001645562373542862</v>
+        <v>0.001645562373563559</v>
       </c>
       <c r="H30">
+        <v>0.01355315697946691</v>
+      </c>
+      <c r="I30">
         <v>0.003342457548259067</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:9">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1186,22 +1279,25 @@
         <v>0.04402483822502326</v>
       </c>
       <c r="D31">
-        <v>4347366.334715841</v>
+        <v>4347366.334718344</v>
       </c>
       <c r="E31">
-        <v>286.6411659805414</v>
+        <v>286.6411659805659</v>
       </c>
       <c r="F31">
-        <v>12.04058717748817</v>
+        <v>12.04058717737235</v>
       </c>
       <c r="G31">
-        <v>0.001662885456364279</v>
+        <v>0.001662885456380096</v>
       </c>
       <c r="H31">
+        <v>0.01425200895139514</v>
+      </c>
+      <c r="I31">
         <v>0.003554012482759693</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:9">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1212,22 +1308,25 @@
         <v>0.04580445015817358</v>
       </c>
       <c r="D32">
-        <v>4348604.301306475</v>
+        <v>4348604.301308795</v>
       </c>
       <c r="E32">
-        <v>286.6532717384537</v>
+        <v>286.6532717384765</v>
       </c>
       <c r="F32">
-        <v>11.59894412069569</v>
+        <v>11.5989441206102</v>
       </c>
       <c r="G32">
-        <v>0.001678537586254865</v>
+        <v>0.001678537586267063</v>
       </c>
       <c r="H32">
+        <v>0.01495086092332337</v>
+      </c>
+      <c r="I32">
         <v>0.003768153435148493</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:9">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1238,22 +1337,25 @@
         <v>0.04758406209132393</v>
       </c>
       <c r="D33">
-        <v>4349574.117167798</v>
+        <v>4349574.117169999</v>
       </c>
       <c r="E33">
-        <v>286.6627535119822</v>
+        <v>286.6627535120037</v>
       </c>
       <c r="F33">
-        <v>11.20933849925048</v>
+        <v>11.20933849918651</v>
       </c>
       <c r="G33">
-        <v>0.001692485354341924</v>
+        <v>0.001692485354351419</v>
       </c>
       <c r="H33">
+        <v>0.0156497128952516</v>
+      </c>
+      <c r="I33">
         <v>0.00398455449254227</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:9">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1264,22 +1366,25 @@
         <v>0.04936367402447427</v>
       </c>
       <c r="D34">
-        <v>4350327.749140552</v>
+        <v>4350327.749142674</v>
       </c>
       <c r="E34">
-        <v>286.6701205856821</v>
+        <v>286.6701205857029</v>
       </c>
       <c r="F34">
-        <v>10.86551848879606</v>
+        <v>10.86551848874752</v>
       </c>
       <c r="G34">
-        <v>0.001704710285471294</v>
+        <v>0.001704710285478743</v>
       </c>
       <c r="H34">
+        <v>0.01634856486717982</v>
+      </c>
+      <c r="I34">
         <v>0.004202908083874748</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:9">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1290,22 +1395,25 @@
         <v>0.05114328595762462</v>
       </c>
       <c r="D35">
-        <v>4350905.409813343</v>
+        <v>4350905.409815411</v>
       </c>
       <c r="E35">
-        <v>286.6757668162787</v>
+        <v>286.6757668162988</v>
       </c>
       <c r="F35">
-        <v>10.56226121732258</v>
+        <v>10.56226121728529</v>
       </c>
       <c r="G35">
-        <v>0.001715205098757368</v>
+        <v>0.001715205098763264</v>
       </c>
       <c r="H35">
+        <v>0.01704741683910806</v>
+      </c>
+      <c r="I35">
         <v>0.004422922689759432</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:9">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1316,22 +1424,25 @@
         <v>0.05292289789077495</v>
       </c>
       <c r="D36">
-        <v>4351338.455339114</v>
+        <v>4351338.455341145</v>
       </c>
       <c r="E36">
-        <v>286.6799991654826</v>
+        <v>286.6799991655026</v>
       </c>
       <c r="F36">
-        <v>10.29518662723297</v>
+        <v>10.29518662720395</v>
       </c>
       <c r="G36">
-        <v>0.001723971009093573</v>
+        <v>0.001723971009098273</v>
       </c>
       <c r="H36">
+        <v>0.01774626881103629</v>
+      </c>
+      <c r="I36">
         <v>0.004644321082536211</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:9">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1342,22 +1453,25 @@
         <v>0.05470250982392529</v>
       </c>
       <c r="D37">
-        <v>4351651.504402515</v>
+        <v>4351651.504404522</v>
       </c>
       <c r="E37">
-        <v>286.6830585382196</v>
+        <v>286.6830585382391</v>
       </c>
       <c r="F37">
-        <v>10.0606097840184</v>
+        <v>10.06060978399551</v>
       </c>
       <c r="G37">
-        <v>0.001731015744256085</v>
+        <v>0.001731015744259866</v>
       </c>
       <c r="H37">
+        <v>0.01844512078296452</v>
+      </c>
+      <c r="I37">
         <v>0.004866838940184393</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:9">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1368,22 +1482,25 @@
         <v>0.05648212175707563</v>
       </c>
       <c r="D38">
-        <v>4351864.00160152</v>
+        <v>4351864.001603508</v>
       </c>
       <c r="E38">
-        <v>286.6851351413467</v>
+        <v>286.6851351413662</v>
       </c>
       <c r="F38">
-        <v>9.855423187576802</v>
+        <v>9.855423187558509</v>
       </c>
       <c r="G38">
-        <v>0.00173635206415255</v>
+        <v>0.001736352064155614</v>
       </c>
       <c r="H38">
+        <v>0.01914397275489275</v>
+      </c>
+      <c r="I38">
         <v>0.005090223730272982</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:9">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1394,22 +1511,25 @@
         <v>0.05826173369022596</v>
       </c>
       <c r="D39">
-        <v>4351991.38098955</v>
+        <v>4351991.380991526</v>
       </c>
       <c r="E39">
-        <v>286.6863799044852</v>
+        <v>286.6863799045047</v>
       </c>
       <c r="F39">
-        <v>9.677002585296568</v>
+        <v>9.677002585281695</v>
       </c>
       <c r="G39">
-        <v>0.001739996638925434</v>
+        <v>0.001739996638927938</v>
       </c>
       <c r="H39">
+        <v>0.01984282472682097</v>
+      </c>
+      <c r="I39">
         <v>0.005314233793212711</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:9">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1420,22 +1540,25 @@
         <v>0.0600413456233763</v>
       </c>
       <c r="D40">
-        <v>4352045.939222693</v>
+        <v>4352045.939224661</v>
       </c>
       <c r="E40">
-        <v>286.6869130442088</v>
+        <v>286.686913044228</v>
       </c>
       <c r="F40">
-        <v>9.523131289230353</v>
+        <v>9.523131289218119</v>
       </c>
       <c r="G40">
-        <v>0.001741969187807049</v>
+        <v>0.001741969187809126</v>
       </c>
       <c r="H40">
+        <v>0.02054167669874921</v>
+      </c>
+      <c r="I40">
         <v>0.005538637575737033</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:9">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1446,22 +1569,25 @@
         <v>0.06182095755652664</v>
       </c>
       <c r="D41">
-        <v>4352037.495846447</v>
+        <v>4352037.495848407</v>
       </c>
       <c r="E41">
-        <v>286.6868305363797</v>
+        <v>286.6868305363989</v>
       </c>
       <c r="F41">
-        <v>9.391939153056438</v>
+        <v>9.391939153046218</v>
       </c>
       <c r="G41">
-        <v>0.00174229181001052</v>
+        <v>0.001742291810012253</v>
       </c>
       <c r="H41">
+        <v>0.02124052867067744</v>
+      </c>
+      <c r="I41">
         <v>0.00576321297895854</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:9">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1472,22 +1598,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D42">
-        <v>4351973.896106312</v>
+        <v>4351973.896108268</v>
       </c>
       <c r="E42">
-        <v>286.6862090422119</v>
+        <v>286.686209042231</v>
       </c>
       <c r="F42">
-        <v>9.298539256005199</v>
+        <v>9.298539255996433</v>
       </c>
       <c r="G42">
-        <v>0.001740998303699879</v>
+        <v>0.001740998303701357</v>
       </c>
       <c r="H42">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I42">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1498,22 +1627,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D43">
-        <v>4351870.426284381</v>
+        <v>4351870.426286334</v>
       </c>
       <c r="E43">
-        <v>286.6851979245957</v>
+        <v>286.6851979246149</v>
       </c>
       <c r="F43">
-        <v>9.495862408080013</v>
+        <v>9.495862408071064</v>
       </c>
       <c r="G43">
-        <v>0.001739137161956372</v>
+        <v>0.001739137161957848</v>
       </c>
       <c r="H43">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I43">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1524,22 +1656,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D44">
-        <v>4350979.6779093</v>
+        <v>4350979.677911255</v>
       </c>
       <c r="E44">
-        <v>286.6764926943393</v>
+        <v>286.6764926943587</v>
       </c>
       <c r="F44">
-        <v>9.702547272165845</v>
+        <v>9.702547272156666</v>
       </c>
       <c r="G44">
-        <v>0.001737122200257145</v>
+        <v>0.001737122200258613</v>
       </c>
       <c r="H44">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I44">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1550,22 +1685,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D45">
-        <v>4350054.490633124</v>
+        <v>4350054.49063508</v>
       </c>
       <c r="E45">
-        <v>286.6674494780508</v>
+        <v>286.6674494780699</v>
       </c>
       <c r="F45">
-        <v>9.917819414423629</v>
+        <v>9.917819414414261</v>
       </c>
       <c r="G45">
-        <v>0.001735130787834604</v>
+        <v>0.001735130787836078</v>
       </c>
       <c r="H45">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I45">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1576,22 +1714,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D46">
-        <v>4349096.536407231</v>
+        <v>4349096.536409191</v>
       </c>
       <c r="E46">
-        <v>286.6580844604522</v>
+        <v>286.6580844604713</v>
       </c>
       <c r="F46">
-        <v>10.14221748562237</v>
+        <v>10.14221748561277</v>
       </c>
       <c r="G46">
-        <v>0.001733165099313345</v>
+        <v>0.001733165099314819</v>
       </c>
       <c r="H46">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I46">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1602,22 +1743,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D47">
-        <v>4348103.942625263</v>
+        <v>4348103.942627224</v>
       </c>
       <c r="E47">
-        <v>286.6483791707414</v>
+        <v>286.6483791707604</v>
       </c>
       <c r="F47">
-        <v>10.37633348400944</v>
+        <v>10.37633348399961</v>
       </c>
       <c r="G47">
-        <v>0.001731226580621842</v>
+        <v>0.001731226580623315</v>
       </c>
       <c r="H47">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I47">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1628,22 +1772,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D48">
-        <v>4347074.665827832</v>
+        <v>4347074.665829796</v>
       </c>
       <c r="E48">
-        <v>286.6383134485919</v>
+        <v>286.638313448611</v>
       </c>
       <c r="F48">
-        <v>10.62081214309105</v>
+        <v>10.62081214308098</v>
       </c>
       <c r="G48">
-        <v>0.001729316752009213</v>
+        <v>0.001729316752010682</v>
       </c>
       <c r="H48">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I48">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1654,22 +1801,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D49">
-        <v>4346006.490889685</v>
+        <v>4346006.490891652</v>
       </c>
       <c r="E49">
-        <v>286.6278654335136</v>
+        <v>286.6278654335329</v>
       </c>
       <c r="F49">
-        <v>10.87635694310267</v>
+        <v>10.87635694309231</v>
       </c>
       <c r="G49">
-        <v>0.001727437215898863</v>
+        <v>0.001727437215900332</v>
       </c>
       <c r="H49">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I49">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1680,22 +1830,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D50">
-        <v>4344897.012154372</v>
+        <v>4344897.012156342</v>
       </c>
       <c r="E50">
-        <v>286.6170113773364</v>
+        <v>286.6170113773557</v>
       </c>
       <c r="F50">
-        <v>11.14373700565148</v>
+        <v>11.14373700564084</v>
       </c>
       <c r="G50">
-        <v>0.001725589661050569</v>
+        <v>0.001725589661052036</v>
       </c>
       <c r="H50">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I50">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1706,22 +1859,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D51">
-        <v>4343743.611877549</v>
+        <v>4343743.611879522</v>
       </c>
       <c r="E51">
-        <v>286.6057254298741</v>
+        <v>286.6057254298934</v>
       </c>
       <c r="F51">
-        <v>11.42379498819539</v>
+        <v>11.42379498818449</v>
       </c>
       <c r="G51">
-        <v>0.001723775866732372</v>
+        <v>0.001723775866733836</v>
       </c>
       <c r="H51">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I51">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -1732,22 +1888,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D52">
-        <v>4342543.435618807</v>
+        <v>4342543.435620781</v>
       </c>
       <c r="E52">
-        <v>286.5939793941415</v>
+        <v>286.5939793941608</v>
       </c>
       <c r="F52">
-        <v>11.71745615217667</v>
+        <v>11.71745615216543</v>
       </c>
       <c r="G52">
-        <v>0.001721997706858604</v>
+        <v>0.001721997706860066</v>
       </c>
       <c r="H52">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I52">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -1758,22 +1917,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D53">
-        <v>4341293.364060117</v>
+        <v>4341293.364062094</v>
       </c>
       <c r="E53">
-        <v>286.581742445909</v>
+        <v>286.5817424459283</v>
       </c>
       <c r="F53">
-        <v>12.02573881434449</v>
+        <v>12.02573881433292</v>
       </c>
       <c r="G53">
-        <v>0.001720257154010054</v>
+        <v>0.001720257154011522</v>
       </c>
       <c r="H53">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I53">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -1784,22 +1946,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D54">
-        <v>4339989.980623025</v>
+        <v>4339989.980625005</v>
       </c>
       <c r="E54">
-        <v>286.5689808112998</v>
+        <v>286.5689808113192</v>
       </c>
       <c r="F54">
-        <v>12.349766434796</v>
+        <v>12.34976643478407</v>
       </c>
       <c r="G54">
-        <v>0.001718556283224599</v>
+        <v>0.001718556283226064</v>
       </c>
       <c r="H54">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I54">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -1810,22 +1975,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D55">
-        <v>4338629.534126318</v>
+        <v>4338629.534128301</v>
       </c>
       <c r="E55">
-        <v>286.5556573948375</v>
+        <v>286.555657394857</v>
       </c>
       <c r="F55">
-        <v>12.69078164994841</v>
+        <v>12.69078164993613</v>
       </c>
       <c r="G55">
-        <v>0.001716897275409922</v>
+        <v>0.001716897275411388</v>
       </c>
       <c r="H55">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I55">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -1836,22 +2004,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D56">
-        <v>4337207.895564079</v>
+        <v>4337207.895566066</v>
       </c>
       <c r="E56">
-        <v>286.5417313487157</v>
+        <v>286.5417313487352</v>
       </c>
       <c r="F56">
-        <v>13.05016262700768</v>
+        <v>13.05016262699501</v>
       </c>
       <c r="G56">
-        <v>0.001715282420182874</v>
+        <v>0.001715282420184344</v>
       </c>
       <c r="H56">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I56">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -1862,22 +2033,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D57">
-        <v>4335720.507882103</v>
+        <v>4335720.507884094</v>
       </c>
       <c r="E57">
-        <v>286.5271575720374</v>
+        <v>286.5271575720569</v>
       </c>
       <c r="F57">
-        <v>13.42944220242173</v>
+        <v>13.42944220240865</v>
       </c>
       <c r="G57">
-        <v>0.001713714117878269</v>
+        <v>0.001713714117879739</v>
       </c>
       <c r="H57">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I57">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -1888,22 +2062,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D58">
-        <v>4334162.327377089</v>
+        <v>4334162.327379082</v>
       </c>
       <c r="E58">
-        <v>286.5118861262139</v>
+        <v>286.5118861262336</v>
       </c>
       <c r="F58">
-        <v>13.83033037548489</v>
+        <v>13.83033037547136</v>
       </c>
       <c r="G58">
-        <v>0.001712194880389476</v>
+        <v>0.001712194880390946</v>
       </c>
       <c r="H58">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I58">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -1914,22 +2091,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D59">
-        <v>4332527.75502286</v>
+        <v>4332527.755024857</v>
       </c>
       <c r="E59">
-        <v>286.4958615494914</v>
+        <v>286.4958615495109</v>
       </c>
       <c r="F59">
-        <v>14.254740866593</v>
+        <v>14.254740866579</v>
       </c>
       <c r="G59">
-        <v>0.001710727330397616</v>
+        <v>0.001710727330399093</v>
       </c>
       <c r="H59">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I59">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -1940,22 +2120,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D60">
-        <v>4330810.555620828</v>
+        <v>4330810.555622828</v>
       </c>
       <c r="E60">
-        <v>286.4790220494679</v>
+        <v>286.4790220494875</v>
       </c>
       <c r="F60">
-        <v>14.70482262693316</v>
+        <v>14.70482262691861</v>
       </c>
       <c r="G60">
-        <v>0.001709314198407353</v>
+        <v>0.001709314198408828</v>
       </c>
       <c r="H60">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I60">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -1966,22 +2149,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D61">
-        <v>4329003.762150983</v>
+        <v>4329003.762152988</v>
       </c>
       <c r="E61">
-        <v>286.4612985472088</v>
+        <v>286.4612985472286</v>
       </c>
       <c r="F61">
-        <v>15.18299741522497</v>
+        <v>15.18299741520985</v>
       </c>
       <c r="G61">
-        <v>0.001707958316823726</v>
+        <v>0.001707958316825201</v>
       </c>
       <c r="H61">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I61">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -1992,22 +2178,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D62">
-        <v>4327099.562028161</v>
+        <v>4327099.562030169</v>
       </c>
       <c r="E62">
-        <v>286.4426135397907</v>
+        <v>286.4426135398105</v>
       </c>
       <c r="F62">
-        <v>15.69200485474936</v>
+        <v>15.69200485473364</v>
       </c>
       <c r="G62">
-        <v>0.00170666261006087</v>
+        <v>0.001706662610062353</v>
       </c>
       <c r="H62">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I62">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -2018,22 +2207,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D63">
-        <v>4325089.16109598</v>
+        <v>4325089.161097992</v>
       </c>
       <c r="E63">
-        <v>286.422879739281</v>
+        <v>286.4228797393008</v>
       </c>
       <c r="F63">
-        <v>16.23495677412526</v>
+        <v>16.23495677410891</v>
       </c>
       <c r="G63">
-        <v>0.00170543007934816</v>
+        <v>0.001705430079349652</v>
       </c>
       <c r="H63">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I63">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -2044,22 +2236,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D64">
-        <v>4322962.620048434</v>
+        <v>4322962.620050452</v>
       </c>
       <c r="E64">
-        <v>286.4019984346125</v>
+        <v>286.4019984346322</v>
       </c>
       <c r="F64">
-        <v>16.81540315133203</v>
+        <v>16.81540315131503</v>
       </c>
       <c r="G64">
-        <v>0.001704263780462241</v>
+        <v>0.001704263780463736</v>
       </c>
       <c r="H64">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I64">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -2070,22 +2265,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D65">
-        <v>4320708.656460021</v>
+        <v>4320708.656462043</v>
       </c>
       <c r="E65">
-        <v>286.3798575075281</v>
+        <v>286.379857507548</v>
       </c>
       <c r="F65">
-        <v>17.43741266917859</v>
+        <v>17.43741266916085</v>
       </c>
       <c r="G65">
-        <v>0.001703166792022714</v>
+        <v>0.001703166792024211</v>
       </c>
       <c r="H65">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I65">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -2096,22 +2294,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D66">
-        <v>4318314.403593316</v>
+        <v>4318314.403595343</v>
       </c>
       <c r="E66">
-        <v>286.3563290133789</v>
+        <v>286.3563290133989</v>
       </c>
       <c r="F66">
-        <v>18.10567181857212</v>
+        <v>18.10567181855349</v>
       </c>
       <c r="G66">
-        <v>0.001702142171184506</v>
+        <v>0.001702142171186009</v>
       </c>
       <c r="H66">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I66">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -2122,22 +2323,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D67">
-        <v>4315765.11444411</v>
+        <v>4315765.114446143</v>
       </c>
       <c r="E67">
-        <v>286.3312662100712</v>
+        <v>286.3312662100912</v>
       </c>
       <c r="F67">
-        <v>18.82560774996692</v>
+        <v>18.82560774994738</v>
       </c>
       <c r="G67">
-        <v>0.001701192892455195</v>
+        <v>0.001701192892456706</v>
       </c>
       <c r="H67">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I67">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -2148,22 +2352,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D68">
-        <v>4313043.795798274</v>
+        <v>4313043.795800313</v>
       </c>
       <c r="E68">
-        <v>286.304499881019</v>
+        <v>286.304499881039</v>
       </c>
       <c r="F68">
-        <v>19.60354181428021</v>
+        <v>19.60354181425968</v>
       </c>
       <c r="G68">
-        <v>0.001700321763835517</v>
+        <v>0.00170032176383704</v>
       </c>
       <c r="H68">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I68">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -2174,22 +2381,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D69">
-        <v>4310130.752002115</v>
+        <v>4310130.752004162</v>
       </c>
       <c r="E69">
-        <v>286.27583374636</v>
+        <v>286.2758337463802</v>
       </c>
       <c r="F69">
-        <v>20.44688316145358</v>
+        <v>20.44688316143189</v>
       </c>
       <c r="G69">
-        <v>0.001699531312341948</v>
+        <v>0.001699531312343475</v>
       </c>
       <c r="H69">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I69">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -2200,22 +2410,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D70">
-        <v>4307003.011081595</v>
+        <v>4307003.011083649</v>
       </c>
       <c r="E70">
-        <v>286.245038684724</v>
+        <v>286.2450386847443</v>
       </c>
       <c r="F70">
-        <v>21.36437519256381</v>
+        <v>21.3643751925409</v>
       </c>
       <c r="G70">
-        <v>0.001698823627947093</v>
+        <v>0.001698823627948628</v>
       </c>
       <c r="H70">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I70">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -2226,22 +2439,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D71">
-        <v>4303633.595870976</v>
+        <v>4303633.595873037</v>
       </c>
       <c r="E71">
-        <v>286.9161296718924</v>
+        <v>286.9161296719123</v>
       </c>
       <c r="F71">
-        <v>22.36394514119429</v>
+        <v>22.3639451411611</v>
       </c>
       <c r="G71">
-        <v>0.001670370942140564</v>
+        <v>0.001670370942141989</v>
       </c>
       <c r="H71">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I71">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -2252,22 +2468,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D72">
-        <v>4299922.856894268</v>
+        <v>4299922.856896363</v>
       </c>
       <c r="E72">
-        <v>287.6097688875745</v>
+        <v>287.6097688875939</v>
       </c>
       <c r="F72">
-        <v>23.02145109070572</v>
+        <v>23.02145109067208</v>
       </c>
       <c r="G72">
-        <v>0.001643579191444813</v>
+        <v>0.001643579191446155</v>
       </c>
       <c r="H72">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I72">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -2278,22 +2497,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D73">
-        <v>4297079.746383652</v>
+        <v>4297079.746385753</v>
       </c>
       <c r="E73">
-        <v>288.325751218678</v>
+        <v>288.325751218697</v>
       </c>
       <c r="F73">
-        <v>23.66859676631845</v>
+        <v>23.66859676599317</v>
       </c>
       <c r="G73">
-        <v>0.00161836921907928</v>
+        <v>0.001618369219100476</v>
       </c>
       <c r="H73">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I73">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -2304,22 +2526,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D74">
-        <v>4294179.467432562</v>
+        <v>4294179.467435568</v>
       </c>
       <c r="E74">
-        <v>289.0632918455577</v>
+        <v>289.0632918455762</v>
       </c>
       <c r="F74">
-        <v>24.32081016359712</v>
+        <v>24.32081016204168</v>
       </c>
       <c r="G74">
-        <v>0.001594217838295722</v>
+        <v>0.001594217838396027</v>
       </c>
       <c r="H74">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I74">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -2330,22 +2555,25 @@
         <v>0.06349999999999997</v>
       </c>
       <c r="D75">
-        <v>4291176.201255948</v>
+        <v>4291176.201262874</v>
       </c>
       <c r="E75">
-        <v>289.8220406967703</v>
+        <v>289.822040696788</v>
       </c>
       <c r="F75">
-        <v>24.97902211172765</v>
+        <v>24.97902210891925</v>
       </c>
       <c r="G75">
-        <v>0.00157102823451052</v>
+        <v>0.001571028234682904</v>
       </c>
       <c r="H75">
-        <v>0.005975062616975481</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8">
+        <v>0.02189988709636259</v>
+      </c>
+      <c r="I75">
+        <v>0.005975062616975481</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -2356,22 +2584,25 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D76">
-        <v>4288064.985995948</v>
+        <v>4288064.986007183</v>
       </c>
       <c r="E76">
-        <v>290.6016559183944</v>
+        <v>290.6016559184096</v>
       </c>
       <c r="F76">
-        <v>25.64349404560835</v>
+        <v>25.64349404156227</v>
       </c>
       <c r="G76">
-        <v>0.001548729145823301</v>
+        <v>0.001548729146060706</v>
       </c>
       <c r="H76">
+        <v>0.0218998870963626</v>
+      </c>
+      <c r="I76">
         <v>0.005975062616975487</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:9">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -2382,22 +2613,25 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D77">
-        <v>4284842.680617458</v>
+        <v>4284842.68063328</v>
       </c>
       <c r="E77">
-        <v>291.401785602836</v>
+        <v>291.4017856028469</v>
       </c>
       <c r="F77">
-        <v>26.31445620236355</v>
+        <v>26.31445619709291</v>
       </c>
       <c r="G77">
-        <v>0.001527256807358545</v>
+        <v>0.001527256807654739</v>
       </c>
       <c r="H77">
+        <v>0.0218998870963626</v>
+      </c>
+      <c r="I77">
         <v>0.005975062616975487</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:9">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -2408,22 +2642,25 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D78">
-        <v>4281506.133331283</v>
+        <v>4281506.133351982</v>
       </c>
       <c r="E78">
-        <v>292.2220678446314</v>
+        <v>292.2220678446363</v>
       </c>
       <c r="F78">
-        <v>26.99213906768586</v>
+        <v>26.99213906120029</v>
       </c>
       <c r="G78">
-        <v>0.001506553363313357</v>
+        <v>0.001506553363662848</v>
       </c>
       <c r="H78">
+        <v>0.0218998870963626</v>
+      </c>
+      <c r="I78">
         <v>0.005975062616975487</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:9">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -2434,22 +2671,25 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D79">
-        <v>4278052.087462561</v>
+        <v>4278052.087488441</v>
       </c>
       <c r="E79">
-        <v>293.0621316674073</v>
+        <v>293.0621316674044</v>
       </c>
       <c r="F79">
-        <v>27.67677657238193</v>
+        <v>27.67677656468764</v>
       </c>
       <c r="G79">
-        <v>0.001486566113951195</v>
+        <v>0.001486566114349133</v>
       </c>
       <c r="H79">
+        <v>0.0218998870963626</v>
+      </c>
+      <c r="I79">
         <v>0.005975062616975487</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:9">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -2460,22 +2700,25 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D80">
-        <v>4274477.16864248</v>
+        <v>4274477.168673862</v>
       </c>
       <c r="E80">
-        <v>293.9215980235363</v>
+        <v>293.9215980235238</v>
       </c>
       <c r="F80">
-        <v>28.36860786399677</v>
+        <v>28.36860785509679</v>
       </c>
       <c r="G80">
-        <v>0.001467246899919296</v>
+        <v>0.001467246900361383</v>
       </c>
       <c r="H80">
+        <v>0.0218998870963626</v>
+      </c>
+      <c r="I80">
         <v>0.005975062616975487</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:9">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -2486,22 +2729,25 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D81">
-        <v>4270777.875391199</v>
+        <v>4270777.875428421</v>
       </c>
       <c r="E81">
-        <v>294.800080822896</v>
+        <v>294.8000808228722</v>
       </c>
       <c r="F81">
-        <v>29.06787888454368</v>
+        <v>29.06787887443823</v>
       </c>
       <c r="G81">
-        <v>0.001448551578555537</v>
+        <v>0.001448551579037949</v>
       </c>
       <c r="H81">
+        <v>0.0218998870963626</v>
+      </c>
+      <c r="I81">
         <v>0.005975062616975487</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:9">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -2512,22 +2758,25 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D82">
-        <v>4266950.569504418</v>
+        <v>4266950.569547836</v>
       </c>
       <c r="E82">
-        <v>295.6971879784436</v>
+        <v>295.6971879784066</v>
       </c>
       <c r="F82">
-        <v>29.77484381135711</v>
+        <v>29.77484382085884</v>
       </c>
       <c r="G82">
-        <v>0.00143043957664683</v>
+        <v>0.001430439576166159</v>
       </c>
       <c r="H82">
+        <v>0.0218998870963626</v>
+      </c>
+      <c r="I82">
         <v>0.005975062616975487</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:9">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -2538,22 +2787,25 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D83">
-        <v>4262991.466116594</v>
+        <v>4262991.466093731</v>
       </c>
       <c r="E83">
-        <v>296.6125224584019</v>
+        <v>296.6125224583499</v>
       </c>
       <c r="F83">
-        <v>30.48976650151139</v>
+        <v>30.48976651170543</v>
       </c>
       <c r="G83">
-        <v>0.001412873501341346</v>
+        <v>0.001412873500880299</v>
       </c>
       <c r="H83">
+        <v>0.0218998870963626</v>
+      </c>
+      <c r="I83">
         <v>0.005975062616975487</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:9">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -2564,22 +2816,25 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D84">
-        <v>4258896.622988237</v>
+        <v>4258896.622960641</v>
       </c>
       <c r="E84">
-        <v>297.5456833352644</v>
+        <v>297.5456833352188</v>
       </c>
       <c r="F84">
-        <v>31.21292165188228</v>
+        <v>31.21292166183678</v>
       </c>
       <c r="G84">
-        <v>0.001395818814041393</v>
+        <v>0.001395818813609843</v>
       </c>
       <c r="H84">
+        <v>0.0218998870963626</v>
+      </c>
+      <c r="I84">
         <v>0.005975062616975487</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:9">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -2590,22 +2845,25 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D85">
-        <v>4254661.930025212</v>
+        <v>4254661.929995999</v>
       </c>
       <c r="E85">
-        <v>298.4962668224942</v>
+        <v>298.4962668224563</v>
       </c>
       <c r="F85">
-        <v>31.94459608072658</v>
+        <v>31.94459609040981</v>
       </c>
       <c r="G85">
-        <v>0.001379243539139381</v>
+        <v>0.001379243538735515</v>
       </c>
       <c r="H85">
+        <v>0.0218998870963626</v>
+      </c>
+      <c r="I85">
         <v>0.005975062616975487</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:9">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -2616,22 +2874,25 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D86">
-        <v>4250283.097674962</v>
+        <v>4250283.097644281</v>
       </c>
       <c r="E86">
-        <v>299.4638672901369</v>
+        <v>299.4638672901071</v>
       </c>
       <c r="F86">
-        <v>32.68508985967521</v>
+        <v>32.68508986909981</v>
       </c>
       <c r="G86">
-        <v>0.001363118015403327</v>
+        <v>0.001363118015025007</v>
       </c>
       <c r="H86">
+        <v>0.0218998870963626</v>
+      </c>
+      <c r="I86">
         <v>0.005975062616975487</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:9">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -2642,22 +2903,25 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D87">
-        <v>4245755.645112409</v>
+        <v>4245755.64508026</v>
       </c>
       <c r="E87">
-        <v>300.4480782517883</v>
+        <v>300.4480782517668</v>
       </c>
       <c r="F87">
-        <v>33.43471741543139</v>
+        <v>33.4347174246114</v>
       </c>
       <c r="G87">
-        <v>0.001347414678428394</v>
+        <v>0.001347414678073661</v>
       </c>
       <c r="H87">
+        <v>0.0218998870963626</v>
+      </c>
+      <c r="I87">
         <v>0.005975062616975487</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:9">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -2668,22 +2932,25 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D88">
-        <v>4241074.887823214</v>
+        <v>4241074.887789587</v>
       </c>
       <c r="E88">
-        <v>301.4484933159262</v>
+        <v>301.4484933159133</v>
       </c>
       <c r="F88">
-        <v>34.1938085993923</v>
+        <v>34.19380860834079</v>
       </c>
       <c r="G88">
-        <v>0.001332107870254679</v>
+        <v>0.001332107869921761</v>
       </c>
       <c r="H88">
+        <v>0.0218998870963626</v>
+      </c>
+      <c r="I88">
         <v>0.005975062616975487</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:9">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -2694,22 +2961,25 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D89">
-        <v>4236235.924582827</v>
+        <v>4236235.924547716</v>
       </c>
       <c r="E89">
-        <v>302.4647070956676</v>
+        <v>302.4647070956636</v>
       </c>
       <c r="F89">
-        <v>34.96270973739635</v>
+        <v>34.96270974612561</v>
       </c>
       <c r="G89">
-        <v>0.001317173672113212</v>
+        <v>0.001317173671800503</v>
       </c>
       <c r="H89">
+        <v>0.0218998870963626</v>
+      </c>
+      <c r="I89">
         <v>0.005975062616975487</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:9">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -2720,22 +2990,25 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D90">
-        <v>4231233.623777163</v>
+        <v>4231233.62374056</v>
       </c>
       <c r="E90">
-        <v>303.4963160719607</v>
+        <v>303.4963160719658</v>
       </c>
       <c r="F90">
-        <v>35.74178467261875</v>
+        <v>35.74178468114025</v>
       </c>
       <c r="G90">
-        <v>0.001302589756899391</v>
+        <v>0.001302589756605431</v>
       </c>
       <c r="H90">
+        <v>0.0218998870963626</v>
+      </c>
+      <c r="I90">
         <v>0.005975062616975487</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:9">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -2746,22 +3019,25 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D91">
-        <v>4226062.60900035</v>
+        <v>4226062.608962249</v>
       </c>
       <c r="E91">
-        <v>304.5429194061869</v>
+        <v>304.5429194062013</v>
       </c>
       <c r="F91">
-        <v>36.53141581482861</v>
+        <v>36.53141582315298</v>
       </c>
       <c r="G91">
-        <v>0.001288335258510794</v>
+        <v>0.001288335258234255</v>
       </c>
       <c r="H91">
+        <v>0.0218998870963626</v>
+      </c>
+      <c r="I91">
         <v>0.005975062616975487</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:9">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -2772,22 +3048,25 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D92">
-        <v>4220717.243856466</v>
+        <v>4220717.24381686</v>
       </c>
       <c r="E92">
-        <v>305.6041196991026</v>
+        <v>305.6041196991266</v>
       </c>
       <c r="F92">
-        <v>37.33200520941668</v>
+        <v>37.33200521755409</v>
       </c>
       <c r="G92">
-        <v>0.001274390655635652</v>
+        <v>0.001274390655375321</v>
       </c>
       <c r="H92">
+        <v>0.0218998870963626</v>
+      </c>
+      <c r="I92">
         <v>0.005975062616975487</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:9">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -2798,18 +3077,21 @@
         <v>0.06349999999999999</v>
       </c>
       <c r="D93">
-        <v>4215191.615883186</v>
+        <v>4215191.615842067</v>
       </c>
       <c r="E93">
-        <v>306.6795236939586</v>
+        <v>306.6795236939923</v>
       </c>
       <c r="F93">
-        <v>38.14397563983406</v>
+        <v>38.14397564779402</v>
       </c>
       <c r="G93">
-        <v>0.001260737667954634</v>
+        <v>0.001260737667709403</v>
       </c>
       <c r="H93">
+        <v>0.0218998870963626</v>
+      </c>
+      <c r="I93">
         <v>0.005975062616975487</v>
       </c>
     </row>

</xml_diff>